<commit_message>
Add more Xlsx Data
</commit_message>
<xml_diff>
--- a/overall.xlsx
+++ b/overall.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="20385" windowHeight="8370"/>
+    <workbookView windowWidth="28695" windowHeight="13065"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19">
   <si>
     <t>model1</t>
   </si>
@@ -70,6 +70,9 @@
   </si>
   <si>
     <t>20_1_500</t>
+  </si>
+  <si>
+    <t>30_1_500</t>
   </si>
 </sst>
 </file>
@@ -77,9 +80,9 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="20">
@@ -92,36 +95,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color rgb="FFFF0000"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -144,7 +118,30 @@
     </font>
     <font>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color rgb="FF9C0006"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -158,62 +155,61 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
       <color rgb="FF3F3F3F"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -229,7 +225,14 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -250,43 +253,169 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -298,139 +427,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFC6EFCE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -441,6 +444,45 @@
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -462,17 +504,8 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -492,30 +525,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
       <top style="thin">
@@ -527,17 +536,11 @@
       <diagonal/>
     </border>
     <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -549,10 +552,10 @@
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="16" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -561,133 +564,133 @@
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="17" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="15" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="15" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="29" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="19" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="19" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="10" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -751,11 +754,6 @@
     <cellStyle name="60% - 强调文字颜色 6" xfId="48" builtinId="52"/>
   </cellStyles>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
@@ -1047,10 +1045,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr/>
-  <dimension ref="A1:J11"/>
+  <dimension ref="A1:J12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
@@ -1254,8 +1252,14 @@
       <c r="C7" s="1">
         <v>0.1865920008359</v>
       </c>
+      <c r="D7">
+        <v>0.378433577300206</v>
+      </c>
       <c r="E7">
         <v>0.132727784529924</v>
+      </c>
+      <c r="F7">
+        <v>0.0461624259826212</v>
       </c>
       <c r="G7">
         <v>0.0788806869391617</v>
@@ -1286,6 +1290,14 @@
       </c>
       <c r="G11">
         <v>0.0550438941415778</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7">
+      <c r="A12" t="s">
+        <v>18</v>
+      </c>
+      <c r="G12">
+        <v>0.0529699223097137</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
try to add all centrality operation in networkx
</commit_message>
<xml_diff>
--- a/overall.xlsx
+++ b/overall.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20">
   <si>
     <t>model1</t>
   </si>
@@ -43,6 +43,9 @@
   </si>
   <si>
     <t>Sum</t>
+  </si>
+  <si>
+    <t>17_07_06_01_01_31_0_1_500</t>
   </si>
   <si>
     <t>17_06_23_10_09_48_1_500_500</t>
@@ -1045,10 +1048,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr/>
-  <dimension ref="A1:J12"/>
+  <dimension ref="A1:J13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="J9" sqref="J9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
@@ -1092,32 +1095,32 @@
         <v>9</v>
       </c>
       <c r="B2">
-        <v>0.22547216918798</v>
+        <v>0.227858305734011</v>
       </c>
       <c r="C2">
-        <v>0.187971179460758</v>
+        <v>0.191372665244543</v>
       </c>
       <c r="D2">
-        <v>0.381244545954397</v>
+        <v>0.379406709533436</v>
       </c>
       <c r="E2">
-        <v>0.14354485128577</v>
+        <v>0.144618203673806</v>
       </c>
       <c r="F2">
-        <v>0.0525030742733086</v>
+        <v>0.0492559229829956</v>
       </c>
       <c r="G2">
-        <v>0.116477888329227</v>
+        <v>0.0689063882558996</v>
       </c>
       <c r="H2">
-        <v>0.112436622599709</v>
+        <v>0.110164559551915</v>
       </c>
       <c r="I2">
-        <v>0.108004071840423</v>
+        <v>0.0921915925927093</v>
       </c>
       <c r="J2">
-        <f t="shared" ref="J2:J6" si="0">SUM(B2:I2)</f>
-        <v>1.32765440293157</v>
+        <f>SUM(B2:I2)</f>
+        <v>1.26377434756932</v>
       </c>
     </row>
     <row r="3" spans="1:10">
@@ -1125,32 +1128,32 @@
         <v>10</v>
       </c>
       <c r="B3">
-        <v>0.224969857301882</v>
+        <v>0.22547216918798</v>
       </c>
       <c r="C3">
-        <v>0.187526913679589</v>
+        <v>0.187971179460758</v>
       </c>
       <c r="D3">
-        <v>0.378769838409116</v>
+        <v>0.381244545954397</v>
       </c>
       <c r="E3">
-        <v>0.132683877664982</v>
+        <v>0.14354485128577</v>
       </c>
       <c r="F3">
-        <v>0.0486031561140874</v>
+        <v>0.0525030742733086</v>
       </c>
       <c r="G3">
-        <v>0.0963747372803096</v>
+        <v>0.116477888329227</v>
       </c>
       <c r="H3">
-        <v>0.110157803486818</v>
+        <v>0.112436622599709</v>
       </c>
       <c r="I3">
-        <v>0.103127095633863</v>
+        <v>0.108004071840423</v>
       </c>
       <c r="J3">
-        <f t="shared" si="0"/>
-        <v>1.28221327957065</v>
+        <f t="shared" ref="J3:J7" si="0">SUM(B3:I3)</f>
+        <v>1.32765440293157</v>
       </c>
     </row>
     <row r="4" spans="1:10">
@@ -1158,88 +1161,88 @@
         <v>11</v>
       </c>
       <c r="B4">
-        <v>0.224198142615622</v>
+        <v>0.224969857301882</v>
       </c>
       <c r="C4">
-        <v>0.186939959056939</v>
+        <v>0.187526913679589</v>
       </c>
       <c r="D4">
-        <v>0.377817335096797</v>
+        <v>0.378769838409116</v>
       </c>
       <c r="E4">
-        <v>0.132004599476253</v>
+        <v>0.132683877664982</v>
       </c>
       <c r="F4">
         <v>0.0486031561140874</v>
       </c>
       <c r="G4">
-        <v>0.0963890777215438</v>
+        <v>0.0963747372803096</v>
       </c>
       <c r="H4">
-        <v>0.10916941910369</v>
+        <v>0.110157803486818</v>
       </c>
       <c r="I4">
-        <v>0.103775756745258</v>
+        <v>0.103127095633863</v>
       </c>
       <c r="J4">
         <f t="shared" si="0"/>
-        <v>1.27889744593019</v>
+        <v>1.28221327957065</v>
       </c>
     </row>
-    <row r="5" spans="1:9">
+    <row r="5" spans="1:10">
       <c r="A5" t="s">
         <v>12</v>
       </c>
-      <c r="B5" s="1">
-        <v>0.223945645080802</v>
+      <c r="B5">
+        <v>0.224198142615622</v>
       </c>
       <c r="C5">
-        <v>0.186709197985794</v>
-      </c>
-      <c r="D5" s="1">
-        <v>0.377672270137459</v>
-      </c>
-      <c r="E5" s="1">
-        <v>0.131740457119956</v>
+        <v>0.186939959056939</v>
+      </c>
+      <c r="D5">
+        <v>0.377817335096797</v>
+      </c>
+      <c r="E5">
+        <v>0.132004599476253</v>
+      </c>
+      <c r="F5">
+        <v>0.0486031561140874</v>
       </c>
       <c r="G5">
-        <v>0.0940710894739789</v>
+        <v>0.0963890777215438</v>
+      </c>
+      <c r="H5">
+        <v>0.10916941910369</v>
       </c>
       <c r="I5">
-        <v>0.0963690477597405</v>
+        <v>0.103775756745258</v>
+      </c>
+      <c r="J5">
+        <f t="shared" si="0"/>
+        <v>1.27889744593019</v>
       </c>
     </row>
-    <row r="6" spans="1:10">
+    <row r="6" spans="1:9">
       <c r="A6" t="s">
         <v>13</v>
       </c>
-      <c r="B6">
-        <v>0.224739363004351</v>
+      <c r="B6" s="1">
+        <v>0.223945645080802</v>
       </c>
       <c r="C6">
-        <v>0.187297215185024</v>
-      </c>
-      <c r="D6">
-        <v>0.379599876421476</v>
-      </c>
-      <c r="E6">
-        <v>0.133204469124497</v>
-      </c>
-      <c r="F6" s="1">
-        <v>0.0457840270181713</v>
+        <v>0.186709197985794</v>
+      </c>
+      <c r="D6" s="1">
+        <v>0.377672270137459</v>
+      </c>
+      <c r="E6" s="1">
+        <v>0.131740457119956</v>
       </c>
       <c r="G6">
-        <v>0.0855973956383197</v>
-      </c>
-      <c r="H6" s="1">
-        <v>0.10823914358667</v>
-      </c>
-      <c r="I6" s="1">
-        <v>0.0727882363083031</v>
-      </c>
-      <c r="J6">
-        <f t="shared" si="0"/>
-        <v>1.23724972628681</v>
+        <v>0.0940710894739789</v>
+      </c>
+      <c r="I6">
+        <v>0.0963690477597405</v>
       </c>
     </row>
     <row r="7" spans="1:10">
@@ -1247,56 +1250,81 @@
         <v>14</v>
       </c>
       <c r="B7">
+        <v>0.224739363004351</v>
+      </c>
+      <c r="C7">
+        <v>0.187297215185024</v>
+      </c>
+      <c r="D7">
+        <v>0.379599876421476</v>
+      </c>
+      <c r="E7">
+        <v>0.133204469124497</v>
+      </c>
+      <c r="F7" s="1">
+        <v>0.0457840270181713</v>
+      </c>
+      <c r="G7">
+        <v>0.0855973956383197</v>
+      </c>
+      <c r="H7" s="1">
+        <v>0.10823914358667</v>
+      </c>
+      <c r="I7" s="1">
+        <v>0.0727882363083031</v>
+      </c>
+      <c r="J7">
+        <f t="shared" si="0"/>
+        <v>1.23724972628681</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10">
+      <c r="A8" t="s">
+        <v>15</v>
+      </c>
+      <c r="B8">
         <v>0.223967412612399</v>
       </c>
-      <c r="C7" s="1">
+      <c r="C8" s="1">
         <v>0.1865920008359</v>
       </c>
-      <c r="D7">
+      <c r="D8">
         <v>0.378433577300206</v>
       </c>
-      <c r="E7">
+      <c r="E8">
         <v>0.132727784529924</v>
       </c>
-      <c r="F7">
+      <c r="F8">
         <v>0.0461624259826212</v>
       </c>
-      <c r="G7">
+      <c r="G8">
         <v>0.0788806869391617</v>
       </c>
-      <c r="H7">
+      <c r="H8">
         <v>0.109294166632193</v>
       </c>
-      <c r="I7">
+      <c r="I8">
         <v>0.0740594403788479</v>
       </c>
-      <c r="J7">
-        <f>SUM(B7:I7)</f>
+      <c r="J8">
+        <f>SUM(B8:I8)</f>
         <v>1.23011749521125</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7">
-      <c r="A9" t="s">
-        <v>15</v>
-      </c>
-      <c r="G9">
-        <v>0.0726150323207724</v>
       </c>
     </row>
     <row r="10" spans="1:7">
       <c r="A10" t="s">
         <v>16</v>
       </c>
-      <c r="G10" s="1">
-        <v>0.0629933219692992</v>
+      <c r="G10">
+        <v>0.0726150323207724</v>
       </c>
     </row>
     <row r="11" spans="1:7">
       <c r="A11" t="s">
         <v>17</v>
       </c>
-      <c r="G11">
-        <v>0.0550438941415778</v>
+      <c r="G11" s="1">
+        <v>0.0629933219692992</v>
       </c>
     </row>
     <row r="12" spans="1:7">
@@ -1304,6 +1332,14 @@
         <v>18</v>
       </c>
       <c r="G12">
+        <v>0.0550438941415778</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7">
+      <c r="A13" t="s">
+        <v>19</v>
+      </c>
+      <c r="G13">
         <v>0.0529699223097137</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Add non-reinsert casefor OpenSouce
</commit_message>
<xml_diff>
--- a/overall.xlsx
+++ b/overall.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="28695" windowHeight="13065"/>
+    <workbookView windowWidth="20385" windowHeight="8370"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25">
   <si>
     <t>model1</t>
   </si>
@@ -48,6 +48,9 @@
     <t>17_07_06_01_01_31_0_1_500</t>
   </si>
   <si>
+    <t>17_07_06_05_09_04_1_1_500</t>
+  </si>
+  <si>
     <t>17_06_23_10_09_48_1_500_500</t>
   </si>
   <si>
@@ -76,6 +79,18 @@
   </si>
   <si>
     <t>30_1_500</t>
+  </si>
+  <si>
+    <t>openSource_reinsert</t>
+  </si>
+  <si>
+    <t>17_07_07_23_04_06_1_1_500_1</t>
+  </si>
+  <si>
+    <t>openSource_noreinsert</t>
+  </si>
+  <si>
+    <t>1_1_500</t>
   </si>
 </sst>
 </file>
@@ -83,9 +98,9 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
   <fonts count="20">
@@ -98,6 +113,44 @@
     </font>
     <font>
       <sz val="11"/>
+      <color theme="0"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="宋体"/>
       <charset val="0"/>
@@ -106,7 +159,7 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
+      <color rgb="FF3F3F3F"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -127,16 +180,53 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
       <color theme="3"/>
       <name val="宋体"/>
       <charset val="134"/>
@@ -145,29 +235,7 @@
     <font>
       <u/>
       <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <color rgb="FF0000FF"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -181,67 +249,14 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
-  <fills count="34">
+  <fills count="35">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -250,25 +265,151 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -280,37 +421,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
+        <fgColor theme="4" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -322,13 +433,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
+        <fgColor theme="7" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -340,55 +445,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
+        <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -400,43 +457,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -447,30 +468,6 @@
       <right/>
       <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -489,17 +486,41 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
-        <color rgb="FFB2B2B2"/>
+        <color rgb="FF7F7F7F"/>
       </left>
       <right style="thin">
-        <color rgb="FFB2B2B2"/>
+        <color rgb="FF7F7F7F"/>
       </right>
       <top style="thin">
-        <color rgb="FFB2B2B2"/>
+        <color rgb="FF7F7F7F"/>
       </top>
       <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -525,16 +546,16 @@
     </border>
     <border>
       <left style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color rgb="FFB2B2B2"/>
       </left>
       <right style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color rgb="FFB2B2B2"/>
       </right>
       <top style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color rgb="FFB2B2B2"/>
       </top>
       <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color rgb="FFB2B2B2"/>
       </bottom>
       <diagonal/>
     </border>
@@ -555,10 +576,10 @@
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="24" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="15" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -567,141 +588,144 @@
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="31" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="10" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="10" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="19" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="16" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="15" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="15" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -757,6 +781,11 @@
     <cellStyle name="60% - 强调文字颜色 6" xfId="48" builtinId="52"/>
   </cellStyles>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -1048,10 +1077,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr/>
-  <dimension ref="A1:J13"/>
+  <dimension ref="A1:J26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J9" sqref="J9"/>
+      <selection activeCell="F25" sqref="F25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
@@ -1128,32 +1157,32 @@
         <v>10</v>
       </c>
       <c r="B3">
-        <v>0.22547216918798</v>
+        <v>0.225286283054075</v>
       </c>
       <c r="C3">
-        <v>0.187971179460758</v>
+        <v>0.187794520641569</v>
       </c>
       <c r="D3">
-        <v>0.381244545954397</v>
+        <v>0.380938188780155</v>
       </c>
       <c r="E3">
-        <v>0.14354485128577</v>
+        <v>0.143376574520423</v>
       </c>
       <c r="F3">
-        <v>0.0525030742733086</v>
-      </c>
-      <c r="G3">
-        <v>0.116477888329227</v>
+        <v>0.0522827100851127</v>
+      </c>
+      <c r="G3" s="1">
+        <v>0.106926203216301</v>
       </c>
       <c r="H3">
-        <v>0.112436622599709</v>
+        <v>0.111811531431783</v>
       </c>
       <c r="I3">
-        <v>0.108004071840423</v>
+        <v>0.102423416293936</v>
       </c>
       <c r="J3">
-        <f t="shared" ref="J3:J7" si="0">SUM(B3:I3)</f>
-        <v>1.32765440293157</v>
+        <f>SUM(B3:I3)</f>
+        <v>1.31083942802335</v>
       </c>
     </row>
     <row r="4" spans="1:10">
@@ -1161,32 +1190,32 @@
         <v>11</v>
       </c>
       <c r="B4">
-        <v>0.224969857301882</v>
+        <v>0.22547216918798</v>
       </c>
       <c r="C4">
-        <v>0.187526913679589</v>
+        <v>0.187971179460758</v>
       </c>
       <c r="D4">
-        <v>0.378769838409116</v>
+        <v>0.381244545954397</v>
       </c>
       <c r="E4">
-        <v>0.132683877664982</v>
+        <v>0.14354485128577</v>
       </c>
       <c r="F4">
-        <v>0.0486031561140874</v>
+        <v>0.0525030742733086</v>
       </c>
       <c r="G4">
-        <v>0.0963747372803096</v>
+        <v>0.116477888329227</v>
       </c>
       <c r="H4">
-        <v>0.110157803486818</v>
+        <v>0.112436622599709</v>
       </c>
       <c r="I4">
-        <v>0.103127095633863</v>
+        <v>0.108004071840423</v>
       </c>
       <c r="J4">
-        <f t="shared" si="0"/>
-        <v>1.28221327957065</v>
+        <f t="shared" ref="J4:J9" si="0">SUM(B4:I4)</f>
+        <v>1.32765440293157</v>
       </c>
     </row>
     <row r="5" spans="1:10">
@@ -1194,88 +1223,88 @@
         <v>12</v>
       </c>
       <c r="B5">
-        <v>0.224198142615622</v>
+        <v>0.224969857301882</v>
       </c>
       <c r="C5">
-        <v>0.186939959056939</v>
+        <v>0.187526913679589</v>
       </c>
       <c r="D5">
-        <v>0.377817335096797</v>
+        <v>0.378769838409116</v>
       </c>
       <c r="E5">
-        <v>0.132004599476253</v>
+        <v>0.132683877664982</v>
       </c>
       <c r="F5">
         <v>0.0486031561140874</v>
       </c>
       <c r="G5">
-        <v>0.0963890777215438</v>
+        <v>0.0963747372803096</v>
       </c>
       <c r="H5">
-        <v>0.10916941910369</v>
+        <v>0.110157803486818</v>
       </c>
       <c r="I5">
-        <v>0.103775756745258</v>
+        <v>0.103127095633863</v>
       </c>
       <c r="J5">
         <f t="shared" si="0"/>
-        <v>1.27889744593019</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9">
+        <v>1.28221327957065</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10">
       <c r="A6" t="s">
         <v>13</v>
       </c>
-      <c r="B6" s="1">
-        <v>0.223945645080802</v>
+      <c r="B6">
+        <v>0.224198142615622</v>
       </c>
       <c r="C6">
-        <v>0.186709197985794</v>
-      </c>
-      <c r="D6" s="1">
-        <v>0.377672270137459</v>
-      </c>
-      <c r="E6" s="1">
-        <v>0.131740457119956</v>
+        <v>0.186939959056939</v>
+      </c>
+      <c r="D6">
+        <v>0.377817335096797</v>
+      </c>
+      <c r="E6">
+        <v>0.132004599476253</v>
+      </c>
+      <c r="F6">
+        <v>0.0486031561140874</v>
       </c>
       <c r="G6">
-        <v>0.0940710894739789</v>
+        <v>0.0963890777215438</v>
+      </c>
+      <c r="H6">
+        <v>0.10916941910369</v>
       </c>
       <c r="I6">
-        <v>0.0963690477597405</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10">
+        <v>0.103775756745258</v>
+      </c>
+      <c r="J6">
+        <f t="shared" si="0"/>
+        <v>1.27889744593019</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9">
       <c r="A7" t="s">
         <v>14</v>
       </c>
-      <c r="B7">
-        <v>0.224739363004351</v>
+      <c r="B7" s="2">
+        <v>0.223945645080802</v>
       </c>
       <c r="C7">
-        <v>0.187297215185024</v>
-      </c>
-      <c r="D7">
-        <v>0.379599876421476</v>
-      </c>
-      <c r="E7">
-        <v>0.133204469124497</v>
-      </c>
-      <c r="F7" s="1">
-        <v>0.0457840270181713</v>
+        <v>0.186709197985794</v>
+      </c>
+      <c r="D7" s="2">
+        <v>0.377672270137459</v>
+      </c>
+      <c r="E7" s="2">
+        <v>0.131740457119956</v>
       </c>
       <c r="G7">
-        <v>0.0855973956383197</v>
-      </c>
-      <c r="H7" s="1">
-        <v>0.10823914358667</v>
-      </c>
-      <c r="I7" s="1">
-        <v>0.0727882363083031</v>
-      </c>
-      <c r="J7">
-        <f t="shared" si="0"/>
-        <v>1.23724972628681</v>
+        <v>0.0940710894739789</v>
+      </c>
+      <c r="I7">
+        <v>0.0963690477597405</v>
       </c>
     </row>
     <row r="8" spans="1:10">
@@ -1283,56 +1312,81 @@
         <v>15</v>
       </c>
       <c r="B8">
+        <v>0.224739363004351</v>
+      </c>
+      <c r="C8">
+        <v>0.187297215185024</v>
+      </c>
+      <c r="D8">
+        <v>0.379599876421476</v>
+      </c>
+      <c r="E8">
+        <v>0.133204469124497</v>
+      </c>
+      <c r="F8" s="2">
+        <v>0.0457840270181713</v>
+      </c>
+      <c r="G8">
+        <v>0.0855973956383197</v>
+      </c>
+      <c r="H8" s="2">
+        <v>0.10823914358667</v>
+      </c>
+      <c r="I8" s="2">
+        <v>0.0727882363083031</v>
+      </c>
+      <c r="J8">
+        <f t="shared" si="0"/>
+        <v>1.23724972628681</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10">
+      <c r="A9" t="s">
+        <v>16</v>
+      </c>
+      <c r="B9">
         <v>0.223967412612399</v>
       </c>
-      <c r="C8" s="1">
+      <c r="C9" s="2">
         <v>0.1865920008359</v>
       </c>
-      <c r="D8">
+      <c r="D9">
         <v>0.378433577300206</v>
       </c>
-      <c r="E8">
+      <c r="E9">
         <v>0.132727784529924</v>
       </c>
-      <c r="F8">
+      <c r="F9">
         <v>0.0461624259826212</v>
       </c>
-      <c r="G8">
+      <c r="G9">
         <v>0.0788806869391617</v>
       </c>
-      <c r="H8">
+      <c r="H9">
         <v>0.109294166632193</v>
       </c>
-      <c r="I8">
+      <c r="I9">
         <v>0.0740594403788479</v>
       </c>
-      <c r="J8">
-        <f>SUM(B8:I8)</f>
+      <c r="J9">
+        <f t="shared" si="0"/>
         <v>1.23011749521125</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7">
-      <c r="A10" t="s">
-        <v>16</v>
-      </c>
-      <c r="G10">
-        <v>0.0726150323207724</v>
       </c>
     </row>
     <row r="11" spans="1:7">
       <c r="A11" t="s">
         <v>17</v>
       </c>
-      <c r="G11" s="1">
-        <v>0.0629933219692992</v>
+      <c r="G11">
+        <v>0.0726150323207724</v>
       </c>
     </row>
     <row r="12" spans="1:7">
       <c r="A12" t="s">
         <v>18</v>
       </c>
-      <c r="G12">
-        <v>0.0550438941415778</v>
+      <c r="G12" s="2">
+        <v>0.0629933219692992</v>
       </c>
     </row>
     <row r="13" spans="1:7">
@@ -1340,7 +1394,66 @@
         <v>19</v>
       </c>
       <c r="G13">
+        <v>0.0550438941415778</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7">
+      <c r="A14" t="s">
+        <v>20</v>
+      </c>
+      <c r="G14">
         <v>0.0529699223097137</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1">
+      <c r="A18" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10">
+      <c r="A19" t="s">
+        <v>22</v>
+      </c>
+      <c r="B19" s="2">
+        <v>0.20800686430345</v>
+      </c>
+      <c r="C19" s="2">
+        <v>0.173239206962822</v>
+      </c>
+      <c r="D19" s="2">
+        <v>0.346041541710196</v>
+      </c>
+      <c r="E19" s="2">
+        <v>0.124928278882666</v>
+      </c>
+      <c r="F19" s="2">
+        <v>0.0409924383808026</v>
+      </c>
+      <c r="G19" s="2">
+        <v>0.0453003114127127</v>
+      </c>
+      <c r="H19" s="2">
+        <v>0.0964368086720679</v>
+      </c>
+      <c r="I19" s="2">
+        <v>0.065879029949852</v>
+      </c>
+      <c r="J19" s="2">
+        <f>SUM(B19:I19)</f>
+        <v>1.10082448027457</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1">
+      <c r="A25" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7">
+      <c r="A26" t="s">
+        <v>24</v>
+      </c>
+      <c r="G26" s="1">
+        <v>0.107332525566182</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
If method not in the list just exit
</commit_message>
<xml_diff>
--- a/overall.xlsx
+++ b/overall.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26">
   <si>
     <t>model1</t>
   </si>
@@ -82,6 +82,9 @@
   </si>
   <si>
     <t>openSource_reinsert</t>
+  </si>
+  <si>
+    <t>17_07_07_23_44_39_0_1_500_1</t>
   </si>
   <si>
     <t>17_07_07_23_04_06_1_1_500_1</t>
@@ -718,7 +721,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -726,6 +729,9 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -1077,10 +1083,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr/>
-  <dimension ref="A1:J26"/>
+  <dimension ref="A1:J27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F25" sqref="F25"/>
+      <selection activeCell="F22" sqref="F22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
@@ -1414,45 +1420,78 @@
       <c r="A19" t="s">
         <v>22</v>
       </c>
-      <c r="B19" s="2">
+      <c r="B19">
+        <v>0.212115440228391</v>
+      </c>
+      <c r="C19">
+        <v>0.177082696994985</v>
+      </c>
+      <c r="D19">
+        <v>0.348478583991745</v>
+      </c>
+      <c r="E19">
+        <v>0.128600159255576</v>
+      </c>
+      <c r="F19">
+        <v>0.0450454702134789</v>
+      </c>
+      <c r="G19">
+        <v>0.0896377651990727</v>
+      </c>
+      <c r="H19">
+        <v>0.102231876751721</v>
+      </c>
+      <c r="I19">
+        <v>0.0755164339928472</v>
+      </c>
+      <c r="J19" s="3">
+        <f>SUM(B19:I19)</f>
+        <v>1.17870842662782</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10">
+      <c r="A20" t="s">
+        <v>23</v>
+      </c>
+      <c r="B20" s="2">
         <v>0.20800686430345</v>
       </c>
-      <c r="C19" s="2">
+      <c r="C20" s="2">
         <v>0.173239206962822</v>
       </c>
-      <c r="D19" s="2">
+      <c r="D20" s="2">
         <v>0.346041541710196</v>
       </c>
-      <c r="E19" s="2">
+      <c r="E20" s="2">
         <v>0.124928278882666</v>
       </c>
-      <c r="F19" s="2">
+      <c r="F20" s="2">
         <v>0.0409924383808026</v>
       </c>
-      <c r="G19" s="2">
+      <c r="G20" s="2">
         <v>0.0453003114127127</v>
       </c>
-      <c r="H19" s="2">
+      <c r="H20" s="2">
         <v>0.0964368086720679</v>
       </c>
-      <c r="I19" s="2">
+      <c r="I20" s="2">
         <v>0.065879029949852</v>
       </c>
-      <c r="J19" s="2">
-        <f>SUM(B19:I19)</f>
+      <c r="J20" s="2">
+        <f>SUM(B20:I20)</f>
         <v>1.10082448027457</v>
       </c>
     </row>
-    <row r="25" spans="1:1">
-      <c r="A25" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7">
+    <row r="26" spans="1:1">
       <c r="A26" t="s">
         <v>24</v>
       </c>
-      <c r="G26" s="1">
+    </row>
+    <row r="27" spans="1:7">
+      <c r="A27" t="s">
+        <v>25</v>
+      </c>
+      <c r="G27" s="1">
         <v>0.107332525566182</v>
       </c>
     </row>

</xml_diff>

<commit_message>
add more statistic data
</commit_message>
<xml_diff>
--- a/overall.xlsx
+++ b/overall.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="20385" windowHeight="8370"/>
+    <workbookView windowWidth="28695" windowHeight="13065"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30">
   <si>
     <t>model1</t>
   </si>
@@ -90,13 +90,22 @@
     <t>17_07_07_23_04_06_1_1_500_1</t>
   </si>
   <si>
+    <t>17_07_08_00_31_54_2_1_500_1</t>
+  </si>
+  <si>
     <t>openSource_noreinsert</t>
   </si>
   <si>
+    <t>17_07_09_18_11_46_0_1_500_2</t>
+  </si>
+  <si>
+    <t>17_07_09_18_14_44_1_1_500_2</t>
+  </si>
+  <si>
+    <t>openSource_citm_noreinsert</t>
+  </si>
+  <si>
     <t>1_1_500</t>
-  </si>
-  <si>
-    <t>openSource_citm_noreinsert</t>
   </si>
 </sst>
 </file>
@@ -105,9 +114,9 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
     <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="20">
     <font>
@@ -119,9 +128,123 @@
     </font>
     <font>
       <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="宋体"/>
       <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -134,76 +257,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="0"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -216,51 +270,6 @@
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="35">
     <fill>
@@ -283,31 +292,145 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -319,151 +442,37 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -477,17 +486,11 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -503,50 +506,6 @@
       </top>
       <bottom style="thin">
         <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -574,6 +533,56 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
@@ -582,10 +591,10 @@
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="12" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -594,137 +603,137 @@
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="23" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="21" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="21" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="19" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="22" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -732,6 +741,9 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1">
@@ -790,11 +802,6 @@
     <cellStyle name="60% - 强调文字颜色 6" xfId="48" builtinId="52"/>
   </cellStyles>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
@@ -1088,8 +1095,8 @@
   <sheetPr/>
   <dimension ref="A1:J34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="A33" sqref="A33"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
@@ -1447,7 +1454,7 @@
       <c r="I19">
         <v>0.0755164339928472</v>
       </c>
-      <c r="J19" s="3">
+      <c r="J19" s="4">
         <f>SUM(B19:I19)</f>
         <v>1.17870842662782</v>
       </c>
@@ -1456,59 +1463,163 @@
       <c r="A20" t="s">
         <v>23</v>
       </c>
-      <c r="B20" s="2">
+      <c r="B20" s="3">
         <v>0.20800686430345</v>
       </c>
-      <c r="C20" s="2">
+      <c r="C20" s="3">
         <v>0.173239206962822</v>
       </c>
-      <c r="D20" s="2">
+      <c r="D20" s="3">
         <v>0.346041541710196</v>
       </c>
-      <c r="E20" s="2">
+      <c r="E20" s="3">
         <v>0.124928278882666</v>
       </c>
-      <c r="F20" s="2">
+      <c r="F20" s="3">
         <v>0.0409924383808026</v>
       </c>
-      <c r="G20" s="2">
+      <c r="G20" s="3">
         <v>0.0453003114127127</v>
       </c>
-      <c r="H20" s="2">
+      <c r="H20" s="3">
         <v>0.0964368086720679</v>
       </c>
-      <c r="I20" s="2">
+      <c r="I20" s="3">
         <v>0.065879029949852</v>
       </c>
-      <c r="J20" s="2">
+      <c r="J20" s="3">
         <f>SUM(B20:I20)</f>
         <v>1.10082448027457</v>
       </c>
     </row>
-    <row r="26" spans="1:1">
+    <row r="21" spans="1:10">
+      <c r="A21" t="s">
+        <v>24</v>
+      </c>
+      <c r="B21" s="2">
+        <v>0.207894527330402</v>
+      </c>
+      <c r="C21" s="2">
+        <v>0.173165858291852</v>
+      </c>
+      <c r="D21" s="2">
+        <v>0.344628020195683</v>
+      </c>
+      <c r="E21" s="2">
+        <v>0.118862297465155</v>
+      </c>
+      <c r="F21" s="2">
+        <v>0.0388983176119749</v>
+      </c>
+      <c r="G21" s="2">
+        <v>0.0422239303614074</v>
+      </c>
+      <c r="H21" s="2">
+        <v>0.0955131594160284</v>
+      </c>
+      <c r="I21" s="2">
+        <v>0.0488732287830458</v>
+      </c>
+      <c r="J21" s="2">
+        <f>SUM(B21:I21)</f>
+        <v>1.07005933945555</v>
+      </c>
+    </row>
+    <row r="22" spans="10:10">
+      <c r="J22" s="3"/>
+    </row>
+    <row r="23" spans="10:10">
+      <c r="J23" s="3"/>
+    </row>
+    <row r="24" spans="10:10">
+      <c r="J24" s="3"/>
+    </row>
+    <row r="25" spans="10:10">
+      <c r="J25" s="3"/>
+    </row>
+    <row r="26" spans="1:10">
       <c r="A26" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="27" spans="1:7">
+        <v>25</v>
+      </c>
+      <c r="J26" s="3"/>
+    </row>
+    <row r="27" spans="1:10">
       <c r="A27" t="s">
-        <v>25</v>
-      </c>
-      <c r="G27" s="1">
-        <v>0.107332525566182</v>
-      </c>
-    </row>
-    <row r="33" spans="1:7">
+        <v>26</v>
+      </c>
+      <c r="B27">
+        <v>0.228152205079095</v>
+      </c>
+      <c r="C27">
+        <v>0.191548875347098</v>
+      </c>
+      <c r="D27">
+        <v>0.379426065867224</v>
+      </c>
+      <c r="E27">
+        <v>0.143834806978518</v>
+      </c>
+      <c r="F27">
+        <v>0.0492015604703379</v>
+      </c>
+      <c r="G27" s="3">
+        <v>0.0766396493470802</v>
+      </c>
+      <c r="H27">
+        <v>0.110167879524473</v>
+      </c>
+      <c r="I27">
+        <v>0.0926905158740254</v>
+      </c>
+      <c r="J27" s="3">
+        <f>SUM(B27:I27)</f>
+        <v>1.27166155848785</v>
+      </c>
+    </row>
+    <row r="28" customFormat="1" spans="1:10">
+      <c r="A28" t="s">
+        <v>27</v>
+      </c>
+      <c r="B28">
+        <v>0.225357832225731</v>
+      </c>
+      <c r="C28">
+        <v>0.187832278626018</v>
+      </c>
+      <c r="D28">
+        <v>0.381070627327604</v>
+      </c>
+      <c r="E28">
+        <v>0.143343517352846</v>
+      </c>
+      <c r="F28">
+        <v>0.0533366743677525</v>
+      </c>
+      <c r="G28" s="1">
+        <v>0.110748101588701</v>
+      </c>
+      <c r="H28">
+        <v>0.111848633104288</v>
+      </c>
+      <c r="I28">
+        <v>0.103230203907768</v>
+      </c>
+      <c r="J28" s="3">
+        <f>SUM(B28:I28)</f>
+        <v>1.31676786850071</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1">
       <c r="A33" t="s">
-        <v>26</v>
-      </c>
-      <c r="G33">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7">
+      <c r="A34" t="s">
+        <v>29</v>
+      </c>
+      <c r="G34">
         <v>0.102480606902965</v>
-      </c>
-    </row>
-    <row r="34" spans="1:1">
-      <c r="A34" t="s">
-        <v>25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Improve Double and int in CITM , still not completed
</commit_message>
<xml_diff>
--- a/overall.xlsx
+++ b/overall.xlsx
@@ -140,10 +140,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="20">
     <font>
@@ -161,8 +161,85 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -183,46 +260,9 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -245,54 +285,14 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
+      <color rgb="FFFA7D00"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF006100"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -319,7 +319,133 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -331,7 +457,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
+        <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -343,73 +469,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFC6EFCE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
+        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
+        <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -421,85 +493,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
+        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -528,24 +528,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color rgb="FF7F7F7F"/>
       </left>
@@ -562,6 +544,30 @@
     </border>
     <border>
       <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
         <color rgb="FFB2B2B2"/>
       </left>
       <right style="thin">
@@ -572,30 +578,6 @@
       </top>
       <bottom style="thin">
         <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -625,6 +607,24 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
@@ -633,10 +633,10 @@
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="25" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="19" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -645,137 +645,137 @@
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="1" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="16" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="15" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="15" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="32" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="22" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -789,12 +789,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1250,7 +1244,7 @@
       <c r="F3">
         <v>0.0522827100851127</v>
       </c>
-      <c r="G3" s="9">
+      <c r="G3" s="7">
         <v>0.106926203216301</v>
       </c>
       <c r="H3">
@@ -1276,7 +1270,7 @@
       <c r="A12" t="s">
         <v>12</v>
       </c>
-      <c r="G12" s="10">
+      <c r="G12" s="8">
         <v>0.0629933219692992</v>
       </c>
     </row>
@@ -1329,7 +1323,7 @@
       <c r="I19">
         <v>0.0755164339928472</v>
       </c>
-      <c r="J19" s="11">
+      <c r="J19" s="9">
         <f t="shared" ref="J19:J21" si="0">SUM(B19:I19)</f>
         <v>1.17870842662782</v>
       </c>
@@ -1338,31 +1332,31 @@
       <c r="A20" t="s">
         <v>17</v>
       </c>
-      <c r="B20" s="11">
+      <c r="B20" s="9">
         <v>0.20800686430345</v>
       </c>
-      <c r="C20" s="11">
+      <c r="C20" s="9">
         <v>0.173239206962822</v>
       </c>
-      <c r="D20" s="11">
+      <c r="D20" s="9">
         <v>0.346041541710196</v>
       </c>
-      <c r="E20" s="11">
+      <c r="E20" s="9">
         <v>0.124928278882666</v>
       </c>
-      <c r="F20" s="11">
+      <c r="F20" s="9">
         <v>0.0409924383808026</v>
       </c>
-      <c r="G20" s="11">
+      <c r="G20" s="9">
         <v>0.0453003114127127</v>
       </c>
-      <c r="H20" s="11">
+      <c r="H20" s="9">
         <v>0.0964368086720679</v>
       </c>
-      <c r="I20" s="11">
+      <c r="I20" s="9">
         <v>0.065879029949852</v>
       </c>
-      <c r="J20" s="11">
+      <c r="J20" s="9">
         <f t="shared" si="0"/>
         <v>1.10082448027457</v>
       </c>
@@ -1371,52 +1365,52 @@
       <c r="A21" t="s">
         <v>18</v>
       </c>
-      <c r="B21" s="10">
+      <c r="B21" s="8">
         <v>0.207894527330402</v>
       </c>
-      <c r="C21" s="10">
+      <c r="C21" s="8">
         <v>0.173165858291852</v>
       </c>
-      <c r="D21" s="10">
+      <c r="D21" s="8">
         <v>0.344628020195683</v>
       </c>
-      <c r="E21" s="10">
+      <c r="E21" s="8">
         <v>0.118862297465155</v>
       </c>
-      <c r="F21" s="10">
+      <c r="F21" s="8">
         <v>0.0388983176119749</v>
       </c>
-      <c r="G21" s="10">
+      <c r="G21" s="8">
         <v>0.0422239303614074</v>
       </c>
-      <c r="H21" s="10">
+      <c r="H21" s="8">
         <v>0.0955131594160284</v>
       </c>
-      <c r="I21" s="10">
+      <c r="I21" s="8">
         <v>0.0488732287830458</v>
       </c>
-      <c r="J21" s="10">
+      <c r="J21" s="8">
         <f t="shared" si="0"/>
         <v>1.07005933945555</v>
       </c>
     </row>
     <row r="22" spans="10:10">
-      <c r="J22" s="11"/>
+      <c r="J22" s="9"/>
     </row>
     <row r="23" spans="10:10">
-      <c r="J23" s="11"/>
+      <c r="J23" s="9"/>
     </row>
     <row r="24" spans="10:10">
-      <c r="J24" s="11"/>
+      <c r="J24" s="9"/>
     </row>
     <row r="25" spans="10:10">
-      <c r="J25" s="11"/>
+      <c r="J25" s="9"/>
     </row>
     <row r="26" spans="1:10">
       <c r="A26" t="s">
         <v>19</v>
       </c>
-      <c r="J26" s="11"/>
+      <c r="J26" s="9"/>
     </row>
     <row r="27" spans="1:10">
       <c r="A27" t="s">
@@ -1437,7 +1431,7 @@
       <c r="F27">
         <v>0.0492015604703379</v>
       </c>
-      <c r="G27" s="11">
+      <c r="G27" s="9">
         <v>0.0766396493470802</v>
       </c>
       <c r="H27">
@@ -1446,7 +1440,7 @@
       <c r="I27">
         <v>0.0926905158740254</v>
       </c>
-      <c r="J27" s="11">
+      <c r="J27" s="9">
         <f>SUM(B27:I27)</f>
         <v>1.27166155848785</v>
       </c>
@@ -1470,7 +1464,7 @@
       <c r="F28">
         <v>0.0533366743677525</v>
       </c>
-      <c r="G28" s="9">
+      <c r="G28" s="7">
         <v>0.110748101588701</v>
       </c>
       <c r="H28">
@@ -1479,7 +1473,7 @@
       <c r="I28">
         <v>0.103230203907768</v>
       </c>
-      <c r="J28" s="11">
+      <c r="J28" s="9">
         <f>SUM(B28:I28)</f>
         <v>1.31676786850071</v>
       </c>
@@ -1509,8 +1503,8 @@
   <sheetPr/>
   <dimension ref="A1:J111"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A78" workbookViewId="0">
-      <selection activeCell="E109" sqref="E109"/>
+    <sheetView tabSelected="1" topLeftCell="A67" workbookViewId="0">
+      <selection activeCell="J98" sqref="J98"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
@@ -2059,16 +2053,16 @@
       <c r="A31" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="B31" s="6">
+      <c r="B31" s="5">
         <v>0.223945645080802</v>
       </c>
       <c r="C31" s="5">
         <v>0.186709197985794</v>
       </c>
-      <c r="D31" s="6">
+      <c r="D31" s="5">
         <v>0.377672270137459</v>
       </c>
-      <c r="E31" s="6">
+      <c r="E31" s="5">
         <v>0.131740457119956</v>
       </c>
       <c r="F31" s="5"/>
@@ -2085,10 +2079,10 @@
       <c r="A32" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="B32" s="6"/>
+      <c r="B32" s="5"/>
       <c r="C32" s="5"/>
-      <c r="D32" s="6"/>
-      <c r="E32" s="6"/>
+      <c r="D32" s="5"/>
+      <c r="E32" s="5"/>
       <c r="F32" s="5"/>
       <c r="G32" s="5"/>
       <c r="H32" s="5"/>
@@ -2139,16 +2133,16 @@
       <c r="E36" s="5">
         <v>0.133204469124497</v>
       </c>
-      <c r="F36" s="6">
+      <c r="F36" s="5">
         <v>0.0457840270181713</v>
       </c>
       <c r="G36" s="5">
         <v>0.0855973956383197</v>
       </c>
-      <c r="H36" s="6">
+      <c r="H36" s="5">
         <v>0.10823914358667</v>
       </c>
-      <c r="I36" s="6">
+      <c r="I36" s="5">
         <v>0.0727882363083031</v>
       </c>
       <c r="J36" s="5">
@@ -2164,10 +2158,10 @@
       <c r="C37" s="5"/>
       <c r="D37" s="5"/>
       <c r="E37" s="5"/>
-      <c r="F37" s="6"/>
+      <c r="F37" s="5"/>
       <c r="G37" s="5"/>
-      <c r="H37" s="6"/>
-      <c r="I37" s="6"/>
+      <c r="H37" s="5"/>
+      <c r="I37" s="5"/>
       <c r="J37" s="5"/>
     </row>
     <row r="38" spans="1:10">
@@ -2178,10 +2172,10 @@
       <c r="C38" s="5"/>
       <c r="D38" s="5"/>
       <c r="E38" s="5"/>
-      <c r="F38" s="6"/>
+      <c r="F38" s="5"/>
       <c r="G38" s="5"/>
-      <c r="H38" s="6"/>
-      <c r="I38" s="6"/>
+      <c r="H38" s="5"/>
+      <c r="I38" s="5"/>
       <c r="J38" s="5"/>
     </row>
     <row r="40" spans="1:10">
@@ -2205,7 +2199,7 @@
       <c r="B41" s="5">
         <v>0.223967412612399</v>
       </c>
-      <c r="C41" s="6">
+      <c r="C41" s="5">
         <v>0.1865920008359</v>
       </c>
       <c r="D41" s="5">
@@ -2239,10 +2233,10 @@
       <c r="C42" s="5"/>
       <c r="D42" s="5"/>
       <c r="E42" s="5"/>
-      <c r="F42" s="6"/>
+      <c r="F42" s="5"/>
       <c r="G42" s="5"/>
-      <c r="H42" s="6"/>
-      <c r="I42" s="6"/>
+      <c r="H42" s="5"/>
+      <c r="I42" s="5"/>
       <c r="J42" s="5"/>
     </row>
     <row r="43" spans="1:10">
@@ -2253,10 +2247,10 @@
       <c r="C43" s="5"/>
       <c r="D43" s="5"/>
       <c r="E43" s="5"/>
-      <c r="F43" s="6"/>
+      <c r="F43" s="5"/>
       <c r="G43" s="5"/>
-      <c r="H43" s="6"/>
-      <c r="I43" s="6"/>
+      <c r="H43" s="5"/>
+      <c r="I43" s="5"/>
       <c r="J43" s="5"/>
     </row>
     <row r="45" spans="1:10">
@@ -2280,7 +2274,7 @@
         <v>26</v>
       </c>
       <c r="B46" s="5"/>
-      <c r="C46" s="6"/>
+      <c r="C46" s="5"/>
       <c r="D46" s="5"/>
       <c r="E46" s="5"/>
       <c r="F46" s="5"/>
@@ -2297,10 +2291,10 @@
       <c r="C47" s="5"/>
       <c r="D47" s="5"/>
       <c r="E47" s="5"/>
-      <c r="F47" s="6"/>
+      <c r="F47" s="5"/>
       <c r="G47" s="5"/>
-      <c r="H47" s="6"/>
-      <c r="I47" s="6"/>
+      <c r="H47" s="5"/>
+      <c r="I47" s="5"/>
       <c r="J47" s="5"/>
     </row>
     <row r="48" spans="1:10">
@@ -2311,10 +2305,10 @@
       <c r="C48" s="5"/>
       <c r="D48" s="5"/>
       <c r="E48" s="5"/>
-      <c r="F48" s="6"/>
+      <c r="F48" s="5"/>
       <c r="G48" s="5"/>
-      <c r="H48" s="6"/>
-      <c r="I48" s="6"/>
+      <c r="H48" s="5"/>
+      <c r="I48" s="5"/>
       <c r="J48" s="5"/>
     </row>
     <row r="50" spans="1:10">
@@ -2326,7 +2320,7 @@
       <c r="D50" s="3"/>
       <c r="E50" s="3"/>
       <c r="F50" s="3"/>
-      <c r="G50" s="6">
+      <c r="G50" s="5">
         <v>0.0629933219692992</v>
       </c>
       <c r="H50" s="3"/>
@@ -2338,7 +2332,7 @@
         <v>26</v>
       </c>
       <c r="B51" s="5"/>
-      <c r="C51" s="6"/>
+      <c r="C51" s="5"/>
       <c r="D51" s="5"/>
       <c r="E51" s="5"/>
       <c r="F51" s="5"/>
@@ -2355,10 +2349,10 @@
       <c r="C52" s="5"/>
       <c r="D52" s="5"/>
       <c r="E52" s="5"/>
-      <c r="F52" s="6"/>
+      <c r="F52" s="5"/>
       <c r="G52" s="5"/>
-      <c r="H52" s="6"/>
-      <c r="I52" s="6"/>
+      <c r="H52" s="5"/>
+      <c r="I52" s="5"/>
       <c r="J52" s="5"/>
     </row>
     <row r="53" spans="1:10">
@@ -2369,10 +2363,10 @@
       <c r="C53" s="5"/>
       <c r="D53" s="5"/>
       <c r="E53" s="5"/>
-      <c r="F53" s="6"/>
+      <c r="F53" s="5"/>
       <c r="G53" s="5"/>
-      <c r="H53" s="6"/>
-      <c r="I53" s="6"/>
+      <c r="H53" s="5"/>
+      <c r="I53" s="5"/>
       <c r="J53" s="5"/>
     </row>
     <row r="55" spans="1:10">
@@ -2396,7 +2390,7 @@
         <v>26</v>
       </c>
       <c r="B56" s="5"/>
-      <c r="C56" s="6"/>
+      <c r="C56" s="5"/>
       <c r="D56" s="5"/>
       <c r="E56" s="5"/>
       <c r="F56" s="5"/>
@@ -2413,10 +2407,10 @@
       <c r="C57" s="5"/>
       <c r="D57" s="5"/>
       <c r="E57" s="5"/>
-      <c r="F57" s="6"/>
+      <c r="F57" s="5"/>
       <c r="G57" s="5"/>
-      <c r="H57" s="6"/>
-      <c r="I57" s="6"/>
+      <c r="H57" s="5"/>
+      <c r="I57" s="5"/>
       <c r="J57" s="5"/>
     </row>
     <row r="58" spans="1:10">
@@ -2427,10 +2421,10 @@
       <c r="C58" s="5"/>
       <c r="D58" s="5"/>
       <c r="E58" s="5"/>
-      <c r="F58" s="6"/>
+      <c r="F58" s="5"/>
       <c r="G58" s="5"/>
-      <c r="H58" s="6"/>
-      <c r="I58" s="6"/>
+      <c r="H58" s="5"/>
+      <c r="I58" s="5"/>
       <c r="J58" s="5"/>
     </row>
     <row r="60" spans="1:10">
@@ -2454,7 +2448,7 @@
         <v>26</v>
       </c>
       <c r="B61" s="5"/>
-      <c r="C61" s="6"/>
+      <c r="C61" s="5"/>
       <c r="D61" s="5"/>
       <c r="E61" s="5"/>
       <c r="F61" s="5"/>
@@ -2471,10 +2465,10 @@
       <c r="C62" s="5"/>
       <c r="D62" s="5"/>
       <c r="E62" s="5"/>
-      <c r="F62" s="6"/>
+      <c r="F62" s="5"/>
       <c r="G62" s="5"/>
-      <c r="H62" s="6"/>
-      <c r="I62" s="6"/>
+      <c r="H62" s="5"/>
+      <c r="I62" s="5"/>
       <c r="J62" s="5"/>
     </row>
     <row r="63" spans="1:10">
@@ -2485,10 +2479,10 @@
       <c r="C63" s="5"/>
       <c r="D63" s="5"/>
       <c r="E63" s="5"/>
-      <c r="F63" s="6"/>
+      <c r="F63" s="5"/>
       <c r="G63" s="5"/>
-      <c r="H63" s="6"/>
-      <c r="I63" s="6"/>
+      <c r="H63" s="5"/>
+      <c r="I63" s="5"/>
       <c r="J63" s="5"/>
     </row>
     <row r="67" spans="1:10">
@@ -2607,7 +2601,7 @@
       <c r="I72" s="3">
         <v>0.0755164339928472</v>
       </c>
-      <c r="J72" s="7">
+      <c r="J72" s="5">
         <f>SUM(B72:I72)</f>
         <v>1.17870842662782</v>
       </c>
@@ -2692,31 +2686,31 @@
       <c r="A77" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="B77" s="7">
+      <c r="B77" s="5">
         <v>0.20800686430345</v>
       </c>
-      <c r="C77" s="7">
+      <c r="C77" s="5">
         <v>0.173239206962822</v>
       </c>
-      <c r="D77" s="7">
+      <c r="D77" s="5">
         <v>0.346041541710196</v>
       </c>
-      <c r="E77" s="7">
+      <c r="E77" s="5">
         <v>0.124928278882666</v>
       </c>
-      <c r="F77" s="7">
+      <c r="F77" s="5">
         <v>0.0409924383808026</v>
       </c>
-      <c r="G77" s="7">
+      <c r="G77" s="5">
         <v>0.0453003114127127</v>
       </c>
-      <c r="H77" s="7">
+      <c r="H77" s="5">
         <v>0.0964368086720679</v>
       </c>
-      <c r="I77" s="7">
+      <c r="I77" s="5">
         <v>0.065879029949852</v>
       </c>
-      <c r="J77" s="7">
+      <c r="J77" s="5">
         <f>SUM(B77:I77)</f>
         <v>1.10082448027457</v>
       </c>
@@ -2813,31 +2807,31 @@
       <c r="A82" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="B82" s="8">
+      <c r="B82" s="6">
         <v>0.207894527330402</v>
       </c>
-      <c r="C82" s="8">
+      <c r="C82" s="6">
         <v>0.173165858291852</v>
       </c>
-      <c r="D82" s="8">
+      <c r="D82" s="6">
         <v>0.344628020195683</v>
       </c>
-      <c r="E82" s="8">
+      <c r="E82" s="6">
         <v>0.118862297465155</v>
       </c>
-      <c r="F82" s="8">
+      <c r="F82" s="6">
         <v>0.0388983176119749</v>
       </c>
-      <c r="G82" s="8">
+      <c r="G82" s="6">
         <v>0.0422239303614074</v>
       </c>
-      <c r="H82" s="8">
+      <c r="H82" s="6">
         <v>0.0955131594160284</v>
       </c>
-      <c r="I82" s="8">
+      <c r="I82" s="6">
         <v>0.0488732287830458</v>
       </c>
-      <c r="J82" s="8">
+      <c r="J82" s="6">
         <f>SUM(B82:I82)</f>
         <v>1.07005933945555</v>
       </c>
@@ -2951,7 +2945,7 @@
       <c r="F88" s="3">
         <v>0.0492015604703379</v>
       </c>
-      <c r="G88" s="7">
+      <c r="G88" s="5">
         <v>0.0766396493470802</v>
       </c>
       <c r="H88" s="3">
@@ -2960,7 +2954,7 @@
       <c r="I88" s="3">
         <v>0.0926905158740254</v>
       </c>
-      <c r="J88" s="7">
+      <c r="J88" s="5">
         <f>SUM(B88:I88)</f>
         <v>1.27166155848785</v>
       </c>
@@ -3069,7 +3063,7 @@
       <c r="I93" s="3">
         <v>0.103230203907768</v>
       </c>
-      <c r="J93" s="7">
+      <c r="J93" s="5">
         <f>SUM(B93:I93)</f>
         <v>1.31676786850071</v>
       </c>
@@ -3154,15 +3148,33 @@
       <c r="A98" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="B98" s="3"/>
-      <c r="C98" s="3"/>
-      <c r="D98" s="3"/>
-      <c r="E98" s="3"/>
-      <c r="F98" s="3"/>
-      <c r="G98" s="6"/>
-      <c r="H98" s="3"/>
-      <c r="I98" s="3"/>
-      <c r="J98" s="7"/>
+      <c r="B98" s="3">
+        <v>0.223944128917166</v>
+      </c>
+      <c r="C98" s="3">
+        <v>0.186722386746853</v>
+      </c>
+      <c r="D98" s="3">
+        <v>0.37770148730091</v>
+      </c>
+      <c r="E98" s="3">
+        <v>0.131732931754474</v>
+      </c>
+      <c r="F98" s="3">
+        <v>0.0490670980855947</v>
+      </c>
+      <c r="G98" s="5">
+        <v>0.0970503709159689</v>
+      </c>
+      <c r="H98" s="3">
+        <v>0.108574350654746</v>
+      </c>
+      <c r="I98" s="3">
+        <v>0.0965472395965962</v>
+      </c>
+      <c r="J98" s="5">
+        <v>1.27133999397231</v>
+      </c>
     </row>
     <row r="99" spans="1:10">
       <c r="A99" s="3" t="s">
@@ -3186,11 +3198,15 @@
       <c r="G99" s="3">
         <v>111</v>
       </c>
-      <c r="H99" s="3"/>
+      <c r="H99" s="3">
+        <v>148014</v>
+      </c>
       <c r="I99" s="3">
         <v>4635</v>
       </c>
-      <c r="J99" s="3"/>
+      <c r="J99" s="3">
+        <v>148014</v>
+      </c>
     </row>
     <row r="100" spans="1:10">
       <c r="A100" s="3" t="s">
@@ -3214,7 +3230,9 @@
       <c r="G100" s="3">
         <v>234841</v>
       </c>
-      <c r="H100" s="3"/>
+      <c r="H100" s="3">
+        <v>85281</v>
+      </c>
       <c r="I100" s="3">
         <v>171161</v>
       </c>
@@ -3255,10 +3273,10 @@
       <c r="D104" s="3"/>
       <c r="E104" s="3"/>
       <c r="F104" s="3"/>
-      <c r="G104" s="7"/>
+      <c r="G104" s="5"/>
       <c r="H104" s="3"/>
       <c r="I104" s="3"/>
-      <c r="J104" s="7"/>
+      <c r="J104" s="5"/>
     </row>
     <row r="105" spans="1:10">
       <c r="A105" s="3" t="s">
@@ -3316,7 +3334,7 @@
       </c>
       <c r="H109" s="3"/>
       <c r="I109" s="3"/>
-      <c r="J109" s="7"/>
+      <c r="J109" s="5"/>
     </row>
     <row r="110" spans="1:10">
       <c r="A110" s="3" t="s">

</xml_diff>

<commit_message>
1. Update more data 2. Start to code the concorrent in CI, not completed
</commit_message>
<xml_diff>
--- a/overall.xlsx
+++ b/overall.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40">
   <si>
     <t>model1</t>
   </si>
@@ -105,7 +105,7 @@
     <t>Min-Point</t>
   </si>
   <si>
-    <t>17_06_23_10_09_48_1_500_500</t>
+    <t>17_07_13_06_28_57_1_500_500_0</t>
   </si>
   <si>
     <t>17_06_28_02_58_04_2_2500_500</t>
@@ -117,13 +117,16 @@
     <t>17_07_12_07_26_07_2_1_500_0</t>
   </si>
   <si>
-    <t>17_06_25_09_58_41_3_2500_500</t>
-  </si>
-  <si>
-    <t>17_06_30_10_46_56_4_500_500</t>
+    <t>17_07_13_07_23_02_3_2500_500_0</t>
+  </si>
+  <si>
+    <t>17_07_13_10_20_51_4_500_500_0</t>
   </si>
   <si>
     <t>OpenSource_with_reinsert</t>
+  </si>
+  <si>
+    <t>30_1_500_reinsert</t>
   </si>
   <si>
     <t>OpenSource_without_reinsert</t>
@@ -913,7 +916,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -980,10 +983,28 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
@@ -1436,7 +1457,7 @@
       <c r="F3">
         <v>0.0522827100851127</v>
       </c>
-      <c r="G3" s="25">
+      <c r="G3" s="31">
         <v>0.106926203216301</v>
       </c>
       <c r="H3">
@@ -1462,7 +1483,7 @@
       <c r="A12" t="s">
         <v>12</v>
       </c>
-      <c r="G12" s="26">
+      <c r="G12" s="32">
         <v>0.0629933219692992</v>
       </c>
     </row>
@@ -1515,7 +1536,7 @@
       <c r="I19">
         <v>0.0755164339928472</v>
       </c>
-      <c r="J19" s="27">
+      <c r="J19" s="33">
         <f t="shared" ref="J19:J21" si="0">SUM(B19:I19)</f>
         <v>1.17870842662782</v>
       </c>
@@ -1524,31 +1545,31 @@
       <c r="A20" t="s">
         <v>17</v>
       </c>
-      <c r="B20" s="27">
+      <c r="B20" s="33">
         <v>0.20800686430345</v>
       </c>
-      <c r="C20" s="27">
+      <c r="C20" s="33">
         <v>0.173239206962822</v>
       </c>
-      <c r="D20" s="27">
+      <c r="D20" s="33">
         <v>0.346041541710196</v>
       </c>
-      <c r="E20" s="27">
+      <c r="E20" s="33">
         <v>0.124928278882666</v>
       </c>
-      <c r="F20" s="27">
+      <c r="F20" s="33">
         <v>0.0409924383808026</v>
       </c>
-      <c r="G20" s="27">
+      <c r="G20" s="33">
         <v>0.0453003114127127</v>
       </c>
-      <c r="H20" s="27">
+      <c r="H20" s="33">
         <v>0.0964368086720679</v>
       </c>
-      <c r="I20" s="27">
+      <c r="I20" s="33">
         <v>0.065879029949852</v>
       </c>
-      <c r="J20" s="27">
+      <c r="J20" s="33">
         <f t="shared" si="0"/>
         <v>1.10082448027457</v>
       </c>
@@ -1557,52 +1578,52 @@
       <c r="A21" t="s">
         <v>18</v>
       </c>
-      <c r="B21" s="26">
+      <c r="B21" s="32">
         <v>0.207894527330402</v>
       </c>
-      <c r="C21" s="26">
+      <c r="C21" s="32">
         <v>0.173165858291852</v>
       </c>
-      <c r="D21" s="26">
+      <c r="D21" s="32">
         <v>0.344628020195683</v>
       </c>
-      <c r="E21" s="26">
+      <c r="E21" s="32">
         <v>0.118862297465155</v>
       </c>
-      <c r="F21" s="26">
+      <c r="F21" s="32">
         <v>0.0388983176119749</v>
       </c>
-      <c r="G21" s="26">
+      <c r="G21" s="32">
         <v>0.0422239303614074</v>
       </c>
-      <c r="H21" s="26">
+      <c r="H21" s="32">
         <v>0.0955131594160284</v>
       </c>
-      <c r="I21" s="26">
+      <c r="I21" s="32">
         <v>0.0488732287830458</v>
       </c>
-      <c r="J21" s="26">
+      <c r="J21" s="32">
         <f t="shared" si="0"/>
         <v>1.07005933945555</v>
       </c>
     </row>
     <row r="22" spans="10:10">
-      <c r="J22" s="27"/>
+      <c r="J22" s="33"/>
     </row>
     <row r="23" spans="10:10">
-      <c r="J23" s="27"/>
+      <c r="J23" s="33"/>
     </row>
     <row r="24" spans="10:10">
-      <c r="J24" s="27"/>
+      <c r="J24" s="33"/>
     </row>
     <row r="25" spans="10:10">
-      <c r="J25" s="27"/>
+      <c r="J25" s="33"/>
     </row>
     <row r="26" spans="1:10">
       <c r="A26" t="s">
         <v>19</v>
       </c>
-      <c r="J26" s="27"/>
+      <c r="J26" s="33"/>
     </row>
     <row r="27" spans="1:10">
       <c r="A27" t="s">
@@ -1623,7 +1644,7 @@
       <c r="F27">
         <v>0.0492015604703379</v>
       </c>
-      <c r="G27" s="27">
+      <c r="G27" s="33">
         <v>0.0766396493470802</v>
       </c>
       <c r="H27">
@@ -1632,7 +1653,7 @@
       <c r="I27">
         <v>0.0926905158740254</v>
       </c>
-      <c r="J27" s="27">
+      <c r="J27" s="33">
         <f>SUM(B27:I27)</f>
         <v>1.27166155848785</v>
       </c>
@@ -1656,7 +1677,7 @@
       <c r="F28">
         <v>0.0533366743677525</v>
       </c>
-      <c r="G28" s="25">
+      <c r="G28" s="31">
         <v>0.110748101588701</v>
       </c>
       <c r="H28">
@@ -1665,7 +1686,7 @@
       <c r="I28">
         <v>0.103230203907768</v>
       </c>
-      <c r="J28" s="27">
+      <c r="J28" s="33">
         <f>SUM(B28:I28)</f>
         <v>1.31676786850071</v>
       </c>
@@ -1693,10 +1714,10 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr/>
-  <dimension ref="A1:J111"/>
+  <dimension ref="A1:J116"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E19" sqref="E19"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="J36" sqref="J36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
@@ -2028,60 +2049,94 @@
         <v>26</v>
       </c>
       <c r="B16" s="10">
-        <v>0.22547216918798</v>
+        <v>0.225470908622326</v>
       </c>
       <c r="C16" s="10">
-        <v>0.187971179460758</v>
+        <v>0.187969567075629</v>
       </c>
       <c r="D16" s="10">
-        <v>0.381244545954397</v>
+        <v>0.381243807789244</v>
       </c>
       <c r="E16" s="10">
-        <v>0.14354485128577</v>
+        <v>0.143543120492896</v>
       </c>
       <c r="F16" s="10">
-        <v>0.0525030742733086</v>
+        <v>0.0524463942386956</v>
       </c>
       <c r="G16" s="10">
-        <v>0.116477888329227</v>
+        <v>0.116477647084075</v>
       </c>
       <c r="H16" s="10">
-        <v>0.112436622599709</v>
+        <v>0.11241776384841</v>
       </c>
       <c r="I16" s="10">
-        <v>0.108004071840423</v>
-      </c>
-      <c r="J16" s="17">
+        <v>0.107949060989036</v>
+      </c>
+      <c r="J16" s="15">
         <f>SUM(B16:I16)</f>
-        <v>1.32765440293157</v>
+        <v>1.32751827014031</v>
       </c>
     </row>
     <row r="17" s="1" customFormat="1" spans="1:10">
       <c r="A17" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="B17" s="10"/>
-      <c r="C17" s="10"/>
-      <c r="D17" s="10"/>
-      <c r="E17" s="10"/>
-      <c r="F17" s="10"/>
-      <c r="G17" s="10"/>
-      <c r="H17" s="10"/>
-      <c r="I17" s="10"/>
-      <c r="J17" s="17"/>
+      <c r="B17" s="10">
+        <v>246</v>
+      </c>
+      <c r="C17" s="10">
+        <v>205</v>
+      </c>
+      <c r="D17" s="10">
+        <v>281</v>
+      </c>
+      <c r="E17" s="10">
+        <v>163</v>
+      </c>
+      <c r="F17" s="10">
+        <v>274</v>
+      </c>
+      <c r="G17" s="10">
+        <v>52</v>
+      </c>
+      <c r="H17" s="10">
+        <v>212</v>
+      </c>
+      <c r="I17" s="10">
+        <v>152</v>
+      </c>
+      <c r="J17" s="17">
+        <v>281</v>
+      </c>
     </row>
     <row r="18" s="1" customFormat="1" spans="1:10">
       <c r="A18" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="B18" s="10"/>
-      <c r="C18" s="10"/>
-      <c r="D18" s="10"/>
-      <c r="E18" s="10"/>
-      <c r="F18" s="10"/>
-      <c r="G18" s="10"/>
-      <c r="H18" s="10"/>
-      <c r="I18" s="10"/>
+      <c r="B18" s="10">
+        <v>676544</v>
+      </c>
+      <c r="C18" s="10">
+        <v>678602</v>
+      </c>
+      <c r="D18" s="10">
+        <v>780097</v>
+      </c>
+      <c r="E18" s="10">
+        <v>632598</v>
+      </c>
+      <c r="F18" s="10">
+        <v>733500</v>
+      </c>
+      <c r="G18" s="10">
+        <v>1632272</v>
+      </c>
+      <c r="H18" s="10">
+        <v>190579</v>
+      </c>
+      <c r="I18" s="10">
+        <v>421334</v>
+      </c>
       <c r="J18" s="17"/>
     </row>
     <row r="19" s="1" customFormat="1" spans="1:10">
@@ -2092,61 +2147,95 @@
       <c r="A20" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="B20" s="10"/>
-      <c r="C20" s="10"/>
-      <c r="D20" s="10"/>
-      <c r="E20" s="10"/>
-      <c r="F20" s="10"/>
-      <c r="G20" s="10"/>
-      <c r="H20" s="10"/>
-      <c r="I20" s="10"/>
-      <c r="J20" s="17"/>
+      <c r="B20" s="10">
+        <v>0.22496788201061</v>
+      </c>
+      <c r="C20" s="10">
+        <v>0.187524905369721</v>
+      </c>
+      <c r="D20" s="10">
+        <v>0.378768597488832</v>
+      </c>
+      <c r="E20" s="10">
+        <v>0.13268127642868</v>
+      </c>
+      <c r="F20" s="10">
+        <v>0.0485509130381507</v>
+      </c>
+      <c r="G20" s="10">
+        <v>0.0963740326795437</v>
+      </c>
+      <c r="H20" s="10">
+        <v>0.110138053342448</v>
+      </c>
+      <c r="I20" s="10">
+        <v>0.103029977777207</v>
+      </c>
+      <c r="J20" s="17">
+        <f>SUM(B20:I20)</f>
+        <v>1.28203563813519</v>
+      </c>
     </row>
     <row r="21" s="1" customFormat="1" spans="1:10">
       <c r="A21" s="5" t="s">
         <v>26</v>
       </c>
       <c r="B21" s="10">
-        <v>0.224969857301882</v>
+        <v>661</v>
       </c>
       <c r="C21" s="10">
-        <v>0.187526913679589</v>
+        <v>496</v>
       </c>
       <c r="D21" s="10">
-        <v>0.378769838409116</v>
+        <v>1058</v>
       </c>
       <c r="E21" s="10">
-        <v>0.132683877664982</v>
+        <v>328</v>
       </c>
       <c r="F21" s="10">
-        <v>0.0486031561140874</v>
+        <v>856</v>
       </c>
       <c r="G21" s="10">
-        <v>0.0963747372803096</v>
+        <v>72</v>
       </c>
       <c r="H21" s="10">
-        <v>0.110157803486818</v>
+        <v>923</v>
       </c>
       <c r="I21" s="10">
-        <v>0.103127095633863</v>
+        <v>335</v>
       </c>
       <c r="J21" s="17">
-        <f>SUM(B21:I21)</f>
-        <v>1.28221327957065</v>
+        <v>1058</v>
       </c>
     </row>
     <row r="22" s="1" customFormat="1" spans="1:10">
       <c r="A22" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="B22" s="10"/>
-      <c r="C22" s="10"/>
-      <c r="D22" s="10"/>
-      <c r="E22" s="10"/>
-      <c r="F22" s="10"/>
-      <c r="G22" s="10"/>
-      <c r="H22" s="10"/>
-      <c r="I22" s="10"/>
+      <c r="B22" s="10">
+        <v>682954</v>
+      </c>
+      <c r="C22" s="10">
+        <v>691497</v>
+      </c>
+      <c r="D22" s="10">
+        <v>772314</v>
+      </c>
+      <c r="E22" s="10">
+        <v>687672</v>
+      </c>
+      <c r="F22" s="10">
+        <v>754610</v>
+      </c>
+      <c r="G22" s="10">
+        <v>1548385</v>
+      </c>
+      <c r="H22" s="10">
+        <v>187357</v>
+      </c>
+      <c r="I22" s="10">
+        <v>500491</v>
+      </c>
       <c r="J22" s="17"/>
     </row>
     <row r="23" s="1" customFormat="1" spans="1:10">
@@ -2186,60 +2275,92 @@
         <v>26</v>
       </c>
       <c r="B26" s="10">
-        <v>0.224198142615622</v>
+        <v>0.224196133336137</v>
       </c>
       <c r="C26" s="10">
-        <v>0.186939959056939</v>
+        <v>0.186937903287681</v>
       </c>
       <c r="D26" s="10">
-        <v>0.377817335096797</v>
-      </c>
-      <c r="E26" s="10">
-        <v>0.132004599476253</v>
+        <v>0.377815991293198</v>
+      </c>
+      <c r="E26" s="2">
+        <v>0.132001795806194</v>
       </c>
       <c r="F26" s="10">
-        <v>0.0486031561140874</v>
+        <v>0.0484972658475219</v>
       </c>
       <c r="G26" s="10">
-        <v>0.0963890777215438</v>
+        <v>0.0963883732701269</v>
       </c>
       <c r="H26" s="10">
-        <v>0.10916941910369</v>
+        <v>0.109148965031763</v>
       </c>
       <c r="I26" s="10">
-        <v>0.103775756745258</v>
+        <v>0.103639895551926</v>
       </c>
       <c r="J26" s="17">
         <f>SUM(B26:I26)</f>
-        <v>1.27889744593019</v>
+        <v>1.27862632342455</v>
       </c>
     </row>
     <row r="27" spans="1:10">
       <c r="A27" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="B27" s="10"/>
-      <c r="C27" s="10"/>
-      <c r="D27" s="10"/>
-      <c r="E27" s="10"/>
-      <c r="F27" s="10"/>
-      <c r="G27" s="10"/>
-      <c r="H27" s="10"/>
-      <c r="I27" s="10"/>
+      <c r="B27" s="10">
+        <v>1239</v>
+      </c>
+      <c r="C27" s="10">
+        <v>835</v>
+      </c>
+      <c r="D27" s="10">
+        <v>1883</v>
+      </c>
+      <c r="E27" s="10">
+        <v>485</v>
+      </c>
+      <c r="F27" s="10">
+        <v>1410</v>
+      </c>
+      <c r="G27" s="10">
+        <v>75</v>
+      </c>
+      <c r="H27" s="10">
+        <v>1332</v>
+      </c>
+      <c r="I27" s="10">
+        <v>488</v>
+      </c>
       <c r="J27" s="17"/>
     </row>
     <row r="28" spans="1:10">
       <c r="A28" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="B28" s="6"/>
-      <c r="C28" s="6"/>
-      <c r="D28" s="6"/>
-      <c r="E28" s="6"/>
-      <c r="F28" s="6"/>
-      <c r="G28" s="6"/>
-      <c r="H28" s="6"/>
-      <c r="I28" s="6"/>
+      <c r="B28" s="6">
+        <v>685552</v>
+      </c>
+      <c r="C28" s="6">
+        <v>694100</v>
+      </c>
+      <c r="D28" s="6">
+        <v>772502</v>
+      </c>
+      <c r="E28" s="10">
+        <v>690048</v>
+      </c>
+      <c r="F28" s="6">
+        <v>763537</v>
+      </c>
+      <c r="G28" s="6">
+        <v>1547683</v>
+      </c>
+      <c r="H28" s="6">
+        <v>189000</v>
+      </c>
+      <c r="I28" s="6">
+        <v>505491</v>
+      </c>
       <c r="J28" s="17"/>
     </row>
     <row r="29" spans="1:10">
@@ -2378,60 +2499,92 @@
         <v>26</v>
       </c>
       <c r="B36" s="10">
-        <v>0.224739363004351</v>
+        <v>0.224736691876997</v>
       </c>
       <c r="C36" s="10">
-        <v>0.187297215185024</v>
+        <v>0.187294567106436</v>
       </c>
       <c r="D36" s="10">
-        <v>0.379599876421476</v>
+        <v>0.379598329129886</v>
       </c>
       <c r="E36" s="10">
-        <v>0.133204469124497</v>
+        <v>0.133199928177059</v>
       </c>
       <c r="F36" s="10">
-        <v>0.0457840270181713</v>
+        <v>0.0457097264452359</v>
       </c>
       <c r="G36" s="10">
-        <v>0.0855973956383197</v>
+        <v>0.0855964570603726</v>
       </c>
       <c r="H36" s="10">
-        <v>0.10823914358667</v>
+        <v>0.108191476936675</v>
       </c>
       <c r="I36" s="10">
-        <v>0.0727882363083031</v>
+        <v>0.0725702160635175</v>
       </c>
       <c r="J36" s="17">
         <f>SUM(B36:I36)</f>
-        <v>1.23724972628681</v>
+        <v>1.23689739279618</v>
       </c>
     </row>
     <row r="37" spans="1:10">
       <c r="A37" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="B37" s="10"/>
-      <c r="C37" s="10"/>
-      <c r="D37" s="10"/>
-      <c r="E37" s="10"/>
-      <c r="F37" s="10"/>
-      <c r="G37" s="10"/>
-      <c r="H37" s="10"/>
-      <c r="I37" s="10"/>
+      <c r="B37" s="10">
+        <v>3171</v>
+      </c>
+      <c r="C37" s="10">
+        <v>1921</v>
+      </c>
+      <c r="D37" s="10">
+        <v>6153</v>
+      </c>
+      <c r="E37" s="10">
+        <v>1233</v>
+      </c>
+      <c r="F37" s="10">
+        <v>7581</v>
+      </c>
+      <c r="G37" s="10">
+        <v>103</v>
+      </c>
+      <c r="H37" s="10">
+        <v>10661</v>
+      </c>
+      <c r="I37" s="10">
+        <v>1797</v>
+      </c>
       <c r="J37" s="17"/>
     </row>
     <row r="38" spans="1:10">
       <c r="A38" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="B38" s="10"/>
-      <c r="C38" s="10"/>
-      <c r="D38" s="10"/>
-      <c r="E38" s="10"/>
-      <c r="F38" s="10"/>
-      <c r="G38" s="10"/>
-      <c r="H38" s="10"/>
-      <c r="I38" s="10"/>
+      <c r="B38" s="10">
+        <v>687917</v>
+      </c>
+      <c r="C38" s="10">
+        <v>698622</v>
+      </c>
+      <c r="D38" s="10">
+        <v>778644</v>
+      </c>
+      <c r="E38" s="10">
+        <v>707502</v>
+      </c>
+      <c r="F38" s="10">
+        <v>845276</v>
+      </c>
+      <c r="G38" s="10">
+        <v>1624434</v>
+      </c>
+      <c r="H38" s="10">
+        <v>198638</v>
+      </c>
+      <c r="I38" s="10">
+        <v>480276</v>
+      </c>
       <c r="J38" s="17"/>
     </row>
     <row r="39" spans="1:10">
@@ -2456,47 +2609,36 @@
       <c r="A41" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="B41" s="10">
-        <v>0.223967412612399</v>
-      </c>
-      <c r="C41" s="10">
-        <v>0.1865920008359</v>
-      </c>
-      <c r="D41" s="10">
-        <v>0.378433577300206</v>
-      </c>
-      <c r="E41" s="10">
-        <v>0.132727784529924</v>
-      </c>
-      <c r="F41" s="10">
-        <v>0.0461624259826212</v>
-      </c>
-      <c r="G41" s="10">
-        <v>0.0788806869391617</v>
-      </c>
-      <c r="H41" s="10">
-        <v>0.109294166632193</v>
-      </c>
-      <c r="I41" s="10">
-        <v>0.0740594403788479</v>
-      </c>
-      <c r="J41" s="17">
-        <f>SUM(B41:I41)</f>
-        <v>1.23011749521125</v>
-      </c>
+      <c r="B41" s="10"/>
+      <c r="C41" s="10"/>
+      <c r="D41" s="10"/>
+      <c r="E41" s="10"/>
+      <c r="F41" s="10"/>
+      <c r="G41" s="10"/>
+      <c r="H41" s="10"/>
+      <c r="I41" s="10"/>
+      <c r="J41" s="17"/>
     </row>
     <row r="42" spans="1:10">
       <c r="A42" s="5" t="s">
         <v>27</v>
       </c>
       <c r="B42" s="10"/>
-      <c r="C42" s="10"/>
+      <c r="C42" s="10">
+        <v>26950</v>
+      </c>
       <c r="D42" s="10"/>
-      <c r="E42" s="10"/>
+      <c r="E42" s="10">
+        <v>13105</v>
+      </c>
       <c r="F42" s="10"/>
-      <c r="G42" s="10"/>
+      <c r="G42" s="10">
+        <v>138</v>
+      </c>
       <c r="H42" s="10"/>
-      <c r="I42" s="10"/>
+      <c r="I42" s="10">
+        <v>15231</v>
+      </c>
       <c r="J42" s="17"/>
     </row>
     <row r="43" spans="1:10">
@@ -2504,13 +2646,21 @@
         <v>28</v>
       </c>
       <c r="B43" s="10"/>
-      <c r="C43" s="10"/>
+      <c r="C43" s="10">
+        <v>699969</v>
+      </c>
       <c r="D43" s="10"/>
-      <c r="E43" s="10"/>
+      <c r="E43" s="10">
+        <v>704981</v>
+      </c>
       <c r="F43" s="10"/>
-      <c r="G43" s="10"/>
+      <c r="G43" s="10">
+        <v>1631177</v>
+      </c>
       <c r="H43" s="10"/>
-      <c r="I43" s="10"/>
+      <c r="I43" s="10">
+        <v>481500</v>
+      </c>
       <c r="J43" s="17"/>
     </row>
     <row r="44" spans="1:10">
@@ -3116,7 +3266,7 @@
       <c r="I82" s="21">
         <v>0.0488732287830458</v>
       </c>
-      <c r="J82" s="23">
+      <c r="J82" s="26">
         <f>SUM(B82:I82)</f>
         <v>1.07005933945555</v>
       </c>
@@ -3153,167 +3303,120 @@
         <v>149985</v>
       </c>
     </row>
-    <row r="84" ht="14.25" spans="1:10">
-      <c r="A84" s="12" t="s">
+    <row r="84" spans="1:10">
+      <c r="A84" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="B84" s="22">
+      <c r="B84" s="6">
         <v>301514</v>
       </c>
-      <c r="C84" s="22">
+      <c r="C84" s="6">
         <v>260041</v>
       </c>
-      <c r="D84" s="22">
+      <c r="D84" s="6">
         <v>518753</v>
       </c>
-      <c r="E84" s="22">
+      <c r="E84" s="6">
         <v>170290</v>
       </c>
-      <c r="F84" s="22">
+      <c r="F84" s="6">
         <v>169461</v>
       </c>
-      <c r="G84" s="22">
+      <c r="G84" s="6">
         <v>234841</v>
       </c>
-      <c r="H84" s="22">
+      <c r="H84" s="6">
         <v>85281</v>
       </c>
-      <c r="I84" s="22">
+      <c r="I84" s="6">
         <v>171161</v>
       </c>
-      <c r="J84" s="24"/>
-    </row>
-    <row r="85" ht="14.25"/>
-    <row r="86" spans="1:10">
-      <c r="A86" s="3" t="s">
+      <c r="J84" s="15"/>
+    </row>
+    <row r="85" spans="1:10">
+      <c r="A85" s="7"/>
+      <c r="J85" s="16"/>
+    </row>
+    <row r="86" s="2" customFormat="1" spans="1:10">
+      <c r="A86" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="B86" s="4"/>
-      <c r="C86" s="4"/>
-      <c r="D86" s="4"/>
-      <c r="E86" s="4"/>
-      <c r="F86" s="4"/>
-      <c r="G86" s="4"/>
-      <c r="H86" s="4"/>
-      <c r="I86" s="4"/>
-      <c r="J86" s="14"/>
-    </row>
-    <row r="87" spans="1:10">
+      <c r="B86" s="6"/>
+      <c r="C86" s="6"/>
+      <c r="D86" s="6"/>
+      <c r="E86" s="6"/>
+      <c r="F86" s="6"/>
+      <c r="G86" s="6"/>
+      <c r="H86" s="6"/>
+      <c r="I86" s="6"/>
+      <c r="J86" s="15"/>
+    </row>
+    <row r="87" s="2" customFormat="1" spans="1:10">
       <c r="A87" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="B87" s="6"/>
-      <c r="C87" s="6"/>
-      <c r="D87" s="6"/>
-      <c r="E87" s="6"/>
-      <c r="F87" s="6"/>
-      <c r="G87" s="6"/>
-      <c r="H87" s="6"/>
-      <c r="I87" s="6"/>
-      <c r="J87" s="15"/>
-    </row>
-    <row r="88" spans="1:10">
+        <v>26</v>
+      </c>
+      <c r="B87" s="22"/>
+      <c r="C87" s="22"/>
+      <c r="D87" s="22"/>
+      <c r="E87" s="22"/>
+      <c r="F87" s="22"/>
+      <c r="G87" s="22">
+        <v>0.0366467058789264</v>
+      </c>
+      <c r="H87" s="22"/>
+      <c r="I87" s="22"/>
+      <c r="J87" s="27"/>
+    </row>
+    <row r="88" s="2" customFormat="1" spans="1:10">
       <c r="A88" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="B88" s="6">
-        <v>0.228152205079095</v>
-      </c>
-      <c r="C88" s="6">
-        <v>0.191548875347098</v>
-      </c>
-      <c r="D88" s="6">
-        <v>0.379426065867224</v>
-      </c>
-      <c r="E88" s="6">
-        <v>0.143834806978518</v>
-      </c>
-      <c r="F88" s="6">
-        <v>0.0492015604703379</v>
-      </c>
-      <c r="G88" s="10">
-        <v>0.0766396493470802</v>
-      </c>
-      <c r="H88" s="6">
-        <v>0.110167879524473</v>
-      </c>
-      <c r="I88" s="6">
-        <v>0.0926905158740254</v>
-      </c>
-      <c r="J88" s="17">
-        <f>SUM(B88:I88)</f>
-        <v>1.27166155848785</v>
-      </c>
-    </row>
-    <row r="89" spans="1:10">
-      <c r="A89" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="B89" s="6">
-        <v>127</v>
-      </c>
-      <c r="C89" s="6">
-        <v>115</v>
-      </c>
-      <c r="D89" s="6">
-        <v>145</v>
-      </c>
-      <c r="E89" s="6">
-        <v>101</v>
-      </c>
-      <c r="F89" s="6">
-        <v>170</v>
-      </c>
-      <c r="G89" s="2">
-        <v>108</v>
-      </c>
-      <c r="H89" s="6">
-        <v>156</v>
-      </c>
-      <c r="I89" s="6">
-        <v>117</v>
-      </c>
-      <c r="J89" s="15">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="90" spans="1:10">
-      <c r="A90" s="5" t="s">
+      <c r="B88" s="23"/>
+      <c r="C88" s="23"/>
+      <c r="D88" s="23"/>
+      <c r="E88" s="23"/>
+      <c r="F88" s="23"/>
+      <c r="G88" s="23">
+        <v>24917</v>
+      </c>
+      <c r="H88" s="23"/>
+      <c r="I88" s="23"/>
+      <c r="J88" s="28"/>
+    </row>
+    <row r="89" s="2" customFormat="1" ht="14.25" spans="1:10">
+      <c r="A89" s="12" t="s">
         <v>28</v>
       </c>
-      <c r="B90" s="6">
-        <v>322308</v>
-      </c>
-      <c r="C90" s="6">
-        <v>281711</v>
-      </c>
-      <c r="D90" s="6">
-        <v>538705</v>
-      </c>
-      <c r="E90" s="6">
-        <v>200341</v>
-      </c>
-      <c r="F90" s="6">
-        <v>220299</v>
-      </c>
-      <c r="G90" s="6">
-        <v>430541</v>
-      </c>
-      <c r="H90" s="6">
-        <v>93809</v>
-      </c>
-      <c r="I90" s="6">
-        <v>171161</v>
-      </c>
-      <c r="J90" s="15"/>
-    </row>
+      <c r="B89" s="24"/>
+      <c r="C89" s="24"/>
+      <c r="D89" s="24"/>
+      <c r="E89" s="24"/>
+      <c r="F89" s="24"/>
+      <c r="G89" s="24">
+        <v>156561</v>
+      </c>
+      <c r="H89" s="24"/>
+      <c r="I89" s="24"/>
+      <c r="J89" s="29"/>
+    </row>
+    <row r="90" ht="14.25"/>
     <row r="91" spans="1:10">
-      <c r="A91" s="7"/>
-      <c r="J91" s="16"/>
+      <c r="A91" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="B91" s="4"/>
+      <c r="C91" s="4"/>
+      <c r="D91" s="4"/>
+      <c r="E91" s="4"/>
+      <c r="F91" s="4"/>
+      <c r="G91" s="4"/>
+      <c r="H91" s="4"/>
+      <c r="I91" s="4"/>
+      <c r="J91" s="14"/>
     </row>
     <row r="92" spans="1:10">
       <c r="A92" s="5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B92" s="6"/>
       <c r="C92" s="6"/>
@@ -3330,32 +3433,32 @@
         <v>26</v>
       </c>
       <c r="B93" s="6">
-        <v>0.225357832225731</v>
+        <v>0.228152205079095</v>
       </c>
       <c r="C93" s="6">
-        <v>0.187832278626018</v>
+        <v>0.191548875347098</v>
       </c>
       <c r="D93" s="6">
-        <v>0.381070627327604</v>
+        <v>0.379426065867224</v>
       </c>
       <c r="E93" s="6">
-        <v>0.143343517352846</v>
+        <v>0.143834806978518</v>
       </c>
       <c r="F93" s="6">
-        <v>0.0533366743677525</v>
-      </c>
-      <c r="G93" s="8">
-        <v>0.110748101588701</v>
+        <v>0.0492015604703379</v>
+      </c>
+      <c r="G93" s="10">
+        <v>0.0766396493470802</v>
       </c>
       <c r="H93" s="6">
-        <v>0.111848633104288</v>
+        <v>0.110167879524473</v>
       </c>
       <c r="I93" s="6">
-        <v>0.103230203907768</v>
+        <v>0.0926905158740254</v>
       </c>
       <c r="J93" s="17">
         <f>SUM(B93:I93)</f>
-        <v>1.31676786850071</v>
+        <v>1.27166155848785</v>
       </c>
     </row>
     <row r="94" spans="1:10">
@@ -3363,31 +3466,31 @@
         <v>27</v>
       </c>
       <c r="B94" s="6">
-        <v>194</v>
+        <v>127</v>
       </c>
       <c r="C94" s="6">
+        <v>115</v>
+      </c>
+      <c r="D94" s="6">
+        <v>145</v>
+      </c>
+      <c r="E94" s="6">
+        <v>101</v>
+      </c>
+      <c r="F94" s="6">
+        <v>170</v>
+      </c>
+      <c r="G94" s="2">
+        <v>108</v>
+      </c>
+      <c r="H94" s="6">
         <v>156</v>
       </c>
-      <c r="D94" s="6">
-        <v>224</v>
-      </c>
-      <c r="E94" s="6">
-        <v>129</v>
-      </c>
-      <c r="F94" s="6">
-        <v>437</v>
-      </c>
-      <c r="G94" s="6">
-        <v>108</v>
-      </c>
-      <c r="H94" s="6">
-        <v>729</v>
-      </c>
       <c r="I94" s="6">
-        <v>151</v>
+        <v>117</v>
       </c>
       <c r="J94" s="15">
-        <v>729</v>
+        <v>170</v>
       </c>
     </row>
     <row r="95" spans="1:10">
@@ -3395,28 +3498,28 @@
         <v>28</v>
       </c>
       <c r="B95" s="6">
-        <v>301514</v>
+        <v>322308</v>
       </c>
       <c r="C95" s="6">
-        <v>260041</v>
+        <v>281711</v>
       </c>
       <c r="D95" s="6">
-        <v>528729</v>
+        <v>538705</v>
       </c>
       <c r="E95" s="6">
-        <v>190324</v>
+        <v>200341</v>
       </c>
       <c r="F95" s="6">
-        <v>186407</v>
+        <v>220299</v>
       </c>
       <c r="G95" s="6">
-        <v>293551</v>
+        <v>430541</v>
       </c>
       <c r="H95" s="6">
-        <v>89545</v>
+        <v>93809</v>
       </c>
       <c r="I95" s="6">
-        <v>162603</v>
+        <v>171161</v>
       </c>
       <c r="J95" s="15"/>
     </row>
@@ -3426,7 +3529,7 @@
     </row>
     <row r="97" spans="1:10">
       <c r="A97" s="5" t="s">
-        <v>37</v>
+        <v>21</v>
       </c>
       <c r="B97" s="6"/>
       <c r="C97" s="6"/>
@@ -3443,31 +3546,32 @@
         <v>26</v>
       </c>
       <c r="B98" s="6">
-        <v>0.223944128917166</v>
+        <v>0.225357832225731</v>
       </c>
       <c r="C98" s="6">
-        <v>0.186722386746853</v>
+        <v>0.187832278626018</v>
       </c>
       <c r="D98" s="6">
-        <v>0.37770148730091</v>
+        <v>0.381070627327604</v>
       </c>
       <c r="E98" s="6">
-        <v>0.131732931754474</v>
+        <v>0.143343517352846</v>
       </c>
       <c r="F98" s="6">
-        <v>0.0490670980855947</v>
-      </c>
-      <c r="G98" s="10">
-        <v>0.0970503709159689</v>
+        <v>0.0533366743677525</v>
+      </c>
+      <c r="G98" s="8">
+        <v>0.110748101588701</v>
       </c>
       <c r="H98" s="6">
-        <v>0.108574350654746</v>
+        <v>0.111848633104288</v>
       </c>
       <c r="I98" s="6">
-        <v>0.0965472395965962</v>
+        <v>0.103230203907768</v>
       </c>
       <c r="J98" s="17">
-        <v>1.27133999397231</v>
+        <f>SUM(B98:I98)</f>
+        <v>1.31676786850071</v>
       </c>
     </row>
     <row r="99" spans="1:10">
@@ -3475,65 +3579,69 @@
         <v>27</v>
       </c>
       <c r="B99" s="6">
-        <v>5546</v>
+        <v>194</v>
       </c>
       <c r="C99" s="6">
-        <v>1533</v>
+        <v>156</v>
       </c>
       <c r="D99" s="6">
-        <v>4598</v>
+        <v>224</v>
       </c>
       <c r="E99" s="6">
-        <v>896</v>
+        <v>129</v>
       </c>
       <c r="F99" s="6">
-        <v>59593</v>
+        <v>437</v>
       </c>
       <c r="G99" s="6">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="H99" s="6">
-        <v>148014</v>
+        <v>729</v>
       </c>
       <c r="I99" s="6">
-        <v>4635</v>
+        <v>151</v>
       </c>
       <c r="J99" s="15">
-        <v>148014</v>
-      </c>
-    </row>
-    <row r="100" ht="14.25" spans="1:10">
-      <c r="A100" s="12" t="s">
+        <v>729</v>
+      </c>
+    </row>
+    <row r="100" spans="1:10">
+      <c r="A100" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="B100" s="22">
+      <c r="B100" s="6">
         <v>301514</v>
       </c>
-      <c r="C100" s="22">
+      <c r="C100" s="6">
         <v>260041</v>
       </c>
-      <c r="D100" s="22">
-        <v>518753</v>
-      </c>
-      <c r="E100" s="22">
-        <v>170290</v>
-      </c>
-      <c r="F100" s="22">
-        <v>169461</v>
-      </c>
-      <c r="G100" s="22">
-        <v>234841</v>
-      </c>
-      <c r="H100" s="22">
-        <v>85281</v>
-      </c>
-      <c r="I100" s="22">
-        <v>171161</v>
-      </c>
-      <c r="J100" s="24"/>
+      <c r="D100" s="6">
+        <v>528729</v>
+      </c>
+      <c r="E100" s="6">
+        <v>190324</v>
+      </c>
+      <c r="F100" s="6">
+        <v>186407</v>
+      </c>
+      <c r="G100" s="6">
+        <v>293551</v>
+      </c>
+      <c r="H100" s="6">
+        <v>89545</v>
+      </c>
+      <c r="I100" s="6">
+        <v>162603</v>
+      </c>
+      <c r="J100" s="15"/>
+    </row>
+    <row r="101" spans="1:10">
+      <c r="A101" s="7"/>
+      <c r="J101" s="16"/>
     </row>
     <row r="102" spans="1:10">
-      <c r="A102" s="6" t="s">
+      <c r="A102" s="5" t="s">
         <v>38</v>
       </c>
       <c r="B102" s="6"/>
@@ -3544,66 +3652,118 @@
       <c r="G102" s="6"/>
       <c r="H102" s="6"/>
       <c r="I102" s="6"/>
-      <c r="J102" s="6"/>
+      <c r="J102" s="15"/>
     </row>
     <row r="103" spans="1:10">
-      <c r="A103" s="6"/>
-      <c r="B103" s="6"/>
-      <c r="C103" s="6"/>
-      <c r="D103" s="6"/>
-      <c r="E103" s="6"/>
-      <c r="F103" s="6"/>
-      <c r="G103" s="6"/>
-      <c r="H103" s="6"/>
-      <c r="I103" s="6"/>
-      <c r="J103" s="6"/>
+      <c r="A103" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="B103" s="6">
+        <v>0.223944128917166</v>
+      </c>
+      <c r="C103" s="6">
+        <v>0.186722386746853</v>
+      </c>
+      <c r="D103" s="6">
+        <v>0.37770148730091</v>
+      </c>
+      <c r="E103" s="6">
+        <v>0.131732931754474</v>
+      </c>
+      <c r="F103" s="6">
+        <v>0.0490670980855947</v>
+      </c>
+      <c r="G103" s="10">
+        <v>0.0970503709159689</v>
+      </c>
+      <c r="H103" s="6">
+        <v>0.108574350654746</v>
+      </c>
+      <c r="I103" s="6">
+        <v>0.0965472395965962</v>
+      </c>
+      <c r="J103" s="17">
+        <v>1.27133999397231</v>
+      </c>
     </row>
     <row r="104" spans="1:10">
-      <c r="A104" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="B104" s="6"/>
-      <c r="C104" s="6"/>
-      <c r="D104" s="6"/>
-      <c r="E104" s="6"/>
-      <c r="F104" s="6"/>
-      <c r="G104" s="10"/>
-      <c r="H104" s="6"/>
-      <c r="I104" s="6"/>
-      <c r="J104" s="10"/>
-    </row>
-    <row r="105" spans="1:10">
-      <c r="A105" s="6" t="s">
+      <c r="A104" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="B105" s="6"/>
-      <c r="C105" s="6"/>
-      <c r="D105" s="6"/>
-      <c r="E105" s="6"/>
-      <c r="F105" s="6"/>
-      <c r="G105" s="6"/>
-      <c r="H105" s="6"/>
-      <c r="I105" s="6"/>
-      <c r="J105" s="6"/>
-    </row>
-    <row r="106" spans="1:10">
-      <c r="A106" s="6" t="s">
+      <c r="B104" s="6">
+        <v>5546</v>
+      </c>
+      <c r="C104" s="6">
+        <v>1533</v>
+      </c>
+      <c r="D104" s="6">
+        <v>4598</v>
+      </c>
+      <c r="E104" s="6">
+        <v>896</v>
+      </c>
+      <c r="F104" s="6">
+        <v>59593</v>
+      </c>
+      <c r="G104" s="6">
+        <v>111</v>
+      </c>
+      <c r="H104" s="6">
+        <v>148014</v>
+      </c>
+      <c r="I104" s="6">
+        <v>4635</v>
+      </c>
+      <c r="J104" s="15">
+        <v>148014</v>
+      </c>
+    </row>
+    <row r="105" ht="14.25" spans="1:10">
+      <c r="A105" s="12" t="s">
         <v>28</v>
       </c>
-      <c r="B106" s="6"/>
-      <c r="C106" s="6"/>
-      <c r="D106" s="6"/>
-      <c r="E106" s="6"/>
-      <c r="F106" s="6"/>
-      <c r="G106" s="6"/>
-      <c r="H106" s="6"/>
-      <c r="I106" s="6"/>
-      <c r="J106" s="6"/>
+      <c r="B105" s="25">
+        <v>301514</v>
+      </c>
+      <c r="C105" s="25">
+        <v>260041</v>
+      </c>
+      <c r="D105" s="25">
+        <v>518753</v>
+      </c>
+      <c r="E105" s="25">
+        <v>170290</v>
+      </c>
+      <c r="F105" s="25">
+        <v>169461</v>
+      </c>
+      <c r="G105" s="25">
+        <v>234841</v>
+      </c>
+      <c r="H105" s="25">
+        <v>85281</v>
+      </c>
+      <c r="I105" s="25">
+        <v>171161</v>
+      </c>
+      <c r="J105" s="30"/>
+    </row>
+    <row r="107" spans="1:10">
+      <c r="A107" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="B107" s="6"/>
+      <c r="C107" s="6"/>
+      <c r="D107" s="6"/>
+      <c r="E107" s="6"/>
+      <c r="F107" s="6"/>
+      <c r="G107" s="6"/>
+      <c r="H107" s="6"/>
+      <c r="I107" s="6"/>
+      <c r="J107" s="6"/>
     </row>
     <row r="108" spans="1:10">
-      <c r="A108" s="6" t="s">
-        <v>23</v>
-      </c>
+      <c r="A108" s="6"/>
       <c r="B108" s="6"/>
       <c r="C108" s="6"/>
       <c r="D108" s="6"/>
@@ -3623,9 +3783,7 @@
       <c r="D109" s="6"/>
       <c r="E109" s="6"/>
       <c r="F109" s="6"/>
-      <c r="G109">
-        <v>0.102480606902965</v>
-      </c>
+      <c r="G109" s="10"/>
       <c r="H109" s="6"/>
       <c r="I109" s="6"/>
       <c r="J109" s="10"/>
@@ -3657,6 +3815,64 @@
       <c r="H111" s="6"/>
       <c r="I111" s="6"/>
       <c r="J111" s="6"/>
+    </row>
+    <row r="113" spans="1:10">
+      <c r="A113" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="B113" s="6"/>
+      <c r="C113" s="6"/>
+      <c r="D113" s="6"/>
+      <c r="E113" s="6"/>
+      <c r="F113" s="6"/>
+      <c r="G113" s="6"/>
+      <c r="H113" s="6"/>
+      <c r="I113" s="6"/>
+      <c r="J113" s="6"/>
+    </row>
+    <row r="114" spans="1:10">
+      <c r="A114" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="B114" s="6"/>
+      <c r="C114" s="6"/>
+      <c r="D114" s="6"/>
+      <c r="E114" s="6"/>
+      <c r="F114" s="6"/>
+      <c r="G114">
+        <v>0.102480606902965</v>
+      </c>
+      <c r="H114" s="6"/>
+      <c r="I114" s="6"/>
+      <c r="J114" s="10"/>
+    </row>
+    <row r="115" spans="1:10">
+      <c r="A115" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="B115" s="6"/>
+      <c r="C115" s="6"/>
+      <c r="D115" s="6"/>
+      <c r="E115" s="6"/>
+      <c r="F115" s="6"/>
+      <c r="G115" s="6"/>
+      <c r="H115" s="6"/>
+      <c r="I115" s="6"/>
+      <c r="J115" s="6"/>
+    </row>
+    <row r="116" spans="1:10">
+      <c r="A116" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="B116" s="6"/>
+      <c r="C116" s="6"/>
+      <c r="D116" s="6"/>
+      <c r="E116" s="6"/>
+      <c r="F116" s="6"/>
+      <c r="G116" s="6"/>
+      <c r="H116" s="6"/>
+      <c r="I116" s="6"/>
+      <c r="J116" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.699305555555556" right="0.699305555555556" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Re-org the Multi-Thread. The result is correct but the performance is not well very because creating thread by async again and again.
</commit_message>
<xml_diff>
--- a/overall.xlsx
+++ b/overall.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="28080" windowHeight="13065" activeTab="1"/>
+    <workbookView windowWidth="20385" windowHeight="8370" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -108,10 +108,10 @@
     <t>17_07_13_06_28_57_1_500_500_0</t>
   </si>
   <si>
-    <t>17_06_28_02_58_04_2_2500_500</t>
-  </si>
-  <si>
-    <t>17_06_23_10_45_37_2_500_500</t>
+    <t>17_07_13_06_33_45_2_2500_500_0</t>
+  </si>
+  <si>
+    <t>17_07_13_06_51_31_2_500_500_0</t>
   </si>
   <si>
     <t>17_07_12_07_26_07_2_1_500_0</t>
@@ -143,10 +143,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="20">
     <font>
@@ -157,6 +157,21 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="宋体"/>
@@ -173,41 +188,10 @@
     </font>
     <font>
       <b/>
-      <sz val="13"/>
+      <sz val="15"/>
       <color theme="3"/>
       <name val="宋体"/>
       <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="宋体"/>
-      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -219,7 +203,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="0"/>
+      <color theme="1"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -228,22 +212,6 @@
       <b/>
       <sz val="11"/>
       <color rgb="FF3F3F3F"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -265,15 +233,39 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color rgb="FFFF0000"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -286,14 +278,22 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <i/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FF7F7F7F"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
       <name val="宋体"/>
@@ -322,7 +322,145 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -334,37 +472,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
+        <fgColor theme="4" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
+        <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
+        <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -376,133 +496,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -669,6 +669,17 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="double">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -694,21 +705,6 @@
     </border>
     <border>
       <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
         <color rgb="FFB2B2B2"/>
       </left>
       <right style="thin">
@@ -723,22 +719,17 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
       <top style="thin">
-        <color theme="4"/>
+        <color rgb="FF3F3F3F"/>
       </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -761,6 +752,15 @@
       <left/>
       <right/>
       <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
       <bottom style="double">
         <color rgb="FFFF8001"/>
       </bottom>
@@ -774,10 +774,10 @@
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="25" borderId="18" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="12" borderId="17" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -786,137 +786,137 @@
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="1" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="15" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="17" borderId="15" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="17" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="16" borderId="14" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="16" borderId="18" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="12" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="19" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="16" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="14" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="14" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="18" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="10" borderId="16" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="10" borderId="17" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="13" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="19" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -953,6 +953,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -974,37 +977,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
@@ -1072,6 +1054,11 @@
     <cellStyle name="60% - 强调文字颜色 6" xfId="48" builtinId="52"/>
   </cellStyles>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -1457,7 +1444,7 @@
       <c r="F3">
         <v>0.0522827100851127</v>
       </c>
-      <c r="G3" s="31">
+      <c r="G3" s="25">
         <v>0.106926203216301</v>
       </c>
       <c r="H3">
@@ -1483,7 +1470,7 @@
       <c r="A12" t="s">
         <v>12</v>
       </c>
-      <c r="G12" s="32">
+      <c r="G12" s="26">
         <v>0.0629933219692992</v>
       </c>
     </row>
@@ -1536,7 +1523,7 @@
       <c r="I19">
         <v>0.0755164339928472</v>
       </c>
-      <c r="J19" s="33">
+      <c r="J19" s="27">
         <f t="shared" ref="J19:J21" si="0">SUM(B19:I19)</f>
         <v>1.17870842662782</v>
       </c>
@@ -1545,31 +1532,31 @@
       <c r="A20" t="s">
         <v>17</v>
       </c>
-      <c r="B20" s="33">
+      <c r="B20" s="27">
         <v>0.20800686430345</v>
       </c>
-      <c r="C20" s="33">
+      <c r="C20" s="27">
         <v>0.173239206962822</v>
       </c>
-      <c r="D20" s="33">
+      <c r="D20" s="27">
         <v>0.346041541710196</v>
       </c>
-      <c r="E20" s="33">
+      <c r="E20" s="27">
         <v>0.124928278882666</v>
       </c>
-      <c r="F20" s="33">
+      <c r="F20" s="27">
         <v>0.0409924383808026</v>
       </c>
-      <c r="G20" s="33">
+      <c r="G20" s="27">
         <v>0.0453003114127127</v>
       </c>
-      <c r="H20" s="33">
+      <c r="H20" s="27">
         <v>0.0964368086720679</v>
       </c>
-      <c r="I20" s="33">
+      <c r="I20" s="27">
         <v>0.065879029949852</v>
       </c>
-      <c r="J20" s="33">
+      <c r="J20" s="27">
         <f t="shared" si="0"/>
         <v>1.10082448027457</v>
       </c>
@@ -1578,52 +1565,52 @@
       <c r="A21" t="s">
         <v>18</v>
       </c>
-      <c r="B21" s="32">
+      <c r="B21" s="26">
         <v>0.207894527330402</v>
       </c>
-      <c r="C21" s="32">
+      <c r="C21" s="26">
         <v>0.173165858291852</v>
       </c>
-      <c r="D21" s="32">
+      <c r="D21" s="26">
         <v>0.344628020195683</v>
       </c>
-      <c r="E21" s="32">
+      <c r="E21" s="26">
         <v>0.118862297465155</v>
       </c>
-      <c r="F21" s="32">
+      <c r="F21" s="26">
         <v>0.0388983176119749</v>
       </c>
-      <c r="G21" s="32">
+      <c r="G21" s="26">
         <v>0.0422239303614074</v>
       </c>
-      <c r="H21" s="32">
+      <c r="H21" s="26">
         <v>0.0955131594160284</v>
       </c>
-      <c r="I21" s="32">
+      <c r="I21" s="26">
         <v>0.0488732287830458</v>
       </c>
-      <c r="J21" s="32">
+      <c r="J21" s="26">
         <f t="shared" si="0"/>
         <v>1.07005933945555</v>
       </c>
     </row>
     <row r="22" spans="10:10">
-      <c r="J22" s="33"/>
+      <c r="J22" s="27"/>
     </row>
     <row r="23" spans="10:10">
-      <c r="J23" s="33"/>
+      <c r="J23" s="27"/>
     </row>
     <row r="24" spans="10:10">
-      <c r="J24" s="33"/>
+      <c r="J24" s="27"/>
     </row>
     <row r="25" spans="10:10">
-      <c r="J25" s="33"/>
+      <c r="J25" s="27"/>
     </row>
     <row r="26" spans="1:10">
       <c r="A26" t="s">
         <v>19</v>
       </c>
-      <c r="J26" s="33"/>
+      <c r="J26" s="27"/>
     </row>
     <row r="27" spans="1:10">
       <c r="A27" t="s">
@@ -1644,7 +1631,7 @@
       <c r="F27">
         <v>0.0492015604703379</v>
       </c>
-      <c r="G27" s="33">
+      <c r="G27" s="27">
         <v>0.0766396493470802</v>
       </c>
       <c r="H27">
@@ -1653,7 +1640,7 @@
       <c r="I27">
         <v>0.0926905158740254</v>
       </c>
-      <c r="J27" s="33">
+      <c r="J27" s="27">
         <f>SUM(B27:I27)</f>
         <v>1.27166155848785</v>
       </c>
@@ -1677,7 +1664,7 @@
       <c r="F28">
         <v>0.0533366743677525</v>
       </c>
-      <c r="G28" s="31">
+      <c r="G28" s="25">
         <v>0.110748101588701</v>
       </c>
       <c r="H28">
@@ -1686,7 +1673,7 @@
       <c r="I28">
         <v>0.103230203907768</v>
       </c>
-      <c r="J28" s="33">
+      <c r="J28" s="27">
         <f>SUM(B28:I28)</f>
         <v>1.31676786850071</v>
       </c>
@@ -1716,8 +1703,8 @@
   <sheetPr/>
   <dimension ref="A1:J116"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="J36" sqref="J36"/>
+    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
+      <selection activeCell="J27" sqref="J27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
@@ -1802,7 +1789,7 @@
       <c r="G4" s="4"/>
       <c r="H4" s="4"/>
       <c r="I4" s="4"/>
-      <c r="J4" s="14"/>
+      <c r="J4" s="15"/>
     </row>
     <row r="5" spans="1:10">
       <c r="A5" s="5" t="s">
@@ -1816,7 +1803,7 @@
       <c r="G5" s="6"/>
       <c r="H5" s="6"/>
       <c r="I5" s="6"/>
-      <c r="J5" s="15"/>
+      <c r="J5" s="16"/>
     </row>
     <row r="6" spans="1:10">
       <c r="A6" s="5" t="s">
@@ -1846,7 +1833,7 @@
       <c r="I6" s="6">
         <v>0.0921915925927093</v>
       </c>
-      <c r="J6" s="15">
+      <c r="J6" s="16">
         <f>SUM(B6:I6)</f>
         <v>1.26377434756932</v>
       </c>
@@ -1879,7 +1866,7 @@
       <c r="I7" s="6">
         <v>109</v>
       </c>
-      <c r="J7" s="15">
+      <c r="J7" s="16">
         <v>139</v>
       </c>
     </row>
@@ -1911,11 +1898,11 @@
       <c r="I8" s="6">
         <v>343549</v>
       </c>
-      <c r="J8" s="15"/>
+      <c r="J8" s="16"/>
     </row>
     <row r="9" spans="1:10">
       <c r="A9" s="7"/>
-      <c r="J9" s="16"/>
+      <c r="J9" s="17"/>
     </row>
     <row r="10" spans="1:10">
       <c r="A10" s="5" t="s">
@@ -1929,7 +1916,7 @@
       <c r="G10" s="6"/>
       <c r="H10" s="6"/>
       <c r="I10" s="6"/>
-      <c r="J10" s="15"/>
+      <c r="J10" s="16"/>
     </row>
     <row r="11" spans="1:10">
       <c r="A11" s="5" t="s">
@@ -1959,7 +1946,7 @@
       <c r="I11" s="6">
         <v>0.102423416293936</v>
       </c>
-      <c r="J11" s="15">
+      <c r="J11" s="16">
         <f>SUM(B11:I11)</f>
         <v>1.31083942802335</v>
       </c>
@@ -1992,7 +1979,7 @@
       <c r="I12" s="6">
         <v>221</v>
       </c>
-      <c r="J12" s="15">
+      <c r="J12" s="16">
         <v>1089</v>
       </c>
     </row>
@@ -2024,11 +2011,11 @@
       <c r="I13" s="6">
         <v>430115</v>
       </c>
-      <c r="J13" s="15"/>
+      <c r="J13" s="16"/>
     </row>
     <row r="14" spans="1:10">
       <c r="A14" s="7"/>
-      <c r="J14" s="16"/>
+      <c r="J14" s="17"/>
     </row>
     <row r="15" spans="1:10">
       <c r="A15" s="9" t="s">
@@ -2042,7 +2029,7 @@
       <c r="G15" s="10"/>
       <c r="H15" s="10"/>
       <c r="I15" s="10"/>
-      <c r="J15" s="17"/>
+      <c r="J15" s="18"/>
     </row>
     <row r="16" s="1" customFormat="1" spans="1:10">
       <c r="A16" s="5" t="s">
@@ -2072,7 +2059,7 @@
       <c r="I16" s="10">
         <v>0.107949060989036</v>
       </c>
-      <c r="J16" s="15">
+      <c r="J16" s="16">
         <f>SUM(B16:I16)</f>
         <v>1.32751827014031</v>
       </c>
@@ -2105,7 +2092,7 @@
       <c r="I17" s="10">
         <v>152</v>
       </c>
-      <c r="J17" s="17">
+      <c r="J17" s="18">
         <v>281</v>
       </c>
     </row>
@@ -2137,124 +2124,124 @@
       <c r="I18" s="10">
         <v>421334</v>
       </c>
-      <c r="J18" s="17"/>
+      <c r="J18" s="18"/>
     </row>
     <row r="19" s="1" customFormat="1" spans="1:10">
       <c r="A19" s="11"/>
-      <c r="J19" s="18"/>
+      <c r="J19" s="19"/>
     </row>
     <row r="20" s="1" customFormat="1" spans="1:10">
-      <c r="A20" s="9" t="s">
+      <c r="A20" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="B20" s="10">
+      <c r="B20" s="12"/>
+      <c r="C20" s="12"/>
+      <c r="D20" s="12"/>
+      <c r="E20" s="12"/>
+      <c r="F20" s="12"/>
+      <c r="G20" s="12"/>
+      <c r="H20" s="12"/>
+      <c r="I20" s="12"/>
+      <c r="J20" s="12"/>
+    </row>
+    <row r="21" s="1" customFormat="1" spans="1:10">
+      <c r="A21" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="B21" s="10">
         <v>0.22496788201061</v>
       </c>
-      <c r="C20" s="10">
+      <c r="C21" s="10">
         <v>0.187524905369721</v>
       </c>
-      <c r="D20" s="10">
+      <c r="D21" s="10">
         <v>0.378768597488832</v>
       </c>
-      <c r="E20" s="10">
+      <c r="E21" s="10">
         <v>0.13268127642868</v>
       </c>
-      <c r="F20" s="10">
+      <c r="F21" s="10">
         <v>0.0485509130381507</v>
       </c>
-      <c r="G20" s="10">
+      <c r="G21" s="10">
         <v>0.0963740326795437</v>
       </c>
-      <c r="H20" s="10">
+      <c r="H21" s="10">
         <v>0.110138053342448</v>
       </c>
-      <c r="I20" s="10">
+      <c r="I21" s="10">
         <v>0.103029977777207</v>
       </c>
-      <c r="J20" s="17">
-        <f>SUM(B20:I20)</f>
+      <c r="J21" s="10">
+        <f>SUM(B21:I21)</f>
         <v>1.28203563813519</v>
       </c>
     </row>
-    <row r="21" s="1" customFormat="1" spans="1:10">
-      <c r="A21" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="B21" s="10">
+    <row r="22" s="1" customFormat="1" spans="1:10">
+      <c r="A22" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="B22" s="10">
         <v>661</v>
       </c>
-      <c r="C21" s="10">
+      <c r="C22" s="10">
         <v>496</v>
       </c>
-      <c r="D21" s="10">
+      <c r="D22" s="10">
         <v>1058</v>
       </c>
-      <c r="E21" s="10">
+      <c r="E22" s="10">
         <v>328</v>
       </c>
-      <c r="F21" s="10">
+      <c r="F22" s="10">
         <v>856</v>
       </c>
-      <c r="G21" s="10">
+      <c r="G22" s="10">
         <v>72</v>
       </c>
-      <c r="H21" s="10">
+      <c r="H22" s="10">
         <v>923</v>
       </c>
-      <c r="I21" s="10">
+      <c r="I22" s="10">
         <v>335</v>
       </c>
-      <c r="J21" s="17">
+      <c r="J22" s="10">
         <v>1058</v>
       </c>
     </row>
-    <row r="22" s="1" customFormat="1" spans="1:10">
-      <c r="A22" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="B22" s="10">
+    <row r="23" s="1" customFormat="1" spans="1:10">
+      <c r="A23" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="B23" s="10">
         <v>682954</v>
       </c>
-      <c r="C22" s="10">
+      <c r="C23" s="10">
         <v>691497</v>
       </c>
-      <c r="D22" s="10">
+      <c r="D23" s="10">
         <v>772314</v>
       </c>
-      <c r="E22" s="10">
+      <c r="E23" s="10">
         <v>687672</v>
       </c>
-      <c r="F22" s="10">
+      <c r="F23" s="10">
         <v>754610</v>
       </c>
-      <c r="G22" s="10">
+      <c r="G23" s="10">
         <v>1548385</v>
       </c>
-      <c r="H22" s="10">
+      <c r="H23" s="10">
         <v>187357</v>
       </c>
-      <c r="I22" s="10">
+      <c r="I23" s="10">
         <v>500491</v>
       </c>
-      <c r="J22" s="17"/>
-    </row>
-    <row r="23" s="1" customFormat="1" spans="1:10">
-      <c r="A23" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="B23" s="10"/>
-      <c r="C23" s="10"/>
-      <c r="D23" s="10"/>
-      <c r="E23" s="10"/>
-      <c r="F23" s="10"/>
-      <c r="G23" s="10"/>
-      <c r="H23" s="10"/>
-      <c r="I23" s="10"/>
-      <c r="J23" s="17"/>
+      <c r="J23" s="10"/>
     </row>
     <row r="24" s="1" customFormat="1" spans="1:10">
       <c r="A24" s="11"/>
-      <c r="J24" s="18"/>
+      <c r="J24" s="19"/>
     </row>
     <row r="25" s="1" customFormat="1" spans="1:10">
       <c r="A25" s="9" t="s">
@@ -2268,7 +2255,7 @@
       <c r="G25" s="6"/>
       <c r="H25" s="6"/>
       <c r="I25" s="6"/>
-      <c r="J25" s="15"/>
+      <c r="J25" s="16"/>
     </row>
     <row r="26" spans="1:10">
       <c r="A26" s="5" t="s">
@@ -2298,7 +2285,7 @@
       <c r="I26" s="10">
         <v>0.103639895551926</v>
       </c>
-      <c r="J26" s="17">
+      <c r="J26" s="18">
         <f>SUM(B26:I26)</f>
         <v>1.27862632342455</v>
       </c>
@@ -2331,7 +2318,9 @@
       <c r="I27" s="10">
         <v>488</v>
       </c>
-      <c r="J27" s="17"/>
+      <c r="J27" s="10">
+        <v>1883</v>
+      </c>
     </row>
     <row r="28" spans="1:10">
       <c r="A28" s="5" t="s">
@@ -2361,7 +2350,7 @@
       <c r="I28" s="6">
         <v>505491</v>
       </c>
-      <c r="J28" s="17"/>
+      <c r="J28" s="18"/>
     </row>
     <row r="29" spans="1:10">
       <c r="A29" s="7"/>
@@ -2379,7 +2368,7 @@
       <c r="G30" s="6"/>
       <c r="H30" s="6"/>
       <c r="I30" s="6"/>
-      <c r="J30" s="17"/>
+      <c r="J30" s="18"/>
     </row>
     <row r="31" spans="1:10">
       <c r="A31" s="5" t="s">
@@ -2409,7 +2398,7 @@
       <c r="I31" s="10">
         <v>0.096234294786308</v>
       </c>
-      <c r="J31" s="17">
+      <c r="J31" s="18">
         <f>SUM(B31:I31)</f>
         <v>1.26709179991234</v>
       </c>
@@ -2442,7 +2431,7 @@
       <c r="I32" s="10">
         <v>2877</v>
       </c>
-      <c r="J32" s="15">
+      <c r="J32" s="16">
         <v>67058</v>
       </c>
     </row>
@@ -2474,11 +2463,11 @@
       <c r="I33" s="6">
         <v>509904</v>
       </c>
-      <c r="J33" s="15"/>
+      <c r="J33" s="16"/>
     </row>
     <row r="34" spans="1:10">
       <c r="A34" s="7"/>
-      <c r="J34" s="16"/>
+      <c r="J34" s="17"/>
     </row>
     <row r="35" spans="1:10">
       <c r="A35" s="9" t="s">
@@ -2492,7 +2481,7 @@
       <c r="G35" s="6"/>
       <c r="H35" s="6"/>
       <c r="I35" s="6"/>
-      <c r="J35" s="15"/>
+      <c r="J35" s="16"/>
     </row>
     <row r="36" spans="1:10">
       <c r="A36" s="5" t="s">
@@ -2522,7 +2511,7 @@
       <c r="I36" s="10">
         <v>0.0725702160635175</v>
       </c>
-      <c r="J36" s="17">
+      <c r="J36" s="18">
         <f>SUM(B36:I36)</f>
         <v>1.23689739279618</v>
       </c>
@@ -2555,7 +2544,9 @@
       <c r="I37" s="10">
         <v>1797</v>
       </c>
-      <c r="J37" s="17"/>
+      <c r="J37" s="10">
+        <v>10661</v>
+      </c>
     </row>
     <row r="38" spans="1:10">
       <c r="A38" s="5" t="s">
@@ -2585,11 +2576,11 @@
       <c r="I38" s="10">
         <v>480276</v>
       </c>
-      <c r="J38" s="17"/>
+      <c r="J38" s="18"/>
     </row>
     <row r="39" spans="1:10">
       <c r="A39" s="7"/>
-      <c r="J39" s="16"/>
+      <c r="J39" s="17"/>
     </row>
     <row r="40" spans="1:10">
       <c r="A40" s="9" t="s">
@@ -2603,7 +2594,7 @@
       <c r="G40" s="6"/>
       <c r="H40" s="6"/>
       <c r="I40" s="6"/>
-      <c r="J40" s="15"/>
+      <c r="J40" s="16"/>
     </row>
     <row r="41" spans="1:10">
       <c r="A41" s="5" t="s">
@@ -2617,7 +2608,7 @@
       <c r="G41" s="10"/>
       <c r="H41" s="10"/>
       <c r="I41" s="10"/>
-      <c r="J41" s="17"/>
+      <c r="J41" s="18"/>
     </row>
     <row r="42" spans="1:10">
       <c r="A42" s="5" t="s">
@@ -2639,7 +2630,7 @@
       <c r="I42" s="10">
         <v>15231</v>
       </c>
-      <c r="J42" s="17"/>
+      <c r="J42" s="18"/>
     </row>
     <row r="43" spans="1:10">
       <c r="A43" s="5" t="s">
@@ -2661,11 +2652,11 @@
       <c r="I43" s="10">
         <v>481500</v>
       </c>
-      <c r="J43" s="17"/>
+      <c r="J43" s="18"/>
     </row>
     <row r="44" spans="1:10">
       <c r="A44" s="7"/>
-      <c r="J44" s="16"/>
+      <c r="J44" s="17"/>
     </row>
     <row r="45" spans="1:10">
       <c r="A45" s="5" t="s">
@@ -2681,7 +2672,7 @@
       </c>
       <c r="H45" s="6"/>
       <c r="I45" s="6"/>
-      <c r="J45" s="15"/>
+      <c r="J45" s="16"/>
     </row>
     <row r="46" spans="1:10">
       <c r="A46" s="5" t="s">
@@ -2695,7 +2686,7 @@
       <c r="G46" s="10"/>
       <c r="H46" s="10"/>
       <c r="I46" s="10"/>
-      <c r="J46" s="17"/>
+      <c r="J46" s="18"/>
     </row>
     <row r="47" spans="1:10">
       <c r="A47" s="5" t="s">
@@ -2709,7 +2700,7 @@
       <c r="G47" s="10"/>
       <c r="H47" s="10"/>
       <c r="I47" s="10"/>
-      <c r="J47" s="17"/>
+      <c r="J47" s="18"/>
     </row>
     <row r="48" spans="1:10">
       <c r="A48" s="5" t="s">
@@ -2723,11 +2714,11 @@
       <c r="G48" s="10"/>
       <c r="H48" s="10"/>
       <c r="I48" s="10"/>
-      <c r="J48" s="17"/>
+      <c r="J48" s="18"/>
     </row>
     <row r="49" spans="1:10">
       <c r="A49" s="7"/>
-      <c r="J49" s="16"/>
+      <c r="J49" s="17"/>
     </row>
     <row r="50" spans="1:10">
       <c r="A50" s="5" t="s">
@@ -2743,7 +2734,7 @@
       </c>
       <c r="H50" s="6"/>
       <c r="I50" s="6"/>
-      <c r="J50" s="15"/>
+      <c r="J50" s="16"/>
     </row>
     <row r="51" spans="1:10">
       <c r="A51" s="5" t="s">
@@ -2757,7 +2748,7 @@
       <c r="G51" s="10"/>
       <c r="H51" s="10"/>
       <c r="I51" s="10"/>
-      <c r="J51" s="17"/>
+      <c r="J51" s="18"/>
     </row>
     <row r="52" spans="1:10">
       <c r="A52" s="5" t="s">
@@ -2771,7 +2762,7 @@
       <c r="G52" s="10"/>
       <c r="H52" s="10"/>
       <c r="I52" s="10"/>
-      <c r="J52" s="17"/>
+      <c r="J52" s="18"/>
     </row>
     <row r="53" spans="1:10">
       <c r="A53" s="5" t="s">
@@ -2785,11 +2776,11 @@
       <c r="G53" s="10"/>
       <c r="H53" s="10"/>
       <c r="I53" s="10"/>
-      <c r="J53" s="17"/>
+      <c r="J53" s="18"/>
     </row>
     <row r="54" spans="1:10">
       <c r="A54" s="7"/>
-      <c r="J54" s="16"/>
+      <c r="J54" s="17"/>
     </row>
     <row r="55" spans="1:10">
       <c r="A55" s="5" t="s">
@@ -2805,7 +2796,7 @@
       </c>
       <c r="H55" s="6"/>
       <c r="I55" s="6"/>
-      <c r="J55" s="15"/>
+      <c r="J55" s="16"/>
     </row>
     <row r="56" spans="1:10">
       <c r="A56" s="5" t="s">
@@ -2819,7 +2810,7 @@
       <c r="G56" s="10"/>
       <c r="H56" s="10"/>
       <c r="I56" s="10"/>
-      <c r="J56" s="17"/>
+      <c r="J56" s="18"/>
     </row>
     <row r="57" spans="1:10">
       <c r="A57" s="5" t="s">
@@ -2833,7 +2824,7 @@
       <c r="G57" s="10"/>
       <c r="H57" s="10"/>
       <c r="I57" s="10"/>
-      <c r="J57" s="17"/>
+      <c r="J57" s="18"/>
     </row>
     <row r="58" spans="1:10">
       <c r="A58" s="5" t="s">
@@ -2847,11 +2838,11 @@
       <c r="G58" s="10"/>
       <c r="H58" s="10"/>
       <c r="I58" s="10"/>
-      <c r="J58" s="17"/>
+      <c r="J58" s="18"/>
     </row>
     <row r="59" spans="1:10">
       <c r="A59" s="7"/>
-      <c r="J59" s="16"/>
+      <c r="J59" s="17"/>
     </row>
     <row r="60" spans="1:10">
       <c r="A60" s="5" t="s">
@@ -2867,7 +2858,7 @@
       </c>
       <c r="H60" s="6"/>
       <c r="I60" s="6"/>
-      <c r="J60" s="15"/>
+      <c r="J60" s="16"/>
     </row>
     <row r="61" spans="1:10">
       <c r="A61" s="5" t="s">
@@ -2881,7 +2872,7 @@
       <c r="G61" s="10"/>
       <c r="H61" s="10"/>
       <c r="I61" s="10"/>
-      <c r="J61" s="17"/>
+      <c r="J61" s="18"/>
     </row>
     <row r="62" spans="1:10">
       <c r="A62" s="5" t="s">
@@ -2895,20 +2886,20 @@
       <c r="G62" s="10"/>
       <c r="H62" s="10"/>
       <c r="I62" s="10"/>
-      <c r="J62" s="17"/>
+      <c r="J62" s="18"/>
     </row>
     <row r="63" ht="14.25" spans="1:10">
-      <c r="A63" s="12" t="s">
+      <c r="A63" s="13" t="s">
         <v>28</v>
       </c>
-      <c r="B63" s="13"/>
-      <c r="C63" s="13"/>
-      <c r="D63" s="13"/>
-      <c r="E63" s="13"/>
-      <c r="F63" s="13"/>
-      <c r="G63" s="13"/>
-      <c r="H63" s="13"/>
-      <c r="I63" s="13"/>
+      <c r="B63" s="14"/>
+      <c r="C63" s="14"/>
+      <c r="D63" s="14"/>
+      <c r="E63" s="14"/>
+      <c r="F63" s="14"/>
+      <c r="G63" s="14"/>
+      <c r="H63" s="14"/>
+      <c r="I63" s="14"/>
       <c r="J63" s="20"/>
     </row>
     <row r="66" ht="14.25"/>
@@ -2938,7 +2929,7 @@
       <c r="I67" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="J67" s="14" t="s">
+      <c r="J67" s="15" t="s">
         <v>8</v>
       </c>
     </row>
@@ -2970,11 +2961,11 @@
       <c r="I68" s="6">
         <v>855802</v>
       </c>
-      <c r="J68" s="15"/>
+      <c r="J68" s="16"/>
     </row>
     <row r="69" spans="1:10">
       <c r="A69" s="7"/>
-      <c r="J69" s="16"/>
+      <c r="J69" s="17"/>
     </row>
     <row r="70" spans="1:10">
       <c r="A70" s="5" t="s">
@@ -2988,7 +2979,7 @@
       <c r="G70" s="6"/>
       <c r="H70" s="6"/>
       <c r="I70" s="6"/>
-      <c r="J70" s="15"/>
+      <c r="J70" s="16"/>
     </row>
     <row r="71" spans="1:10">
       <c r="A71" s="7" t="s">
@@ -3002,7 +2993,7 @@
       <c r="G71" s="6"/>
       <c r="H71" s="6"/>
       <c r="I71" s="6"/>
-      <c r="J71" s="15"/>
+      <c r="J71" s="16"/>
     </row>
     <row r="72" spans="1:10">
       <c r="A72" s="5" t="s">
@@ -3032,7 +3023,7 @@
       <c r="I72" s="6">
         <v>0.0755164339928472</v>
       </c>
-      <c r="J72" s="17">
+      <c r="J72" s="18">
         <f>SUM(B72:I72)</f>
         <v>1.17870842662782</v>
       </c>
@@ -3065,7 +3056,7 @@
       <c r="I73" s="6">
         <v>634</v>
       </c>
-      <c r="J73" s="15">
+      <c r="J73" s="16">
         <v>1792</v>
       </c>
     </row>
@@ -3097,11 +3088,11 @@
       <c r="I74" s="6">
         <v>171161</v>
       </c>
-      <c r="J74" s="15"/>
+      <c r="J74" s="16"/>
     </row>
     <row r="75" spans="1:10">
       <c r="A75" s="7"/>
-      <c r="J75" s="16"/>
+      <c r="J75" s="17"/>
     </row>
     <row r="76" s="2" customFormat="1" spans="1:10">
       <c r="A76" s="5" t="s">
@@ -3115,7 +3106,7 @@
       <c r="G76" s="6"/>
       <c r="H76" s="6"/>
       <c r="I76" s="6"/>
-      <c r="J76" s="15"/>
+      <c r="J76" s="16"/>
     </row>
     <row r="77" s="2" customFormat="1" spans="1:10">
       <c r="A77" s="5" t="s">
@@ -3145,7 +3136,7 @@
       <c r="I77" s="10">
         <v>0.065879029949852</v>
       </c>
-      <c r="J77" s="17">
+      <c r="J77" s="18">
         <f>SUM(B77:I77)</f>
         <v>1.10082448027457</v>
       </c>
@@ -3178,7 +3169,7 @@
       <c r="I78" s="6">
         <v>633</v>
       </c>
-      <c r="J78" s="15">
+      <c r="J78" s="16">
         <v>1864</v>
       </c>
     </row>
@@ -3210,7 +3201,7 @@
       <c r="I79" s="6">
         <v>162603</v>
       </c>
-      <c r="J79" s="15"/>
+      <c r="J79" s="16"/>
     </row>
     <row r="80" customFormat="1" spans="1:10">
       <c r="A80" s="7"/>
@@ -3222,7 +3213,7 @@
       <c r="G80" s="2"/>
       <c r="H80" s="2"/>
       <c r="I80" s="2"/>
-      <c r="J80" s="16"/>
+      <c r="J80" s="17"/>
     </row>
     <row r="81" spans="1:10">
       <c r="A81" s="5" t="s">
@@ -3236,7 +3227,7 @@
       <c r="G81" s="6"/>
       <c r="H81" s="6"/>
       <c r="I81" s="6"/>
-      <c r="J81" s="15"/>
+      <c r="J81" s="16"/>
     </row>
     <row r="82" spans="1:10">
       <c r="A82" s="5" t="s">
@@ -3266,7 +3257,7 @@
       <c r="I82" s="21">
         <v>0.0488732287830458</v>
       </c>
-      <c r="J82" s="26">
+      <c r="J82" s="23">
         <f>SUM(B82:I82)</f>
         <v>1.07005933945555</v>
       </c>
@@ -3299,7 +3290,7 @@
       <c r="I83" s="6">
         <v>5050</v>
       </c>
-      <c r="J83" s="15">
+      <c r="J83" s="16">
         <v>149985</v>
       </c>
     </row>
@@ -3331,11 +3322,11 @@
       <c r="I84" s="6">
         <v>171161</v>
       </c>
-      <c r="J84" s="15"/>
+      <c r="J84" s="16"/>
     </row>
     <row r="85" spans="1:10">
       <c r="A85" s="7"/>
-      <c r="J85" s="16"/>
+      <c r="J85" s="17"/>
     </row>
     <row r="86" s="2" customFormat="1" spans="1:10">
       <c r="A86" s="5" t="s">
@@ -3349,55 +3340,55 @@
       <c r="G86" s="6"/>
       <c r="H86" s="6"/>
       <c r="I86" s="6"/>
-      <c r="J86" s="15"/>
+      <c r="J86" s="16"/>
     </row>
     <row r="87" s="2" customFormat="1" spans="1:10">
       <c r="A87" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="B87" s="22"/>
-      <c r="C87" s="22"/>
-      <c r="D87" s="22"/>
-      <c r="E87" s="22"/>
-      <c r="F87" s="22"/>
-      <c r="G87" s="22">
+      <c r="B87" s="10"/>
+      <c r="C87" s="10"/>
+      <c r="D87" s="10"/>
+      <c r="E87" s="10"/>
+      <c r="F87" s="10"/>
+      <c r="G87" s="10">
         <v>0.0366467058789264</v>
       </c>
-      <c r="H87" s="22"/>
-      <c r="I87" s="22"/>
-      <c r="J87" s="27"/>
+      <c r="H87" s="10"/>
+      <c r="I87" s="10"/>
+      <c r="J87" s="18"/>
     </row>
     <row r="88" s="2" customFormat="1" spans="1:10">
       <c r="A88" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="B88" s="23"/>
-      <c r="C88" s="23"/>
-      <c r="D88" s="23"/>
-      <c r="E88" s="23"/>
-      <c r="F88" s="23"/>
-      <c r="G88" s="23">
+      <c r="B88" s="10"/>
+      <c r="C88" s="10"/>
+      <c r="D88" s="10"/>
+      <c r="E88" s="10"/>
+      <c r="F88" s="10"/>
+      <c r="G88" s="10">
         <v>24917</v>
       </c>
-      <c r="H88" s="23"/>
-      <c r="I88" s="23"/>
-      <c r="J88" s="28"/>
+      <c r="H88" s="10"/>
+      <c r="I88" s="10"/>
+      <c r="J88" s="18"/>
     </row>
     <row r="89" s="2" customFormat="1" ht="14.25" spans="1:10">
-      <c r="A89" s="12" t="s">
+      <c r="A89" s="13" t="s">
         <v>28</v>
       </c>
-      <c r="B89" s="24"/>
-      <c r="C89" s="24"/>
-      <c r="D89" s="24"/>
-      <c r="E89" s="24"/>
-      <c r="F89" s="24"/>
-      <c r="G89" s="24">
+      <c r="B89" s="14"/>
+      <c r="C89" s="14"/>
+      <c r="D89" s="14"/>
+      <c r="E89" s="14"/>
+      <c r="F89" s="14"/>
+      <c r="G89" s="14">
         <v>156561</v>
       </c>
-      <c r="H89" s="24"/>
-      <c r="I89" s="24"/>
-      <c r="J89" s="29"/>
+      <c r="H89" s="14"/>
+      <c r="I89" s="14"/>
+      <c r="J89" s="20"/>
     </row>
     <row r="90" ht="14.25"/>
     <row r="91" spans="1:10">
@@ -3412,7 +3403,7 @@
       <c r="G91" s="4"/>
       <c r="H91" s="4"/>
       <c r="I91" s="4"/>
-      <c r="J91" s="14"/>
+      <c r="J91" s="15"/>
     </row>
     <row r="92" spans="1:10">
       <c r="A92" s="5" t="s">
@@ -3426,7 +3417,7 @@
       <c r="G92" s="6"/>
       <c r="H92" s="6"/>
       <c r="I92" s="6"/>
-      <c r="J92" s="15"/>
+      <c r="J92" s="16"/>
     </row>
     <row r="93" spans="1:10">
       <c r="A93" s="5" t="s">
@@ -3456,7 +3447,7 @@
       <c r="I93" s="6">
         <v>0.0926905158740254</v>
       </c>
-      <c r="J93" s="17">
+      <c r="J93" s="18">
         <f>SUM(B93:I93)</f>
         <v>1.27166155848785</v>
       </c>
@@ -3489,7 +3480,7 @@
       <c r="I94" s="6">
         <v>117</v>
       </c>
-      <c r="J94" s="15">
+      <c r="J94" s="16">
         <v>170</v>
       </c>
     </row>
@@ -3521,11 +3512,11 @@
       <c r="I95" s="6">
         <v>171161</v>
       </c>
-      <c r="J95" s="15"/>
+      <c r="J95" s="16"/>
     </row>
     <row r="96" spans="1:10">
       <c r="A96" s="7"/>
-      <c r="J96" s="16"/>
+      <c r="J96" s="17"/>
     </row>
     <row r="97" spans="1:10">
       <c r="A97" s="5" t="s">
@@ -3539,7 +3530,7 @@
       <c r="G97" s="6"/>
       <c r="H97" s="6"/>
       <c r="I97" s="6"/>
-      <c r="J97" s="15"/>
+      <c r="J97" s="16"/>
     </row>
     <row r="98" spans="1:10">
       <c r="A98" s="5" t="s">
@@ -3569,7 +3560,7 @@
       <c r="I98" s="6">
         <v>0.103230203907768</v>
       </c>
-      <c r="J98" s="17">
+      <c r="J98" s="18">
         <f>SUM(B98:I98)</f>
         <v>1.31676786850071</v>
       </c>
@@ -3602,7 +3593,7 @@
       <c r="I99" s="6">
         <v>151</v>
       </c>
-      <c r="J99" s="15">
+      <c r="J99" s="16">
         <v>729</v>
       </c>
     </row>
@@ -3634,11 +3625,11 @@
       <c r="I100" s="6">
         <v>162603</v>
       </c>
-      <c r="J100" s="15"/>
+      <c r="J100" s="16"/>
     </row>
     <row r="101" spans="1:10">
       <c r="A101" s="7"/>
-      <c r="J101" s="16"/>
+      <c r="J101" s="17"/>
     </row>
     <row r="102" spans="1:10">
       <c r="A102" s="5" t="s">
@@ -3652,7 +3643,7 @@
       <c r="G102" s="6"/>
       <c r="H102" s="6"/>
       <c r="I102" s="6"/>
-      <c r="J102" s="15"/>
+      <c r="J102" s="16"/>
     </row>
     <row r="103" spans="1:10">
       <c r="A103" s="5" t="s">
@@ -3682,7 +3673,7 @@
       <c r="I103" s="6">
         <v>0.0965472395965962</v>
       </c>
-      <c r="J103" s="17">
+      <c r="J103" s="18">
         <v>1.27133999397231</v>
       </c>
     </row>
@@ -3714,39 +3705,39 @@
       <c r="I104" s="6">
         <v>4635</v>
       </c>
-      <c r="J104" s="15">
+      <c r="J104" s="16">
         <v>148014</v>
       </c>
     </row>
     <row r="105" ht="14.25" spans="1:10">
-      <c r="A105" s="12" t="s">
+      <c r="A105" s="13" t="s">
         <v>28</v>
       </c>
-      <c r="B105" s="25">
+      <c r="B105" s="22">
         <v>301514</v>
       </c>
-      <c r="C105" s="25">
+      <c r="C105" s="22">
         <v>260041</v>
       </c>
-      <c r="D105" s="25">
+      <c r="D105" s="22">
         <v>518753</v>
       </c>
-      <c r="E105" s="25">
+      <c r="E105" s="22">
         <v>170290</v>
       </c>
-      <c r="F105" s="25">
+      <c r="F105" s="22">
         <v>169461</v>
       </c>
-      <c r="G105" s="25">
+      <c r="G105" s="22">
         <v>234841</v>
       </c>
-      <c r="H105" s="25">
+      <c r="H105" s="22">
         <v>85281</v>
       </c>
-      <c r="I105" s="25">
+      <c r="I105" s="22">
         <v>171161</v>
       </c>
-      <c r="J105" s="30"/>
+      <c r="J105" s="24"/>
     </row>
     <row r="107" spans="1:10">
       <c r="A107" s="6" t="s">

</xml_diff>

<commit_message>
reInsert algorithm. Not Completed and Not Tested
</commit_message>
<xml_diff>
--- a/overall.xlsx
+++ b/overall.xlsx
@@ -143,10 +143,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="20">
     <font>
@@ -157,15 +157,31 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color theme="0"/>
+      <color rgb="FFFFFFFF"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <color rgb="FF9C0006"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -179,39 +195,15 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <color rgb="FFFA7D00"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <color theme="0"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -233,14 +225,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color rgb="FF3F3F76"/>
       <name val="宋体"/>
@@ -248,16 +232,15 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
       <name val="宋体"/>
-      <charset val="134"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <color rgb="FF9C6500"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -266,13 +249,6 @@
       <b/>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -294,8 +270,32 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -322,7 +322,73 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -334,97 +400,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -436,19 +412,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
+        <fgColor rgb="FFFFFFCC"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -466,7 +430,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
+        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -478,7 +442,31 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6"/>
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -490,19 +478,31 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8"/>
+        <fgColor theme="4" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5"/>
+        <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -669,6 +669,21 @@
       <diagonal/>
     </border>
     <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
       <right/>
       <top style="thin">
@@ -680,16 +695,40 @@
       <diagonal/>
     </border>
     <border>
-      <left style="double">
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
         <color rgb="FF3F3F3F"/>
       </left>
-      <right style="double">
+      <right style="thin">
         <color rgb="FF3F3F3F"/>
       </right>
-      <top style="double">
+      <top style="thin">
         <color rgb="FF3F3F3F"/>
       </top>
-      <bottom style="double">
+      <bottom style="thin">
         <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
@@ -719,36 +758,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
       <top/>
@@ -757,15 +766,6 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
@@ -774,149 +774,149 @@
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="8" borderId="15" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="18" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="17" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="17" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="19" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="17" borderId="16" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="17" borderId="15" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="12" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="14" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="12" borderId="17" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="15" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="14" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="14" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="18" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="10" borderId="16" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="10" borderId="17" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="13" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="19" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -951,9 +951,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
@@ -1444,7 +1441,7 @@
       <c r="F3">
         <v>0.0522827100851127</v>
       </c>
-      <c r="G3" s="25">
+      <c r="G3" s="24">
         <v>0.106926203216301</v>
       </c>
       <c r="H3">
@@ -1470,7 +1467,7 @@
       <c r="A12" t="s">
         <v>12</v>
       </c>
-      <c r="G12" s="26">
+      <c r="G12" s="25">
         <v>0.0629933219692992</v>
       </c>
     </row>
@@ -1523,7 +1520,7 @@
       <c r="I19">
         <v>0.0755164339928472</v>
       </c>
-      <c r="J19" s="27">
+      <c r="J19" s="26">
         <f t="shared" ref="J19:J21" si="0">SUM(B19:I19)</f>
         <v>1.17870842662782</v>
       </c>
@@ -1532,31 +1529,31 @@
       <c r="A20" t="s">
         <v>17</v>
       </c>
-      <c r="B20" s="27">
+      <c r="B20" s="26">
         <v>0.20800686430345</v>
       </c>
-      <c r="C20" s="27">
+      <c r="C20" s="26">
         <v>0.173239206962822</v>
       </c>
-      <c r="D20" s="27">
+      <c r="D20" s="26">
         <v>0.346041541710196</v>
       </c>
-      <c r="E20" s="27">
+      <c r="E20" s="26">
         <v>0.124928278882666</v>
       </c>
-      <c r="F20" s="27">
+      <c r="F20" s="26">
         <v>0.0409924383808026</v>
       </c>
-      <c r="G20" s="27">
+      <c r="G20" s="26">
         <v>0.0453003114127127</v>
       </c>
-      <c r="H20" s="27">
+      <c r="H20" s="26">
         <v>0.0964368086720679</v>
       </c>
-      <c r="I20" s="27">
+      <c r="I20" s="26">
         <v>0.065879029949852</v>
       </c>
-      <c r="J20" s="27">
+      <c r="J20" s="26">
         <f t="shared" si="0"/>
         <v>1.10082448027457</v>
       </c>
@@ -1565,52 +1562,52 @@
       <c r="A21" t="s">
         <v>18</v>
       </c>
-      <c r="B21" s="26">
+      <c r="B21" s="25">
         <v>0.207894527330402</v>
       </c>
-      <c r="C21" s="26">
+      <c r="C21" s="25">
         <v>0.173165858291852</v>
       </c>
-      <c r="D21" s="26">
+      <c r="D21" s="25">
         <v>0.344628020195683</v>
       </c>
-      <c r="E21" s="26">
+      <c r="E21" s="25">
         <v>0.118862297465155</v>
       </c>
-      <c r="F21" s="26">
+      <c r="F21" s="25">
         <v>0.0388983176119749</v>
       </c>
-      <c r="G21" s="26">
+      <c r="G21" s="25">
         <v>0.0422239303614074</v>
       </c>
-      <c r="H21" s="26">
+      <c r="H21" s="25">
         <v>0.0955131594160284</v>
       </c>
-      <c r="I21" s="26">
+      <c r="I21" s="25">
         <v>0.0488732287830458</v>
       </c>
-      <c r="J21" s="26">
+      <c r="J21" s="25">
         <f t="shared" si="0"/>
         <v>1.07005933945555</v>
       </c>
     </row>
     <row r="22" spans="10:10">
-      <c r="J22" s="27"/>
+      <c r="J22" s="26"/>
     </row>
     <row r="23" spans="10:10">
-      <c r="J23" s="27"/>
+      <c r="J23" s="26"/>
     </row>
     <row r="24" spans="10:10">
-      <c r="J24" s="27"/>
+      <c r="J24" s="26"/>
     </row>
     <row r="25" spans="10:10">
-      <c r="J25" s="27"/>
+      <c r="J25" s="26"/>
     </row>
     <row r="26" spans="1:10">
       <c r="A26" t="s">
         <v>19</v>
       </c>
-      <c r="J26" s="27"/>
+      <c r="J26" s="26"/>
     </row>
     <row r="27" spans="1:10">
       <c r="A27" t="s">
@@ -1631,7 +1628,7 @@
       <c r="F27">
         <v>0.0492015604703379</v>
       </c>
-      <c r="G27" s="27">
+      <c r="G27" s="26">
         <v>0.0766396493470802</v>
       </c>
       <c r="H27">
@@ -1640,7 +1637,7 @@
       <c r="I27">
         <v>0.0926905158740254</v>
       </c>
-      <c r="J27" s="27">
+      <c r="J27" s="26">
         <f>SUM(B27:I27)</f>
         <v>1.27166155848785</v>
       </c>
@@ -1664,7 +1661,7 @@
       <c r="F28">
         <v>0.0533366743677525</v>
       </c>
-      <c r="G28" s="25">
+      <c r="G28" s="24">
         <v>0.110748101588701</v>
       </c>
       <c r="H28">
@@ -1673,7 +1670,7 @@
       <c r="I28">
         <v>0.103230203907768</v>
       </c>
-      <c r="J28" s="27">
+      <c r="J28" s="26">
         <f>SUM(B28:I28)</f>
         <v>1.31676786850071</v>
       </c>
@@ -1703,8 +1700,8 @@
   <sheetPr/>
   <dimension ref="A1:J116"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
-      <selection activeCell="J27" sqref="J27"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="A40" sqref="A40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
@@ -1789,7 +1786,7 @@
       <c r="G4" s="4"/>
       <c r="H4" s="4"/>
       <c r="I4" s="4"/>
-      <c r="J4" s="15"/>
+      <c r="J4" s="14"/>
     </row>
     <row r="5" spans="1:10">
       <c r="A5" s="5" t="s">
@@ -1803,7 +1800,7 @@
       <c r="G5" s="6"/>
       <c r="H5" s="6"/>
       <c r="I5" s="6"/>
-      <c r="J5" s="16"/>
+      <c r="J5" s="15"/>
     </row>
     <row r="6" spans="1:10">
       <c r="A6" s="5" t="s">
@@ -1833,7 +1830,7 @@
       <c r="I6" s="6">
         <v>0.0921915925927093</v>
       </c>
-      <c r="J6" s="16">
+      <c r="J6" s="15">
         <f>SUM(B6:I6)</f>
         <v>1.26377434756932</v>
       </c>
@@ -1866,7 +1863,7 @@
       <c r="I7" s="6">
         <v>109</v>
       </c>
-      <c r="J7" s="16">
+      <c r="J7" s="15">
         <v>139</v>
       </c>
     </row>
@@ -1898,11 +1895,11 @@
       <c r="I8" s="6">
         <v>343549</v>
       </c>
-      <c r="J8" s="16"/>
+      <c r="J8" s="15"/>
     </row>
     <row r="9" spans="1:10">
       <c r="A9" s="7"/>
-      <c r="J9" s="17"/>
+      <c r="J9" s="16"/>
     </row>
     <row r="10" spans="1:10">
       <c r="A10" s="5" t="s">
@@ -1916,7 +1913,7 @@
       <c r="G10" s="6"/>
       <c r="H10" s="6"/>
       <c r="I10" s="6"/>
-      <c r="J10" s="16"/>
+      <c r="J10" s="15"/>
     </row>
     <row r="11" spans="1:10">
       <c r="A11" s="5" t="s">
@@ -1946,7 +1943,7 @@
       <c r="I11" s="6">
         <v>0.102423416293936</v>
       </c>
-      <c r="J11" s="16">
+      <c r="J11" s="15">
         <f>SUM(B11:I11)</f>
         <v>1.31083942802335</v>
       </c>
@@ -1979,7 +1976,7 @@
       <c r="I12" s="6">
         <v>221</v>
       </c>
-      <c r="J12" s="16">
+      <c r="J12" s="15">
         <v>1089</v>
       </c>
     </row>
@@ -2011,11 +2008,11 @@
       <c r="I13" s="6">
         <v>430115</v>
       </c>
-      <c r="J13" s="16"/>
+      <c r="J13" s="15"/>
     </row>
     <row r="14" spans="1:10">
       <c r="A14" s="7"/>
-      <c r="J14" s="17"/>
+      <c r="J14" s="16"/>
     </row>
     <row r="15" spans="1:10">
       <c r="A15" s="9" t="s">
@@ -2029,7 +2026,7 @@
       <c r="G15" s="10"/>
       <c r="H15" s="10"/>
       <c r="I15" s="10"/>
-      <c r="J15" s="18"/>
+      <c r="J15" s="17"/>
     </row>
     <row r="16" s="1" customFormat="1" spans="1:10">
       <c r="A16" s="5" t="s">
@@ -2059,7 +2056,7 @@
       <c r="I16" s="10">
         <v>0.107949060989036</v>
       </c>
-      <c r="J16" s="16">
+      <c r="J16" s="15">
         <f>SUM(B16:I16)</f>
         <v>1.32751827014031</v>
       </c>
@@ -2092,7 +2089,7 @@
       <c r="I17" s="10">
         <v>152</v>
       </c>
-      <c r="J17" s="18">
+      <c r="J17" s="17">
         <v>281</v>
       </c>
     </row>
@@ -2124,25 +2121,25 @@
       <c r="I18" s="10">
         <v>421334</v>
       </c>
-      <c r="J18" s="18"/>
+      <c r="J18" s="17"/>
     </row>
     <row r="19" s="1" customFormat="1" spans="1:10">
       <c r="A19" s="11"/>
-      <c r="J19" s="19"/>
+      <c r="J19" s="18"/>
     </row>
     <row r="20" s="1" customFormat="1" spans="1:10">
       <c r="A20" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="B20" s="12"/>
-      <c r="C20" s="12"/>
-      <c r="D20" s="12"/>
-      <c r="E20" s="12"/>
-      <c r="F20" s="12"/>
-      <c r="G20" s="12"/>
-      <c r="H20" s="12"/>
-      <c r="I20" s="12"/>
-      <c r="J20" s="12"/>
+      <c r="B20" s="10"/>
+      <c r="C20" s="10"/>
+      <c r="D20" s="10"/>
+      <c r="E20" s="10"/>
+      <c r="F20" s="10"/>
+      <c r="G20" s="10"/>
+      <c r="H20" s="10"/>
+      <c r="I20" s="10"/>
+      <c r="J20" s="10"/>
     </row>
     <row r="21" s="1" customFormat="1" spans="1:10">
       <c r="A21" s="6" t="s">
@@ -2241,7 +2238,7 @@
     </row>
     <row r="24" s="1" customFormat="1" spans="1:10">
       <c r="A24" s="11"/>
-      <c r="J24" s="19"/>
+      <c r="J24" s="18"/>
     </row>
     <row r="25" s="1" customFormat="1" spans="1:10">
       <c r="A25" s="9" t="s">
@@ -2255,7 +2252,7 @@
       <c r="G25" s="6"/>
       <c r="H25" s="6"/>
       <c r="I25" s="6"/>
-      <c r="J25" s="16"/>
+      <c r="J25" s="15"/>
     </row>
     <row r="26" spans="1:10">
       <c r="A26" s="5" t="s">
@@ -2285,7 +2282,7 @@
       <c r="I26" s="10">
         <v>0.103639895551926</v>
       </c>
-      <c r="J26" s="18">
+      <c r="J26" s="17">
         <f>SUM(B26:I26)</f>
         <v>1.27862632342455</v>
       </c>
@@ -2350,11 +2347,11 @@
       <c r="I28" s="6">
         <v>505491</v>
       </c>
-      <c r="J28" s="18"/>
+      <c r="J28" s="17"/>
     </row>
     <row r="29" spans="1:10">
       <c r="A29" s="7"/>
-      <c r="J29" s="19"/>
+      <c r="J29" s="18"/>
     </row>
     <row r="30" spans="1:10">
       <c r="A30" s="9" t="s">
@@ -2368,7 +2365,7 @@
       <c r="G30" s="6"/>
       <c r="H30" s="6"/>
       <c r="I30" s="6"/>
-      <c r="J30" s="18"/>
+      <c r="J30" s="17"/>
     </row>
     <row r="31" spans="1:10">
       <c r="A31" s="5" t="s">
@@ -2398,7 +2395,7 @@
       <c r="I31" s="10">
         <v>0.096234294786308</v>
       </c>
-      <c r="J31" s="18">
+      <c r="J31" s="17">
         <f>SUM(B31:I31)</f>
         <v>1.26709179991234</v>
       </c>
@@ -2431,7 +2428,7 @@
       <c r="I32" s="10">
         <v>2877</v>
       </c>
-      <c r="J32" s="16">
+      <c r="J32" s="15">
         <v>67058</v>
       </c>
     </row>
@@ -2463,11 +2460,11 @@
       <c r="I33" s="6">
         <v>509904</v>
       </c>
-      <c r="J33" s="16"/>
+      <c r="J33" s="15"/>
     </row>
     <row r="34" spans="1:10">
       <c r="A34" s="7"/>
-      <c r="J34" s="17"/>
+      <c r="J34" s="16"/>
     </row>
     <row r="35" spans="1:10">
       <c r="A35" s="9" t="s">
@@ -2481,7 +2478,7 @@
       <c r="G35" s="6"/>
       <c r="H35" s="6"/>
       <c r="I35" s="6"/>
-      <c r="J35" s="16"/>
+      <c r="J35" s="15"/>
     </row>
     <row r="36" spans="1:10">
       <c r="A36" s="5" t="s">
@@ -2511,7 +2508,7 @@
       <c r="I36" s="10">
         <v>0.0725702160635175</v>
       </c>
-      <c r="J36" s="18">
+      <c r="J36" s="17">
         <f>SUM(B36:I36)</f>
         <v>1.23689739279618</v>
       </c>
@@ -2576,11 +2573,11 @@
       <c r="I38" s="10">
         <v>480276</v>
       </c>
-      <c r="J38" s="18"/>
+      <c r="J38" s="17"/>
     </row>
     <row r="39" spans="1:10">
       <c r="A39" s="7"/>
-      <c r="J39" s="17"/>
+      <c r="J39" s="16"/>
     </row>
     <row r="40" spans="1:10">
       <c r="A40" s="9" t="s">
@@ -2594,7 +2591,7 @@
       <c r="G40" s="6"/>
       <c r="H40" s="6"/>
       <c r="I40" s="6"/>
-      <c r="J40" s="16"/>
+      <c r="J40" s="15"/>
     </row>
     <row r="41" spans="1:10">
       <c r="A41" s="5" t="s">
@@ -2608,7 +2605,7 @@
       <c r="G41" s="10"/>
       <c r="H41" s="10"/>
       <c r="I41" s="10"/>
-      <c r="J41" s="18"/>
+      <c r="J41" s="17"/>
     </row>
     <row r="42" spans="1:10">
       <c r="A42" s="5" t="s">
@@ -2630,7 +2627,7 @@
       <c r="I42" s="10">
         <v>15231</v>
       </c>
-      <c r="J42" s="18"/>
+      <c r="J42" s="17"/>
     </row>
     <row r="43" spans="1:10">
       <c r="A43" s="5" t="s">
@@ -2652,11 +2649,11 @@
       <c r="I43" s="10">
         <v>481500</v>
       </c>
-      <c r="J43" s="18"/>
+      <c r="J43" s="17"/>
     </row>
     <row r="44" spans="1:10">
       <c r="A44" s="7"/>
-      <c r="J44" s="17"/>
+      <c r="J44" s="16"/>
     </row>
     <row r="45" spans="1:10">
       <c r="A45" s="5" t="s">
@@ -2672,7 +2669,7 @@
       </c>
       <c r="H45" s="6"/>
       <c r="I45" s="6"/>
-      <c r="J45" s="16"/>
+      <c r="J45" s="15"/>
     </row>
     <row r="46" spans="1:10">
       <c r="A46" s="5" t="s">
@@ -2686,7 +2683,7 @@
       <c r="G46" s="10"/>
       <c r="H46" s="10"/>
       <c r="I46" s="10"/>
-      <c r="J46" s="18"/>
+      <c r="J46" s="17"/>
     </row>
     <row r="47" spans="1:10">
       <c r="A47" s="5" t="s">
@@ -2700,7 +2697,7 @@
       <c r="G47" s="10"/>
       <c r="H47" s="10"/>
       <c r="I47" s="10"/>
-      <c r="J47" s="18"/>
+      <c r="J47" s="17"/>
     </row>
     <row r="48" spans="1:10">
       <c r="A48" s="5" t="s">
@@ -2714,11 +2711,11 @@
       <c r="G48" s="10"/>
       <c r="H48" s="10"/>
       <c r="I48" s="10"/>
-      <c r="J48" s="18"/>
+      <c r="J48" s="17"/>
     </row>
     <row r="49" spans="1:10">
       <c r="A49" s="7"/>
-      <c r="J49" s="17"/>
+      <c r="J49" s="16"/>
     </row>
     <row r="50" spans="1:10">
       <c r="A50" s="5" t="s">
@@ -2734,7 +2731,7 @@
       </c>
       <c r="H50" s="6"/>
       <c r="I50" s="6"/>
-      <c r="J50" s="16"/>
+      <c r="J50" s="15"/>
     </row>
     <row r="51" spans="1:10">
       <c r="A51" s="5" t="s">
@@ -2748,7 +2745,7 @@
       <c r="G51" s="10"/>
       <c r="H51" s="10"/>
       <c r="I51" s="10"/>
-      <c r="J51" s="18"/>
+      <c r="J51" s="17"/>
     </row>
     <row r="52" spans="1:10">
       <c r="A52" s="5" t="s">
@@ -2762,7 +2759,7 @@
       <c r="G52" s="10"/>
       <c r="H52" s="10"/>
       <c r="I52" s="10"/>
-      <c r="J52" s="18"/>
+      <c r="J52" s="17"/>
     </row>
     <row r="53" spans="1:10">
       <c r="A53" s="5" t="s">
@@ -2776,11 +2773,11 @@
       <c r="G53" s="10"/>
       <c r="H53" s="10"/>
       <c r="I53" s="10"/>
-      <c r="J53" s="18"/>
+      <c r="J53" s="17"/>
     </row>
     <row r="54" spans="1:10">
       <c r="A54" s="7"/>
-      <c r="J54" s="17"/>
+      <c r="J54" s="16"/>
     </row>
     <row r="55" spans="1:10">
       <c r="A55" s="5" t="s">
@@ -2796,7 +2793,7 @@
       </c>
       <c r="H55" s="6"/>
       <c r="I55" s="6"/>
-      <c r="J55" s="16"/>
+      <c r="J55" s="15"/>
     </row>
     <row r="56" spans="1:10">
       <c r="A56" s="5" t="s">
@@ -2810,7 +2807,7 @@
       <c r="G56" s="10"/>
       <c r="H56" s="10"/>
       <c r="I56" s="10"/>
-      <c r="J56" s="18"/>
+      <c r="J56" s="17"/>
     </row>
     <row r="57" spans="1:10">
       <c r="A57" s="5" t="s">
@@ -2824,7 +2821,7 @@
       <c r="G57" s="10"/>
       <c r="H57" s="10"/>
       <c r="I57" s="10"/>
-      <c r="J57" s="18"/>
+      <c r="J57" s="17"/>
     </row>
     <row r="58" spans="1:10">
       <c r="A58" s="5" t="s">
@@ -2838,11 +2835,11 @@
       <c r="G58" s="10"/>
       <c r="H58" s="10"/>
       <c r="I58" s="10"/>
-      <c r="J58" s="18"/>
+      <c r="J58" s="17"/>
     </row>
     <row r="59" spans="1:10">
       <c r="A59" s="7"/>
-      <c r="J59" s="17"/>
+      <c r="J59" s="16"/>
     </row>
     <row r="60" spans="1:10">
       <c r="A60" s="5" t="s">
@@ -2858,7 +2855,7 @@
       </c>
       <c r="H60" s="6"/>
       <c r="I60" s="6"/>
-      <c r="J60" s="16"/>
+      <c r="J60" s="15"/>
     </row>
     <row r="61" spans="1:10">
       <c r="A61" s="5" t="s">
@@ -2872,7 +2869,7 @@
       <c r="G61" s="10"/>
       <c r="H61" s="10"/>
       <c r="I61" s="10"/>
-      <c r="J61" s="18"/>
+      <c r="J61" s="17"/>
     </row>
     <row r="62" spans="1:10">
       <c r="A62" s="5" t="s">
@@ -2886,21 +2883,21 @@
       <c r="G62" s="10"/>
       <c r="H62" s="10"/>
       <c r="I62" s="10"/>
-      <c r="J62" s="18"/>
+      <c r="J62" s="17"/>
     </row>
     <row r="63" ht="14.25" spans="1:10">
-      <c r="A63" s="13" t="s">
+      <c r="A63" s="12" t="s">
         <v>28</v>
       </c>
-      <c r="B63" s="14"/>
-      <c r="C63" s="14"/>
-      <c r="D63" s="14"/>
-      <c r="E63" s="14"/>
-      <c r="F63" s="14"/>
-      <c r="G63" s="14"/>
-      <c r="H63" s="14"/>
-      <c r="I63" s="14"/>
-      <c r="J63" s="20"/>
+      <c r="B63" s="13"/>
+      <c r="C63" s="13"/>
+      <c r="D63" s="13"/>
+      <c r="E63" s="13"/>
+      <c r="F63" s="13"/>
+      <c r="G63" s="13"/>
+      <c r="H63" s="13"/>
+      <c r="I63" s="13"/>
+      <c r="J63" s="19"/>
     </row>
     <row r="66" ht="14.25"/>
     <row r="67" spans="1:10">
@@ -2929,7 +2926,7 @@
       <c r="I67" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="J67" s="15" t="s">
+      <c r="J67" s="14" t="s">
         <v>8</v>
       </c>
     </row>
@@ -2961,11 +2958,11 @@
       <c r="I68" s="6">
         <v>855802</v>
       </c>
-      <c r="J68" s="16"/>
+      <c r="J68" s="15"/>
     </row>
     <row r="69" spans="1:10">
       <c r="A69" s="7"/>
-      <c r="J69" s="17"/>
+      <c r="J69" s="16"/>
     </row>
     <row r="70" spans="1:10">
       <c r="A70" s="5" t="s">
@@ -2979,7 +2976,7 @@
       <c r="G70" s="6"/>
       <c r="H70" s="6"/>
       <c r="I70" s="6"/>
-      <c r="J70" s="16"/>
+      <c r="J70" s="15"/>
     </row>
     <row r="71" spans="1:10">
       <c r="A71" s="7" t="s">
@@ -2993,7 +2990,7 @@
       <c r="G71" s="6"/>
       <c r="H71" s="6"/>
       <c r="I71" s="6"/>
-      <c r="J71" s="16"/>
+      <c r="J71" s="15"/>
     </row>
     <row r="72" spans="1:10">
       <c r="A72" s="5" t="s">
@@ -3023,7 +3020,7 @@
       <c r="I72" s="6">
         <v>0.0755164339928472</v>
       </c>
-      <c r="J72" s="18">
+      <c r="J72" s="17">
         <f>SUM(B72:I72)</f>
         <v>1.17870842662782</v>
       </c>
@@ -3056,7 +3053,7 @@
       <c r="I73" s="6">
         <v>634</v>
       </c>
-      <c r="J73" s="16">
+      <c r="J73" s="15">
         <v>1792</v>
       </c>
     </row>
@@ -3088,11 +3085,11 @@
       <c r="I74" s="6">
         <v>171161</v>
       </c>
-      <c r="J74" s="16"/>
+      <c r="J74" s="15"/>
     </row>
     <row r="75" spans="1:10">
       <c r="A75" s="7"/>
-      <c r="J75" s="17"/>
+      <c r="J75" s="16"/>
     </row>
     <row r="76" s="2" customFormat="1" spans="1:10">
       <c r="A76" s="5" t="s">
@@ -3106,7 +3103,7 @@
       <c r="G76" s="6"/>
       <c r="H76" s="6"/>
       <c r="I76" s="6"/>
-      <c r="J76" s="16"/>
+      <c r="J76" s="15"/>
     </row>
     <row r="77" s="2" customFormat="1" spans="1:10">
       <c r="A77" s="5" t="s">
@@ -3136,7 +3133,7 @@
       <c r="I77" s="10">
         <v>0.065879029949852</v>
       </c>
-      <c r="J77" s="18">
+      <c r="J77" s="17">
         <f>SUM(B77:I77)</f>
         <v>1.10082448027457</v>
       </c>
@@ -3169,7 +3166,7 @@
       <c r="I78" s="6">
         <v>633</v>
       </c>
-      <c r="J78" s="16">
+      <c r="J78" s="15">
         <v>1864</v>
       </c>
     </row>
@@ -3201,7 +3198,7 @@
       <c r="I79" s="6">
         <v>162603</v>
       </c>
-      <c r="J79" s="16"/>
+      <c r="J79" s="15"/>
     </row>
     <row r="80" customFormat="1" spans="1:10">
       <c r="A80" s="7"/>
@@ -3213,7 +3210,7 @@
       <c r="G80" s="2"/>
       <c r="H80" s="2"/>
       <c r="I80" s="2"/>
-      <c r="J80" s="17"/>
+      <c r="J80" s="16"/>
     </row>
     <row r="81" spans="1:10">
       <c r="A81" s="5" t="s">
@@ -3227,37 +3224,37 @@
       <c r="G81" s="6"/>
       <c r="H81" s="6"/>
       <c r="I81" s="6"/>
-      <c r="J81" s="16"/>
+      <c r="J81" s="15"/>
     </row>
     <row r="82" spans="1:10">
       <c r="A82" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="B82" s="21">
+      <c r="B82" s="20">
         <v>0.207894527330402</v>
       </c>
-      <c r="C82" s="21">
+      <c r="C82" s="20">
         <v>0.173165858291852</v>
       </c>
-      <c r="D82" s="21">
+      <c r="D82" s="20">
         <v>0.344628020195683</v>
       </c>
-      <c r="E82" s="21">
+      <c r="E82" s="20">
         <v>0.118862297465155</v>
       </c>
-      <c r="F82" s="21">
+      <c r="F82" s="20">
         <v>0.0388983176119749</v>
       </c>
-      <c r="G82" s="21">
+      <c r="G82" s="20">
         <v>0.0422239303614074</v>
       </c>
-      <c r="H82" s="21">
+      <c r="H82" s="20">
         <v>0.0955131594160284</v>
       </c>
-      <c r="I82" s="21">
+      <c r="I82" s="20">
         <v>0.0488732287830458</v>
       </c>
-      <c r="J82" s="23">
+      <c r="J82" s="22">
         <f>SUM(B82:I82)</f>
         <v>1.07005933945555</v>
       </c>
@@ -3290,7 +3287,7 @@
       <c r="I83" s="6">
         <v>5050</v>
       </c>
-      <c r="J83" s="16">
+      <c r="J83" s="15">
         <v>149985</v>
       </c>
     </row>
@@ -3322,11 +3319,11 @@
       <c r="I84" s="6">
         <v>171161</v>
       </c>
-      <c r="J84" s="16"/>
+      <c r="J84" s="15"/>
     </row>
     <row r="85" spans="1:10">
       <c r="A85" s="7"/>
-      <c r="J85" s="17"/>
+      <c r="J85" s="16"/>
     </row>
     <row r="86" s="2" customFormat="1" spans="1:10">
       <c r="A86" s="5" t="s">
@@ -3340,7 +3337,7 @@
       <c r="G86" s="6"/>
       <c r="H86" s="6"/>
       <c r="I86" s="6"/>
-      <c r="J86" s="16"/>
+      <c r="J86" s="15"/>
     </row>
     <row r="87" s="2" customFormat="1" spans="1:10">
       <c r="A87" s="5" t="s">
@@ -3356,7 +3353,7 @@
       </c>
       <c r="H87" s="10"/>
       <c r="I87" s="10"/>
-      <c r="J87" s="18"/>
+      <c r="J87" s="17"/>
     </row>
     <row r="88" s="2" customFormat="1" spans="1:10">
       <c r="A88" s="5" t="s">
@@ -3372,23 +3369,23 @@
       </c>
       <c r="H88" s="10"/>
       <c r="I88" s="10"/>
-      <c r="J88" s="18"/>
+      <c r="J88" s="17"/>
     </row>
     <row r="89" s="2" customFormat="1" ht="14.25" spans="1:10">
-      <c r="A89" s="13" t="s">
+      <c r="A89" s="12" t="s">
         <v>28</v>
       </c>
-      <c r="B89" s="14"/>
-      <c r="C89" s="14"/>
-      <c r="D89" s="14"/>
-      <c r="E89" s="14"/>
-      <c r="F89" s="14"/>
-      <c r="G89" s="14">
+      <c r="B89" s="13"/>
+      <c r="C89" s="13"/>
+      <c r="D89" s="13"/>
+      <c r="E89" s="13"/>
+      <c r="F89" s="13"/>
+      <c r="G89" s="13">
         <v>156561</v>
       </c>
-      <c r="H89" s="14"/>
-      <c r="I89" s="14"/>
-      <c r="J89" s="20"/>
+      <c r="H89" s="13"/>
+      <c r="I89" s="13"/>
+      <c r="J89" s="19"/>
     </row>
     <row r="90" ht="14.25"/>
     <row r="91" spans="1:10">
@@ -3403,7 +3400,7 @@
       <c r="G91" s="4"/>
       <c r="H91" s="4"/>
       <c r="I91" s="4"/>
-      <c r="J91" s="15"/>
+      <c r="J91" s="14"/>
     </row>
     <row r="92" spans="1:10">
       <c r="A92" s="5" t="s">
@@ -3417,7 +3414,7 @@
       <c r="G92" s="6"/>
       <c r="H92" s="6"/>
       <c r="I92" s="6"/>
-      <c r="J92" s="16"/>
+      <c r="J92" s="15"/>
     </row>
     <row r="93" spans="1:10">
       <c r="A93" s="5" t="s">
@@ -3447,7 +3444,7 @@
       <c r="I93" s="6">
         <v>0.0926905158740254</v>
       </c>
-      <c r="J93" s="18">
+      <c r="J93" s="17">
         <f>SUM(B93:I93)</f>
         <v>1.27166155848785</v>
       </c>
@@ -3480,7 +3477,7 @@
       <c r="I94" s="6">
         <v>117</v>
       </c>
-      <c r="J94" s="16">
+      <c r="J94" s="15">
         <v>170</v>
       </c>
     </row>
@@ -3512,11 +3509,11 @@
       <c r="I95" s="6">
         <v>171161</v>
       </c>
-      <c r="J95" s="16"/>
+      <c r="J95" s="15"/>
     </row>
     <row r="96" spans="1:10">
       <c r="A96" s="7"/>
-      <c r="J96" s="17"/>
+      <c r="J96" s="16"/>
     </row>
     <row r="97" spans="1:10">
       <c r="A97" s="5" t="s">
@@ -3530,7 +3527,7 @@
       <c r="G97" s="6"/>
       <c r="H97" s="6"/>
       <c r="I97" s="6"/>
-      <c r="J97" s="16"/>
+      <c r="J97" s="15"/>
     </row>
     <row r="98" spans="1:10">
       <c r="A98" s="5" t="s">
@@ -3560,7 +3557,7 @@
       <c r="I98" s="6">
         <v>0.103230203907768</v>
       </c>
-      <c r="J98" s="18">
+      <c r="J98" s="17">
         <f>SUM(B98:I98)</f>
         <v>1.31676786850071</v>
       </c>
@@ -3593,7 +3590,7 @@
       <c r="I99" s="6">
         <v>151</v>
       </c>
-      <c r="J99" s="16">
+      <c r="J99" s="15">
         <v>729</v>
       </c>
     </row>
@@ -3625,11 +3622,11 @@
       <c r="I100" s="6">
         <v>162603</v>
       </c>
-      <c r="J100" s="16"/>
+      <c r="J100" s="15"/>
     </row>
     <row r="101" spans="1:10">
       <c r="A101" s="7"/>
-      <c r="J101" s="17"/>
+      <c r="J101" s="16"/>
     </row>
     <row r="102" spans="1:10">
       <c r="A102" s="5" t="s">
@@ -3643,7 +3640,7 @@
       <c r="G102" s="6"/>
       <c r="H102" s="6"/>
       <c r="I102" s="6"/>
-      <c r="J102" s="16"/>
+      <c r="J102" s="15"/>
     </row>
     <row r="103" spans="1:10">
       <c r="A103" s="5" t="s">
@@ -3673,7 +3670,7 @@
       <c r="I103" s="6">
         <v>0.0965472395965962</v>
       </c>
-      <c r="J103" s="18">
+      <c r="J103" s="17">
         <v>1.27133999397231</v>
       </c>
     </row>
@@ -3705,39 +3702,39 @@
       <c r="I104" s="6">
         <v>4635</v>
       </c>
-      <c r="J104" s="16">
+      <c r="J104" s="15">
         <v>148014</v>
       </c>
     </row>
     <row r="105" ht="14.25" spans="1:10">
-      <c r="A105" s="13" t="s">
+      <c r="A105" s="12" t="s">
         <v>28</v>
       </c>
-      <c r="B105" s="22">
+      <c r="B105" s="21">
         <v>301514</v>
       </c>
-      <c r="C105" s="22">
+      <c r="C105" s="21">
         <v>260041</v>
       </c>
-      <c r="D105" s="22">
+      <c r="D105" s="21">
         <v>518753</v>
       </c>
-      <c r="E105" s="22">
+      <c r="E105" s="21">
         <v>170290</v>
       </c>
-      <c r="F105" s="22">
+      <c r="F105" s="21">
         <v>169461</v>
       </c>
-      <c r="G105" s="22">
+      <c r="G105" s="21">
         <v>234841</v>
       </c>
-      <c r="H105" s="22">
+      <c r="H105" s="21">
         <v>85281</v>
       </c>
-      <c r="I105" s="22">
+      <c r="I105" s="21">
         <v>171161</v>
       </c>
-      <c r="J105" s="24"/>
+      <c r="J105" s="23"/>
     </row>
     <row r="107" spans="1:10">
       <c r="A107" s="6" t="s">

</xml_diff>

<commit_message>
Add more data and modify the concurrentBasicCiAlgo with reinsert
</commit_message>
<xml_diff>
--- a/overall.xlsx
+++ b/overall.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48">
   <si>
     <t>model1</t>
   </si>
@@ -102,7 +102,13 @@
     <t>Time</t>
   </si>
   <si>
+    <t>17_07_19_03_29_17_0_1_500_4/Concurrent Time</t>
+  </si>
+  <si>
     <t>Min-Point</t>
+  </si>
+  <si>
+    <t>17_07_19_07_15_58_1_1_500_4/Concurrent Time</t>
   </si>
   <si>
     <t>17_07_13_06_28_57_1_500_500_0</t>
@@ -127,6 +133,21 @@
   </si>
   <si>
     <t>OpenSource_with_reinsert</t>
+  </si>
+  <si>
+    <t>0.01/JustCount/mycode_reinsert</t>
+  </si>
+  <si>
+    <t>0.01/Rank/mycode_reinsert</t>
+  </si>
+  <si>
+    <t>17_07_19_02_59_23_0_1_500_5</t>
+  </si>
+  <si>
+    <t>17_07_20_16_16_33_0_1_500_5</t>
+  </si>
+  <si>
+    <t>17_07_19_01_59_02_1_1_500_5</t>
   </si>
   <si>
     <t>30_1_500_reinsert</t>
@@ -927,7 +948,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1021,7 +1042,13 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1">
@@ -1471,7 +1498,7 @@
       <c r="F3">
         <v>0.0522827100851127</v>
       </c>
-      <c r="G3" s="32">
+      <c r="G3" s="34">
         <v>0.106926203216301</v>
       </c>
       <c r="H3">
@@ -1497,7 +1524,7 @@
       <c r="A12" t="s">
         <v>12</v>
       </c>
-      <c r="G12" s="33">
+      <c r="G12" s="35">
         <v>0.0629933219692992</v>
       </c>
     </row>
@@ -1550,7 +1577,7 @@
       <c r="I19">
         <v>0.0755164339928472</v>
       </c>
-      <c r="J19" s="34">
+      <c r="J19" s="36">
         <f t="shared" ref="J19:J21" si="0">SUM(B19:I19)</f>
         <v>1.17870842662782</v>
       </c>
@@ -1559,31 +1586,31 @@
       <c r="A20" t="s">
         <v>17</v>
       </c>
-      <c r="B20" s="34">
+      <c r="B20" s="36">
         <v>0.20800686430345</v>
       </c>
-      <c r="C20" s="34">
+      <c r="C20" s="36">
         <v>0.173239206962822</v>
       </c>
-      <c r="D20" s="34">
+      <c r="D20" s="36">
         <v>0.346041541710196</v>
       </c>
-      <c r="E20" s="34">
+      <c r="E20" s="36">
         <v>0.124928278882666</v>
       </c>
-      <c r="F20" s="34">
+      <c r="F20" s="36">
         <v>0.0409924383808026</v>
       </c>
-      <c r="G20" s="34">
+      <c r="G20" s="36">
         <v>0.0453003114127127</v>
       </c>
-      <c r="H20" s="34">
+      <c r="H20" s="36">
         <v>0.0964368086720679</v>
       </c>
-      <c r="I20" s="34">
+      <c r="I20" s="36">
         <v>0.065879029949852</v>
       </c>
-      <c r="J20" s="34">
+      <c r="J20" s="36">
         <f t="shared" si="0"/>
         <v>1.10082448027457</v>
       </c>
@@ -1592,52 +1619,52 @@
       <c r="A21" t="s">
         <v>18</v>
       </c>
-      <c r="B21" s="33">
+      <c r="B21" s="35">
         <v>0.207894527330402</v>
       </c>
-      <c r="C21" s="33">
+      <c r="C21" s="35">
         <v>0.173165858291852</v>
       </c>
-      <c r="D21" s="33">
+      <c r="D21" s="35">
         <v>0.344628020195683</v>
       </c>
-      <c r="E21" s="33">
+      <c r="E21" s="35">
         <v>0.118862297465155</v>
       </c>
-      <c r="F21" s="33">
+      <c r="F21" s="35">
         <v>0.0388983176119749</v>
       </c>
-      <c r="G21" s="33">
+      <c r="G21" s="35">
         <v>0.0422239303614074</v>
       </c>
-      <c r="H21" s="33">
+      <c r="H21" s="35">
         <v>0.0955131594160284</v>
       </c>
-      <c r="I21" s="33">
+      <c r="I21" s="35">
         <v>0.0488732287830458</v>
       </c>
-      <c r="J21" s="33">
+      <c r="J21" s="35">
         <f t="shared" si="0"/>
         <v>1.07005933945555</v>
       </c>
     </row>
     <row r="22" spans="10:10">
-      <c r="J22" s="34"/>
+      <c r="J22" s="36"/>
     </row>
     <row r="23" spans="10:10">
-      <c r="J23" s="34"/>
+      <c r="J23" s="36"/>
     </row>
     <row r="24" spans="10:10">
-      <c r="J24" s="34"/>
+      <c r="J24" s="36"/>
     </row>
     <row r="25" spans="10:10">
-      <c r="J25" s="34"/>
+      <c r="J25" s="36"/>
     </row>
     <row r="26" spans="1:10">
       <c r="A26" t="s">
         <v>19</v>
       </c>
-      <c r="J26" s="34"/>
+      <c r="J26" s="36"/>
     </row>
     <row r="27" spans="1:10">
       <c r="A27" t="s">
@@ -1658,7 +1685,7 @@
       <c r="F27">
         <v>0.0492015604703379</v>
       </c>
-      <c r="G27" s="34">
+      <c r="G27" s="36">
         <v>0.0766396493470802</v>
       </c>
       <c r="H27">
@@ -1667,7 +1694,7 @@
       <c r="I27">
         <v>0.0926905158740254</v>
       </c>
-      <c r="J27" s="34">
+      <c r="J27" s="36">
         <f>SUM(B27:I27)</f>
         <v>1.27166155848785</v>
       </c>
@@ -1691,7 +1718,7 @@
       <c r="F28">
         <v>0.0533366743677525</v>
       </c>
-      <c r="G28" s="32">
+      <c r="G28" s="34">
         <v>0.110748101588701</v>
       </c>
       <c r="H28">
@@ -1700,7 +1727,7 @@
       <c r="I28">
         <v>0.103230203907768</v>
       </c>
-      <c r="J28" s="34">
+      <c r="J28" s="36">
         <f>SUM(B28:I28)</f>
         <v>1.31676786850071</v>
       </c>
@@ -1728,21 +1755,27 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr/>
-  <dimension ref="A1:J121"/>
+  <dimension ref="A1:AF123"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I42" sqref="I42"/>
+    <sheetView tabSelected="1" topLeftCell="R61" workbookViewId="0">
+      <selection activeCell="AE84" sqref="AE84"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
   <cols>
-    <col min="1" max="1" width="36" style="2" customWidth="1"/>
+    <col min="1" max="1" width="48.25" style="2" customWidth="1"/>
     <col min="2" max="3" width="12.625" style="2" customWidth="1"/>
     <col min="4" max="4" width="11.5" style="2" customWidth="1"/>
     <col min="5" max="7" width="12.625" style="2" customWidth="1"/>
     <col min="8" max="8" width="11.5" style="2" customWidth="1"/>
     <col min="9" max="10" width="12.625" style="2" customWidth="1"/>
-    <col min="11" max="16384" width="9" style="2"/>
+    <col min="11" max="11" width="9" style="2"/>
+    <col min="12" max="12" width="33.75" style="2" customWidth="1"/>
+    <col min="13" max="21" width="12.625" style="2" customWidth="1"/>
+    <col min="22" max="22" width="9" style="2"/>
+    <col min="23" max="23" width="33.75" style="2" customWidth="1"/>
+    <col min="24" max="32" width="12.625" style="2" customWidth="1"/>
+    <col min="33" max="16384" width="9" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10">
@@ -1904,994 +1937,1030 @@
         <v>28</v>
       </c>
       <c r="B8" s="7">
+        <v>9014</v>
+      </c>
+      <c r="C8" s="7">
+        <v>8950</v>
+      </c>
+      <c r="D8" s="7">
+        <v>9831</v>
+      </c>
+      <c r="E8" s="7">
+        <v>8346</v>
+      </c>
+      <c r="F8" s="7">
+        <v>9789</v>
+      </c>
+      <c r="G8" s="7">
+        <v>13594</v>
+      </c>
+      <c r="H8" s="7">
+        <v>2424</v>
+      </c>
+      <c r="I8" s="7">
+        <v>5519</v>
+      </c>
+      <c r="J8" s="14">
+        <v>13594</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10">
+      <c r="A9" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="B9" s="7">
         <v>583934</v>
       </c>
-      <c r="C8" s="7">
+      <c r="C9" s="7">
         <v>573704</v>
       </c>
-      <c r="D8" s="7">
+      <c r="D9" s="7">
         <v>719722</v>
       </c>
-      <c r="E8" s="7">
+      <c r="E9" s="7">
         <v>534504</v>
       </c>
-      <c r="F8" s="7">
+      <c r="F9" s="7">
         <v>529690</v>
       </c>
-      <c r="G8" s="7">
+      <c r="G9" s="7">
         <v>1054742</v>
       </c>
-      <c r="H8" s="7">
+      <c r="H9" s="7">
         <v>151903</v>
       </c>
-      <c r="I8" s="7">
+      <c r="I9" s="7">
         <v>343549</v>
       </c>
-      <c r="J8" s="14"/>
-    </row>
-    <row r="9" spans="1:10">
-      <c r="A9" s="8"/>
-      <c r="J9" s="15"/>
+      <c r="J9" s="14"/>
     </row>
     <row r="10" spans="1:10">
-      <c r="A10" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="B10" s="7"/>
-      <c r="C10" s="7"/>
-      <c r="D10" s="7"/>
-      <c r="E10" s="7"/>
-      <c r="F10" s="7"/>
-      <c r="G10" s="7"/>
-      <c r="H10" s="7"/>
-      <c r="I10" s="7"/>
-      <c r="J10" s="14"/>
+      <c r="A10" s="8"/>
+      <c r="J10" s="15"/>
     </row>
     <row r="11" spans="1:10">
       <c r="A11" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="B11" s="7">
-        <v>0.225286283054075</v>
-      </c>
-      <c r="C11" s="7">
-        <v>0.187794520641569</v>
-      </c>
-      <c r="D11" s="7">
-        <v>0.380938188780155</v>
-      </c>
-      <c r="E11" s="7">
-        <v>0.143376574520423</v>
-      </c>
-      <c r="F11" s="7">
-        <v>0.0522827100851127</v>
-      </c>
-      <c r="G11" s="9">
-        <v>0.106926203216301</v>
-      </c>
-      <c r="H11" s="7">
-        <v>0.111811531431783</v>
-      </c>
-      <c r="I11" s="7">
-        <v>0.102423416293936</v>
-      </c>
-      <c r="J11" s="14">
-        <f>SUM(B11:I11)</f>
-        <v>1.31083942802335</v>
-      </c>
+        <v>10</v>
+      </c>
+      <c r="B11" s="7"/>
+      <c r="C11" s="7"/>
+      <c r="D11" s="7"/>
+      <c r="E11" s="7"/>
+      <c r="F11" s="7"/>
+      <c r="G11" s="7"/>
+      <c r="H11" s="7"/>
+      <c r="I11" s="7"/>
+      <c r="J11" s="14"/>
     </row>
     <row r="12" spans="1:10">
       <c r="A12" s="6" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B12" s="7">
-        <v>379</v>
+        <v>0.225286283054075</v>
       </c>
       <c r="C12" s="7">
-        <v>277</v>
+        <v>0.187794520641569</v>
       </c>
       <c r="D12" s="7">
-        <v>437</v>
+        <v>0.380938188780155</v>
       </c>
       <c r="E12" s="7">
-        <v>210</v>
+        <v>0.143376574520423</v>
       </c>
       <c r="F12" s="7">
-        <v>817</v>
-      </c>
-      <c r="G12" s="7">
-        <v>65</v>
+        <v>0.0522827100851127</v>
+      </c>
+      <c r="G12" s="9">
+        <v>0.106926203216301</v>
       </c>
       <c r="H12" s="7">
-        <v>1089</v>
+        <v>0.111811531431783</v>
       </c>
       <c r="I12" s="7">
-        <v>221</v>
+        <v>0.102423416293936</v>
       </c>
       <c r="J12" s="14">
-        <v>1089</v>
+        <f>SUM(B12:I12)</f>
+        <v>1.31083942802335</v>
       </c>
     </row>
     <row r="13" spans="1:10">
       <c r="A13" s="6" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B13" s="7">
+        <v>379</v>
+      </c>
+      <c r="C13" s="7">
+        <v>277</v>
+      </c>
+      <c r="D13" s="7">
+        <v>437</v>
+      </c>
+      <c r="E13" s="7">
+        <v>210</v>
+      </c>
+      <c r="F13" s="7">
+        <v>817</v>
+      </c>
+      <c r="G13" s="7">
+        <v>65</v>
+      </c>
+      <c r="H13" s="7">
+        <v>1089</v>
+      </c>
+      <c r="I13" s="7">
+        <v>221</v>
+      </c>
+      <c r="J13" s="14">
+        <v>1089</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10">
+      <c r="A14" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="B14" s="7">
+        <v>11340</v>
+      </c>
+      <c r="C14" s="7">
+        <v>11503</v>
+      </c>
+      <c r="D14" s="7">
+        <v>12019</v>
+      </c>
+      <c r="E14" s="7">
+        <v>10611</v>
+      </c>
+      <c r="F14" s="7">
+        <v>13407</v>
+      </c>
+      <c r="G14" s="7">
+        <v>17334</v>
+      </c>
+      <c r="H14" s="7">
+        <v>5942</v>
+      </c>
+      <c r="I14" s="7">
+        <v>7573</v>
+      </c>
+      <c r="J14" s="14">
+        <v>17334</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10">
+      <c r="A15" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="B15" s="7">
         <v>675627</v>
       </c>
-      <c r="C13" s="7">
+      <c r="C15" s="7">
         <v>677816</v>
       </c>
-      <c r="D13" s="7">
+      <c r="D15" s="7">
         <v>779027</v>
       </c>
-      <c r="E13" s="7">
+      <c r="E15" s="7">
         <v>632197</v>
       </c>
-      <c r="F13" s="7">
+      <c r="F15" s="7">
         <v>718846</v>
       </c>
-      <c r="G13" s="7">
+      <c r="G15" s="7">
         <v>1293988</v>
       </c>
-      <c r="H13" s="7">
+      <c r="H15" s="7">
         <v>186872</v>
       </c>
-      <c r="I13" s="7">
+      <c r="I15" s="7">
         <v>430115</v>
       </c>
-      <c r="J13" s="14"/>
-    </row>
-    <row r="14" spans="1:10">
-      <c r="A14" s="8"/>
-      <c r="J14" s="15"/>
-    </row>
-    <row r="15" spans="1:10">
-      <c r="A15" s="10" t="s">
-        <v>29</v>
-      </c>
-      <c r="B15" s="11"/>
-      <c r="C15" s="11"/>
-      <c r="D15" s="11"/>
-      <c r="E15" s="11"/>
-      <c r="F15" s="11"/>
-      <c r="G15" s="11"/>
-      <c r="H15" s="11"/>
-      <c r="I15" s="11"/>
-      <c r="J15" s="16"/>
-    </row>
-    <row r="16" s="1" customFormat="1" spans="1:10">
-      <c r="A16" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="B16" s="11">
-        <v>0.225470908622326</v>
-      </c>
-      <c r="C16" s="11">
-        <v>0.187969567075629</v>
-      </c>
-      <c r="D16" s="11">
-        <v>0.381243807789244</v>
-      </c>
-      <c r="E16" s="11">
-        <v>0.143543120492896</v>
-      </c>
-      <c r="F16" s="11">
-        <v>0.0524463942386956</v>
-      </c>
-      <c r="G16" s="11">
-        <v>0.116477647084075</v>
-      </c>
-      <c r="H16" s="11">
-        <v>0.11241776384841</v>
-      </c>
-      <c r="I16" s="11">
-        <v>0.107949060989036</v>
-      </c>
-      <c r="J16" s="14">
-        <f>SUM(B16:I16)</f>
-        <v>1.32751827014031</v>
-      </c>
-    </row>
-    <row r="17" s="1" customFormat="1" spans="1:10">
-      <c r="A17" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="B17" s="11">
-        <v>246</v>
-      </c>
-      <c r="C17" s="11">
-        <v>205</v>
-      </c>
-      <c r="D17" s="11">
-        <v>281</v>
-      </c>
-      <c r="E17" s="11">
-        <v>163</v>
-      </c>
-      <c r="F17" s="11">
-        <v>274</v>
-      </c>
-      <c r="G17" s="11">
-        <v>52</v>
-      </c>
-      <c r="H17" s="11">
-        <v>212</v>
-      </c>
-      <c r="I17" s="11">
-        <v>152</v>
-      </c>
-      <c r="J17" s="16">
-        <v>281</v>
-      </c>
+      <c r="J15" s="14"/>
+    </row>
+    <row r="16" spans="1:10">
+      <c r="A16" s="8"/>
+      <c r="J16" s="15"/>
+    </row>
+    <row r="17" spans="1:10">
+      <c r="A17" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="B17" s="11"/>
+      <c r="C17" s="11"/>
+      <c r="D17" s="11"/>
+      <c r="E17" s="11"/>
+      <c r="F17" s="11"/>
+      <c r="G17" s="11"/>
+      <c r="H17" s="11"/>
+      <c r="I17" s="11"/>
+      <c r="J17" s="16"/>
     </row>
     <row r="18" s="1" customFormat="1" spans="1:10">
       <c r="A18" s="6" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B18" s="11">
+        <v>0.225470908622326</v>
+      </c>
+      <c r="C18" s="11">
+        <v>0.187969567075629</v>
+      </c>
+      <c r="D18" s="11">
+        <v>0.381243807789244</v>
+      </c>
+      <c r="E18" s="11">
+        <v>0.143543120492896</v>
+      </c>
+      <c r="F18" s="11">
+        <v>0.0524463942386956</v>
+      </c>
+      <c r="G18" s="11">
+        <v>0.116477647084075</v>
+      </c>
+      <c r="H18" s="11">
+        <v>0.11241776384841</v>
+      </c>
+      <c r="I18" s="11">
+        <v>0.107949060989036</v>
+      </c>
+      <c r="J18" s="14">
+        <f>SUM(B18:I18)</f>
+        <v>1.32751827014031</v>
+      </c>
+    </row>
+    <row r="19" s="1" customFormat="1" spans="1:10">
+      <c r="A19" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="B19" s="11">
+        <v>246</v>
+      </c>
+      <c r="C19" s="11">
+        <v>205</v>
+      </c>
+      <c r="D19" s="11">
+        <v>281</v>
+      </c>
+      <c r="E19" s="11">
+        <v>163</v>
+      </c>
+      <c r="F19" s="11">
+        <v>274</v>
+      </c>
+      <c r="G19" s="11">
+        <v>52</v>
+      </c>
+      <c r="H19" s="11">
+        <v>212</v>
+      </c>
+      <c r="I19" s="11">
+        <v>152</v>
+      </c>
+      <c r="J19" s="16">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="20" s="1" customFormat="1" spans="1:10">
+      <c r="A20" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="B20" s="11">
         <v>676544</v>
       </c>
-      <c r="C18" s="11">
+      <c r="C20" s="11">
         <v>678602</v>
       </c>
-      <c r="D18" s="11">
+      <c r="D20" s="11">
         <v>780097</v>
       </c>
-      <c r="E18" s="11">
+      <c r="E20" s="11">
         <v>632598</v>
       </c>
-      <c r="F18" s="11">
+      <c r="F20" s="11">
         <v>733500</v>
       </c>
-      <c r="G18" s="11">
+      <c r="G20" s="11">
         <v>1632272</v>
       </c>
-      <c r="H18" s="11">
+      <c r="H20" s="11">
         <v>190579</v>
       </c>
-      <c r="I18" s="11">
+      <c r="I20" s="11">
         <v>421334</v>
       </c>
-      <c r="J18" s="16"/>
-    </row>
-    <row r="19" s="1" customFormat="1" spans="1:10">
-      <c r="A19" s="12"/>
-      <c r="J19" s="17"/>
-    </row>
-    <row r="20" s="1" customFormat="1" spans="1:10">
-      <c r="A20" s="10" t="s">
-        <v>30</v>
-      </c>
-      <c r="B20" s="11"/>
-      <c r="C20" s="11"/>
-      <c r="D20" s="11"/>
-      <c r="E20" s="11"/>
-      <c r="F20" s="11"/>
-      <c r="G20" s="11"/>
-      <c r="H20" s="11"/>
-      <c r="I20" s="11"/>
       <c r="J20" s="16"/>
     </row>
     <row r="21" s="1" customFormat="1" spans="1:10">
-      <c r="A21" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="B21" s="11">
-        <v>0.22496788201061</v>
-      </c>
-      <c r="C21" s="11">
-        <v>0.187524905369721</v>
-      </c>
-      <c r="D21" s="11">
-        <v>0.378768597488832</v>
-      </c>
-      <c r="E21" s="11">
-        <v>0.13268127642868</v>
-      </c>
-      <c r="F21" s="11">
-        <v>0.0485509130381507</v>
-      </c>
-      <c r="G21" s="11">
-        <v>0.0963740326795437</v>
-      </c>
-      <c r="H21" s="11">
-        <v>0.110138053342448</v>
-      </c>
-      <c r="I21" s="11">
-        <v>0.103029977777207</v>
-      </c>
-      <c r="J21" s="16">
-        <f>SUM(B21:I21)</f>
-        <v>1.28203563813519</v>
-      </c>
+      <c r="A21" s="12"/>
+      <c r="J21" s="17"/>
     </row>
     <row r="22" s="1" customFormat="1" spans="1:10">
-      <c r="A22" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="B22" s="11">
-        <v>661</v>
-      </c>
-      <c r="C22" s="11">
-        <v>496</v>
-      </c>
-      <c r="D22" s="11">
-        <v>1058</v>
-      </c>
-      <c r="E22" s="11">
-        <v>328</v>
-      </c>
-      <c r="F22" s="11">
-        <v>856</v>
-      </c>
-      <c r="G22" s="11">
-        <v>72</v>
-      </c>
-      <c r="H22" s="11">
-        <v>923</v>
-      </c>
-      <c r="I22" s="11">
-        <v>335</v>
-      </c>
-      <c r="J22" s="16">
-        <v>1058</v>
-      </c>
+      <c r="A22" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="B22" s="11"/>
+      <c r="C22" s="11"/>
+      <c r="D22" s="11"/>
+      <c r="E22" s="11"/>
+      <c r="F22" s="11"/>
+      <c r="G22" s="11"/>
+      <c r="H22" s="11"/>
+      <c r="I22" s="11"/>
+      <c r="J22" s="16"/>
     </row>
     <row r="23" s="1" customFormat="1" spans="1:10">
       <c r="A23" s="6" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B23" s="11">
+        <v>0.22496788201061</v>
+      </c>
+      <c r="C23" s="11">
+        <v>0.187524905369721</v>
+      </c>
+      <c r="D23" s="11">
+        <v>0.378768597488832</v>
+      </c>
+      <c r="E23" s="11">
+        <v>0.13268127642868</v>
+      </c>
+      <c r="F23" s="11">
+        <v>0.0485509130381507</v>
+      </c>
+      <c r="G23" s="11">
+        <v>0.0963740326795437</v>
+      </c>
+      <c r="H23" s="11">
+        <v>0.110138053342448</v>
+      </c>
+      <c r="I23" s="11">
+        <v>0.103029977777207</v>
+      </c>
+      <c r="J23" s="16">
+        <f>SUM(B23:I23)</f>
+        <v>1.28203563813519</v>
+      </c>
+    </row>
+    <row r="24" s="1" customFormat="1" spans="1:10">
+      <c r="A24" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="B24" s="11">
+        <v>661</v>
+      </c>
+      <c r="C24" s="11">
+        <v>496</v>
+      </c>
+      <c r="D24" s="11">
+        <v>1058</v>
+      </c>
+      <c r="E24" s="11">
+        <v>328</v>
+      </c>
+      <c r="F24" s="11">
+        <v>856</v>
+      </c>
+      <c r="G24" s="11">
+        <v>72</v>
+      </c>
+      <c r="H24" s="11">
+        <v>923</v>
+      </c>
+      <c r="I24" s="11">
+        <v>335</v>
+      </c>
+      <c r="J24" s="16">
+        <v>1058</v>
+      </c>
+    </row>
+    <row r="25" s="1" customFormat="1" spans="1:10">
+      <c r="A25" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="B25" s="11">
         <v>682954</v>
       </c>
-      <c r="C23" s="11">
+      <c r="C25" s="11">
         <v>691497</v>
       </c>
-      <c r="D23" s="11">
+      <c r="D25" s="11">
         <v>772314</v>
       </c>
-      <c r="E23" s="11">
+      <c r="E25" s="11">
         <v>687672</v>
       </c>
-      <c r="F23" s="11">
+      <c r="F25" s="11">
         <v>754610</v>
       </c>
-      <c r="G23" s="11">
+      <c r="G25" s="11">
         <v>1548385</v>
       </c>
-      <c r="H23" s="11">
+      <c r="H25" s="11">
         <v>187357</v>
       </c>
-      <c r="I23" s="11">
+      <c r="I25" s="11">
         <v>500491</v>
       </c>
-      <c r="J23" s="16"/>
-    </row>
-    <row r="24" s="1" customFormat="1" spans="1:10">
-      <c r="A24" s="12"/>
-      <c r="J24" s="17"/>
-    </row>
-    <row r="25" s="1" customFormat="1" spans="1:10">
-      <c r="A25" s="10" t="s">
-        <v>31</v>
-      </c>
-      <c r="B25" s="7"/>
-      <c r="C25" s="7"/>
-      <c r="D25" s="7"/>
-      <c r="E25" s="7"/>
-      <c r="F25" s="7"/>
-      <c r="G25" s="7"/>
-      <c r="H25" s="7"/>
-      <c r="I25" s="7"/>
-      <c r="J25" s="14"/>
-    </row>
-    <row r="26" spans="1:10">
-      <c r="A26" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="B26" s="11">
-        <v>0.224196133336137</v>
-      </c>
-      <c r="C26" s="11">
-        <v>0.186937903287681</v>
-      </c>
-      <c r="D26" s="11">
-        <v>0.377815991293198</v>
-      </c>
-      <c r="E26" s="2">
-        <v>0.132001795806194</v>
-      </c>
-      <c r="F26" s="11">
-        <v>0.0484972658475219</v>
-      </c>
-      <c r="G26" s="11">
-        <v>0.0963883732701269</v>
-      </c>
-      <c r="H26" s="11">
-        <v>0.109148965031763</v>
-      </c>
-      <c r="I26" s="11">
-        <v>0.103639895551926</v>
-      </c>
-      <c r="J26" s="16">
-        <f>SUM(B26:I26)</f>
-        <v>1.27862632342455</v>
-      </c>
-    </row>
-    <row r="27" spans="1:10">
-      <c r="A27" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="B27" s="11">
-        <v>1239</v>
-      </c>
-      <c r="C27" s="11">
-        <v>835</v>
-      </c>
-      <c r="D27" s="11">
-        <v>1883</v>
-      </c>
-      <c r="E27" s="11">
-        <v>485</v>
-      </c>
-      <c r="F27" s="11">
-        <v>1410</v>
-      </c>
-      <c r="G27" s="11">
-        <v>75</v>
-      </c>
-      <c r="H27" s="11">
-        <v>1332</v>
-      </c>
-      <c r="I27" s="11">
-        <v>488</v>
-      </c>
-      <c r="J27" s="16">
-        <v>1883</v>
-      </c>
+      <c r="J25" s="16"/>
+    </row>
+    <row r="26" s="1" customFormat="1" spans="1:10">
+      <c r="A26" s="12"/>
+      <c r="J26" s="17"/>
+    </row>
+    <row r="27" s="1" customFormat="1" spans="1:10">
+      <c r="A27" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="B27" s="7"/>
+      <c r="C27" s="7"/>
+      <c r="D27" s="7"/>
+      <c r="E27" s="7"/>
+      <c r="F27" s="7"/>
+      <c r="G27" s="7"/>
+      <c r="H27" s="7"/>
+      <c r="I27" s="7"/>
+      <c r="J27" s="14"/>
     </row>
     <row r="28" spans="1:10">
       <c r="A28" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="B28" s="7">
+        <v>26</v>
+      </c>
+      <c r="B28" s="11">
+        <v>0.224196133336137</v>
+      </c>
+      <c r="C28" s="11">
+        <v>0.186937903287681</v>
+      </c>
+      <c r="D28" s="11">
+        <v>0.377815991293198</v>
+      </c>
+      <c r="E28" s="2">
+        <v>0.132001795806194</v>
+      </c>
+      <c r="F28" s="11">
+        <v>0.0484972658475219</v>
+      </c>
+      <c r="G28" s="11">
+        <v>0.0963883732701269</v>
+      </c>
+      <c r="H28" s="11">
+        <v>0.109148965031763</v>
+      </c>
+      <c r="I28" s="11">
+        <v>0.103639895551926</v>
+      </c>
+      <c r="J28" s="16">
+        <f>SUM(B28:I28)</f>
+        <v>1.27862632342455</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10">
+      <c r="A29" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="B29" s="11">
+        <v>1239</v>
+      </c>
+      <c r="C29" s="11">
+        <v>835</v>
+      </c>
+      <c r="D29" s="11">
+        <v>1883</v>
+      </c>
+      <c r="E29" s="11">
+        <v>485</v>
+      </c>
+      <c r="F29" s="11">
+        <v>1410</v>
+      </c>
+      <c r="G29" s="11">
+        <v>75</v>
+      </c>
+      <c r="H29" s="11">
+        <v>1332</v>
+      </c>
+      <c r="I29" s="11">
+        <v>488</v>
+      </c>
+      <c r="J29" s="16">
+        <v>1883</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10">
+      <c r="A30" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="B30" s="7">
         <v>685552</v>
       </c>
-      <c r="C28" s="7">
+      <c r="C30" s="7">
         <v>694100</v>
       </c>
-      <c r="D28" s="7">
+      <c r="D30" s="7">
         <v>772502</v>
       </c>
-      <c r="E28" s="11">
+      <c r="E30" s="11">
         <v>690048</v>
       </c>
-      <c r="F28" s="7">
+      <c r="F30" s="7">
         <v>763537</v>
       </c>
-      <c r="G28" s="7">
+      <c r="G30" s="7">
         <v>1547683</v>
       </c>
-      <c r="H28" s="7">
+      <c r="H30" s="7">
         <v>189000</v>
       </c>
-      <c r="I28" s="7">
+      <c r="I30" s="7">
         <v>505491</v>
       </c>
-      <c r="J28" s="16"/>
-    </row>
-    <row r="29" spans="1:10">
-      <c r="A29" s="8"/>
-      <c r="J29" s="17"/>
-    </row>
-    <row r="30" spans="1:10">
-      <c r="A30" s="10" t="s">
-        <v>32</v>
-      </c>
-      <c r="B30" s="7"/>
-      <c r="C30" s="7"/>
-      <c r="D30" s="7"/>
-      <c r="E30" s="7"/>
-      <c r="F30" s="7"/>
-      <c r="G30" s="7"/>
-      <c r="H30" s="7"/>
-      <c r="I30" s="7"/>
       <c r="J30" s="16"/>
     </row>
     <row r="31" spans="1:10">
-      <c r="A31" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="B31" s="11">
-        <v>0.223943658885033</v>
-      </c>
-      <c r="C31" s="11">
-        <v>0.186707045902669</v>
-      </c>
-      <c r="D31" s="11">
-        <v>0.377670940701938</v>
-      </c>
-      <c r="E31" s="11">
-        <v>0.13173763980523</v>
-      </c>
-      <c r="F31" s="11">
-        <v>0.0481836597937725</v>
-      </c>
-      <c r="G31" s="11">
-        <v>0.0940700052880424</v>
-      </c>
-      <c r="H31" s="11">
-        <v>0.108544554749352</v>
-      </c>
-      <c r="I31" s="11">
-        <v>0.096234294786308</v>
-      </c>
-      <c r="J31" s="16">
-        <f>SUM(B31:I31)</f>
-        <v>1.26709179991234</v>
-      </c>
+      <c r="A31" s="8"/>
+      <c r="J31" s="17"/>
     </row>
     <row r="32" spans="1:10">
-      <c r="A32" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="B32" s="11">
-        <v>4789</v>
-      </c>
-      <c r="C32" s="11">
-        <v>1982</v>
-      </c>
-      <c r="D32" s="11">
-        <v>4399</v>
-      </c>
-      <c r="E32" s="11">
-        <v>1209</v>
-      </c>
-      <c r="F32" s="11">
-        <v>38714</v>
-      </c>
-      <c r="G32" s="11">
-        <v>82</v>
-      </c>
-      <c r="H32" s="11">
-        <v>67058</v>
-      </c>
-      <c r="I32" s="11">
-        <v>2877</v>
-      </c>
-      <c r="J32" s="14">
-        <v>67058</v>
-      </c>
+      <c r="A32" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="B32" s="7"/>
+      <c r="C32" s="7"/>
+      <c r="D32" s="7"/>
+      <c r="E32" s="7"/>
+      <c r="F32" s="7"/>
+      <c r="G32" s="7"/>
+      <c r="H32" s="7"/>
+      <c r="I32" s="7"/>
+      <c r="J32" s="16"/>
     </row>
     <row r="33" spans="1:10">
       <c r="A33" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="B33" s="7">
+        <v>26</v>
+      </c>
+      <c r="B33" s="11">
+        <v>0.223943658885033</v>
+      </c>
+      <c r="C33" s="11">
+        <v>0.186707045902669</v>
+      </c>
+      <c r="D33" s="11">
+        <v>0.377670940701938</v>
+      </c>
+      <c r="E33" s="11">
+        <v>0.13173763980523</v>
+      </c>
+      <c r="F33" s="11">
+        <v>0.0481836597937725</v>
+      </c>
+      <c r="G33" s="11">
+        <v>0.0940700052880424</v>
+      </c>
+      <c r="H33" s="11">
+        <v>0.108544554749352</v>
+      </c>
+      <c r="I33" s="11">
+        <v>0.096234294786308</v>
+      </c>
+      <c r="J33" s="16">
+        <f>SUM(B33:I33)</f>
+        <v>1.26709179991234</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10">
+      <c r="A34" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="B34" s="11">
+        <v>4789</v>
+      </c>
+      <c r="C34" s="11">
+        <v>1982</v>
+      </c>
+      <c r="D34" s="11">
+        <v>4399</v>
+      </c>
+      <c r="E34" s="11">
+        <v>1209</v>
+      </c>
+      <c r="F34" s="11">
+        <v>38714</v>
+      </c>
+      <c r="G34" s="11">
+        <v>82</v>
+      </c>
+      <c r="H34" s="11">
+        <v>67058</v>
+      </c>
+      <c r="I34" s="11">
+        <v>2877</v>
+      </c>
+      <c r="J34" s="14">
+        <v>67058</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10">
+      <c r="A35" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="B35" s="7">
         <v>686650</v>
       </c>
-      <c r="C33" s="7">
+      <c r="C35" s="7">
         <v>695091</v>
       </c>
-      <c r="D33" s="7">
+      <c r="D35" s="7">
         <v>772235</v>
       </c>
-      <c r="E33" s="7">
+      <c r="E35" s="7">
         <v>690491</v>
       </c>
-      <c r="F33" s="7">
+      <c r="F35" s="7">
         <v>766671</v>
       </c>
-      <c r="G33" s="7">
+      <c r="G35" s="7">
         <v>1355969</v>
       </c>
-      <c r="H33" s="7">
+      <c r="H35" s="7">
         <v>189648</v>
       </c>
-      <c r="I33" s="7">
+      <c r="I35" s="7">
         <v>509904</v>
       </c>
-      <c r="J33" s="14"/>
-    </row>
-    <row r="34" spans="1:10">
-      <c r="A34" s="8"/>
-      <c r="J34" s="15"/>
-    </row>
-    <row r="35" spans="1:10">
-      <c r="A35" s="10" t="s">
-        <v>33</v>
-      </c>
-      <c r="B35" s="7"/>
-      <c r="C35" s="7"/>
-      <c r="D35" s="7"/>
-      <c r="E35" s="7"/>
-      <c r="F35" s="7"/>
-      <c r="G35" s="7"/>
-      <c r="H35" s="7"/>
-      <c r="I35" s="7"/>
       <c r="J35" s="14"/>
     </row>
     <row r="36" spans="1:10">
-      <c r="A36" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="B36" s="11">
-        <v>0.224736691876997</v>
-      </c>
-      <c r="C36" s="11">
-        <v>0.187294567106436</v>
-      </c>
-      <c r="D36" s="11">
-        <v>0.379598329129886</v>
-      </c>
-      <c r="E36" s="11">
-        <v>0.133199928177059</v>
-      </c>
-      <c r="F36" s="11">
-        <v>0.0457097264452359</v>
-      </c>
-      <c r="G36" s="11">
-        <v>0.0855964570603726</v>
-      </c>
-      <c r="H36" s="11">
-        <v>0.108191476936675</v>
-      </c>
-      <c r="I36" s="11">
-        <v>0.0725702160635175</v>
-      </c>
-      <c r="J36" s="16">
-        <f>SUM(B36:I36)</f>
-        <v>1.23689739279618</v>
-      </c>
+      <c r="A36" s="8"/>
+      <c r="J36" s="15"/>
     </row>
     <row r="37" spans="1:10">
-      <c r="A37" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="B37" s="11">
-        <v>3171</v>
-      </c>
-      <c r="C37" s="11">
-        <v>1921</v>
-      </c>
-      <c r="D37" s="11">
-        <v>6153</v>
-      </c>
-      <c r="E37" s="11">
-        <v>1233</v>
-      </c>
-      <c r="F37" s="11">
-        <v>7581</v>
-      </c>
-      <c r="G37" s="11">
-        <v>103</v>
-      </c>
-      <c r="H37" s="11">
-        <v>10661</v>
-      </c>
-      <c r="I37" s="11">
-        <v>1797</v>
-      </c>
-      <c r="J37" s="16">
-        <v>10661</v>
-      </c>
+      <c r="A37" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="B37" s="7"/>
+      <c r="C37" s="7"/>
+      <c r="D37" s="7"/>
+      <c r="E37" s="7"/>
+      <c r="F37" s="7"/>
+      <c r="G37" s="7"/>
+      <c r="H37" s="7"/>
+      <c r="I37" s="7"/>
+      <c r="J37" s="14"/>
     </row>
     <row r="38" spans="1:10">
       <c r="A38" s="6" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B38" s="11">
+        <v>0.224736691876997</v>
+      </c>
+      <c r="C38" s="11">
+        <v>0.187294567106436</v>
+      </c>
+      <c r="D38" s="11">
+        <v>0.379598329129886</v>
+      </c>
+      <c r="E38" s="11">
+        <v>0.133199928177059</v>
+      </c>
+      <c r="F38" s="11">
+        <v>0.0457097264452359</v>
+      </c>
+      <c r="G38" s="11">
+        <v>0.0855964570603726</v>
+      </c>
+      <c r="H38" s="11">
+        <v>0.108191476936675</v>
+      </c>
+      <c r="I38" s="11">
+        <v>0.0725702160635175</v>
+      </c>
+      <c r="J38" s="16">
+        <f>SUM(B38:I38)</f>
+        <v>1.23689739279618</v>
+      </c>
+    </row>
+    <row r="39" spans="1:10">
+      <c r="A39" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="B39" s="11">
+        <v>3171</v>
+      </c>
+      <c r="C39" s="11">
+        <v>1921</v>
+      </c>
+      <c r="D39" s="11">
+        <v>6153</v>
+      </c>
+      <c r="E39" s="11">
+        <v>1233</v>
+      </c>
+      <c r="F39" s="11">
+        <v>7581</v>
+      </c>
+      <c r="G39" s="11">
+        <v>103</v>
+      </c>
+      <c r="H39" s="11">
+        <v>10661</v>
+      </c>
+      <c r="I39" s="11">
+        <v>1797</v>
+      </c>
+      <c r="J39" s="16">
+        <v>10661</v>
+      </c>
+    </row>
+    <row r="40" spans="1:10">
+      <c r="A40" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="B40" s="11">
         <v>687917</v>
       </c>
-      <c r="C38" s="11">
+      <c r="C40" s="11">
         <v>698622</v>
       </c>
-      <c r="D38" s="11">
+      <c r="D40" s="11">
         <v>778644</v>
       </c>
-      <c r="E38" s="11">
+      <c r="E40" s="11">
         <v>707502</v>
       </c>
-      <c r="F38" s="11">
+      <c r="F40" s="11">
         <v>845276</v>
       </c>
-      <c r="G38" s="11">
+      <c r="G40" s="11">
         <v>1624434</v>
       </c>
-      <c r="H38" s="11">
+      <c r="H40" s="11">
         <v>198638</v>
       </c>
-      <c r="I38" s="11">
+      <c r="I40" s="11">
         <v>480276</v>
       </c>
-      <c r="J38" s="16"/>
-    </row>
-    <row r="39" s="2" customFormat="1" spans="1:10">
-      <c r="A39" s="8"/>
-      <c r="B39" s="2"/>
-      <c r="C39" s="2"/>
-      <c r="D39" s="2"/>
-      <c r="E39" s="2"/>
-      <c r="F39" s="2"/>
-      <c r="G39" s="2"/>
-      <c r="H39" s="2"/>
-      <c r="I39" s="2"/>
-      <c r="J39" s="15"/>
-    </row>
-    <row r="40" s="2" customFormat="1" spans="1:10">
-      <c r="A40" s="10" t="s">
-        <v>34</v>
-      </c>
-      <c r="B40" s="7"/>
-      <c r="C40" s="7"/>
-      <c r="D40" s="7"/>
-      <c r="E40" s="7"/>
-      <c r="F40" s="7"/>
-      <c r="G40" s="7"/>
-      <c r="H40" s="7"/>
-      <c r="I40" s="7"/>
-      <c r="J40" s="14"/>
+      <c r="J40" s="16"/>
     </row>
     <row r="41" s="2" customFormat="1" spans="1:10">
-      <c r="A41" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="B41" s="11">
-        <v>0.223983742272348</v>
-      </c>
-      <c r="C41" s="11">
-        <v>0.186591074650024</v>
-      </c>
-      <c r="D41" s="11">
-        <v>0.378466722022617</v>
-      </c>
-      <c r="E41" s="11">
-        <v>0.132694963136445</v>
-      </c>
-      <c r="F41" s="11">
-        <v>0.0457305927623964</v>
-      </c>
-      <c r="G41" s="11">
-        <v>0.0851383095332634</v>
-      </c>
-      <c r="H41" s="11">
-        <v>0.107004318017908</v>
-      </c>
-      <c r="I41" s="11">
-        <v>0.0720747850122068</v>
-      </c>
-      <c r="J41" s="16">
-        <f>SUM(B41:I41)</f>
-        <v>1.23168450740721</v>
-      </c>
+      <c r="A41" s="8"/>
+      <c r="B41" s="2"/>
+      <c r="C41" s="2"/>
+      <c r="D41" s="2"/>
+      <c r="E41" s="2"/>
+      <c r="F41" s="2"/>
+      <c r="G41" s="2"/>
+      <c r="H41" s="2"/>
+      <c r="I41" s="2"/>
+      <c r="J41" s="15"/>
     </row>
     <row r="42" s="2" customFormat="1" spans="1:10">
-      <c r="A42" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="B42" s="11">
-        <v>8356</v>
-      </c>
-      <c r="C42" s="11">
-        <v>4527</v>
-      </c>
-      <c r="D42" s="11">
-        <v>19594</v>
-      </c>
-      <c r="E42" s="11">
-        <v>2189</v>
-      </c>
-      <c r="F42" s="11">
-        <v>14796</v>
-      </c>
-      <c r="G42" s="11">
-        <v>101</v>
-      </c>
-      <c r="H42" s="11">
-        <v>20417</v>
-      </c>
-      <c r="I42" s="11">
-        <v>2480</v>
-      </c>
-      <c r="J42" s="11">
-        <v>20417</v>
-      </c>
+      <c r="A42" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="B42" s="7"/>
+      <c r="C42" s="7"/>
+      <c r="D42" s="7"/>
+      <c r="E42" s="7"/>
+      <c r="F42" s="7"/>
+      <c r="G42" s="7"/>
+      <c r="H42" s="7"/>
+      <c r="I42" s="7"/>
+      <c r="J42" s="14"/>
     </row>
     <row r="43" s="2" customFormat="1" spans="1:10">
       <c r="A43" s="6" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B43" s="11">
+        <v>0.223983742272348</v>
+      </c>
+      <c r="C43" s="11">
+        <v>0.186591074650024</v>
+      </c>
+      <c r="D43" s="11">
+        <v>0.378466722022617</v>
+      </c>
+      <c r="E43" s="11">
+        <v>0.132694963136445</v>
+      </c>
+      <c r="F43" s="11">
+        <v>0.0457305927623964</v>
+      </c>
+      <c r="G43" s="11">
+        <v>0.0851383095332634</v>
+      </c>
+      <c r="H43" s="11">
+        <v>0.107004318017908</v>
+      </c>
+      <c r="I43" s="11">
+        <v>0.0720747850122068</v>
+      </c>
+      <c r="J43" s="16">
+        <f>SUM(B43:I43)</f>
+        <v>1.23168450740721</v>
+      </c>
+    </row>
+    <row r="44" s="2" customFormat="1" spans="1:10">
+      <c r="A44" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="B44" s="11">
+        <v>8356</v>
+      </c>
+      <c r="C44" s="11">
+        <v>4527</v>
+      </c>
+      <c r="D44" s="11">
+        <v>19594</v>
+      </c>
+      <c r="E44" s="11">
+        <v>2189</v>
+      </c>
+      <c r="F44" s="11">
+        <v>14796</v>
+      </c>
+      <c r="G44" s="11">
+        <v>101</v>
+      </c>
+      <c r="H44" s="11">
+        <v>20417</v>
+      </c>
+      <c r="I44" s="11">
+        <v>2480</v>
+      </c>
+      <c r="J44" s="11">
+        <v>20417</v>
+      </c>
+    </row>
+    <row r="45" s="2" customFormat="1" spans="1:10">
+      <c r="A45" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="B45" s="11">
         <v>689016</v>
       </c>
-      <c r="C43" s="11">
+      <c r="C45" s="11">
         <v>699728</v>
       </c>
-      <c r="D43" s="11">
+      <c r="D45" s="11">
         <v>777577</v>
       </c>
-      <c r="E43" s="11">
+      <c r="E45" s="11">
         <v>709351</v>
       </c>
-      <c r="F43" s="11">
+      <c r="F45" s="11">
         <v>845206</v>
       </c>
-      <c r="G43" s="11">
+      <c r="G45" s="11">
         <v>1619385</v>
       </c>
-      <c r="H43" s="11">
+      <c r="H45" s="11">
         <v>199841</v>
       </c>
-      <c r="I43" s="11">
+      <c r="I45" s="11">
         <v>482183</v>
       </c>
-      <c r="J43" s="18"/>
-    </row>
-    <row r="44" spans="1:10">
-      <c r="A44" s="8"/>
-      <c r="J44" s="15"/>
-    </row>
-    <row r="45" spans="1:10">
-      <c r="A45" s="10" t="s">
-        <v>35</v>
-      </c>
-      <c r="B45" s="7"/>
-      <c r="C45" s="7"/>
-      <c r="D45" s="7"/>
-      <c r="E45" s="7"/>
-      <c r="F45" s="7"/>
-      <c r="G45" s="7"/>
-      <c r="H45" s="7"/>
-      <c r="I45" s="7"/>
-      <c r="J45" s="14"/>
+      <c r="J45" s="18"/>
     </row>
     <row r="46" spans="1:10">
-      <c r="A46" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="B46" s="7">
-        <v>0.223964152036268</v>
-      </c>
-      <c r="C46" s="7">
-        <v>0.186588808844244</v>
-      </c>
-      <c r="D46" s="7">
-        <v>0.378431358303736</v>
-      </c>
-      <c r="E46" s="7">
-        <v>0.132723134356391</v>
-      </c>
-      <c r="F46" s="7">
-        <v>0.0460582563706361</v>
-      </c>
-      <c r="G46" s="7">
-        <v>0.0788786927184357</v>
-      </c>
-      <c r="H46" s="7">
-        <v>0.1092624567126</v>
-      </c>
-      <c r="I46" s="7">
-        <v>0.0737819749366587</v>
-      </c>
-      <c r="J46" s="16">
-        <f>SUM(B46:I46)</f>
-        <v>1.22968883427897</v>
-      </c>
+      <c r="A46" s="8"/>
+      <c r="J46" s="15"/>
     </row>
     <row r="47" spans="1:10">
-      <c r="A47" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="B47" s="11">
-        <v>65144</v>
-      </c>
-      <c r="C47" s="11">
-        <v>26950</v>
-      </c>
-      <c r="D47" s="11">
-        <v>171525</v>
-      </c>
-      <c r="E47" s="11">
-        <v>13105</v>
-      </c>
-      <c r="F47" s="11">
-        <v>207291</v>
-      </c>
-      <c r="G47" s="11">
-        <v>138</v>
-      </c>
-      <c r="H47" s="11">
-        <v>461178</v>
-      </c>
-      <c r="I47" s="11">
-        <v>15231</v>
-      </c>
-      <c r="J47" s="11">
-        <v>461178</v>
-      </c>
+      <c r="A47" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="B47" s="7"/>
+      <c r="C47" s="7"/>
+      <c r="D47" s="7"/>
+      <c r="E47" s="7"/>
+      <c r="F47" s="7"/>
+      <c r="G47" s="7"/>
+      <c r="H47" s="7"/>
+      <c r="I47" s="7"/>
+      <c r="J47" s="14"/>
     </row>
     <row r="48" spans="1:10">
       <c r="A48" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="B48" s="11">
-        <v>688906</v>
-      </c>
-      <c r="C48" s="11">
-        <v>699969</v>
-      </c>
-      <c r="D48" s="11">
-        <v>775773</v>
-      </c>
-      <c r="E48" s="11">
-        <v>704981</v>
-      </c>
-      <c r="F48" s="11">
-        <v>872391</v>
-      </c>
-      <c r="G48" s="11">
-        <v>1631177</v>
-      </c>
-      <c r="H48" s="11">
-        <v>200427</v>
-      </c>
-      <c r="I48" s="11">
-        <v>481500</v>
-      </c>
-      <c r="J48" s="16"/>
+        <v>26</v>
+      </c>
+      <c r="B48" s="7">
+        <v>0.223964152036268</v>
+      </c>
+      <c r="C48" s="7">
+        <v>0.186588808844244</v>
+      </c>
+      <c r="D48" s="7">
+        <v>0.378431358303736</v>
+      </c>
+      <c r="E48" s="7">
+        <v>0.132723134356391</v>
+      </c>
+      <c r="F48" s="7">
+        <v>0.0460582563706361</v>
+      </c>
+      <c r="G48" s="7">
+        <v>0.0788786927184357</v>
+      </c>
+      <c r="H48" s="7">
+        <v>0.1092624567126</v>
+      </c>
+      <c r="I48" s="7">
+        <v>0.0737819749366587</v>
+      </c>
+      <c r="J48" s="16">
+        <f>SUM(B48:I48)</f>
+        <v>1.22968883427897</v>
+      </c>
     </row>
     <row r="49" spans="1:10">
-      <c r="A49" s="8"/>
-      <c r="J49" s="15"/>
+      <c r="A49" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="B49" s="11">
+        <v>65144</v>
+      </c>
+      <c r="C49" s="11">
+        <v>26950</v>
+      </c>
+      <c r="D49" s="11">
+        <v>171525</v>
+      </c>
+      <c r="E49" s="11">
+        <v>13105</v>
+      </c>
+      <c r="F49" s="11">
+        <v>207291</v>
+      </c>
+      <c r="G49" s="11">
+        <v>138</v>
+      </c>
+      <c r="H49" s="11">
+        <v>461178</v>
+      </c>
+      <c r="I49" s="11">
+        <v>15231</v>
+      </c>
+      <c r="J49" s="11">
+        <v>461178</v>
+      </c>
     </row>
     <row r="50" spans="1:10">
       <c r="A50" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="B50" s="7"/>
-      <c r="C50" s="7"/>
-      <c r="D50" s="7"/>
-      <c r="E50" s="7"/>
-      <c r="F50" s="7"/>
-      <c r="G50" s="7">
-        <v>0.0726150323207724</v>
-      </c>
-      <c r="H50" s="7"/>
-      <c r="I50" s="7"/>
-      <c r="J50" s="14"/>
+        <v>29</v>
+      </c>
+      <c r="B50" s="11">
+        <v>688906</v>
+      </c>
+      <c r="C50" s="11">
+        <v>699969</v>
+      </c>
+      <c r="D50" s="11">
+        <v>775773</v>
+      </c>
+      <c r="E50" s="11">
+        <v>704981</v>
+      </c>
+      <c r="F50" s="11">
+        <v>872391</v>
+      </c>
+      <c r="G50" s="11">
+        <v>1631177</v>
+      </c>
+      <c r="H50" s="11">
+        <v>200427</v>
+      </c>
+      <c r="I50" s="11">
+        <v>481500</v>
+      </c>
+      <c r="J50" s="16"/>
     </row>
     <row r="51" spans="1:10">
-      <c r="A51" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="B51" s="11"/>
-      <c r="C51" s="11"/>
-      <c r="D51" s="11"/>
-      <c r="E51" s="11"/>
-      <c r="F51" s="11"/>
-      <c r="G51" s="11"/>
-      <c r="H51" s="11"/>
-      <c r="I51" s="11"/>
-      <c r="J51" s="16"/>
+      <c r="A51" s="8"/>
+      <c r="J51" s="15"/>
     </row>
     <row r="52" spans="1:10">
       <c r="A52" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="B52" s="11"/>
-      <c r="C52" s="11"/>
-      <c r="D52" s="11"/>
-      <c r="E52" s="11"/>
-      <c r="F52" s="11"/>
-      <c r="G52" s="11"/>
-      <c r="H52" s="11"/>
-      <c r="I52" s="11"/>
-      <c r="J52" s="16"/>
+        <v>11</v>
+      </c>
+      <c r="B52" s="7"/>
+      <c r="C52" s="7"/>
+      <c r="D52" s="7"/>
+      <c r="E52" s="7"/>
+      <c r="F52" s="7"/>
+      <c r="G52" s="7">
+        <v>0.0726150323207724</v>
+      </c>
+      <c r="H52" s="7"/>
+      <c r="I52" s="7"/>
+      <c r="J52" s="14"/>
     </row>
     <row r="53" spans="1:10">
       <c r="A53" s="6" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B53" s="11"/>
       <c r="C53" s="11"/>
@@ -2904,56 +2973,56 @@
       <c r="J53" s="16"/>
     </row>
     <row r="54" spans="1:10">
-      <c r="A54" s="8"/>
-      <c r="J54" s="15"/>
+      <c r="A54" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="B54" s="11"/>
+      <c r="C54" s="11"/>
+      <c r="D54" s="11"/>
+      <c r="E54" s="11"/>
+      <c r="F54" s="11"/>
+      <c r="G54" s="11"/>
+      <c r="H54" s="11"/>
+      <c r="I54" s="11"/>
+      <c r="J54" s="16"/>
     </row>
     <row r="55" spans="1:10">
       <c r="A55" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="B55" s="7"/>
-      <c r="C55" s="7"/>
-      <c r="D55" s="7"/>
-      <c r="E55" s="7"/>
-      <c r="F55" s="7"/>
-      <c r="G55" s="11">
-        <v>0.0629933219692992</v>
-      </c>
-      <c r="H55" s="7"/>
-      <c r="I55" s="7"/>
-      <c r="J55" s="14"/>
+        <v>29</v>
+      </c>
+      <c r="B55" s="11"/>
+      <c r="C55" s="11"/>
+      <c r="D55" s="11"/>
+      <c r="E55" s="11"/>
+      <c r="F55" s="11"/>
+      <c r="G55" s="11"/>
+      <c r="H55" s="11"/>
+      <c r="I55" s="11"/>
+      <c r="J55" s="16"/>
     </row>
     <row r="56" spans="1:10">
-      <c r="A56" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="B56" s="11"/>
-      <c r="C56" s="11"/>
-      <c r="D56" s="11"/>
-      <c r="E56" s="11"/>
-      <c r="F56" s="11"/>
-      <c r="G56" s="11"/>
-      <c r="H56" s="11"/>
-      <c r="I56" s="11"/>
-      <c r="J56" s="16"/>
+      <c r="A56" s="8"/>
+      <c r="J56" s="15"/>
     </row>
     <row r="57" spans="1:10">
       <c r="A57" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="B57" s="11"/>
-      <c r="C57" s="11"/>
-      <c r="D57" s="11"/>
-      <c r="E57" s="11"/>
-      <c r="F57" s="11"/>
-      <c r="G57" s="11"/>
-      <c r="H57" s="11"/>
-      <c r="I57" s="11"/>
-      <c r="J57" s="16"/>
+        <v>12</v>
+      </c>
+      <c r="B57" s="7"/>
+      <c r="C57" s="7"/>
+      <c r="D57" s="7"/>
+      <c r="E57" s="7"/>
+      <c r="F57" s="7"/>
+      <c r="G57" s="11">
+        <v>0.0629933219692992</v>
+      </c>
+      <c r="H57" s="7"/>
+      <c r="I57" s="7"/>
+      <c r="J57" s="14"/>
     </row>
     <row r="58" spans="1:10">
       <c r="A58" s="6" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B58" s="11"/>
       <c r="C58" s="11"/>
@@ -2966,56 +3035,56 @@
       <c r="J58" s="16"/>
     </row>
     <row r="59" spans="1:10">
-      <c r="A59" s="8"/>
-      <c r="J59" s="15"/>
+      <c r="A59" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="B59" s="11"/>
+      <c r="C59" s="11"/>
+      <c r="D59" s="11"/>
+      <c r="E59" s="11"/>
+      <c r="F59" s="11"/>
+      <c r="G59" s="11"/>
+      <c r="H59" s="11"/>
+      <c r="I59" s="11"/>
+      <c r="J59" s="16"/>
     </row>
     <row r="60" spans="1:10">
       <c r="A60" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="B60" s="7"/>
-      <c r="C60" s="7"/>
-      <c r="D60" s="7"/>
-      <c r="E60" s="7"/>
-      <c r="F60" s="7"/>
-      <c r="G60" s="7">
-        <v>0.0550438941415778</v>
-      </c>
-      <c r="H60" s="7"/>
-      <c r="I60" s="7"/>
-      <c r="J60" s="14"/>
+        <v>29</v>
+      </c>
+      <c r="B60" s="11"/>
+      <c r="C60" s="11"/>
+      <c r="D60" s="11"/>
+      <c r="E60" s="11"/>
+      <c r="F60" s="11"/>
+      <c r="G60" s="11"/>
+      <c r="H60" s="11"/>
+      <c r="I60" s="11"/>
+      <c r="J60" s="16"/>
     </row>
     <row r="61" spans="1:10">
-      <c r="A61" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="B61" s="11"/>
-      <c r="C61" s="11"/>
-      <c r="D61" s="11"/>
-      <c r="E61" s="11"/>
-      <c r="F61" s="11"/>
-      <c r="G61" s="11"/>
-      <c r="H61" s="11"/>
-      <c r="I61" s="11"/>
-      <c r="J61" s="16"/>
+      <c r="A61" s="8"/>
+      <c r="J61" s="15"/>
     </row>
     <row r="62" spans="1:10">
       <c r="A62" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="B62" s="11"/>
-      <c r="C62" s="11"/>
-      <c r="D62" s="11"/>
-      <c r="E62" s="11"/>
-      <c r="F62" s="11"/>
-      <c r="G62" s="11"/>
-      <c r="H62" s="11"/>
-      <c r="I62" s="11"/>
-      <c r="J62" s="16"/>
+        <v>13</v>
+      </c>
+      <c r="B62" s="7"/>
+      <c r="C62" s="7"/>
+      <c r="D62" s="7"/>
+      <c r="E62" s="7"/>
+      <c r="F62" s="7"/>
+      <c r="G62" s="7">
+        <v>0.0550438941415778</v>
+      </c>
+      <c r="H62" s="7"/>
+      <c r="I62" s="7"/>
+      <c r="J62" s="14"/>
     </row>
     <row r="63" spans="1:10">
       <c r="A63" s="6" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B63" s="11"/>
       <c r="C63" s="11"/>
@@ -3028,948 +3097,1632 @@
       <c r="J63" s="16"/>
     </row>
     <row r="64" spans="1:10">
-      <c r="A64" s="8"/>
-      <c r="J64" s="15"/>
+      <c r="A64" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="B64" s="11"/>
+      <c r="C64" s="11"/>
+      <c r="D64" s="11"/>
+      <c r="E64" s="11"/>
+      <c r="F64" s="11"/>
+      <c r="G64" s="11"/>
+      <c r="H64" s="11"/>
+      <c r="I64" s="11"/>
+      <c r="J64" s="16"/>
     </row>
     <row r="65" spans="1:10">
       <c r="A65" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="B65" s="7"/>
-      <c r="C65" s="7"/>
-      <c r="D65" s="7"/>
-      <c r="E65" s="7"/>
-      <c r="F65" s="7"/>
-      <c r="G65" s="7">
-        <v>0.0529699223097137</v>
-      </c>
-      <c r="H65" s="7"/>
-      <c r="I65" s="7"/>
-      <c r="J65" s="14"/>
+        <v>29</v>
+      </c>
+      <c r="B65" s="11"/>
+      <c r="C65" s="11"/>
+      <c r="D65" s="11"/>
+      <c r="E65" s="11"/>
+      <c r="F65" s="11"/>
+      <c r="G65" s="11"/>
+      <c r="H65" s="11"/>
+      <c r="I65" s="11"/>
+      <c r="J65" s="16"/>
     </row>
     <row r="66" spans="1:10">
-      <c r="A66" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="B66" s="11"/>
-      <c r="C66" s="11"/>
-      <c r="D66" s="11"/>
-      <c r="E66" s="11"/>
-      <c r="F66" s="11"/>
-      <c r="G66" s="11"/>
-      <c r="H66" s="11"/>
-      <c r="I66" s="11"/>
-      <c r="J66" s="16"/>
+      <c r="A66" s="8"/>
+      <c r="J66" s="15"/>
     </row>
     <row r="67" spans="1:10">
       <c r="A67" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="B67" s="7"/>
+      <c r="C67" s="7"/>
+      <c r="D67" s="7"/>
+      <c r="E67" s="7"/>
+      <c r="F67" s="7"/>
+      <c r="G67" s="7">
+        <v>0.0529699223097137</v>
+      </c>
+      <c r="H67" s="7"/>
+      <c r="I67" s="7"/>
+      <c r="J67" s="14"/>
+    </row>
+    <row r="68" spans="1:10">
+      <c r="A68" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="B68" s="11"/>
+      <c r="C68" s="11"/>
+      <c r="D68" s="11"/>
+      <c r="E68" s="11"/>
+      <c r="F68" s="11"/>
+      <c r="G68" s="11"/>
+      <c r="H68" s="11"/>
+      <c r="I68" s="11"/>
+      <c r="J68" s="16"/>
+    </row>
+    <row r="69" spans="1:10">
+      <c r="A69" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="B67" s="11"/>
-      <c r="C67" s="11"/>
-      <c r="D67" s="11"/>
-      <c r="E67" s="11"/>
-      <c r="F67" s="11"/>
-      <c r="G67" s="11"/>
-      <c r="H67" s="11"/>
-      <c r="I67" s="11"/>
-      <c r="J67" s="16"/>
-    </row>
-    <row r="68" ht="14.25" spans="1:10">
-      <c r="A68" s="19" t="s">
-        <v>28</v>
-      </c>
-      <c r="B68" s="20"/>
-      <c r="C68" s="20"/>
-      <c r="D68" s="20"/>
-      <c r="E68" s="20"/>
-      <c r="F68" s="20"/>
-      <c r="G68" s="20"/>
-      <c r="H68" s="20"/>
-      <c r="I68" s="20"/>
-      <c r="J68" s="27"/>
-    </row>
-    <row r="71" ht="14.25"/>
-    <row r="72" spans="1:10">
-      <c r="A72" s="21"/>
-      <c r="B72" s="22" t="s">
+      <c r="B69" s="11"/>
+      <c r="C69" s="11"/>
+      <c r="D69" s="11"/>
+      <c r="E69" s="11"/>
+      <c r="F69" s="11"/>
+      <c r="G69" s="11"/>
+      <c r="H69" s="11"/>
+      <c r="I69" s="11"/>
+      <c r="J69" s="16"/>
+    </row>
+    <row r="70" ht="14.25" spans="1:10">
+      <c r="A70" s="19" t="s">
+        <v>29</v>
+      </c>
+      <c r="B70" s="20"/>
+      <c r="C70" s="20"/>
+      <c r="D70" s="20"/>
+      <c r="E70" s="20"/>
+      <c r="F70" s="20"/>
+      <c r="G70" s="20"/>
+      <c r="H70" s="20"/>
+      <c r="I70" s="20"/>
+      <c r="J70" s="27"/>
+    </row>
+    <row r="73" ht="14.25"/>
+    <row r="74" spans="1:32">
+      <c r="A74" s="21"/>
+      <c r="B74" s="22" t="s">
         <v>0</v>
       </c>
-      <c r="C72" s="22" t="s">
+      <c r="C74" s="22" t="s">
         <v>1</v>
       </c>
-      <c r="D72" s="22" t="s">
+      <c r="D74" s="22" t="s">
         <v>2</v>
       </c>
-      <c r="E72" s="22" t="s">
+      <c r="E74" s="22" t="s">
         <v>3</v>
       </c>
-      <c r="F72" s="22" t="s">
+      <c r="F74" s="22" t="s">
         <v>4</v>
       </c>
-      <c r="G72" s="22" t="s">
+      <c r="G74" s="22" t="s">
         <v>5</v>
       </c>
-      <c r="H72" s="22" t="s">
+      <c r="H74" s="22" t="s">
         <v>6</v>
       </c>
-      <c r="I72" s="22" t="s">
+      <c r="I74" s="22" t="s">
         <v>7</v>
       </c>
-      <c r="J72" s="28" t="s">
+      <c r="J74" s="28" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="73" spans="1:10">
-      <c r="A73" s="23" t="s">
+      <c r="L74" s="21"/>
+      <c r="M74" s="22" t="s">
+        <v>0</v>
+      </c>
+      <c r="N74" s="22" t="s">
+        <v>1</v>
+      </c>
+      <c r="O74" s="22" t="s">
+        <v>2</v>
+      </c>
+      <c r="P74" s="22" t="s">
+        <v>3</v>
+      </c>
+      <c r="Q74" s="22" t="s">
+        <v>4</v>
+      </c>
+      <c r="R74" s="22" t="s">
+        <v>5</v>
+      </c>
+      <c r="S74" s="22" t="s">
+        <v>6</v>
+      </c>
+      <c r="T74" s="22" t="s">
+        <v>7</v>
+      </c>
+      <c r="U74" s="28" t="s">
+        <v>8</v>
+      </c>
+      <c r="W74" s="21"/>
+      <c r="X74" s="22" t="s">
+        <v>0</v>
+      </c>
+      <c r="Y74" s="22" t="s">
+        <v>1</v>
+      </c>
+      <c r="Z74" s="22" t="s">
+        <v>2</v>
+      </c>
+      <c r="AA74" s="22" t="s">
+        <v>3</v>
+      </c>
+      <c r="AB74" s="22" t="s">
+        <v>4</v>
+      </c>
+      <c r="AC74" s="22" t="s">
+        <v>5</v>
+      </c>
+      <c r="AD74" s="22" t="s">
+        <v>6</v>
+      </c>
+      <c r="AE74" s="22" t="s">
+        <v>7</v>
+      </c>
+      <c r="AF74" s="28" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="75" spans="1:32">
+      <c r="A75" s="23" t="s">
         <v>24</v>
       </c>
-      <c r="B73" s="24">
+      <c r="B75" s="24">
         <v>1039722</v>
       </c>
-      <c r="C73" s="24">
+      <c r="C75" s="24">
         <v>1083568</v>
       </c>
-      <c r="D73" s="24">
+      <c r="D75" s="24">
         <v>997663</v>
       </c>
-      <c r="E73" s="24">
+      <c r="E75" s="24">
         <v>1001733</v>
       </c>
-      <c r="F73" s="24">
+      <c r="F75" s="24">
         <v>1694616</v>
       </c>
-      <c r="G73" s="24">
+      <c r="G75" s="24">
         <v>1957027</v>
       </c>
-      <c r="H73" s="24">
+      <c r="H75" s="24">
         <v>426485</v>
       </c>
-      <c r="I73" s="24">
+      <c r="I75" s="24">
         <v>855802</v>
       </c>
-      <c r="J73" s="29"/>
-    </row>
-    <row r="74" spans="1:10">
-      <c r="A74" s="8"/>
-      <c r="J74" s="15"/>
-    </row>
-    <row r="75" spans="1:10">
-      <c r="A75" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="B75" s="7"/>
-      <c r="C75" s="7"/>
-      <c r="D75" s="7"/>
-      <c r="E75" s="7"/>
-      <c r="F75" s="7"/>
-      <c r="G75" s="7"/>
-      <c r="H75" s="7"/>
-      <c r="I75" s="7"/>
-      <c r="J75" s="14"/>
-    </row>
-    <row r="76" spans="1:10">
-      <c r="A76" s="8" t="s">
+      <c r="J75" s="29"/>
+      <c r="L75" s="23" t="s">
+        <v>24</v>
+      </c>
+      <c r="M75" s="24">
+        <v>1039722</v>
+      </c>
+      <c r="N75" s="24">
+        <v>1083568</v>
+      </c>
+      <c r="O75" s="24">
+        <v>997663</v>
+      </c>
+      <c r="P75" s="24">
+        <v>1001733</v>
+      </c>
+      <c r="Q75" s="24">
+        <v>1694616</v>
+      </c>
+      <c r="R75" s="24">
+        <v>1957027</v>
+      </c>
+      <c r="S75" s="24">
+        <v>426485</v>
+      </c>
+      <c r="T75" s="24">
+        <v>855802</v>
+      </c>
+      <c r="U75" s="29"/>
+      <c r="W75" s="23" t="s">
+        <v>24</v>
+      </c>
+      <c r="X75" s="24">
+        <v>1039722</v>
+      </c>
+      <c r="Y75" s="24">
+        <v>1083568</v>
+      </c>
+      <c r="Z75" s="24">
+        <v>997663</v>
+      </c>
+      <c r="AA75" s="24">
+        <v>1001733</v>
+      </c>
+      <c r="AB75" s="24">
+        <v>1694616</v>
+      </c>
+      <c r="AC75" s="24">
+        <v>1957027</v>
+      </c>
+      <c r="AD75" s="24">
+        <v>426485</v>
+      </c>
+      <c r="AE75" s="24">
+        <v>855802</v>
+      </c>
+      <c r="AF75" s="29"/>
+    </row>
+    <row r="76" spans="1:32">
+      <c r="A76" s="8"/>
+      <c r="J76" s="15"/>
+      <c r="L76" s="8"/>
+      <c r="U76" s="15"/>
+      <c r="W76" s="8"/>
+      <c r="AF76" s="15"/>
+    </row>
+    <row r="77" spans="1:32">
+      <c r="A77" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="B77" s="7"/>
+      <c r="C77" s="7"/>
+      <c r="D77" s="7"/>
+      <c r="E77" s="7"/>
+      <c r="F77" s="7"/>
+      <c r="G77" s="7"/>
+      <c r="H77" s="7"/>
+      <c r="I77" s="7"/>
+      <c r="J77" s="14"/>
+      <c r="L77" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="M77" s="7"/>
+      <c r="N77" s="7"/>
+      <c r="O77" s="7"/>
+      <c r="P77" s="7"/>
+      <c r="Q77" s="7"/>
+      <c r="R77" s="7"/>
+      <c r="S77" s="7"/>
+      <c r="T77" s="7"/>
+      <c r="U77" s="14"/>
+      <c r="W77" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="X77" s="7"/>
+      <c r="Y77" s="7"/>
+      <c r="Z77" s="7"/>
+      <c r="AA77" s="7"/>
+      <c r="AB77" s="7"/>
+      <c r="AC77" s="7"/>
+      <c r="AD77" s="7"/>
+      <c r="AE77" s="7"/>
+      <c r="AF77" s="14"/>
+    </row>
+    <row r="78" spans="1:32">
+      <c r="A78" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="B76" s="7"/>
-      <c r="C76" s="7"/>
-      <c r="D76" s="7"/>
-      <c r="E76" s="7"/>
-      <c r="F76" s="7"/>
-      <c r="G76" s="7"/>
-      <c r="H76" s="7"/>
-      <c r="I76" s="7"/>
-      <c r="J76" s="14"/>
-    </row>
-    <row r="77" spans="1:10">
-      <c r="A77" s="6" t="s">
+      <c r="B78" s="7"/>
+      <c r="C78" s="7"/>
+      <c r="D78" s="7"/>
+      <c r="E78" s="7"/>
+      <c r="F78" s="7"/>
+      <c r="G78" s="7"/>
+      <c r="H78" s="7"/>
+      <c r="I78" s="7"/>
+      <c r="J78" s="14"/>
+      <c r="L78" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="M78" s="7"/>
+      <c r="N78" s="7"/>
+      <c r="O78" s="7"/>
+      <c r="P78" s="7"/>
+      <c r="Q78" s="7"/>
+      <c r="R78" s="7"/>
+      <c r="S78" s="7"/>
+      <c r="T78" s="7"/>
+      <c r="U78" s="14"/>
+      <c r="W78" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="X78" s="7"/>
+      <c r="Y78" s="7"/>
+      <c r="Z78" s="7"/>
+      <c r="AA78" s="7"/>
+      <c r="AB78" s="7"/>
+      <c r="AC78" s="7"/>
+      <c r="AD78" s="7"/>
+      <c r="AE78" s="7"/>
+      <c r="AF78" s="14"/>
+    </row>
+    <row r="79" spans="1:32">
+      <c r="A79" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="B77" s="7">
+      <c r="B79" s="7">
         <v>0.212115440228391</v>
       </c>
-      <c r="C77" s="7">
+      <c r="C79" s="7">
         <v>0.177082696994985</v>
       </c>
-      <c r="D77" s="7">
+      <c r="D79" s="7">
         <v>0.348478583991745</v>
       </c>
-      <c r="E77" s="7">
+      <c r="E79" s="7">
         <v>0.128600159255576</v>
       </c>
-      <c r="F77" s="7">
+      <c r="F79" s="7">
         <v>0.0450454702134789</v>
       </c>
-      <c r="G77" s="7">
+      <c r="G79" s="7">
         <v>0.0896377651990727</v>
       </c>
-      <c r="H77" s="7">
+      <c r="H79" s="7">
         <v>0.102231876751721</v>
       </c>
-      <c r="I77" s="7">
+      <c r="I79" s="7">
         <v>0.0755164339928472</v>
       </c>
-      <c r="J77" s="16">
-        <f>SUM(B77:I77)</f>
+      <c r="J79" s="16">
+        <f>SUM(B79:I79)</f>
         <v>1.17870842662782</v>
       </c>
-    </row>
-    <row r="78" spans="1:10">
-      <c r="A78" s="6" t="s">
+      <c r="L79" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="M79" s="7">
+        <v>0.212610083091798</v>
+      </c>
+      <c r="N79" s="7">
+        <v>0.178048147162705</v>
+      </c>
+      <c r="O79" s="7">
+        <v>0.348811049361099</v>
+      </c>
+      <c r="P79" s="7">
+        <v>0.130516545288126</v>
+      </c>
+      <c r="Q79" s="7">
+        <v>0.0457448107661841</v>
+      </c>
+      <c r="R79" s="7">
+        <v>0.090839203886208</v>
+      </c>
+      <c r="S79" s="7">
+        <v>0.102366838709629</v>
+      </c>
+      <c r="T79" s="7">
+        <v>0.0753235418226055</v>
+      </c>
+      <c r="U79" s="16">
+        <f>SUM(M79:T79)</f>
+        <v>1.18426022008835</v>
+      </c>
+      <c r="W79" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="X79" s="7">
+        <v>0.208021298270889</v>
+      </c>
+      <c r="Y79" s="7">
+        <v>0.172066303803264</v>
+      </c>
+      <c r="Z79" s="7">
+        <v>0.359688816767279</v>
+      </c>
+      <c r="AA79" s="7">
+        <v>0.114825911730544</v>
+      </c>
+      <c r="AB79" s="7">
+        <v>0.0299016358139109</v>
+      </c>
+      <c r="AC79" s="7">
+        <v>0.00561278468943498</v>
+      </c>
+      <c r="AD79" s="7">
+        <v>0.0966504431290623</v>
+      </c>
+      <c r="AE79" s="7">
+        <v>0.0421888953279342</v>
+      </c>
+      <c r="AF79" s="16">
+        <f>SUM(X79:AE79)</f>
+        <v>1.02895608953232</v>
+      </c>
+    </row>
+    <row r="80" spans="1:32">
+      <c r="A80" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="B78" s="7">
+      <c r="B80" s="7">
         <v>681</v>
       </c>
-      <c r="C78" s="7">
+      <c r="C80" s="7">
         <v>549</v>
       </c>
-      <c r="D78" s="7">
+      <c r="D80" s="7">
         <v>960</v>
       </c>
-      <c r="E78" s="7">
+      <c r="E80" s="7">
         <v>412</v>
       </c>
-      <c r="F78" s="7">
+      <c r="F80" s="7">
         <v>1792</v>
       </c>
-      <c r="G78" s="7">
+      <c r="G80" s="7">
         <v>329</v>
       </c>
-      <c r="H78" s="7">
+      <c r="H80" s="7">
         <v>1441</v>
       </c>
-      <c r="I78" s="7">
+      <c r="I80" s="7">
         <v>634</v>
       </c>
-      <c r="J78" s="14">
+      <c r="J80" s="14">
         <v>1792</v>
       </c>
-    </row>
-    <row r="79" spans="1:10">
-      <c r="A79" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="B79" s="7">
+      <c r="L80" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="M80" s="7">
+        <v>1220</v>
+      </c>
+      <c r="N80" s="7">
+        <v>1123</v>
+      </c>
+      <c r="O80" s="2">
+        <v>1490</v>
+      </c>
+      <c r="P80" s="7">
+        <v>850</v>
+      </c>
+      <c r="Q80" s="7">
+        <v>1185</v>
+      </c>
+      <c r="R80" s="7">
+        <v>690</v>
+      </c>
+      <c r="S80" s="7">
+        <v>1115</v>
+      </c>
+      <c r="T80" s="7">
+        <v>1020</v>
+      </c>
+      <c r="U80" s="2">
+        <v>1490</v>
+      </c>
+      <c r="W80" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="X80" s="7">
+        <v>392</v>
+      </c>
+      <c r="Y80" s="7">
+        <v>293</v>
+      </c>
+      <c r="Z80" s="2">
+        <v>645</v>
+      </c>
+      <c r="AA80" s="7">
+        <v>191</v>
+      </c>
+      <c r="AB80" s="7">
+        <v>504</v>
+      </c>
+      <c r="AC80" s="7">
+        <v>280</v>
+      </c>
+      <c r="AD80" s="7">
+        <v>213</v>
+      </c>
+      <c r="AE80" s="7">
+        <v>223</v>
+      </c>
+      <c r="AF80" s="2">
+        <v>645</v>
+      </c>
+    </row>
+    <row r="81" spans="1:32">
+      <c r="A81" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="B81" s="7">
         <v>322308</v>
       </c>
-      <c r="C79" s="7">
+      <c r="C81" s="7">
         <v>281711</v>
       </c>
-      <c r="D79" s="7">
+      <c r="D81" s="7">
         <v>538705</v>
       </c>
-      <c r="E79" s="7">
+      <c r="E81" s="7">
         <v>200341</v>
       </c>
-      <c r="F79" s="7">
+      <c r="F81" s="7">
         <v>220299</v>
       </c>
-      <c r="G79" s="7">
+      <c r="G81" s="7">
         <v>430541</v>
       </c>
-      <c r="H79" s="7">
+      <c r="H81" s="7">
         <v>93809</v>
       </c>
-      <c r="I79" s="7">
+      <c r="I81" s="7">
         <v>171161</v>
       </c>
-      <c r="J79" s="14"/>
-    </row>
-    <row r="80" spans="1:10">
-      <c r="A80" s="8"/>
-      <c r="J80" s="15"/>
-    </row>
-    <row r="81" s="2" customFormat="1" spans="1:10">
-      <c r="A81" s="6" t="s">
+      <c r="J81" s="14"/>
+      <c r="L81" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="M81" s="7"/>
+      <c r="N81" s="7"/>
+      <c r="O81" s="7"/>
+      <c r="P81" s="7"/>
+      <c r="Q81" s="7"/>
+      <c r="R81" s="7"/>
+      <c r="S81" s="7"/>
+      <c r="T81" s="7"/>
+      <c r="U81" s="14"/>
+      <c r="W81" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="X81" s="7"/>
+      <c r="Y81" s="7"/>
+      <c r="Z81" s="7"/>
+      <c r="AA81" s="7"/>
+      <c r="AB81" s="7"/>
+      <c r="AC81" s="7"/>
+      <c r="AD81" s="7"/>
+      <c r="AE81" s="7"/>
+      <c r="AF81" s="14"/>
+    </row>
+    <row r="82" spans="1:32">
+      <c r="A82" s="8"/>
+      <c r="J82" s="15"/>
+      <c r="L82" s="8"/>
+      <c r="U82" s="15"/>
+      <c r="W82" s="8"/>
+      <c r="AF82" s="15"/>
+    </row>
+    <row r="83" s="2" customFormat="1" spans="1:32">
+      <c r="A83" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="B81" s="7"/>
-      <c r="C81" s="7"/>
-      <c r="D81" s="7"/>
-      <c r="E81" s="7"/>
-      <c r="F81" s="7"/>
-      <c r="G81" s="7"/>
-      <c r="H81" s="7"/>
-      <c r="I81" s="7"/>
-      <c r="J81" s="14"/>
-    </row>
-    <row r="82" s="2" customFormat="1" spans="1:10">
-      <c r="A82" s="6" t="s">
+      <c r="B83" s="7"/>
+      <c r="C83" s="7"/>
+      <c r="D83" s="7"/>
+      <c r="E83" s="7"/>
+      <c r="F83" s="7"/>
+      <c r="G83" s="7"/>
+      <c r="H83" s="7"/>
+      <c r="I83" s="7"/>
+      <c r="J83" s="14"/>
+      <c r="L83" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="M83" s="7"/>
+      <c r="N83" s="7"/>
+      <c r="O83" s="7"/>
+      <c r="P83" s="7"/>
+      <c r="Q83" s="7"/>
+      <c r="R83" s="7"/>
+      <c r="S83" s="7"/>
+      <c r="T83" s="7"/>
+      <c r="U83" s="14"/>
+      <c r="W83" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="X83" s="7"/>
+      <c r="Y83" s="7"/>
+      <c r="Z83" s="7"/>
+      <c r="AA83" s="7"/>
+      <c r="AB83" s="7"/>
+      <c r="AC83" s="7"/>
+      <c r="AD83" s="7"/>
+      <c r="AE83" s="7"/>
+      <c r="AF83" s="14"/>
+    </row>
+    <row r="84" s="2" customFormat="1" spans="1:32">
+      <c r="A84" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="B82" s="11">
+      <c r="B84" s="11">
         <v>0.20800686430345</v>
       </c>
-      <c r="C82" s="11">
+      <c r="C84" s="11">
         <v>0.173239206962822</v>
       </c>
-      <c r="D82" s="11">
+      <c r="D84" s="11">
         <v>0.346041541710196</v>
       </c>
-      <c r="E82" s="11">
+      <c r="E84" s="11">
         <v>0.124928278882666</v>
       </c>
-      <c r="F82" s="11">
+      <c r="F84" s="11">
         <v>0.0409924383808026</v>
       </c>
-      <c r="G82" s="11">
+      <c r="G84" s="11">
         <v>0.0453003114127127</v>
       </c>
-      <c r="H82" s="11">
+      <c r="H84" s="11">
         <v>0.0964368086720679</v>
       </c>
-      <c r="I82" s="11">
+      <c r="I84" s="11">
         <v>0.065879029949852</v>
       </c>
-      <c r="J82" s="16">
-        <f>SUM(B82:I82)</f>
+      <c r="J84" s="16">
+        <f>SUM(B84:I84)</f>
         <v>1.10082448027457</v>
       </c>
-    </row>
-    <row r="83" s="2" customFormat="1" spans="1:10">
-      <c r="A83" s="6" t="s">
+      <c r="L84" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="M84" s="11">
+        <v>0.207737472172823</v>
+      </c>
+      <c r="N84" s="11">
+        <v>0.172864798071239</v>
+      </c>
+      <c r="O84" s="11">
+        <v>0.346185146605167</v>
+      </c>
+      <c r="P84" s="11">
+        <v>0.126695077773503</v>
+      </c>
+      <c r="Q84" s="11">
+        <v>0.0405881734554024</v>
+      </c>
+      <c r="R84" s="11">
+        <v>0.0542699172938978</v>
+      </c>
+      <c r="S84" s="11">
+        <v>0.0968620615813381</v>
+      </c>
+      <c r="T84" s="11">
+        <v>0.0653439800586281</v>
+      </c>
+      <c r="U84" s="16">
+        <f>SUM(M84:T84)</f>
+        <v>1.110546627012</v>
+      </c>
+      <c r="W84" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="X84" s="11">
+        <v>0.207936098099326</v>
+      </c>
+      <c r="Y84" s="11">
+        <v>0.173133066835469</v>
+      </c>
+      <c r="Z84" s="11">
+        <v>0.36086728230694</v>
+      </c>
+      <c r="AA84" s="11">
+        <v>0.117444985416314</v>
+      </c>
+      <c r="AB84" s="11">
+        <v>0.0308039492387758</v>
+      </c>
+      <c r="AC84" s="11">
+        <v>0.0043669430886191</v>
+      </c>
+      <c r="AD84" s="11">
+        <v>0.0963550348991925</v>
+      </c>
+      <c r="AE84" s="11">
+        <v>0.0426430113460201</v>
+      </c>
+      <c r="AF84" s="16">
+        <f>SUM(X84:AE84)</f>
+        <v>1.03355037123066</v>
+      </c>
+    </row>
+    <row r="85" s="2" customFormat="1" spans="1:32">
+      <c r="A85" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="B83" s="7">
+      <c r="B85" s="7">
         <v>723</v>
       </c>
-      <c r="C83" s="7">
+      <c r="C85" s="7">
         <v>545</v>
       </c>
-      <c r="D83" s="7">
+      <c r="D85" s="7">
         <v>1028</v>
       </c>
-      <c r="E83" s="7">
+      <c r="E85" s="7">
         <v>416</v>
       </c>
-      <c r="F83" s="7">
+      <c r="F85" s="7">
         <v>1666</v>
       </c>
-      <c r="G83" s="7">
+      <c r="G85" s="7">
         <v>255</v>
       </c>
-      <c r="H83" s="7">
+      <c r="H85" s="7">
         <v>1864</v>
       </c>
-      <c r="I83" s="7">
+      <c r="I85" s="7">
         <v>633</v>
       </c>
-      <c r="J83" s="14">
+      <c r="J85" s="14">
         <v>1864</v>
       </c>
-    </row>
-    <row r="84" s="2" customFormat="1" spans="1:10">
-      <c r="A84" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="B84" s="7">
+      <c r="L85" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="M85" s="7">
+        <v>1425</v>
+      </c>
+      <c r="N85" s="7">
+        <v>1199</v>
+      </c>
+      <c r="O85" s="7">
+        <v>1900</v>
+      </c>
+      <c r="P85" s="7">
+        <v>902</v>
+      </c>
+      <c r="Q85" s="7">
+        <v>1774</v>
+      </c>
+      <c r="R85" s="7">
+        <v>495</v>
+      </c>
+      <c r="S85" s="7">
+        <v>1966</v>
+      </c>
+      <c r="T85" s="7">
+        <v>1044</v>
+      </c>
+      <c r="U85" s="14">
+        <v>1966</v>
+      </c>
+      <c r="W85" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="X85" s="7">
+        <v>417</v>
+      </c>
+      <c r="Y85" s="7">
+        <v>301</v>
+      </c>
+      <c r="Z85" s="7">
+        <v>697</v>
+      </c>
+      <c r="AA85" s="7">
+        <v>198</v>
+      </c>
+      <c r="AB85" s="7">
+        <v>649</v>
+      </c>
+      <c r="AC85" s="7">
+        <v>171</v>
+      </c>
+      <c r="AD85" s="7">
+        <v>586</v>
+      </c>
+      <c r="AE85" s="7">
+        <v>250</v>
+      </c>
+      <c r="AF85" s="14"/>
+    </row>
+    <row r="86" s="2" customFormat="1" spans="1:32">
+      <c r="A86" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="B86" s="7">
         <v>301514</v>
       </c>
-      <c r="C84" s="7">
+      <c r="C86" s="7">
         <v>260041</v>
       </c>
-      <c r="D84" s="7">
+      <c r="D86" s="7">
         <v>528729</v>
       </c>
-      <c r="E84" s="7">
+      <c r="E86" s="7">
         <v>190324</v>
       </c>
-      <c r="F84" s="7">
+      <c r="F86" s="7">
         <v>186407</v>
       </c>
-      <c r="G84" s="7">
+      <c r="G86" s="7">
         <v>293551</v>
       </c>
-      <c r="H84" s="7">
+      <c r="H86" s="7">
         <v>89545</v>
       </c>
-      <c r="I84" s="7">
+      <c r="I86" s="7">
         <v>162603</v>
       </c>
-      <c r="J84" s="14"/>
-    </row>
-    <row r="85" customFormat="1" spans="1:10">
-      <c r="A85" s="8"/>
-      <c r="B85" s="2"/>
-      <c r="C85" s="2"/>
-      <c r="D85" s="2"/>
-      <c r="E85" s="2"/>
-      <c r="F85" s="2"/>
-      <c r="G85" s="2"/>
-      <c r="H85" s="2"/>
-      <c r="I85" s="2"/>
-      <c r="J85" s="15"/>
-    </row>
-    <row r="86" spans="1:10">
-      <c r="A86" s="6" t="s">
+      <c r="J86" s="14"/>
+      <c r="L86" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="M86" s="7"/>
+      <c r="N86" s="7"/>
+      <c r="O86" s="7"/>
+      <c r="P86" s="7"/>
+      <c r="Q86" s="7"/>
+      <c r="R86" s="7"/>
+      <c r="S86" s="7"/>
+      <c r="T86" s="7"/>
+      <c r="U86" s="14"/>
+      <c r="W86" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="X86" s="7"/>
+      <c r="Y86" s="7"/>
+      <c r="Z86" s="7"/>
+      <c r="AA86" s="7"/>
+      <c r="AB86" s="7"/>
+      <c r="AC86" s="7"/>
+      <c r="AD86" s="7"/>
+      <c r="AE86" s="7"/>
+      <c r="AF86" s="14"/>
+    </row>
+    <row r="87" customFormat="1" spans="1:32">
+      <c r="A87" s="8"/>
+      <c r="B87" s="2"/>
+      <c r="C87" s="2"/>
+      <c r="D87" s="2"/>
+      <c r="E87" s="2"/>
+      <c r="F87" s="2"/>
+      <c r="G87" s="2"/>
+      <c r="H87" s="2"/>
+      <c r="I87" s="2"/>
+      <c r="J87" s="15"/>
+      <c r="L87" s="8"/>
+      <c r="M87" s="2"/>
+      <c r="N87" s="2"/>
+      <c r="O87" s="2"/>
+      <c r="P87" s="2"/>
+      <c r="Q87" s="2"/>
+      <c r="R87" s="2"/>
+      <c r="S87" s="2"/>
+      <c r="T87" s="2"/>
+      <c r="U87" s="15"/>
+      <c r="W87" s="8"/>
+      <c r="X87" s="2"/>
+      <c r="Y87" s="2"/>
+      <c r="Z87" s="2"/>
+      <c r="AA87" s="2"/>
+      <c r="AB87" s="2"/>
+      <c r="AC87" s="2"/>
+      <c r="AD87" s="2"/>
+      <c r="AE87" s="2"/>
+      <c r="AF87" s="15"/>
+    </row>
+    <row r="88" spans="1:32">
+      <c r="A88" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="B86" s="7"/>
-      <c r="C86" s="7"/>
-      <c r="D86" s="7"/>
-      <c r="E86" s="7"/>
-      <c r="F86" s="7"/>
-      <c r="G86" s="7"/>
-      <c r="H86" s="7"/>
-      <c r="I86" s="7"/>
-      <c r="J86" s="14"/>
-    </row>
-    <row r="87" spans="1:10">
-      <c r="A87" s="6" t="s">
+      <c r="B88" s="7"/>
+      <c r="C88" s="7"/>
+      <c r="D88" s="7"/>
+      <c r="E88" s="7"/>
+      <c r="F88" s="7"/>
+      <c r="G88" s="7"/>
+      <c r="H88" s="7"/>
+      <c r="I88" s="7"/>
+      <c r="J88" s="14"/>
+      <c r="L88" s="6"/>
+      <c r="M88" s="7"/>
+      <c r="N88" s="7"/>
+      <c r="O88" s="7"/>
+      <c r="P88" s="7"/>
+      <c r="Q88" s="7"/>
+      <c r="R88" s="7"/>
+      <c r="S88" s="7"/>
+      <c r="T88" s="7"/>
+      <c r="U88" s="14"/>
+      <c r="W88" s="6"/>
+      <c r="X88" s="7"/>
+      <c r="Y88" s="7"/>
+      <c r="Z88" s="7"/>
+      <c r="AA88" s="7"/>
+      <c r="AB88" s="7"/>
+      <c r="AC88" s="7"/>
+      <c r="AD88" s="7"/>
+      <c r="AE88" s="7"/>
+      <c r="AF88" s="14"/>
+    </row>
+    <row r="89" spans="1:32">
+      <c r="A89" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="B87" s="25">
+      <c r="B89" s="25">
         <v>0.207894527330402</v>
       </c>
-      <c r="C87" s="25">
+      <c r="C89" s="25">
         <v>0.173165858291852</v>
       </c>
-      <c r="D87" s="25">
+      <c r="D89" s="25">
         <v>0.344628020195683</v>
       </c>
-      <c r="E87" s="25">
+      <c r="E89" s="25">
         <v>0.118862297465155</v>
       </c>
-      <c r="F87" s="25">
+      <c r="F89" s="25">
         <v>0.0388983176119749</v>
       </c>
-      <c r="G87" s="25">
+      <c r="G89" s="25">
         <v>0.0422239303614074</v>
       </c>
-      <c r="H87" s="25">
+      <c r="H89" s="25">
         <v>0.0955131594160284</v>
       </c>
-      <c r="I87" s="25">
+      <c r="I89" s="25">
         <v>0.0488732287830458</v>
       </c>
-      <c r="J87" s="30">
-        <f>SUM(B87:I87)</f>
+      <c r="J89" s="30">
+        <f>SUM(B89:I89)</f>
         <v>1.07005933945555</v>
       </c>
-    </row>
-    <row r="88" spans="1:10">
-      <c r="A88" s="6" t="s">
+      <c r="L89" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="M89" s="31"/>
+      <c r="N89" s="31"/>
+      <c r="O89" s="31"/>
+      <c r="P89" s="31"/>
+      <c r="Q89" s="31"/>
+      <c r="R89" s="31"/>
+      <c r="S89" s="31"/>
+      <c r="T89" s="31"/>
+      <c r="U89" s="33">
+        <f>SUM(M89:T89)</f>
+        <v>0</v>
+      </c>
+      <c r="W89" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="X89" s="31"/>
+      <c r="Y89" s="31"/>
+      <c r="Z89" s="31"/>
+      <c r="AA89" s="31"/>
+      <c r="AB89" s="31"/>
+      <c r="AC89" s="31"/>
+      <c r="AD89" s="31"/>
+      <c r="AE89" s="31"/>
+      <c r="AF89" s="33">
+        <f>SUM(X89:AE89)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="90" spans="1:32">
+      <c r="A90" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="B88" s="7">
+      <c r="B90" s="7">
         <v>6112</v>
       </c>
-      <c r="C88" s="7">
+      <c r="C90" s="7">
         <v>1905</v>
       </c>
-      <c r="D88" s="7">
+      <c r="D90" s="7">
         <v>5427</v>
       </c>
-      <c r="E88" s="7">
+      <c r="E90" s="7">
         <v>1162</v>
       </c>
-      <c r="F88" s="7">
+      <c r="F90" s="7">
         <v>60491</v>
       </c>
-      <c r="G88" s="7">
+      <c r="G90" s="7">
         <v>223</v>
       </c>
-      <c r="H88" s="7">
+      <c r="H90" s="7">
         <v>149985</v>
       </c>
-      <c r="I88" s="7">
+      <c r="I90" s="7">
         <v>5050</v>
       </c>
-      <c r="J88" s="14">
+      <c r="J90" s="14">
         <v>149985</v>
       </c>
-    </row>
-    <row r="89" spans="1:10">
-      <c r="A89" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="B89" s="7">
+      <c r="L90" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="M90" s="7"/>
+      <c r="N90" s="7"/>
+      <c r="O90" s="7"/>
+      <c r="P90" s="7"/>
+      <c r="Q90" s="7"/>
+      <c r="R90" s="7"/>
+      <c r="S90" s="7"/>
+      <c r="T90" s="7"/>
+      <c r="U90" s="14"/>
+      <c r="W90" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="X90" s="7"/>
+      <c r="Y90" s="7"/>
+      <c r="Z90" s="7"/>
+      <c r="AA90" s="7"/>
+      <c r="AB90" s="7"/>
+      <c r="AC90" s="7"/>
+      <c r="AD90" s="7"/>
+      <c r="AE90" s="7"/>
+      <c r="AF90" s="14"/>
+    </row>
+    <row r="91" spans="1:32">
+      <c r="A91" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="B91" s="7">
         <v>301514</v>
       </c>
-      <c r="C89" s="7">
+      <c r="C91" s="7">
         <v>260041</v>
       </c>
-      <c r="D89" s="7">
+      <c r="D91" s="7">
         <v>518753</v>
       </c>
-      <c r="E89" s="7">
+      <c r="E91" s="7">
         <v>170290</v>
       </c>
-      <c r="F89" s="7">
+      <c r="F91" s="7">
         <v>169461</v>
       </c>
-      <c r="G89" s="7">
+      <c r="G91" s="7">
         <v>234841</v>
       </c>
-      <c r="H89" s="7">
+      <c r="H91" s="7">
         <v>85281</v>
       </c>
-      <c r="I89" s="7">
+      <c r="I91" s="7">
         <v>171161</v>
       </c>
-      <c r="J89" s="14"/>
-    </row>
-    <row r="90" spans="1:10">
-      <c r="A90" s="8"/>
-      <c r="J90" s="15"/>
-    </row>
-    <row r="91" s="2" customFormat="1" spans="1:10">
-      <c r="A91" s="6" t="s">
-        <v>37</v>
-      </c>
-      <c r="B91" s="7"/>
-      <c r="C91" s="7"/>
-      <c r="D91" s="7"/>
-      <c r="E91" s="7"/>
-      <c r="F91" s="7"/>
-      <c r="G91" s="7"/>
-      <c r="H91" s="7"/>
-      <c r="I91" s="7"/>
       <c r="J91" s="14"/>
-    </row>
-    <row r="92" s="2" customFormat="1" spans="1:10">
-      <c r="A92" s="6" t="s">
+      <c r="L91" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="M91" s="7"/>
+      <c r="N91" s="7"/>
+      <c r="O91" s="7"/>
+      <c r="P91" s="7"/>
+      <c r="Q91" s="7"/>
+      <c r="R91" s="7"/>
+      <c r="S91" s="7"/>
+      <c r="T91" s="7"/>
+      <c r="U91" s="14"/>
+      <c r="W91" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="X91" s="7"/>
+      <c r="Y91" s="7"/>
+      <c r="Z91" s="7"/>
+      <c r="AA91" s="7"/>
+      <c r="AB91" s="7"/>
+      <c r="AC91" s="7"/>
+      <c r="AD91" s="7"/>
+      <c r="AE91" s="7"/>
+      <c r="AF91" s="14"/>
+    </row>
+    <row r="92" spans="1:32">
+      <c r="A92" s="8"/>
+      <c r="J92" s="15"/>
+      <c r="L92" s="8"/>
+      <c r="U92" s="15"/>
+      <c r="W92" s="8"/>
+      <c r="AF92" s="15"/>
+    </row>
+    <row r="93" s="2" customFormat="1" spans="1:32">
+      <c r="A93" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="B93" s="7"/>
+      <c r="C93" s="7"/>
+      <c r="D93" s="7"/>
+      <c r="E93" s="7"/>
+      <c r="F93" s="7"/>
+      <c r="G93" s="7"/>
+      <c r="H93" s="7"/>
+      <c r="I93" s="7"/>
+      <c r="J93" s="14"/>
+      <c r="L93" s="6"/>
+      <c r="M93" s="7"/>
+      <c r="N93" s="7"/>
+      <c r="O93" s="7"/>
+      <c r="P93" s="7"/>
+      <c r="Q93" s="7"/>
+      <c r="R93" s="7"/>
+      <c r="S93" s="7"/>
+      <c r="T93" s="7"/>
+      <c r="U93" s="14"/>
+      <c r="W93" s="6"/>
+      <c r="X93" s="7"/>
+      <c r="Y93" s="7"/>
+      <c r="Z93" s="7"/>
+      <c r="AA93" s="7"/>
+      <c r="AB93" s="7"/>
+      <c r="AC93" s="7"/>
+      <c r="AD93" s="7"/>
+      <c r="AE93" s="7"/>
+      <c r="AF93" s="14"/>
+    </row>
+    <row r="94" s="2" customFormat="1" spans="1:32">
+      <c r="A94" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="B92" s="11"/>
-      <c r="C92" s="11"/>
-      <c r="D92" s="11"/>
-      <c r="E92" s="11"/>
-      <c r="F92" s="11"/>
-      <c r="G92" s="11">
+      <c r="B94" s="11"/>
+      <c r="C94" s="11"/>
+      <c r="D94" s="11"/>
+      <c r="E94" s="11"/>
+      <c r="F94" s="11"/>
+      <c r="G94" s="11">
         <v>0.0366467058789264</v>
       </c>
-      <c r="H92" s="11"/>
-      <c r="I92" s="11"/>
-      <c r="J92" s="16"/>
-    </row>
-    <row r="93" s="2" customFormat="1" spans="1:10">
-      <c r="A93" s="6" t="s">
+      <c r="H94" s="11"/>
+      <c r="I94" s="11"/>
+      <c r="J94" s="16"/>
+      <c r="L94" s="6"/>
+      <c r="M94" s="11"/>
+      <c r="N94" s="11"/>
+      <c r="O94" s="11"/>
+      <c r="P94" s="11"/>
+      <c r="Q94" s="11"/>
+      <c r="R94" s="11"/>
+      <c r="S94" s="11"/>
+      <c r="T94" s="11"/>
+      <c r="U94" s="16"/>
+      <c r="W94" s="6"/>
+      <c r="X94" s="11"/>
+      <c r="Y94" s="11"/>
+      <c r="Z94" s="11"/>
+      <c r="AA94" s="11"/>
+      <c r="AB94" s="11"/>
+      <c r="AC94" s="11"/>
+      <c r="AD94" s="11"/>
+      <c r="AE94" s="11"/>
+      <c r="AF94" s="16"/>
+    </row>
+    <row r="95" s="2" customFormat="1" spans="1:32">
+      <c r="A95" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="B93" s="11"/>
-      <c r="C93" s="11"/>
-      <c r="D93" s="11"/>
-      <c r="E93" s="11"/>
-      <c r="F93" s="11"/>
-      <c r="G93" s="11">
+      <c r="B95" s="11"/>
+      <c r="C95" s="11"/>
+      <c r="D95" s="11"/>
+      <c r="E95" s="11"/>
+      <c r="F95" s="11"/>
+      <c r="G95" s="11">
         <v>24917</v>
       </c>
-      <c r="H93" s="11"/>
-      <c r="I93" s="11"/>
-      <c r="J93" s="16"/>
-    </row>
-    <row r="94" s="2" customFormat="1" ht="14.25" spans="1:10">
-      <c r="A94" s="19" t="s">
-        <v>28</v>
-      </c>
-      <c r="B94" s="20"/>
-      <c r="C94" s="20"/>
-      <c r="D94" s="20"/>
-      <c r="E94" s="20"/>
-      <c r="F94" s="20"/>
-      <c r="G94" s="20">
+      <c r="H95" s="11"/>
+      <c r="I95" s="11"/>
+      <c r="J95" s="16"/>
+      <c r="L95" s="6"/>
+      <c r="M95" s="11"/>
+      <c r="N95" s="11"/>
+      <c r="O95" s="11"/>
+      <c r="P95" s="11"/>
+      <c r="Q95" s="11"/>
+      <c r="R95" s="11"/>
+      <c r="S95" s="11"/>
+      <c r="T95" s="11"/>
+      <c r="U95" s="16"/>
+      <c r="W95" s="6"/>
+      <c r="X95" s="11"/>
+      <c r="Y95" s="11"/>
+      <c r="Z95" s="11"/>
+      <c r="AA95" s="11"/>
+      <c r="AB95" s="11"/>
+      <c r="AC95" s="11"/>
+      <c r="AD95" s="11"/>
+      <c r="AE95" s="11"/>
+      <c r="AF95" s="16"/>
+    </row>
+    <row r="96" s="2" customFormat="1" ht="14.25" spans="1:32">
+      <c r="A96" s="19" t="s">
+        <v>29</v>
+      </c>
+      <c r="B96" s="20"/>
+      <c r="C96" s="20"/>
+      <c r="D96" s="20"/>
+      <c r="E96" s="20"/>
+      <c r="F96" s="20"/>
+      <c r="G96" s="20">
         <v>156561</v>
       </c>
-      <c r="H94" s="20"/>
-      <c r="I94" s="20"/>
-      <c r="J94" s="27"/>
-    </row>
-    <row r="95" ht="14.25"/>
-    <row r="96" spans="1:10">
-      <c r="A96" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="B96" s="5"/>
-      <c r="C96" s="5"/>
-      <c r="D96" s="5"/>
-      <c r="E96" s="5"/>
-      <c r="F96" s="5"/>
-      <c r="G96" s="5"/>
-      <c r="H96" s="5"/>
-      <c r="I96" s="5"/>
-      <c r="J96" s="13"/>
-    </row>
-    <row r="97" spans="1:10">
-      <c r="A97" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="B97" s="7"/>
-      <c r="C97" s="7"/>
-      <c r="D97" s="7"/>
-      <c r="E97" s="7"/>
-      <c r="F97" s="7"/>
-      <c r="G97" s="7"/>
-      <c r="H97" s="7"/>
-      <c r="I97" s="7"/>
-      <c r="J97" s="14"/>
-    </row>
+      <c r="H96" s="20"/>
+      <c r="I96" s="20"/>
+      <c r="J96" s="27"/>
+      <c r="L96" s="19"/>
+      <c r="M96" s="20"/>
+      <c r="N96" s="20"/>
+      <c r="O96" s="20"/>
+      <c r="P96" s="20"/>
+      <c r="Q96" s="20"/>
+      <c r="R96" s="20"/>
+      <c r="S96" s="20"/>
+      <c r="T96" s="20"/>
+      <c r="U96" s="27"/>
+      <c r="W96" s="19"/>
+      <c r="X96" s="20"/>
+      <c r="Y96" s="20"/>
+      <c r="Z96" s="20"/>
+      <c r="AA96" s="20"/>
+      <c r="AB96" s="20"/>
+      <c r="AC96" s="20"/>
+      <c r="AD96" s="20"/>
+      <c r="AE96" s="20"/>
+      <c r="AF96" s="27"/>
+    </row>
+    <row r="97" ht="14.25"/>
     <row r="98" spans="1:10">
-      <c r="A98" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="B98" s="7">
-        <v>0.228152205079095</v>
-      </c>
-      <c r="C98" s="7">
-        <v>0.191548875347098</v>
-      </c>
-      <c r="D98" s="7">
-        <v>0.379426065867224</v>
-      </c>
-      <c r="E98" s="7">
-        <v>0.143834806978518</v>
-      </c>
-      <c r="F98" s="7">
-        <v>0.0492015604703379</v>
-      </c>
-      <c r="G98" s="11">
-        <v>0.0766396493470802</v>
-      </c>
-      <c r="H98" s="7">
-        <v>0.110167879524473</v>
-      </c>
-      <c r="I98" s="7">
-        <v>0.0926905158740254</v>
-      </c>
-      <c r="J98" s="16">
-        <f>SUM(B98:I98)</f>
-        <v>1.27166155848785</v>
-      </c>
+      <c r="A98" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="B98" s="5"/>
+      <c r="C98" s="5"/>
+      <c r="D98" s="5"/>
+      <c r="E98" s="5"/>
+      <c r="F98" s="5"/>
+      <c r="G98" s="5"/>
+      <c r="H98" s="5"/>
+      <c r="I98" s="5"/>
+      <c r="J98" s="13"/>
     </row>
     <row r="99" spans="1:10">
       <c r="A99" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="B99" s="7">
-        <v>127</v>
-      </c>
-      <c r="C99" s="7">
-        <v>115</v>
-      </c>
-      <c r="D99" s="7">
-        <v>145</v>
-      </c>
-      <c r="E99" s="7">
-        <v>101</v>
-      </c>
-      <c r="F99" s="7">
-        <v>170</v>
-      </c>
-      <c r="G99" s="2">
-        <v>108</v>
-      </c>
-      <c r="H99" s="7">
-        <v>156</v>
-      </c>
-      <c r="I99" s="7">
-        <v>117</v>
-      </c>
-      <c r="J99" s="14">
-        <v>170</v>
-      </c>
+        <v>20</v>
+      </c>
+      <c r="B99" s="7"/>
+      <c r="C99" s="7"/>
+      <c r="D99" s="7"/>
+      <c r="E99" s="7"/>
+      <c r="F99" s="7"/>
+      <c r="G99" s="7"/>
+      <c r="H99" s="7"/>
+      <c r="I99" s="7"/>
+      <c r="J99" s="14"/>
     </row>
     <row r="100" spans="1:10">
       <c r="A100" s="6" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B100" s="7">
-        <v>322308</v>
+        <v>0.228152205079095</v>
       </c>
       <c r="C100" s="7">
-        <v>281711</v>
+        <v>0.191548875347098</v>
       </c>
       <c r="D100" s="7">
-        <v>538705</v>
+        <v>0.379426065867224</v>
       </c>
       <c r="E100" s="7">
-        <v>200341</v>
+        <v>0.143834806978518</v>
       </c>
       <c r="F100" s="7">
-        <v>220299</v>
-      </c>
-      <c r="G100" s="7">
-        <v>430541</v>
+        <v>0.0492015604703379</v>
+      </c>
+      <c r="G100" s="11">
+        <v>0.0766396493470802</v>
       </c>
       <c r="H100" s="7">
-        <v>93809</v>
+        <v>0.110167879524473</v>
       </c>
       <c r="I100" s="7">
-        <v>171161</v>
-      </c>
-      <c r="J100" s="14"/>
+        <v>0.0926905158740254</v>
+      </c>
+      <c r="J100" s="16">
+        <f>SUM(B100:I100)</f>
+        <v>1.27166155848785</v>
+      </c>
     </row>
     <row r="101" spans="1:10">
-      <c r="A101" s="8"/>
-      <c r="J101" s="15"/>
+      <c r="A101" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="B101" s="7">
+        <v>127</v>
+      </c>
+      <c r="C101" s="7">
+        <v>115</v>
+      </c>
+      <c r="D101" s="7">
+        <v>145</v>
+      </c>
+      <c r="E101" s="7">
+        <v>101</v>
+      </c>
+      <c r="F101" s="7">
+        <v>170</v>
+      </c>
+      <c r="G101" s="2">
+        <v>108</v>
+      </c>
+      <c r="H101" s="7">
+        <v>156</v>
+      </c>
+      <c r="I101" s="7">
+        <v>117</v>
+      </c>
+      <c r="J101" s="14">
+        <v>170</v>
+      </c>
     </row>
     <row r="102" spans="1:10">
       <c r="A102" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="B102" s="7"/>
-      <c r="C102" s="7"/>
-      <c r="D102" s="7"/>
-      <c r="E102" s="7"/>
-      <c r="F102" s="7"/>
-      <c r="G102" s="7"/>
-      <c r="H102" s="7"/>
-      <c r="I102" s="7"/>
+        <v>29</v>
+      </c>
+      <c r="B102" s="7">
+        <v>322308</v>
+      </c>
+      <c r="C102" s="7">
+        <v>281711</v>
+      </c>
+      <c r="D102" s="7">
+        <v>538705</v>
+      </c>
+      <c r="E102" s="7">
+        <v>200341</v>
+      </c>
+      <c r="F102" s="7">
+        <v>220299</v>
+      </c>
+      <c r="G102" s="7">
+        <v>430541</v>
+      </c>
+      <c r="H102" s="7">
+        <v>93809</v>
+      </c>
+      <c r="I102" s="7">
+        <v>171161</v>
+      </c>
       <c r="J102" s="14"/>
     </row>
     <row r="103" spans="1:10">
-      <c r="A103" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="B103" s="7">
-        <v>0.225357832225731</v>
-      </c>
-      <c r="C103" s="7">
-        <v>0.187832278626018</v>
-      </c>
-      <c r="D103" s="7">
-        <v>0.381070627327604</v>
-      </c>
-      <c r="E103" s="7">
-        <v>0.143343517352846</v>
-      </c>
-      <c r="F103" s="7">
-        <v>0.0533366743677525</v>
-      </c>
-      <c r="G103" s="9">
-        <v>0.110748101588701</v>
-      </c>
-      <c r="H103" s="7">
-        <v>0.111848633104288</v>
-      </c>
-      <c r="I103" s="7">
-        <v>0.103230203907768</v>
-      </c>
-      <c r="J103" s="16">
-        <f>SUM(B103:I103)</f>
-        <v>1.31676786850071</v>
-      </c>
+      <c r="A103" s="8"/>
+      <c r="J103" s="15"/>
     </row>
     <row r="104" spans="1:10">
       <c r="A104" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="B104" s="7">
-        <v>194</v>
-      </c>
-      <c r="C104" s="7">
-        <v>156</v>
-      </c>
-      <c r="D104" s="7">
-        <v>224</v>
-      </c>
-      <c r="E104" s="7">
-        <v>129</v>
-      </c>
-      <c r="F104" s="7">
-        <v>437</v>
-      </c>
-      <c r="G104" s="7">
-        <v>108</v>
-      </c>
-      <c r="H104" s="7">
-        <v>729</v>
-      </c>
-      <c r="I104" s="7">
-        <v>151</v>
-      </c>
-      <c r="J104" s="14">
-        <v>729</v>
-      </c>
+        <v>21</v>
+      </c>
+      <c r="B104" s="7"/>
+      <c r="C104" s="7"/>
+      <c r="D104" s="7"/>
+      <c r="E104" s="7"/>
+      <c r="F104" s="7"/>
+      <c r="G104" s="7"/>
+      <c r="H104" s="7"/>
+      <c r="I104" s="7"/>
+      <c r="J104" s="14"/>
     </row>
     <row r="105" spans="1:10">
       <c r="A105" s="6" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B105" s="7">
-        <v>301514</v>
+        <v>0.225357832225731</v>
       </c>
       <c r="C105" s="7">
-        <v>260041</v>
+        <v>0.187832278626018</v>
       </c>
       <c r="D105" s="7">
-        <v>528729</v>
+        <v>0.381070627327604</v>
       </c>
       <c r="E105" s="7">
-        <v>190324</v>
+        <v>0.143343517352846</v>
       </c>
       <c r="F105" s="7">
-        <v>186407</v>
-      </c>
-      <c r="G105" s="7">
-        <v>293551</v>
+        <v>0.0533366743677525</v>
+      </c>
+      <c r="G105" s="9">
+        <v>0.110748101588701</v>
       </c>
       <c r="H105" s="7">
-        <v>89545</v>
+        <v>0.111848633104288</v>
       </c>
       <c r="I105" s="7">
-        <v>162603</v>
-      </c>
-      <c r="J105" s="14"/>
+        <v>0.103230203907768</v>
+      </c>
+      <c r="J105" s="16">
+        <f>SUM(B105:I105)</f>
+        <v>1.31676786850071</v>
+      </c>
     </row>
     <row r="106" spans="1:10">
-      <c r="A106" s="8"/>
-      <c r="J106" s="15"/>
+      <c r="A106" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="B106" s="7">
+        <v>194</v>
+      </c>
+      <c r="C106" s="7">
+        <v>156</v>
+      </c>
+      <c r="D106" s="7">
+        <v>224</v>
+      </c>
+      <c r="E106" s="7">
+        <v>129</v>
+      </c>
+      <c r="F106" s="7">
+        <v>437</v>
+      </c>
+      <c r="G106" s="7">
+        <v>108</v>
+      </c>
+      <c r="H106" s="7">
+        <v>729</v>
+      </c>
+      <c r="I106" s="7">
+        <v>151</v>
+      </c>
+      <c r="J106" s="14">
+        <v>729</v>
+      </c>
     </row>
     <row r="107" spans="1:10">
       <c r="A107" s="6" t="s">
-        <v>39</v>
-      </c>
-      <c r="B107" s="7"/>
-      <c r="C107" s="7"/>
-      <c r="D107" s="7"/>
-      <c r="E107" s="7"/>
-      <c r="F107" s="7"/>
-      <c r="G107" s="7"/>
-      <c r="H107" s="7"/>
-      <c r="I107" s="7"/>
+        <v>29</v>
+      </c>
+      <c r="B107" s="7">
+        <v>301514</v>
+      </c>
+      <c r="C107" s="7">
+        <v>260041</v>
+      </c>
+      <c r="D107" s="7">
+        <v>528729</v>
+      </c>
+      <c r="E107" s="7">
+        <v>190324</v>
+      </c>
+      <c r="F107" s="7">
+        <v>186407</v>
+      </c>
+      <c r="G107" s="7">
+        <v>293551</v>
+      </c>
+      <c r="H107" s="7">
+        <v>89545</v>
+      </c>
+      <c r="I107" s="7">
+        <v>162603</v>
+      </c>
       <c r="J107" s="14"/>
     </row>
     <row r="108" spans="1:10">
-      <c r="A108" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="B108" s="7">
-        <v>0.223944128917166</v>
-      </c>
-      <c r="C108" s="7">
-        <v>0.186722386746853</v>
-      </c>
-      <c r="D108" s="7">
-        <v>0.37770148730091</v>
-      </c>
-      <c r="E108" s="7">
-        <v>0.131732931754474</v>
-      </c>
-      <c r="F108" s="7">
-        <v>0.0490670980855947</v>
-      </c>
-      <c r="G108" s="11">
-        <v>0.0970503709159689</v>
-      </c>
-      <c r="H108" s="7">
-        <v>0.108574350654746</v>
-      </c>
-      <c r="I108" s="7">
-        <v>0.0965472395965962</v>
-      </c>
-      <c r="J108" s="16">
-        <v>1.27133999397231</v>
-      </c>
+      <c r="A108" s="8"/>
+      <c r="J108" s="15"/>
     </row>
     <row r="109" spans="1:10">
       <c r="A109" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="B109" s="7"/>
+      <c r="C109" s="7"/>
+      <c r="D109" s="7"/>
+      <c r="E109" s="7"/>
+      <c r="F109" s="7"/>
+      <c r="G109" s="7"/>
+      <c r="H109" s="7"/>
+      <c r="I109" s="7"/>
+      <c r="J109" s="14"/>
+    </row>
+    <row r="110" spans="1:10">
+      <c r="A110" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="B110" s="7">
+        <v>0.223944128917166</v>
+      </c>
+      <c r="C110" s="7">
+        <v>0.186722386746853</v>
+      </c>
+      <c r="D110" s="7">
+        <v>0.37770148730091</v>
+      </c>
+      <c r="E110" s="7">
+        <v>0.131732931754474</v>
+      </c>
+      <c r="F110" s="7">
+        <v>0.0490670980855947</v>
+      </c>
+      <c r="G110" s="11">
+        <v>0.0970503709159689</v>
+      </c>
+      <c r="H110" s="7">
+        <v>0.108574350654746</v>
+      </c>
+      <c r="I110" s="7">
+        <v>0.0965472395965962</v>
+      </c>
+      <c r="J110" s="16">
+        <v>1.27133999397231</v>
+      </c>
+    </row>
+    <row r="111" spans="1:10">
+      <c r="A111" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="B109" s="7">
+      <c r="B111" s="7">
         <v>5546</v>
       </c>
-      <c r="C109" s="7">
+      <c r="C111" s="7">
         <v>1533</v>
       </c>
-      <c r="D109" s="7">
+      <c r="D111" s="7">
         <v>4598</v>
       </c>
-      <c r="E109" s="7">
+      <c r="E111" s="7">
         <v>896</v>
       </c>
-      <c r="F109" s="7">
+      <c r="F111" s="7">
         <v>59593</v>
       </c>
-      <c r="G109" s="7">
+      <c r="G111" s="7">
         <v>111</v>
       </c>
-      <c r="H109" s="7">
+      <c r="H111" s="7">
         <v>148014</v>
       </c>
-      <c r="I109" s="7">
+      <c r="I111" s="7">
         <v>4635</v>
       </c>
-      <c r="J109" s="14">
+      <c r="J111" s="14">
         <v>148014</v>
       </c>
     </row>
-    <row r="110" ht="14.25" spans="1:10">
-      <c r="A110" s="19" t="s">
-        <v>28</v>
-      </c>
-      <c r="B110" s="26">
+    <row r="112" ht="14.25" spans="1:10">
+      <c r="A112" s="19" t="s">
+        <v>29</v>
+      </c>
+      <c r="B112" s="26">
         <v>301514</v>
       </c>
-      <c r="C110" s="26">
+      <c r="C112" s="26">
         <v>260041</v>
       </c>
-      <c r="D110" s="26">
+      <c r="D112" s="26">
         <v>518753</v>
       </c>
-      <c r="E110" s="26">
+      <c r="E112" s="26">
         <v>170290</v>
       </c>
-      <c r="F110" s="26">
+      <c r="F112" s="26">
         <v>169461</v>
       </c>
-      <c r="G110" s="26">
+      <c r="G112" s="26">
         <v>234841</v>
       </c>
-      <c r="H110" s="26">
+      <c r="H112" s="26">
         <v>85281</v>
       </c>
-      <c r="I110" s="26">
+      <c r="I112" s="26">
         <v>171161</v>
       </c>
-      <c r="J110" s="31"/>
-    </row>
-    <row r="112" spans="1:10">
-      <c r="A112" s="7" t="s">
-        <v>40</v>
-      </c>
-      <c r="B112" s="7"/>
-      <c r="C112" s="7"/>
-      <c r="D112" s="7"/>
-      <c r="E112" s="7"/>
-      <c r="F112" s="7"/>
-      <c r="G112" s="7"/>
-      <c r="H112" s="7"/>
-      <c r="I112" s="7"/>
-      <c r="J112" s="7"/>
-    </row>
-    <row r="113" spans="1:10">
-      <c r="A113" s="7"/>
-      <c r="B113" s="7"/>
-      <c r="C113" s="7"/>
-      <c r="D113" s="7"/>
-      <c r="E113" s="7"/>
-      <c r="F113" s="7"/>
-      <c r="G113" s="7"/>
-      <c r="H113" s="7"/>
-      <c r="I113" s="7"/>
-      <c r="J113" s="7"/>
+      <c r="J112" s="32"/>
     </row>
     <row r="114" spans="1:10">
       <c r="A114" s="7" t="s">
-        <v>26</v>
+        <v>47</v>
       </c>
       <c r="B114" s="7"/>
       <c r="C114" s="7"/>
       <c r="D114" s="7"/>
       <c r="E114" s="7"/>
       <c r="F114" s="7"/>
-      <c r="G114" s="11"/>
+      <c r="G114" s="7"/>
       <c r="H114" s="7"/>
       <c r="I114" s="7"/>
-      <c r="J114" s="11"/>
+      <c r="J114" s="7"/>
     </row>
     <row r="115" spans="1:10">
-      <c r="A115" s="7" t="s">
-        <v>27</v>
-      </c>
+      <c r="A115" s="7"/>
       <c r="B115" s="7"/>
       <c r="C115" s="7"/>
       <c r="D115" s="7"/>
@@ -3982,21 +4735,35 @@
     </row>
     <row r="116" spans="1:10">
       <c r="A116" s="7" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B116" s="7"/>
       <c r="C116" s="7"/>
       <c r="D116" s="7"/>
       <c r="E116" s="7"/>
       <c r="F116" s="7"/>
-      <c r="G116" s="7"/>
+      <c r="G116" s="11"/>
       <c r="H116" s="7"/>
       <c r="I116" s="7"/>
-      <c r="J116" s="7"/>
+      <c r="J116" s="11"/>
+    </row>
+    <row r="117" spans="1:10">
+      <c r="A117" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="B117" s="7"/>
+      <c r="C117" s="7"/>
+      <c r="D117" s="7"/>
+      <c r="E117" s="7"/>
+      <c r="F117" s="7"/>
+      <c r="G117" s="7"/>
+      <c r="H117" s="7"/>
+      <c r="I117" s="7"/>
+      <c r="J117" s="7"/>
     </row>
     <row r="118" spans="1:10">
       <c r="A118" s="7" t="s">
-        <v>23</v>
+        <v>29</v>
       </c>
       <c r="B118" s="7"/>
       <c r="C118" s="7"/>
@@ -4008,25 +4775,9 @@
       <c r="I118" s="7"/>
       <c r="J118" s="7"/>
     </row>
-    <row r="119" spans="1:10">
-      <c r="A119" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="B119" s="7"/>
-      <c r="C119" s="7"/>
-      <c r="D119" s="7"/>
-      <c r="E119" s="7"/>
-      <c r="F119" s="7"/>
-      <c r="G119">
-        <v>0.102480606902965</v>
-      </c>
-      <c r="H119" s="7"/>
-      <c r="I119" s="7"/>
-      <c r="J119" s="11"/>
-    </row>
     <row r="120" spans="1:10">
       <c r="A120" s="7" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="B120" s="7"/>
       <c r="C120" s="7"/>
@@ -4040,17 +4791,47 @@
     </row>
     <row r="121" spans="1:10">
       <c r="A121" s="7" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B121" s="7"/>
       <c r="C121" s="7"/>
       <c r="D121" s="7"/>
       <c r="E121" s="7"/>
       <c r="F121" s="7"/>
-      <c r="G121" s="7"/>
+      <c r="G121">
+        <v>0.102480606902965</v>
+      </c>
       <c r="H121" s="7"/>
       <c r="I121" s="7"/>
-      <c r="J121" s="7"/>
+      <c r="J121" s="11"/>
+    </row>
+    <row r="122" spans="1:10">
+      <c r="A122" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="B122" s="7"/>
+      <c r="C122" s="7"/>
+      <c r="D122" s="7"/>
+      <c r="E122" s="7"/>
+      <c r="F122" s="7"/>
+      <c r="G122" s="7"/>
+      <c r="H122" s="7"/>
+      <c r="I122" s="7"/>
+      <c r="J122" s="7"/>
+    </row>
+    <row r="123" spans="1:10">
+      <c r="A123" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="B123" s="7"/>
+      <c r="C123" s="7"/>
+      <c r="D123" s="7"/>
+      <c r="E123" s="7"/>
+      <c r="F123" s="7"/>
+      <c r="G123" s="7"/>
+      <c r="H123" s="7"/>
+      <c r="I123" s="7"/>
+      <c r="J123" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.699305555555556" right="0.699305555555556" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Add more data and it seems that the lower ratio the better performance in RANK REINSERT
</commit_message>
<xml_diff>
--- a/overall.xlsx
+++ b/overall.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="28080" windowHeight="13065" activeTab="1"/>
+    <workbookView windowWidth="20385" windowHeight="8370" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70">
   <si>
     <t>model1</t>
   </si>
@@ -198,7 +198,34 @@
     <t>17_07_09_18_27_01_2_1_500_2</t>
   </si>
   <si>
+    <t>0.01/eachStep20/JustCount/mycode_reinsert</t>
+  </si>
+  <si>
+    <t>0.01/eachStep20/Rank/mycode_reinsert</t>
+  </si>
+  <si>
+    <t>17_07_21_21_44_14_2_1_500_5_0.01</t>
+  </si>
+  <si>
+    <t>17_07_22_12_43_32_0_1_500_7_0.01</t>
+  </si>
+  <si>
     <t>OpenSource_citm_without_reinsert</t>
+  </si>
+  <si>
+    <t>17_07_22_14_26_14_1_1_500_7_0.01</t>
+  </si>
+  <si>
+    <t>17_07_22_15_50_45_2_1_500_7_0.01</t>
+  </si>
+  <si>
+    <t>17_07_23_02_42_52_2_1_500_8_0.01/Concurrent Time</t>
+  </si>
+  <si>
+    <t>17_07_23_09_39_27_2_500_500_7_0.01</t>
+  </si>
+  <si>
+    <t>17_07_23_11_10_43_2_500_500_8_0.01/Concurrent Time</t>
   </si>
 </sst>
 </file>
@@ -206,10 +233,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="23">
     <font>
@@ -242,6 +269,13 @@
     </font>
     <font>
       <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="宋体"/>
       <charset val="0"/>
@@ -249,23 +283,8 @@
     </font>
     <font>
       <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FFFFFFFF"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -278,17 +297,23 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
       <name val="宋体"/>
-      <charset val="134"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="宋体"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
+      <color rgb="FF3F3F3F"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -302,46 +327,9 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <u/>
       <sz val="11"/>
       <color rgb="FF0000FF"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -363,8 +351,54 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <color rgb="FFFF0000"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -373,13 +407,6 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -406,7 +433,55 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -418,7 +493,67 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -430,7 +565,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8"/>
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -442,91 +589,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
+        <fgColor theme="4" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -538,55 +601,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
+        <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
+        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -753,11 +780,17 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -777,16 +810,16 @@
       <diagonal/>
     </border>
     <border>
-      <left style="double">
+      <left style="thin">
         <color rgb="FF3F3F3F"/>
       </left>
-      <right style="double">
+      <right style="thin">
         <color rgb="FF3F3F3F"/>
       </right>
-      <top style="double">
+      <top style="thin">
         <color rgb="FF3F3F3F"/>
       </top>
-      <bottom style="double">
+      <bottom style="thin">
         <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
@@ -796,7 +829,7 @@
       <right/>
       <top/>
       <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -819,23 +852,17 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -858,10 +885,10 @@
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="13" borderId="13" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="12" borderId="13" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -870,137 +897,137 @@
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="16" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="16" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="15" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="15" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="15" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="17" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="6" borderId="18" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="13" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="16" borderId="14" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="10" borderId="14" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="16" borderId="13" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="12" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="17" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="19" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="18" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="19" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="43">
+  <cellXfs count="51">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1103,22 +1130,46 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1">
@@ -1183,6 +1234,11 @@
     <cellStyle name="60% - 强调文字颜色 6" xfId="48" builtinId="52"/>
   </cellStyles>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -1568,7 +1624,7 @@
       <c r="F3">
         <v>0.0522827100851127</v>
       </c>
-      <c r="G3" s="40">
+      <c r="G3" s="48">
         <v>0.106926203216301</v>
       </c>
       <c r="H3">
@@ -1594,7 +1650,7 @@
       <c r="A12" t="s">
         <v>12</v>
       </c>
-      <c r="G12" s="41">
+      <c r="G12" s="49">
         <v>0.0629933219692992</v>
       </c>
     </row>
@@ -1647,7 +1703,7 @@
       <c r="I19">
         <v>0.0755164339928472</v>
       </c>
-      <c r="J19" s="42">
+      <c r="J19" s="50">
         <f t="shared" ref="J19:J21" si="0">SUM(B19:I19)</f>
         <v>1.17870842662782</v>
       </c>
@@ -1656,31 +1712,31 @@
       <c r="A20" t="s">
         <v>17</v>
       </c>
-      <c r="B20" s="42">
+      <c r="B20" s="50">
         <v>0.20800686430345</v>
       </c>
-      <c r="C20" s="42">
+      <c r="C20" s="50">
         <v>0.173239206962822</v>
       </c>
-      <c r="D20" s="42">
+      <c r="D20" s="50">
         <v>0.346041541710196</v>
       </c>
-      <c r="E20" s="42">
+      <c r="E20" s="50">
         <v>0.124928278882666</v>
       </c>
-      <c r="F20" s="42">
+      <c r="F20" s="50">
         <v>0.0409924383808026</v>
       </c>
-      <c r="G20" s="42">
+      <c r="G20" s="50">
         <v>0.0453003114127127</v>
       </c>
-      <c r="H20" s="42">
+      <c r="H20" s="50">
         <v>0.0964368086720679</v>
       </c>
-      <c r="I20" s="42">
+      <c r="I20" s="50">
         <v>0.065879029949852</v>
       </c>
-      <c r="J20" s="42">
+      <c r="J20" s="50">
         <f t="shared" si="0"/>
         <v>1.10082448027457</v>
       </c>
@@ -1689,52 +1745,52 @@
       <c r="A21" t="s">
         <v>18</v>
       </c>
-      <c r="B21" s="41">
+      <c r="B21" s="49">
         <v>0.207894527330402</v>
       </c>
-      <c r="C21" s="41">
+      <c r="C21" s="49">
         <v>0.173165858291852</v>
       </c>
-      <c r="D21" s="41">
+      <c r="D21" s="49">
         <v>0.344628020195683</v>
       </c>
-      <c r="E21" s="41">
+      <c r="E21" s="49">
         <v>0.118862297465155</v>
       </c>
-      <c r="F21" s="41">
+      <c r="F21" s="49">
         <v>0.0388983176119749</v>
       </c>
-      <c r="G21" s="41">
+      <c r="G21" s="49">
         <v>0.0422239303614074</v>
       </c>
-      <c r="H21" s="41">
+      <c r="H21" s="49">
         <v>0.0955131594160284</v>
       </c>
-      <c r="I21" s="41">
+      <c r="I21" s="49">
         <v>0.0488732287830458</v>
       </c>
-      <c r="J21" s="41">
+      <c r="J21" s="49">
         <f t="shared" si="0"/>
         <v>1.07005933945555</v>
       </c>
     </row>
     <row r="22" spans="10:10">
-      <c r="J22" s="42"/>
+      <c r="J22" s="50"/>
     </row>
     <row r="23" spans="10:10">
-      <c r="J23" s="42"/>
+      <c r="J23" s="50"/>
     </row>
     <row r="24" spans="10:10">
-      <c r="J24" s="42"/>
+      <c r="J24" s="50"/>
     </row>
     <row r="25" spans="10:10">
-      <c r="J25" s="42"/>
+      <c r="J25" s="50"/>
     </row>
     <row r="26" spans="1:10">
       <c r="A26" t="s">
         <v>19</v>
       </c>
-      <c r="J26" s="42"/>
+      <c r="J26" s="50"/>
     </row>
     <row r="27" spans="1:10">
       <c r="A27" t="s">
@@ -1755,7 +1811,7 @@
       <c r="F27">
         <v>0.0492015604703379</v>
       </c>
-      <c r="G27" s="42">
+      <c r="G27" s="50">
         <v>0.0766396493470802</v>
       </c>
       <c r="H27">
@@ -1764,7 +1820,7 @@
       <c r="I27">
         <v>0.0926905158740254</v>
       </c>
-      <c r="J27" s="42">
+      <c r="J27" s="50">
         <f>SUM(B27:I27)</f>
         <v>1.27166155848785</v>
       </c>
@@ -1788,7 +1844,7 @@
       <c r="F28">
         <v>0.0533366743677525</v>
       </c>
-      <c r="G28" s="40">
+      <c r="G28" s="48">
         <v>0.110748101588701</v>
       </c>
       <c r="H28">
@@ -1797,7 +1853,7 @@
       <c r="I28">
         <v>0.103230203907768</v>
       </c>
-      <c r="J28" s="42">
+      <c r="J28" s="50">
         <f>SUM(B28:I28)</f>
         <v>1.31676786850071</v>
       </c>
@@ -1825,10 +1881,10 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr/>
-  <dimension ref="A1:AF126"/>
+  <dimension ref="A1:AF144"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="S64" workbookViewId="0">
-      <selection activeCell="J35" sqref="J35"/>
+    <sheetView tabSelected="1" topLeftCell="X121" workbookViewId="0">
+      <selection activeCell="AF135" sqref="AF135"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
@@ -1840,12 +1896,15 @@
     <col min="8" max="8" width="11.5" style="2" customWidth="1"/>
     <col min="9" max="10" width="12.625" style="2" customWidth="1"/>
     <col min="11" max="11" width="9" style="2"/>
-    <col min="12" max="12" width="33.75" style="2" customWidth="1"/>
+    <col min="12" max="12" width="46" style="2" customWidth="1"/>
     <col min="13" max="21" width="12.625" style="2" customWidth="1"/>
     <col min="22" max="22" width="9" style="2"/>
-    <col min="23" max="23" width="50.375" style="2" customWidth="1"/>
+    <col min="23" max="23" width="56" style="2" customWidth="1"/>
     <col min="24" max="32" width="12.625" style="2" customWidth="1"/>
-    <col min="33" max="16384" width="9" style="2"/>
+    <col min="33" max="33" width="9" style="2"/>
+    <col min="34" max="34" width="50.375" style="2" customWidth="1"/>
+    <col min="35" max="43" width="12.625" style="2" customWidth="1"/>
+    <col min="44" max="16384" width="9" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10">
@@ -3760,31 +3819,31 @@
       <c r="W83" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="X83" s="37">
+      <c r="X83" s="34">
         <v>392</v>
       </c>
-      <c r="Y83" s="37">
+      <c r="Y83" s="34">
         <v>293</v>
       </c>
-      <c r="Z83" s="39">
+      <c r="Z83" s="37">
         <v>645</v>
       </c>
-      <c r="AA83" s="37">
+      <c r="AA83" s="34">
         <v>191</v>
       </c>
-      <c r="AB83" s="37">
+      <c r="AB83" s="34">
         <v>504</v>
       </c>
-      <c r="AC83" s="37">
+      <c r="AC83" s="34">
         <v>280</v>
       </c>
-      <c r="AD83" s="37">
+      <c r="AD83" s="34">
         <v>213</v>
       </c>
-      <c r="AE83" s="37">
+      <c r="AE83" s="34">
         <v>223</v>
       </c>
-      <c r="AF83" s="39">
+      <c r="AF83" s="37">
         <v>645</v>
       </c>
     </row>
@@ -4041,37 +4100,37 @@
       <c r="T88" s="29">
         <v>1044</v>
       </c>
-      <c r="U88" s="38">
+      <c r="U88" s="36">
         <v>1966</v>
       </c>
       <c r="W88" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="X88" s="37">
+      <c r="X88" s="34">
         <v>417</v>
       </c>
-      <c r="Y88" s="37">
+      <c r="Y88" s="34">
         <v>301</v>
       </c>
-      <c r="Z88" s="37">
+      <c r="Z88" s="34">
         <v>697</v>
       </c>
-      <c r="AA88" s="37">
+      <c r="AA88" s="34">
         <v>198</v>
       </c>
-      <c r="AB88" s="37">
+      <c r="AB88" s="34">
         <v>649</v>
       </c>
-      <c r="AC88" s="37">
+      <c r="AC88" s="34">
         <v>171</v>
       </c>
-      <c r="AD88" s="37">
+      <c r="AD88" s="34">
         <v>586</v>
       </c>
-      <c r="AE88" s="37">
+      <c r="AE88" s="34">
         <v>250</v>
       </c>
-      <c r="AF88" s="37">
+      <c r="AF88" s="34">
         <v>697</v>
       </c>
     </row>
@@ -4358,31 +4417,31 @@
       <c r="W93" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="X93" s="37">
+      <c r="X93" s="34">
         <v>1319</v>
       </c>
-      <c r="Y93" s="37">
+      <c r="Y93" s="34">
         <v>558</v>
       </c>
-      <c r="Z93" s="37">
+      <c r="Z93" s="34">
         <v>1593</v>
       </c>
-      <c r="AA93" s="37">
+      <c r="AA93" s="34">
         <v>317</v>
       </c>
-      <c r="AB93" s="37">
+      <c r="AB93" s="34">
         <v>21857</v>
       </c>
-      <c r="AC93" s="37">
+      <c r="AC93" s="34">
         <v>117</v>
       </c>
-      <c r="AD93" s="37">
+      <c r="AD93" s="34">
         <v>36466</v>
       </c>
-      <c r="AE93" s="37">
+      <c r="AE93" s="34">
         <v>641</v>
       </c>
-      <c r="AF93" s="37">
+      <c r="AF93" s="34">
         <v>36466</v>
       </c>
     </row>
@@ -4666,48 +4725,48 @@
       <c r="S99" s="11"/>
       <c r="T99" s="11"/>
       <c r="U99" s="11"/>
-      <c r="W99" s="34" t="s">
+      <c r="W99" s="7" t="s">
         <v>53</v>
       </c>
-      <c r="X99" s="35">
+      <c r="X99" s="34">
         <v>763</v>
       </c>
-      <c r="Y99" s="35">
+      <c r="Y99" s="34">
         <v>583</v>
       </c>
-      <c r="Z99" s="35">
+      <c r="Z99" s="34">
         <v>1150</v>
       </c>
-      <c r="AA99" s="35">
+      <c r="AA99" s="34">
         <v>407</v>
       </c>
-      <c r="AB99" s="35">
+      <c r="AB99" s="34">
         <v>841</v>
       </c>
-      <c r="AC99" s="35">
+      <c r="AC99" s="34">
         <v>465</v>
       </c>
-      <c r="AD99" s="35">
+      <c r="AD99" s="34">
         <v>544</v>
       </c>
-      <c r="AE99" s="35">
+      <c r="AE99" s="34">
         <v>458</v>
       </c>
-      <c r="AF99" s="35">
+      <c r="AF99" s="34">
         <v>1150</v>
       </c>
     </row>
     <row r="100" ht="14.25" spans="12:32">
-      <c r="L100" s="34"/>
-      <c r="M100" s="34"/>
-      <c r="N100" s="34"/>
-      <c r="O100" s="34"/>
-      <c r="P100" s="34"/>
-      <c r="Q100" s="34"/>
-      <c r="R100" s="34"/>
-      <c r="S100" s="34"/>
-      <c r="T100" s="34"/>
-      <c r="U100" s="34"/>
+      <c r="L100" s="7"/>
+      <c r="M100" s="7"/>
+      <c r="N100" s="7"/>
+      <c r="O100" s="7"/>
+      <c r="P100" s="7"/>
+      <c r="Q100" s="7"/>
+      <c r="R100" s="7"/>
+      <c r="S100" s="7"/>
+      <c r="T100" s="7"/>
+      <c r="U100" s="7"/>
       <c r="W100" s="6" t="s">
         <v>29</v>
       </c>
@@ -4737,15 +4796,15 @@
       <c r="L101" s="6" t="s">
         <v>55</v>
       </c>
-      <c r="M101" s="34"/>
-      <c r="N101" s="34"/>
-      <c r="O101" s="34"/>
-      <c r="P101" s="34"/>
-      <c r="Q101" s="34"/>
-      <c r="R101" s="34"/>
-      <c r="S101" s="34"/>
-      <c r="T101" s="34"/>
-      <c r="U101" s="34"/>
+      <c r="M101" s="7"/>
+      <c r="N101" s="7"/>
+      <c r="O101" s="7"/>
+      <c r="P101" s="7"/>
+      <c r="Q101" s="7"/>
+      <c r="R101" s="7"/>
+      <c r="S101" s="7"/>
+      <c r="T101" s="7"/>
+      <c r="U101" s="7"/>
     </row>
     <row r="102" spans="1:32">
       <c r="A102" s="6" t="s">
@@ -4763,45 +4822,45 @@
       <c r="L102" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="M102" s="34">
+      <c r="M102" s="7">
         <v>0.208166067302931</v>
       </c>
-      <c r="N102" s="34">
+      <c r="N102" s="7">
         <v>0.173241272969537</v>
       </c>
-      <c r="O102" s="34">
+      <c r="O102" s="7">
         <v>0.345212092248508</v>
       </c>
-      <c r="P102" s="34">
+      <c r="P102" s="7">
         <v>0.12026906042781</v>
       </c>
-      <c r="Q102" s="34">
+      <c r="Q102" s="7">
         <v>0.0370820736036616</v>
       </c>
-      <c r="R102" s="34">
+      <c r="R102" s="7">
         <v>0.0343696785040505</v>
       </c>
-      <c r="S102" s="34">
+      <c r="S102" s="7">
         <v>0.0953451042202933</v>
       </c>
-      <c r="T102" s="34">
+      <c r="T102" s="7">
         <v>0.0545283599763373</v>
       </c>
-      <c r="U102" s="34">
+      <c r="U102" s="7">
         <v>1.06821370925313</v>
       </c>
-      <c r="W102" s="34" t="s">
+      <c r="W102" s="7" t="s">
         <v>56</v>
       </c>
-      <c r="X102" s="34"/>
-      <c r="Y102" s="34"/>
-      <c r="Z102" s="34"/>
-      <c r="AA102" s="34"/>
-      <c r="AB102" s="34"/>
-      <c r="AC102" s="34"/>
-      <c r="AD102" s="34"/>
-      <c r="AE102" s="34"/>
-      <c r="AF102" s="34"/>
+      <c r="X102" s="7"/>
+      <c r="Y102" s="7"/>
+      <c r="Z102" s="7"/>
+      <c r="AA102" s="7"/>
+      <c r="AB102" s="7"/>
+      <c r="AC102" s="7"/>
+      <c r="AD102" s="7"/>
+      <c r="AE102" s="7"/>
+      <c r="AF102" s="7"/>
     </row>
     <row r="103" spans="1:32">
       <c r="A103" s="6" t="s">
@@ -4838,58 +4897,58 @@
       <c r="L103" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="M103" s="35">
+      <c r="M103" s="34">
         <v>5597</v>
       </c>
-      <c r="N103" s="35">
+      <c r="N103" s="34">
         <v>2831</v>
       </c>
-      <c r="O103" s="35">
+      <c r="O103" s="34">
         <v>17495</v>
       </c>
-      <c r="P103" s="35">
+      <c r="P103" s="34">
         <v>1535</v>
       </c>
-      <c r="Q103" s="35">
+      <c r="Q103" s="34">
         <v>11640</v>
       </c>
-      <c r="R103" s="35">
+      <c r="R103" s="34">
         <v>210</v>
       </c>
-      <c r="S103" s="35">
+      <c r="S103" s="34">
         <v>18972</v>
       </c>
-      <c r="T103" s="35">
+      <c r="T103" s="34">
         <v>1683</v>
       </c>
-      <c r="U103" s="35">
+      <c r="U103" s="34">
         <v>18972</v>
       </c>
       <c r="W103" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="X103" s="34">
+      <c r="X103" s="7">
         <v>0.207425728462033</v>
       </c>
-      <c r="Y103" s="34">
+      <c r="Y103" s="7">
         <v>0.171338688646963</v>
       </c>
-      <c r="Z103" s="34">
+      <c r="Z103" s="7">
         <v>0.361491291979076</v>
       </c>
-      <c r="AA103" s="34">
+      <c r="AA103" s="7">
         <v>0.113168213422427</v>
       </c>
-      <c r="AB103" s="34">
+      <c r="AB103" s="7">
         <v>0.0289916134188518</v>
       </c>
-      <c r="AC103" s="34">
+      <c r="AC103" s="7">
         <v>0.00374726353544287</v>
       </c>
-      <c r="AD103" s="34">
+      <c r="AD103" s="7">
         <v>0.0962610952368913</v>
       </c>
-      <c r="AE103" s="34">
+      <c r="AE103" s="7">
         <v>0.0403390626919688</v>
       </c>
       <c r="AF103" s="16">
@@ -4931,43 +4990,43 @@
       <c r="L104" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="M104" s="34"/>
-      <c r="N104" s="34"/>
-      <c r="O104" s="34"/>
-      <c r="P104" s="34"/>
-      <c r="Q104" s="34"/>
-      <c r="R104" s="34"/>
-      <c r="S104" s="34"/>
-      <c r="T104" s="34"/>
-      <c r="U104" s="34"/>
+      <c r="M104" s="7"/>
+      <c r="N104" s="7"/>
+      <c r="O104" s="7"/>
+      <c r="P104" s="7"/>
+      <c r="Q104" s="7"/>
+      <c r="R104" s="7"/>
+      <c r="S104" s="7"/>
+      <c r="T104" s="7"/>
+      <c r="U104" s="7"/>
       <c r="W104" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="X104" s="35">
+      <c r="X104" s="34">
         <v>2141</v>
       </c>
-      <c r="Y104" s="35">
+      <c r="Y104" s="34">
         <v>993</v>
       </c>
-      <c r="Z104" s="35">
+      <c r="Z104" s="34">
         <v>7592</v>
       </c>
-      <c r="AA104" s="35">
+      <c r="AA104" s="34">
         <v>524</v>
       </c>
-      <c r="AB104" s="35">
+      <c r="AB104" s="34">
         <v>5101</v>
       </c>
-      <c r="AC104" s="35">
+      <c r="AC104" s="34">
         <v>102</v>
       </c>
-      <c r="AD104" s="35">
+      <c r="AD104" s="34">
         <v>8317</v>
       </c>
-      <c r="AE104" s="35">
+      <c r="AE104" s="34">
         <v>562</v>
       </c>
-      <c r="AF104" s="35">
+      <c r="AF104" s="34">
         <v>8317</v>
       </c>
     </row>
@@ -5000,44 +5059,44 @@
         <v>171161</v>
       </c>
       <c r="J105" s="14"/>
-      <c r="L105" s="34"/>
-      <c r="M105" s="34"/>
-      <c r="N105" s="34"/>
-      <c r="O105" s="34"/>
-      <c r="P105" s="34"/>
-      <c r="Q105" s="34"/>
-      <c r="R105" s="34"/>
-      <c r="S105" s="34"/>
-      <c r="T105" s="34"/>
-      <c r="U105" s="34"/>
+      <c r="L105" s="7"/>
+      <c r="M105" s="7"/>
+      <c r="N105" s="7"/>
+      <c r="O105" s="7"/>
+      <c r="P105" s="7"/>
+      <c r="Q105" s="7"/>
+      <c r="R105" s="7"/>
+      <c r="S105" s="7"/>
+      <c r="T105" s="7"/>
+      <c r="U105" s="7"/>
       <c r="W105" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="X105" s="35">
+      <c r="X105" s="34">
         <v>3301</v>
       </c>
-      <c r="Y105" s="35">
+      <c r="Y105" s="34">
         <v>2368</v>
       </c>
-      <c r="Z105" s="35">
+      <c r="Z105" s="34">
         <v>4715</v>
       </c>
-      <c r="AA105" s="35">
+      <c r="AA105" s="34">
         <v>1554</v>
       </c>
-      <c r="AB105" s="35">
+      <c r="AB105" s="34">
         <v>3776</v>
       </c>
-      <c r="AC105" s="35">
+      <c r="AC105" s="34">
         <v>893</v>
       </c>
-      <c r="AD105" s="35">
+      <c r="AD105" s="34">
         <v>3791</v>
       </c>
-      <c r="AE105" s="35">
+      <c r="AE105" s="34">
         <v>1340</v>
       </c>
-      <c r="AF105" s="35">
+      <c r="AF105" s="34">
         <v>4715</v>
       </c>
     </row>
@@ -5047,27 +5106,27 @@
       <c r="L106" s="6" t="s">
         <v>58</v>
       </c>
-      <c r="M106" s="34"/>
-      <c r="N106" s="34"/>
-      <c r="O106" s="34"/>
-      <c r="P106" s="34"/>
-      <c r="Q106" s="34"/>
-      <c r="R106" s="34"/>
-      <c r="S106" s="34"/>
-      <c r="T106" s="34"/>
-      <c r="U106" s="34"/>
+      <c r="M106" s="7"/>
+      <c r="N106" s="7"/>
+      <c r="O106" s="7"/>
+      <c r="P106" s="7"/>
+      <c r="Q106" s="7"/>
+      <c r="R106" s="7"/>
+      <c r="S106" s="7"/>
+      <c r="T106" s="7"/>
+      <c r="U106" s="7"/>
       <c r="W106" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="X106" s="34"/>
-      <c r="Y106" s="34"/>
-      <c r="Z106" s="34"/>
-      <c r="AA106" s="34"/>
-      <c r="AB106" s="34"/>
-      <c r="AC106" s="34"/>
-      <c r="AD106" s="34"/>
-      <c r="AE106" s="34"/>
-      <c r="AF106" s="34"/>
+      <c r="X106" s="7"/>
+      <c r="Y106" s="7"/>
+      <c r="Z106" s="7"/>
+      <c r="AA106" s="7"/>
+      <c r="AB106" s="7"/>
+      <c r="AC106" s="7"/>
+      <c r="AD106" s="7"/>
+      <c r="AE106" s="7"/>
+      <c r="AF106" s="7"/>
     </row>
     <row r="107" spans="1:32">
       <c r="A107" s="6" t="s">
@@ -5085,25 +5144,25 @@
       <c r="L107" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="M107" s="34"/>
-      <c r="N107" s="34"/>
-      <c r="O107" s="34"/>
-      <c r="P107" s="34"/>
-      <c r="Q107" s="34"/>
-      <c r="R107" s="34"/>
-      <c r="S107" s="34"/>
-      <c r="T107" s="34"/>
-      <c r="U107" s="34"/>
-      <c r="W107" s="34"/>
-      <c r="X107" s="34"/>
-      <c r="Y107" s="34"/>
-      <c r="Z107" s="34"/>
-      <c r="AA107" s="34"/>
-      <c r="AB107" s="34"/>
-      <c r="AC107" s="34"/>
-      <c r="AD107" s="34"/>
-      <c r="AE107" s="34"/>
-      <c r="AF107" s="34"/>
+      <c r="M107" s="7"/>
+      <c r="N107" s="7"/>
+      <c r="O107" s="7"/>
+      <c r="P107" s="7"/>
+      <c r="Q107" s="7"/>
+      <c r="R107" s="7"/>
+      <c r="S107" s="7"/>
+      <c r="T107" s="7"/>
+      <c r="U107" s="7"/>
+      <c r="W107" s="7"/>
+      <c r="X107" s="7"/>
+      <c r="Y107" s="7"/>
+      <c r="Z107" s="7"/>
+      <c r="AA107" s="7"/>
+      <c r="AB107" s="7"/>
+      <c r="AC107" s="7"/>
+      <c r="AD107" s="7"/>
+      <c r="AE107" s="7"/>
+      <c r="AF107" s="7"/>
     </row>
     <row r="108" spans="1:32">
       <c r="A108" s="6" t="s">
@@ -5140,35 +5199,35 @@
       <c r="L108" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="M108" s="35">
+      <c r="M108" s="34">
         <v>38223</v>
       </c>
-      <c r="N108" s="35">
+      <c r="N108" s="34">
         <v>13177</v>
       </c>
-      <c r="O108" s="35"/>
-      <c r="P108" s="35">
+      <c r="O108" s="34"/>
+      <c r="P108" s="34">
         <v>6386</v>
       </c>
-      <c r="Q108" s="35"/>
-      <c r="R108" s="35">
+      <c r="Q108" s="34"/>
+      <c r="R108" s="34">
         <v>212</v>
       </c>
-      <c r="S108" s="35"/>
-      <c r="T108" s="35">
+      <c r="S108" s="34"/>
+      <c r="T108" s="34">
         <v>7979</v>
       </c>
-      <c r="U108" s="35"/>
-      <c r="W108" s="34"/>
-      <c r="X108" s="34"/>
-      <c r="Y108" s="34"/>
-      <c r="Z108" s="34"/>
-      <c r="AA108" s="34"/>
-      <c r="AB108" s="34"/>
-      <c r="AC108" s="34"/>
-      <c r="AD108" s="34"/>
-      <c r="AE108" s="34"/>
-      <c r="AF108" s="34"/>
+      <c r="U108" s="34"/>
+      <c r="W108" s="7"/>
+      <c r="X108" s="7"/>
+      <c r="Y108" s="7"/>
+      <c r="Z108" s="7"/>
+      <c r="AA108" s="7"/>
+      <c r="AB108" s="7"/>
+      <c r="AC108" s="7"/>
+      <c r="AD108" s="7"/>
+      <c r="AE108" s="7"/>
+      <c r="AF108" s="7"/>
     </row>
     <row r="109" spans="1:32">
       <c r="A109" s="6" t="s">
@@ -5204,25 +5263,25 @@
       <c r="L109" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="M109" s="34"/>
-      <c r="N109" s="34"/>
-      <c r="O109" s="34"/>
-      <c r="P109" s="34"/>
-      <c r="Q109" s="34"/>
-      <c r="R109" s="34"/>
-      <c r="S109" s="34"/>
-      <c r="T109" s="34"/>
-      <c r="U109" s="34"/>
-      <c r="W109" s="34"/>
-      <c r="X109" s="34"/>
-      <c r="Y109" s="34"/>
-      <c r="Z109" s="34"/>
-      <c r="AA109" s="34"/>
-      <c r="AB109" s="34"/>
-      <c r="AC109" s="34"/>
-      <c r="AD109" s="34"/>
-      <c r="AE109" s="34"/>
-      <c r="AF109" s="34"/>
+      <c r="M109" s="7"/>
+      <c r="N109" s="7"/>
+      <c r="O109" s="7"/>
+      <c r="P109" s="7"/>
+      <c r="Q109" s="7"/>
+      <c r="R109" s="7"/>
+      <c r="S109" s="7"/>
+      <c r="T109" s="7"/>
+      <c r="U109" s="7"/>
+      <c r="W109" s="7"/>
+      <c r="X109" s="7"/>
+      <c r="Y109" s="7"/>
+      <c r="Z109" s="7"/>
+      <c r="AA109" s="7"/>
+      <c r="AB109" s="7"/>
+      <c r="AC109" s="7"/>
+      <c r="AD109" s="7"/>
+      <c r="AE109" s="7"/>
+      <c r="AF109" s="7"/>
     </row>
     <row r="110" spans="1:10">
       <c r="A110" s="6" t="s">
@@ -5254,11 +5313,11 @@
       </c>
       <c r="J110" s="14"/>
     </row>
-    <row r="111" spans="1:10">
+    <row r="111" ht="14.25" spans="1:10">
       <c r="A111" s="8"/>
       <c r="J111" s="15"/>
     </row>
-    <row r="112" spans="1:10">
+    <row r="112" spans="1:32">
       <c r="A112" s="6" t="s">
         <v>59</v>
       </c>
@@ -5271,8 +5330,64 @@
       <c r="H112" s="7"/>
       <c r="I112" s="7"/>
       <c r="J112" s="14"/>
-    </row>
-    <row r="113" spans="1:10">
+      <c r="L112" s="20"/>
+      <c r="M112" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="N112" s="21" t="s">
+        <v>1</v>
+      </c>
+      <c r="O112" s="21" t="s">
+        <v>2</v>
+      </c>
+      <c r="P112" s="21" t="s">
+        <v>3</v>
+      </c>
+      <c r="Q112" s="21" t="s">
+        <v>4</v>
+      </c>
+      <c r="R112" s="21" t="s">
+        <v>5</v>
+      </c>
+      <c r="S112" s="21" t="s">
+        <v>6</v>
+      </c>
+      <c r="T112" s="21" t="s">
+        <v>7</v>
+      </c>
+      <c r="U112" s="27" t="s">
+        <v>8</v>
+      </c>
+      <c r="W112" s="20"/>
+      <c r="X112" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="Y112" s="21" t="s">
+        <v>1</v>
+      </c>
+      <c r="Z112" s="21" t="s">
+        <v>2</v>
+      </c>
+      <c r="AA112" s="21" t="s">
+        <v>3</v>
+      </c>
+      <c r="AB112" s="21" t="s">
+        <v>4</v>
+      </c>
+      <c r="AC112" s="21" t="s">
+        <v>5</v>
+      </c>
+      <c r="AD112" s="21" t="s">
+        <v>6</v>
+      </c>
+      <c r="AE112" s="21" t="s">
+        <v>7</v>
+      </c>
+      <c r="AF112" s="27" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="113" spans="1:32">
       <c r="A113" s="6" t="s">
         <v>26</v>
       </c>
@@ -5303,8 +5418,64 @@
       <c r="J113" s="16">
         <v>1.27133999397231</v>
       </c>
-    </row>
-    <row r="114" spans="1:10">
+      <c r="L113" s="22" t="s">
+        <v>24</v>
+      </c>
+      <c r="M113" s="23">
+        <v>1039722</v>
+      </c>
+      <c r="N113" s="23">
+        <v>1083568</v>
+      </c>
+      <c r="O113" s="23">
+        <v>997663</v>
+      </c>
+      <c r="P113" s="23">
+        <v>1001733</v>
+      </c>
+      <c r="Q113" s="23">
+        <v>1694616</v>
+      </c>
+      <c r="R113" s="23">
+        <v>1957027</v>
+      </c>
+      <c r="S113" s="23">
+        <v>426485</v>
+      </c>
+      <c r="T113" s="23">
+        <v>855802</v>
+      </c>
+      <c r="U113" s="28"/>
+      <c r="W113" s="22" t="s">
+        <v>24</v>
+      </c>
+      <c r="X113" s="23">
+        <v>1039722</v>
+      </c>
+      <c r="Y113" s="23">
+        <v>1083568</v>
+      </c>
+      <c r="Z113" s="23">
+        <v>997663</v>
+      </c>
+      <c r="AA113" s="23">
+        <v>1001733</v>
+      </c>
+      <c r="AB113" s="23">
+        <v>1694616</v>
+      </c>
+      <c r="AC113" s="23">
+        <v>1957027</v>
+      </c>
+      <c r="AD113" s="23">
+        <v>426485</v>
+      </c>
+      <c r="AE113" s="23">
+        <v>855802</v>
+      </c>
+      <c r="AF113" s="28"/>
+    </row>
+    <row r="114" spans="1:32">
       <c r="A114" s="6" t="s">
         <v>27</v>
       </c>
@@ -5335,8 +5506,12 @@
       <c r="J114" s="14">
         <v>148014</v>
       </c>
-    </row>
-    <row r="115" ht="14.25" spans="1:10">
+      <c r="L114" s="8"/>
+      <c r="U114" s="15"/>
+      <c r="W114" s="8"/>
+      <c r="AF114" s="15"/>
+    </row>
+    <row r="115" ht="14.25" spans="1:32">
       <c r="A115" s="18" t="s">
         <v>29</v>
       </c>
@@ -5364,11 +5539,61 @@
       <c r="I115" s="25">
         <v>171161</v>
       </c>
-      <c r="J115" s="36"/>
-    </row>
-    <row r="117" spans="1:10">
+      <c r="J115" s="35"/>
+      <c r="L115" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="M115" s="7"/>
+      <c r="N115" s="7"/>
+      <c r="O115" s="7"/>
+      <c r="P115" s="7"/>
+      <c r="Q115" s="7"/>
+      <c r="R115" s="7"/>
+      <c r="S115" s="7"/>
+      <c r="T115" s="7"/>
+      <c r="U115" s="14"/>
+      <c r="W115" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="X115" s="7"/>
+      <c r="Y115" s="7"/>
+      <c r="Z115" s="7"/>
+      <c r="AA115" s="7"/>
+      <c r="AB115" s="7"/>
+      <c r="AC115" s="7"/>
+      <c r="AD115" s="7"/>
+      <c r="AE115" s="7"/>
+      <c r="AF115" s="14"/>
+    </row>
+    <row r="116" spans="12:32">
+      <c r="L116" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="M116" s="7"/>
+      <c r="N116" s="7"/>
+      <c r="O116" s="7"/>
+      <c r="P116" s="7"/>
+      <c r="Q116" s="7"/>
+      <c r="R116" s="7"/>
+      <c r="S116" s="7"/>
+      <c r="T116" s="7"/>
+      <c r="U116" s="14"/>
+      <c r="W116" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="X116" s="7"/>
+      <c r="Y116" s="7"/>
+      <c r="Z116" s="7"/>
+      <c r="AA116" s="7"/>
+      <c r="AB116" s="7"/>
+      <c r="AC116" s="7"/>
+      <c r="AD116" s="7"/>
+      <c r="AE116" s="7"/>
+      <c r="AF116" s="14"/>
+    </row>
+    <row r="117" spans="1:32">
       <c r="A117" s="7" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="B117" s="7"/>
       <c r="C117" s="7"/>
@@ -5379,8 +5604,70 @@
       <c r="H117" s="7"/>
       <c r="I117" s="7"/>
       <c r="J117" s="7"/>
-    </row>
-    <row r="118" spans="1:10">
+      <c r="L117" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="M117" s="24">
+        <v>0.207415508016323</v>
+      </c>
+      <c r="N117" s="24">
+        <v>0.172532787111305</v>
+      </c>
+      <c r="O117" s="24">
+        <v>0.344112563328489</v>
+      </c>
+      <c r="P117" s="24">
+        <v>0.119256905360069</v>
+      </c>
+      <c r="Q117" s="24">
+        <v>0.0384065562330173</v>
+      </c>
+      <c r="R117" s="24">
+        <v>0.0392393556327599</v>
+      </c>
+      <c r="S117" s="24">
+        <v>0.0955505944283637</v>
+      </c>
+      <c r="T117" s="24">
+        <v>0.0497067152013686</v>
+      </c>
+      <c r="U117" s="31">
+        <f>SUM(M117:T117)</f>
+        <v>1.0662209853117</v>
+      </c>
+      <c r="W117" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="X117" s="7">
+        <v>0.207556270545581</v>
+      </c>
+      <c r="Y117" s="7">
+        <v>0.171427585198946</v>
+      </c>
+      <c r="Z117" s="7">
+        <v>0.358987447595345</v>
+      </c>
+      <c r="AA117" s="7">
+        <v>0.113874655842349</v>
+      </c>
+      <c r="AB117" s="7">
+        <v>0.0301842154410243</v>
+      </c>
+      <c r="AC117" s="7">
+        <v>0.00604113167826786</v>
+      </c>
+      <c r="AD117" s="7">
+        <v>0.0958264187741892</v>
+      </c>
+      <c r="AE117" s="7">
+        <v>0.0415976352932399</v>
+      </c>
+      <c r="AF117" s="16">
+        <f>SUM(X117:AE117)</f>
+        <v>1.02549536036894</v>
+      </c>
+    </row>
+    <row r="118" spans="1:32">
       <c r="A118" s="7"/>
       <c r="B118" s="7"/>
       <c r="C118" s="7"/>
@@ -5391,8 +5678,68 @@
       <c r="H118" s="7"/>
       <c r="I118" s="7"/>
       <c r="J118" s="7"/>
-    </row>
-    <row r="119" spans="1:10">
+      <c r="L118" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="M118" s="29">
+        <v>19989</v>
+      </c>
+      <c r="N118" s="29">
+        <v>14795</v>
+      </c>
+      <c r="O118" s="30">
+        <v>27624</v>
+      </c>
+      <c r="P118" s="29">
+        <v>8798</v>
+      </c>
+      <c r="Q118" s="29">
+        <v>60769</v>
+      </c>
+      <c r="R118" s="29">
+        <v>6889</v>
+      </c>
+      <c r="S118" s="29">
+        <v>82492</v>
+      </c>
+      <c r="T118" s="29">
+        <v>14696</v>
+      </c>
+      <c r="U118" s="30">
+        <v>82492</v>
+      </c>
+      <c r="W118" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="X118" s="34">
+        <v>3182</v>
+      </c>
+      <c r="Y118" s="34">
+        <v>2477</v>
+      </c>
+      <c r="Z118" s="37">
+        <v>5445</v>
+      </c>
+      <c r="AA118" s="34">
+        <v>1524</v>
+      </c>
+      <c r="AB118" s="34">
+        <v>6156</v>
+      </c>
+      <c r="AC118" s="34">
+        <v>3611</v>
+      </c>
+      <c r="AD118" s="34">
+        <v>1722</v>
+      </c>
+      <c r="AE118" s="34">
+        <v>2258</v>
+      </c>
+      <c r="AF118" s="37">
+        <v>6156</v>
+      </c>
+    </row>
+    <row r="119" spans="1:32">
       <c r="A119" s="7" t="s">
         <v>26</v>
       </c>
@@ -5405,8 +5752,32 @@
       <c r="H119" s="7"/>
       <c r="I119" s="7"/>
       <c r="J119" s="11"/>
-    </row>
-    <row r="120" spans="1:10">
+      <c r="L119" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="M119" s="7"/>
+      <c r="N119" s="7"/>
+      <c r="O119" s="7"/>
+      <c r="P119" s="7"/>
+      <c r="Q119" s="7"/>
+      <c r="R119" s="7"/>
+      <c r="S119" s="7"/>
+      <c r="T119" s="7"/>
+      <c r="U119" s="14"/>
+      <c r="W119" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="X119" s="7"/>
+      <c r="Y119" s="7"/>
+      <c r="Z119" s="7"/>
+      <c r="AA119" s="7"/>
+      <c r="AB119" s="7"/>
+      <c r="AC119" s="7"/>
+      <c r="AD119" s="7"/>
+      <c r="AE119" s="7"/>
+      <c r="AF119" s="14"/>
+    </row>
+    <row r="120" spans="1:32">
       <c r="A120" s="7" t="s">
         <v>27</v>
       </c>
@@ -5419,8 +5790,12 @@
       <c r="H120" s="7"/>
       <c r="I120" s="7"/>
       <c r="J120" s="7"/>
-    </row>
-    <row r="121" spans="1:10">
+      <c r="L120" s="8"/>
+      <c r="U120" s="15"/>
+      <c r="W120" s="8"/>
+      <c r="AF120" s="15"/>
+    </row>
+    <row r="121" spans="1:32">
       <c r="A121" s="7" t="s">
         <v>29</v>
       </c>
@@ -5433,8 +5808,75 @@
       <c r="H121" s="7"/>
       <c r="I121" s="7"/>
       <c r="J121" s="7"/>
-    </row>
-    <row r="123" spans="1:10">
+      <c r="L121" s="6"/>
+      <c r="M121" s="7"/>
+      <c r="N121" s="7"/>
+      <c r="O121" s="7"/>
+      <c r="P121" s="7"/>
+      <c r="Q121" s="7"/>
+      <c r="R121" s="7"/>
+      <c r="S121" s="7"/>
+      <c r="T121" s="7"/>
+      <c r="U121" s="14"/>
+      <c r="W121" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="X121" s="7"/>
+      <c r="Y121" s="7"/>
+      <c r="Z121" s="7"/>
+      <c r="AA121" s="7"/>
+      <c r="AB121" s="7"/>
+      <c r="AC121" s="7"/>
+      <c r="AD121" s="7"/>
+      <c r="AE121" s="7"/>
+      <c r="AF121" s="14"/>
+    </row>
+    <row r="122" spans="12:32">
+      <c r="L122" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="M122" s="11"/>
+      <c r="N122" s="11"/>
+      <c r="O122" s="11"/>
+      <c r="P122" s="11"/>
+      <c r="Q122" s="11"/>
+      <c r="R122" s="11"/>
+      <c r="S122" s="11"/>
+      <c r="T122" s="11"/>
+      <c r="U122" s="16"/>
+      <c r="W122" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="X122" s="11">
+        <v>0.207472081813346</v>
+      </c>
+      <c r="Y122" s="11">
+        <v>0.170950889306181</v>
+      </c>
+      <c r="Z122" s="11">
+        <v>0.36282036402299</v>
+      </c>
+      <c r="AA122" s="11">
+        <v>0.113974022322701</v>
+      </c>
+      <c r="AB122" s="11">
+        <v>0.0300290446697214</v>
+      </c>
+      <c r="AC122" s="11">
+        <v>0.00419404141156328</v>
+      </c>
+      <c r="AD122" s="11">
+        <v>0.0955072693879415</v>
+      </c>
+      <c r="AE122" s="11">
+        <v>0.041785489936455</v>
+      </c>
+      <c r="AF122" s="16">
+        <f>SUM(X122:AE122)</f>
+        <v>1.0267332028709</v>
+      </c>
+    </row>
+    <row r="123" spans="1:32">
       <c r="A123" s="7" t="s">
         <v>23</v>
       </c>
@@ -5447,8 +5889,50 @@
       <c r="H123" s="7"/>
       <c r="I123" s="7"/>
       <c r="J123" s="7"/>
-    </row>
-    <row r="124" spans="1:10">
+      <c r="L123" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="M123" s="29"/>
+      <c r="N123" s="29"/>
+      <c r="O123" s="29"/>
+      <c r="P123" s="29"/>
+      <c r="Q123" s="29"/>
+      <c r="R123" s="29"/>
+      <c r="S123" s="29"/>
+      <c r="T123" s="29"/>
+      <c r="U123" s="36"/>
+      <c r="W123" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="X123" s="34">
+        <v>2787</v>
+      </c>
+      <c r="Y123" s="34">
+        <v>2181</v>
+      </c>
+      <c r="Z123" s="34">
+        <v>4953</v>
+      </c>
+      <c r="AA123" s="34">
+        <v>1450</v>
+      </c>
+      <c r="AB123" s="34">
+        <v>5066</v>
+      </c>
+      <c r="AC123" s="34">
+        <v>1942</v>
+      </c>
+      <c r="AD123" s="34">
+        <v>2176</v>
+      </c>
+      <c r="AE123" s="34">
+        <v>2185</v>
+      </c>
+      <c r="AF123" s="34">
+        <v>5066</v>
+      </c>
+    </row>
+    <row r="124" spans="1:32">
       <c r="A124" s="7" t="s">
         <v>26</v>
       </c>
@@ -5463,8 +5947,32 @@
       <c r="H124" s="7"/>
       <c r="I124" s="7"/>
       <c r="J124" s="11"/>
-    </row>
-    <row r="125" spans="1:10">
+      <c r="L124" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="M124" s="7"/>
+      <c r="N124" s="7"/>
+      <c r="O124" s="7"/>
+      <c r="P124" s="7"/>
+      <c r="Q124" s="7"/>
+      <c r="R124" s="7"/>
+      <c r="S124" s="7"/>
+      <c r="T124" s="7"/>
+      <c r="U124" s="14"/>
+      <c r="W124" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="X124" s="7"/>
+      <c r="Y124" s="7"/>
+      <c r="Z124" s="7"/>
+      <c r="AA124" s="7"/>
+      <c r="AB124" s="7"/>
+      <c r="AC124" s="7"/>
+      <c r="AD124" s="7"/>
+      <c r="AE124" s="7"/>
+      <c r="AF124" s="14"/>
+    </row>
+    <row r="125" spans="1:32">
       <c r="A125" s="7" t="s">
         <v>27</v>
       </c>
@@ -5477,8 +5985,28 @@
       <c r="H125" s="7"/>
       <c r="I125" s="7"/>
       <c r="J125" s="7"/>
-    </row>
-    <row r="126" spans="1:10">
+      <c r="L125" s="8"/>
+      <c r="M125" s="2"/>
+      <c r="N125" s="2"/>
+      <c r="O125" s="2"/>
+      <c r="P125" s="2"/>
+      <c r="Q125" s="2"/>
+      <c r="R125" s="2"/>
+      <c r="S125" s="2"/>
+      <c r="T125" s="2"/>
+      <c r="U125" s="15"/>
+      <c r="W125" s="8"/>
+      <c r="X125" s="2"/>
+      <c r="Y125" s="2"/>
+      <c r="Z125" s="2"/>
+      <c r="AA125" s="2"/>
+      <c r="AB125" s="2"/>
+      <c r="AC125" s="2"/>
+      <c r="AD125" s="2"/>
+      <c r="AE125" s="2"/>
+      <c r="AF125" s="15"/>
+    </row>
+    <row r="126" spans="1:32">
       <c r="A126" s="7" t="s">
         <v>29</v>
       </c>
@@ -5491,6 +6019,361 @@
       <c r="H126" s="7"/>
       <c r="I126" s="7"/>
       <c r="J126" s="7"/>
+      <c r="W126" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="X126" s="7"/>
+      <c r="Y126" s="7"/>
+      <c r="Z126" s="7"/>
+      <c r="AA126" s="7"/>
+      <c r="AB126" s="7"/>
+      <c r="AC126" s="7"/>
+      <c r="AD126" s="7"/>
+      <c r="AE126" s="7"/>
+      <c r="AF126" s="14"/>
+    </row>
+    <row r="127" spans="23:32">
+      <c r="W127" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="X127" s="24">
+        <v>0.207161871096565</v>
+      </c>
+      <c r="Y127" s="24">
+        <v>0.170991786306423</v>
+      </c>
+      <c r="Z127" s="24">
+        <v>0.359560380608134</v>
+      </c>
+      <c r="AA127" s="24">
+        <v>0.11219873018098</v>
+      </c>
+      <c r="AB127" s="24">
+        <v>0.0289002342497625</v>
+      </c>
+      <c r="AC127" s="24">
+        <v>0.00419168030842799</v>
+      </c>
+      <c r="AD127" s="24">
+        <v>0.0953063317967282</v>
+      </c>
+      <c r="AE127" s="24">
+        <v>0.0364761403932048</v>
+      </c>
+      <c r="AF127" s="31">
+        <f>SUM(X127:AE127)</f>
+        <v>1.01478715494023</v>
+      </c>
+    </row>
+    <row r="128" spans="23:32">
+      <c r="W128" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="X128" s="34">
+        <v>3737</v>
+      </c>
+      <c r="Y128" s="34">
+        <v>2472</v>
+      </c>
+      <c r="Z128" s="34">
+        <v>6392</v>
+      </c>
+      <c r="AA128" s="34">
+        <v>1323</v>
+      </c>
+      <c r="AB128" s="34">
+        <v>25852</v>
+      </c>
+      <c r="AC128" s="34">
+        <v>1209</v>
+      </c>
+      <c r="AD128" s="34">
+        <v>39122</v>
+      </c>
+      <c r="AE128" s="34">
+        <v>2279</v>
+      </c>
+      <c r="AF128" s="34">
+        <v>39122</v>
+      </c>
+    </row>
+    <row r="129" spans="23:32">
+      <c r="W129" s="38" t="s">
+        <v>67</v>
+      </c>
+      <c r="X129" s="39">
+        <v>16817</v>
+      </c>
+      <c r="Y129" s="39">
+        <v>17542</v>
+      </c>
+      <c r="Z129" s="39">
+        <v>24991</v>
+      </c>
+      <c r="AA129" s="39">
+        <v>12636</v>
+      </c>
+      <c r="AB129" s="39">
+        <v>22954</v>
+      </c>
+      <c r="AC129" s="39">
+        <v>16443</v>
+      </c>
+      <c r="AD129" s="39">
+        <v>19135</v>
+      </c>
+      <c r="AE129" s="39">
+        <v>10620</v>
+      </c>
+      <c r="AF129" s="45">
+        <v>24991</v>
+      </c>
+    </row>
+    <row r="130" spans="23:32">
+      <c r="W130" s="40" t="s">
+        <v>29</v>
+      </c>
+      <c r="X130" s="41"/>
+      <c r="Y130" s="41"/>
+      <c r="Z130" s="41"/>
+      <c r="AA130" s="41"/>
+      <c r="AB130" s="41"/>
+      <c r="AC130" s="41"/>
+      <c r="AD130" s="41"/>
+      <c r="AE130" s="41"/>
+      <c r="AF130" s="46"/>
+    </row>
+    <row r="131" spans="23:32">
+      <c r="W131" s="42"/>
+      <c r="X131" s="43"/>
+      <c r="Y131" s="43"/>
+      <c r="Z131" s="43"/>
+      <c r="AA131" s="43"/>
+      <c r="AB131" s="43"/>
+      <c r="AC131" s="43"/>
+      <c r="AD131" s="43"/>
+      <c r="AE131" s="43"/>
+      <c r="AF131" s="47"/>
+    </row>
+    <row r="132" spans="23:32">
+      <c r="W132" s="41" t="s">
+        <v>68</v>
+      </c>
+      <c r="X132" s="41"/>
+      <c r="Y132" s="41"/>
+      <c r="Z132" s="41"/>
+      <c r="AA132" s="41"/>
+      <c r="AB132" s="41"/>
+      <c r="AC132" s="41"/>
+      <c r="AD132" s="41"/>
+      <c r="AE132" s="41"/>
+      <c r="AF132" s="41"/>
+    </row>
+    <row r="133" spans="23:32">
+      <c r="W133" s="40" t="s">
+        <v>26</v>
+      </c>
+      <c r="X133" s="41">
+        <v>0.20726823279994</v>
+      </c>
+      <c r="Y133" s="41">
+        <v>0.170985023438374</v>
+      </c>
+      <c r="Z133" s="41">
+        <v>0.359664208360988</v>
+      </c>
+      <c r="AA133" s="41">
+        <v>0.112089923569473</v>
+      </c>
+      <c r="AB133" s="41">
+        <v>0.029467659671068</v>
+      </c>
+      <c r="AC133" s="41">
+        <v>0.00370557094652351</v>
+      </c>
+      <c r="AD133" s="41">
+        <v>0.0955302550359815</v>
+      </c>
+      <c r="AE133" s="41">
+        <v>0.0365722018037902</v>
+      </c>
+      <c r="AF133" s="46">
+        <f>SUM(X133:AE133)</f>
+        <v>1.01528307562614</v>
+      </c>
+    </row>
+    <row r="134" spans="23:32">
+      <c r="W134" s="40" t="s">
+        <v>27</v>
+      </c>
+      <c r="X134" s="44">
+        <v>2823</v>
+      </c>
+      <c r="Y134" s="44">
+        <v>2132</v>
+      </c>
+      <c r="Z134" s="44">
+        <v>5470</v>
+      </c>
+      <c r="AA134" s="44">
+        <v>1219</v>
+      </c>
+      <c r="AB134" s="44">
+        <v>4589</v>
+      </c>
+      <c r="AC134" s="44">
+        <v>1263</v>
+      </c>
+      <c r="AD134" s="44">
+        <v>1942</v>
+      </c>
+      <c r="AE134" s="44">
+        <v>1983</v>
+      </c>
+      <c r="AF134" s="44">
+        <v>5470</v>
+      </c>
+    </row>
+    <row r="135" spans="23:32">
+      <c r="W135" s="41" t="s">
+        <v>69</v>
+      </c>
+      <c r="X135" s="44">
+        <v>3058</v>
+      </c>
+      <c r="Y135" s="44">
+        <v>2310</v>
+      </c>
+      <c r="Z135" s="44">
+        <v>5664</v>
+      </c>
+      <c r="AA135" s="44">
+        <v>1409</v>
+      </c>
+      <c r="AB135" s="44">
+        <v>5226</v>
+      </c>
+      <c r="AC135" s="44">
+        <v>1514</v>
+      </c>
+      <c r="AD135" s="44">
+        <v>2020</v>
+      </c>
+      <c r="AE135" s="44">
+        <v>2294</v>
+      </c>
+      <c r="AF135" s="44">
+        <v>5664</v>
+      </c>
+    </row>
+    <row r="136" spans="23:32">
+      <c r="W136" s="40" t="s">
+        <v>29</v>
+      </c>
+      <c r="X136" s="41"/>
+      <c r="Y136" s="41"/>
+      <c r="Z136" s="41"/>
+      <c r="AA136" s="41"/>
+      <c r="AB136" s="41"/>
+      <c r="AC136" s="41"/>
+      <c r="AD136" s="41"/>
+      <c r="AE136" s="41"/>
+      <c r="AF136" s="41"/>
+    </row>
+    <row r="137" spans="23:32">
+      <c r="W137" s="7"/>
+      <c r="X137" s="7"/>
+      <c r="Y137" s="7"/>
+      <c r="Z137" s="7"/>
+      <c r="AA137" s="7"/>
+      <c r="AB137" s="7"/>
+      <c r="AC137" s="7"/>
+      <c r="AD137" s="7"/>
+      <c r="AE137" s="7"/>
+      <c r="AF137" s="7"/>
+    </row>
+    <row r="138" spans="23:32">
+      <c r="W138" s="6"/>
+      <c r="X138" s="7"/>
+      <c r="Y138" s="7"/>
+      <c r="Z138" s="7"/>
+      <c r="AA138" s="7"/>
+      <c r="AB138" s="7"/>
+      <c r="AC138" s="7"/>
+      <c r="AD138" s="7"/>
+      <c r="AE138" s="7"/>
+      <c r="AF138" s="16"/>
+    </row>
+    <row r="139" spans="23:32">
+      <c r="W139" s="6"/>
+      <c r="X139" s="34"/>
+      <c r="Y139" s="34"/>
+      <c r="Z139" s="34"/>
+      <c r="AA139" s="34"/>
+      <c r="AB139" s="34"/>
+      <c r="AC139" s="34"/>
+      <c r="AD139" s="34"/>
+      <c r="AE139" s="34"/>
+      <c r="AF139" s="34"/>
+    </row>
+    <row r="140" spans="24:32">
+      <c r="X140" s="34"/>
+      <c r="Y140" s="34"/>
+      <c r="Z140" s="34"/>
+      <c r="AA140" s="34"/>
+      <c r="AB140" s="34"/>
+      <c r="AC140" s="34"/>
+      <c r="AD140" s="34"/>
+      <c r="AE140" s="34"/>
+      <c r="AF140" s="34"/>
+    </row>
+    <row r="141" spans="23:32">
+      <c r="W141" s="6"/>
+      <c r="X141" s="7"/>
+      <c r="Y141" s="7"/>
+      <c r="Z141" s="7"/>
+      <c r="AA141" s="7"/>
+      <c r="AB141" s="7"/>
+      <c r="AC141" s="7"/>
+      <c r="AD141" s="7"/>
+      <c r="AE141" s="7"/>
+      <c r="AF141" s="7"/>
+    </row>
+    <row r="142" spans="23:32">
+      <c r="W142" s="7"/>
+      <c r="X142" s="7"/>
+      <c r="Y142" s="7"/>
+      <c r="Z142" s="7"/>
+      <c r="AA142" s="7"/>
+      <c r="AB142" s="7"/>
+      <c r="AC142" s="7"/>
+      <c r="AD142" s="7"/>
+      <c r="AE142" s="7"/>
+      <c r="AF142" s="7"/>
+    </row>
+    <row r="143" spans="23:32">
+      <c r="W143" s="7"/>
+      <c r="X143" s="7"/>
+      <c r="Y143" s="7"/>
+      <c r="Z143" s="7"/>
+      <c r="AA143" s="7"/>
+      <c r="AB143" s="7"/>
+      <c r="AC143" s="7"/>
+      <c r="AD143" s="7"/>
+      <c r="AE143" s="7"/>
+      <c r="AF143" s="7"/>
+    </row>
+    <row r="144" spans="23:32">
+      <c r="W144" s="7"/>
+      <c r="X144" s="7"/>
+      <c r="Y144" s="7"/>
+      <c r="Z144" s="7"/>
+      <c r="AA144" s="7"/>
+      <c r="AB144" s="7"/>
+      <c r="AC144" s="7"/>
+      <c r="AD144" s="7"/>
+      <c r="AE144" s="7"/>
+      <c r="AF144" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.699305555555556" right="0.699305555555556" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
1. Update the current constructor to builder mode. 2. Update cpp file to more modern/clear style. 3. Improve python script 4. Add more data
</commit_message>
<xml_diff>
--- a/overall.xlsx
+++ b/overall.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="20385" windowHeight="8370" activeTab="1"/>
+    <workbookView windowWidth="20385" windowHeight="8370"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91">
   <si>
     <t>model1</t>
   </si>
@@ -274,6 +274,21 @@
   </si>
   <si>
     <t>17_07_29_11_48_52_2_1_500_12_-1</t>
+  </si>
+  <si>
+    <t>17_07_30_13_04_32_3_1_500_8_0.001</t>
+  </si>
+  <si>
+    <t>pythonResults/17_07_11_23_45_34_-1_2000000_500_3/./pythonControl.sh -1 2000000 3</t>
+  </si>
+  <si>
+    <t>17_08_02_12_47_32_2_1_500_6_0.001/FirstInFirstOut</t>
+  </si>
+  <si>
+    <t>17_08_01_18_07_17_2_1_500_8_0.001/FirstInFirstOut</t>
+  </si>
+  <si>
+    <t>17_08_02_08_20_59_2_1_500_7_0.001/Multiple_reinsert</t>
   </si>
 </sst>
 </file>
@@ -281,10 +296,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
   <fonts count="23">
     <font>
@@ -317,7 +332,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <color theme="0"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -330,38 +345,16 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="0"/>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
       <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="宋体"/>
-      <charset val="0"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF9C0006"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -377,6 +370,35 @@
     <font>
       <b/>
       <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color rgb="FFFA7D00"/>
       <name val="宋体"/>
       <charset val="0"/>
@@ -385,14 +407,6 @@
     <font>
       <b/>
       <sz val="13"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
       <color theme="3"/>
       <name val="宋体"/>
       <charset val="134"/>
@@ -415,27 +429,26 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <color rgb="FF006100"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
-      <sz val="15"/>
-      <color theme="3"/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
       <name val="宋体"/>
-      <charset val="134"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
+      <sz val="18"/>
+      <color theme="3"/>
       <name val="宋体"/>
-      <charset val="0"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -446,15 +459,17 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color rgb="FF3F3F3F"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <i/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FF7F7F7F"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -487,19 +502,73 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8"/>
+        <fgColor theme="4"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -511,31 +580,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
+        <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -553,7 +598,31 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -565,19 +634,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFFFFFCC"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
+        <fgColor theme="7" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -589,31 +652,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
+        <fgColor rgb="FFC6EFCE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
+        <fgColor rgb="FFF2F2F2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -631,43 +676,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
+        <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -834,6 +849,30 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
         <color rgb="FF7F7F7F"/>
       </left>
@@ -863,8 +902,17 @@
       <left/>
       <right/>
       <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
       <bottom style="medium">
-        <color theme="4"/>
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -898,39 +946,6 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
@@ -939,149 +954,149 @@
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="17" borderId="14" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="27" borderId="18" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="17" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="31" borderId="19" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="31" borderId="14" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="16" borderId="13" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="16" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="15" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="8" borderId="12" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="19" borderId="15" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="14" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="14" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="18" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="16" borderId="16" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="16" borderId="12" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="26" borderId="17" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="19" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
   </cellStyleXfs>
-  <cellXfs count="52">
+  <cellXfs count="55">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1202,6 +1217,9 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1237,6 +1255,12 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="49">
@@ -1587,10 +1611,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr/>
-  <dimension ref="A1:J34"/>
+  <dimension ref="A1:J42"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G34" sqref="G34"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="B42" sqref="B42:J42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
@@ -1681,7 +1705,7 @@
       <c r="F3">
         <v>0.0522827100851127</v>
       </c>
-      <c r="G3" s="49">
+      <c r="G3" s="50">
         <v>0.106926203216301</v>
       </c>
       <c r="H3">
@@ -1707,7 +1731,7 @@
       <c r="A12" t="s">
         <v>12</v>
       </c>
-      <c r="G12" s="50">
+      <c r="G12" s="51">
         <v>0.0629933219692992</v>
       </c>
     </row>
@@ -1760,7 +1784,7 @@
       <c r="I19">
         <v>0.0755164339928472</v>
       </c>
-      <c r="J19" s="51">
+      <c r="J19" s="52">
         <f t="shared" ref="J19:J21" si="0">SUM(B19:I19)</f>
         <v>1.17870842662782</v>
       </c>
@@ -1769,31 +1793,31 @@
       <c r="A20" t="s">
         <v>17</v>
       </c>
-      <c r="B20" s="51">
+      <c r="B20" s="52">
         <v>0.20800686430345</v>
       </c>
-      <c r="C20" s="51">
+      <c r="C20" s="52">
         <v>0.173239206962822</v>
       </c>
-      <c r="D20" s="51">
+      <c r="D20" s="52">
         <v>0.346041541710196</v>
       </c>
-      <c r="E20" s="51">
+      <c r="E20" s="52">
         <v>0.124928278882666</v>
       </c>
-      <c r="F20" s="51">
+      <c r="F20" s="52">
         <v>0.0409924383808026</v>
       </c>
-      <c r="G20" s="51">
+      <c r="G20" s="52">
         <v>0.0453003114127127</v>
       </c>
-      <c r="H20" s="51">
+      <c r="H20" s="52">
         <v>0.0964368086720679</v>
       </c>
-      <c r="I20" s="51">
+      <c r="I20" s="52">
         <v>0.065879029949852</v>
       </c>
-      <c r="J20" s="51">
+      <c r="J20" s="52">
         <f t="shared" si="0"/>
         <v>1.10082448027457</v>
       </c>
@@ -1802,52 +1826,52 @@
       <c r="A21" t="s">
         <v>18</v>
       </c>
-      <c r="B21" s="50">
+      <c r="B21" s="51">
         <v>0.207894527330402</v>
       </c>
-      <c r="C21" s="50">
+      <c r="C21" s="51">
         <v>0.173165858291852</v>
       </c>
-      <c r="D21" s="50">
+      <c r="D21" s="51">
         <v>0.344628020195683</v>
       </c>
-      <c r="E21" s="50">
+      <c r="E21" s="51">
         <v>0.118862297465155</v>
       </c>
-      <c r="F21" s="50">
+      <c r="F21" s="51">
         <v>0.0388983176119749</v>
       </c>
-      <c r="G21" s="50">
+      <c r="G21" s="51">
         <v>0.0422239303614074</v>
       </c>
-      <c r="H21" s="50">
+      <c r="H21" s="51">
         <v>0.0955131594160284</v>
       </c>
-      <c r="I21" s="50">
+      <c r="I21" s="51">
         <v>0.0488732287830458</v>
       </c>
-      <c r="J21" s="50">
+      <c r="J21" s="51">
         <f t="shared" si="0"/>
         <v>1.07005933945555</v>
       </c>
     </row>
     <row r="22" spans="10:10">
-      <c r="J22" s="51"/>
+      <c r="J22" s="52"/>
     </row>
     <row r="23" spans="10:10">
-      <c r="J23" s="51"/>
+      <c r="J23" s="52"/>
     </row>
     <row r="24" spans="10:10">
-      <c r="J24" s="51"/>
+      <c r="J24" s="52"/>
     </row>
     <row r="25" spans="10:10">
-      <c r="J25" s="51"/>
+      <c r="J25" s="52"/>
     </row>
     <row r="26" spans="1:10">
       <c r="A26" t="s">
         <v>19</v>
       </c>
-      <c r="J26" s="51"/>
+      <c r="J26" s="52"/>
     </row>
     <row r="27" spans="1:10">
       <c r="A27" t="s">
@@ -1868,7 +1892,7 @@
       <c r="F27">
         <v>0.0492015604703379</v>
       </c>
-      <c r="G27" s="51">
+      <c r="G27" s="52">
         <v>0.0766396493470802</v>
       </c>
       <c r="H27">
@@ -1877,7 +1901,7 @@
       <c r="I27">
         <v>0.0926905158740254</v>
       </c>
-      <c r="J27" s="51">
+      <c r="J27" s="52">
         <f>SUM(B27:I27)</f>
         <v>1.27166155848785</v>
       </c>
@@ -1901,7 +1925,7 @@
       <c r="F28">
         <v>0.0533366743677525</v>
       </c>
-      <c r="G28" s="49">
+      <c r="G28" s="50">
         <v>0.110748101588701</v>
       </c>
       <c r="H28">
@@ -1910,7 +1934,7 @@
       <c r="I28">
         <v>0.103230203907768</v>
       </c>
-      <c r="J28" s="51">
+      <c r="J28" s="52">
         <f>SUM(B28:I28)</f>
         <v>1.31676786850071</v>
       </c>
@@ -1926,6 +1950,36 @@
       </c>
       <c r="G34">
         <v>0.102480606902965</v>
+      </c>
+    </row>
+    <row r="42" spans="2:10">
+      <c r="B42" s="53">
+        <v>0.206049947306921</v>
+      </c>
+      <c r="C42" s="53">
+        <v>0.169594488695383</v>
+      </c>
+      <c r="D42" s="53">
+        <v>0.343962910788856</v>
+      </c>
+      <c r="E42" s="53">
+        <v>0.110748998587646</v>
+      </c>
+      <c r="F42" s="53">
+        <v>0.0286448603212694</v>
+      </c>
+      <c r="G42" s="53">
+        <v>0.00216421261328103</v>
+      </c>
+      <c r="H42" s="53">
+        <v>0.093607987367592</v>
+      </c>
+      <c r="I42" s="46">
+        <v>0.0354465761733521</v>
+      </c>
+      <c r="J42" s="54">
+        <f>SUM(B42:I42)</f>
+        <v>0.990219981854301</v>
       </c>
     </row>
   </sheetData>
@@ -1938,10 +1992,10 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr/>
-  <dimension ref="A1:AF173"/>
+  <dimension ref="A1:AF195"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="X154" workbookViewId="0">
-      <selection activeCell="AF173" sqref="AF173"/>
+    <sheetView topLeftCell="Z178" workbookViewId="0">
+      <selection activeCell="AF195" sqref="X195:AF195"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
@@ -1959,7 +2013,7 @@
     <col min="23" max="23" width="56" style="2" customWidth="1"/>
     <col min="24" max="32" width="12.625" style="2" customWidth="1"/>
     <col min="33" max="33" width="9" style="2"/>
-    <col min="34" max="34" width="50.375" style="2" customWidth="1"/>
+    <col min="34" max="34" width="89.375" style="2" customWidth="1"/>
     <col min="35" max="43" width="12.625" style="2" customWidth="1"/>
     <col min="44" max="16384" width="9" style="2"/>
   </cols>
@@ -6276,7 +6330,7 @@
       </c>
     </row>
     <row r="129" spans="23:32">
-      <c r="W129" s="40" t="s">
+      <c r="W129" s="41" t="s">
         <v>69</v>
       </c>
       <c r="X129" s="34">
@@ -6320,18 +6374,18 @@
       <c r="S130" s="7"/>
       <c r="T130" s="7"/>
       <c r="U130" s="14"/>
-      <c r="W130" s="41" t="s">
+      <c r="W130" s="42" t="s">
         <v>29</v>
       </c>
-      <c r="X130" s="42"/>
-      <c r="Y130" s="42"/>
-      <c r="Z130" s="42"/>
-      <c r="AA130" s="42"/>
-      <c r="AB130" s="42"/>
-      <c r="AC130" s="42"/>
-      <c r="AD130" s="42"/>
-      <c r="AE130" s="42"/>
-      <c r="AF130" s="46"/>
+      <c r="X130" s="43"/>
+      <c r="Y130" s="43"/>
+      <c r="Z130" s="43"/>
+      <c r="AA130" s="43"/>
+      <c r="AB130" s="43"/>
+      <c r="AC130" s="43"/>
+      <c r="AD130" s="43"/>
+      <c r="AE130" s="43"/>
+      <c r="AF130" s="47"/>
     </row>
     <row r="131" spans="12:32">
       <c r="L131" s="6" t="s">
@@ -6365,16 +6419,16 @@
         <f>SUM(M131:T131)</f>
         <v>1.19427920902361</v>
       </c>
-      <c r="W131" s="43"/>
-      <c r="X131" s="44"/>
-      <c r="Y131" s="44"/>
-      <c r="Z131" s="44"/>
-      <c r="AA131" s="44"/>
-      <c r="AB131" s="44"/>
-      <c r="AC131" s="44"/>
-      <c r="AD131" s="44"/>
-      <c r="AE131" s="44"/>
-      <c r="AF131" s="47"/>
+      <c r="W131" s="44"/>
+      <c r="X131" s="45"/>
+      <c r="Y131" s="45"/>
+      <c r="Z131" s="45"/>
+      <c r="AA131" s="45"/>
+      <c r="AB131" s="45"/>
+      <c r="AC131" s="45"/>
+      <c r="AD131" s="45"/>
+      <c r="AE131" s="45"/>
+      <c r="AF131" s="48"/>
     </row>
     <row r="132" spans="12:32">
       <c r="L132" s="6" t="s">
@@ -6407,48 +6461,48 @@
       <c r="U132" s="38">
         <v>8928</v>
       </c>
-      <c r="W132" s="42" t="s">
+      <c r="W132" s="43" t="s">
         <v>71</v>
       </c>
-      <c r="X132" s="42"/>
-      <c r="Y132" s="42"/>
-      <c r="Z132" s="42"/>
-      <c r="AA132" s="42"/>
-      <c r="AB132" s="42"/>
-      <c r="AC132" s="42"/>
-      <c r="AD132" s="42"/>
-      <c r="AE132" s="42"/>
-      <c r="AF132" s="42"/>
+      <c r="X132" s="43"/>
+      <c r="Y132" s="43"/>
+      <c r="Z132" s="43"/>
+      <c r="AA132" s="43"/>
+      <c r="AB132" s="43"/>
+      <c r="AC132" s="43"/>
+      <c r="AD132" s="43"/>
+      <c r="AE132" s="43"/>
+      <c r="AF132" s="43"/>
     </row>
     <row r="133" spans="23:32">
-      <c r="W133" s="41" t="s">
+      <c r="W133" s="42" t="s">
         <v>26</v>
       </c>
-      <c r="X133" s="42">
+      <c r="X133" s="43">
         <v>0.20726823279994</v>
       </c>
-      <c r="Y133" s="42">
+      <c r="Y133" s="43">
         <v>0.170985023438374</v>
       </c>
-      <c r="Z133" s="42">
+      <c r="Z133" s="43">
         <v>0.359664208360988</v>
       </c>
-      <c r="AA133" s="42">
+      <c r="AA133" s="43">
         <v>0.112089923569473</v>
       </c>
-      <c r="AB133" s="42">
+      <c r="AB133" s="43">
         <v>0.029467659671068</v>
       </c>
-      <c r="AC133" s="42">
+      <c r="AC133" s="43">
         <v>0.00370557094652351</v>
       </c>
-      <c r="AD133" s="42">
+      <c r="AD133" s="43">
         <v>0.0955302550359815</v>
       </c>
-      <c r="AE133" s="42">
+      <c r="AE133" s="43">
         <v>0.0365722018037902</v>
       </c>
-      <c r="AF133" s="46">
+      <c r="AF133" s="47">
         <f>SUM(X133:AE133)</f>
         <v>1.01528307562614</v>
       </c>
@@ -6466,7 +6520,7 @@
       <c r="S134" s="7"/>
       <c r="T134" s="7"/>
       <c r="U134" s="14"/>
-      <c r="W134" s="41" t="s">
+      <c r="W134" s="42" t="s">
         <v>27</v>
       </c>
       <c r="X134" s="33">
@@ -6529,7 +6583,7 @@
         <f>SUM(M135:T135)</f>
         <v>1.11768511223654</v>
       </c>
-      <c r="W135" s="42" t="s">
+      <c r="W135" s="43" t="s">
         <v>73</v>
       </c>
       <c r="X135" s="33">
@@ -6591,18 +6645,18 @@
       <c r="U136" s="34">
         <v>49407</v>
       </c>
-      <c r="W136" s="41" t="s">
+      <c r="W136" s="42" t="s">
         <v>29</v>
       </c>
-      <c r="X136" s="42"/>
-      <c r="Y136" s="42"/>
-      <c r="Z136" s="42"/>
-      <c r="AA136" s="42"/>
-      <c r="AB136" s="42"/>
-      <c r="AC136" s="42"/>
-      <c r="AD136" s="42"/>
-      <c r="AE136" s="42"/>
-      <c r="AF136" s="42"/>
+      <c r="X136" s="43"/>
+      <c r="Y136" s="43"/>
+      <c r="Z136" s="43"/>
+      <c r="AA136" s="43"/>
+      <c r="AB136" s="43"/>
+      <c r="AC136" s="43"/>
+      <c r="AD136" s="43"/>
+      <c r="AE136" s="43"/>
+      <c r="AF136" s="43"/>
     </row>
     <row r="137" spans="23:32">
       <c r="W137" s="7"/>
@@ -6706,7 +6760,7 @@
       <c r="U140" s="38">
         <v>10515</v>
       </c>
-      <c r="W140" s="41" t="s">
+      <c r="W140" s="42" t="s">
         <v>26</v>
       </c>
       <c r="X140" s="34">
@@ -6733,13 +6787,13 @@
       <c r="AE140" s="34">
         <v>0.0400224015997118</v>
       </c>
-      <c r="AF140" s="48">
+      <c r="AF140" s="49">
         <f>SUM(X140:AE140)</f>
         <v>1.01852769482818</v>
       </c>
     </row>
     <row r="141" spans="23:32">
-      <c r="W141" s="41" t="s">
+      <c r="W141" s="42" t="s">
         <v>27</v>
       </c>
       <c r="X141" s="34">
@@ -6860,7 +6914,7 @@
       <c r="U144" s="38">
         <v>53817</v>
       </c>
-      <c r="W144" s="41" t="s">
+      <c r="W144" s="42" t="s">
         <v>26</v>
       </c>
       <c r="X144" s="34">
@@ -6893,7 +6947,7 @@
       </c>
     </row>
     <row r="145" spans="23:32">
-      <c r="W145" s="41" t="s">
+      <c r="W145" s="42" t="s">
         <v>27</v>
       </c>
       <c r="X145" s="34">
@@ -7024,7 +7078,7 @@
       <c r="U148" s="38">
         <v>21172</v>
       </c>
-      <c r="W148" s="41" t="s">
+      <c r="W148" s="42" t="s">
         <v>26</v>
       </c>
       <c r="X148" s="34">
@@ -7057,7 +7111,7 @@
       </c>
     </row>
     <row r="149" spans="23:32">
-      <c r="W149" s="41" t="s">
+      <c r="W149" s="42" t="s">
         <v>27</v>
       </c>
       <c r="X149" s="34">
@@ -7178,31 +7232,31 @@
       <c r="U152" s="38">
         <v>88904</v>
       </c>
-      <c r="W152" s="41" t="s">
+      <c r="W152" s="42" t="s">
         <v>26</v>
       </c>
-      <c r="X152" s="45">
+      <c r="X152" s="46">
         <v>0.207255996600315</v>
       </c>
-      <c r="Y152" s="45">
+      <c r="Y152" s="46">
         <v>0.170827487785851</v>
       </c>
       <c r="Z152" s="33">
         <v>0.359711307241924</v>
       </c>
-      <c r="AA152" s="45">
+      <c r="AA152" s="46">
         <v>0.11166110429993</v>
       </c>
-      <c r="AB152" s="45">
+      <c r="AB152" s="46">
         <v>0.0287592032379425</v>
       </c>
-      <c r="AC152" s="45">
+      <c r="AC152" s="46">
         <v>0.0031382201640017</v>
       </c>
-      <c r="AD152" s="45">
+      <c r="AD152" s="46">
         <v>0.0948727773946742</v>
       </c>
-      <c r="AE152" s="45">
+      <c r="AE152" s="46">
         <v>0.0354465761733521</v>
       </c>
       <c r="AF152" s="34">
@@ -7211,7 +7265,7 @@
       </c>
     </row>
     <row r="153" spans="23:32">
-      <c r="W153" s="41" t="s">
+      <c r="W153" s="42" t="s">
         <v>27</v>
       </c>
       <c r="X153" s="34">
@@ -7257,7 +7311,7 @@
       <c r="AF155" s="16"/>
     </row>
     <row r="156" spans="23:32">
-      <c r="W156" s="41" t="s">
+      <c r="W156" s="42" t="s">
         <v>26</v>
       </c>
       <c r="X156" s="34">
@@ -7290,7 +7344,7 @@
       </c>
     </row>
     <row r="157" spans="23:32">
-      <c r="W157" s="41" t="s">
+      <c r="W157" s="42" t="s">
         <v>27</v>
       </c>
       <c r="X157" s="34">
@@ -7336,7 +7390,7 @@
       <c r="AF159" s="16"/>
     </row>
     <row r="160" spans="23:32">
-      <c r="W160" s="41" t="s">
+      <c r="W160" s="42" t="s">
         <v>26</v>
       </c>
       <c r="X160" s="34">
@@ -7369,7 +7423,7 @@
       </c>
     </row>
     <row r="161" spans="23:32">
-      <c r="W161" s="41" t="s">
+      <c r="W161" s="42" t="s">
         <v>27</v>
       </c>
       <c r="X161" s="34">
@@ -7415,7 +7469,7 @@
       <c r="AF163" s="16"/>
     </row>
     <row r="164" spans="23:32">
-      <c r="W164" s="41" t="s">
+      <c r="W164" s="42" t="s">
         <v>26</v>
       </c>
       <c r="X164" s="34">
@@ -7448,7 +7502,7 @@
       </c>
     </row>
     <row r="165" spans="23:32">
-      <c r="W165" s="41" t="s">
+      <c r="W165" s="42" t="s">
         <v>27</v>
       </c>
       <c r="X165" s="34">
@@ -7494,7 +7548,7 @@
       <c r="AF167" s="16"/>
     </row>
     <row r="168" spans="23:32">
-      <c r="W168" s="41" t="s">
+      <c r="W168" s="42" t="s">
         <v>26</v>
       </c>
       <c r="X168" s="34">
@@ -7527,7 +7581,7 @@
       </c>
     </row>
     <row r="169" spans="23:32">
-      <c r="W169" s="41" t="s">
+      <c r="W169" s="42" t="s">
         <v>27</v>
       </c>
       <c r="X169" s="34">
@@ -7573,7 +7627,7 @@
       <c r="AF171" s="16"/>
     </row>
     <row r="172" spans="23:32">
-      <c r="W172" s="41" t="s">
+      <c r="W172" s="42" t="s">
         <v>26</v>
       </c>
       <c r="X172" s="34">
@@ -7606,7 +7660,7 @@
       </c>
     </row>
     <row r="173" spans="23:32">
-      <c r="W173" s="41" t="s">
+      <c r="W173" s="42" t="s">
         <v>27</v>
       </c>
       <c r="X173" s="34">
@@ -7636,6 +7690,533 @@
       <c r="AF173" s="39">
         <v>77314</v>
       </c>
+    </row>
+    <row r="175" spans="23:32">
+      <c r="W175" s="6" t="s">
+        <v>86</v>
+      </c>
+      <c r="X175" s="7"/>
+      <c r="Y175" s="7"/>
+      <c r="Z175" s="7"/>
+      <c r="AA175" s="7"/>
+      <c r="AB175" s="7"/>
+      <c r="AC175" s="7"/>
+      <c r="AD175" s="7"/>
+      <c r="AE175" s="7"/>
+      <c r="AF175" s="16"/>
+    </row>
+    <row r="176" spans="23:32">
+      <c r="W176" s="42" t="s">
+        <v>26</v>
+      </c>
+      <c r="X176" s="34">
+        <v>0.2071090173021</v>
+      </c>
+      <c r="Y176" s="34">
+        <v>0.170847728774746</v>
+      </c>
+      <c r="Z176" s="34">
+        <v>0.360110402187012</v>
+      </c>
+      <c r="AA176" s="34">
+        <v>0.112401221529825</v>
+      </c>
+      <c r="AB176" s="34">
+        <v>0.0280359899357589</v>
+      </c>
+      <c r="AC176" s="34">
+        <v>0.00249966325506939</v>
+      </c>
+      <c r="AD176" s="34">
+        <v>0.0946217254799631</v>
+      </c>
+      <c r="AE176" s="34">
+        <v>0.0385427196683573</v>
+      </c>
+      <c r="AF176" s="34">
+        <f>SUM(X176:AE176)</f>
+        <v>1.01416846813283</v>
+      </c>
+    </row>
+    <row r="177" spans="23:32">
+      <c r="W177" s="42" t="s">
+        <v>27</v>
+      </c>
+      <c r="X177" s="34">
+        <v>67449</v>
+      </c>
+      <c r="Y177" s="34">
+        <v>40216</v>
+      </c>
+      <c r="Z177" s="34">
+        <v>92779</v>
+      </c>
+      <c r="AA177" s="34">
+        <v>19998</v>
+      </c>
+      <c r="AB177" s="34">
+        <v>347379</v>
+      </c>
+      <c r="AC177" s="34">
+        <v>38781</v>
+      </c>
+      <c r="AD177" s="34">
+        <v>472450</v>
+      </c>
+      <c r="AE177" s="39">
+        <v>19029</v>
+      </c>
+      <c r="AF177" s="34">
+        <v>472450</v>
+      </c>
+    </row>
+    <row r="178" ht="14.25"/>
+    <row r="179" spans="23:32">
+      <c r="W179" s="20"/>
+      <c r="X179" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="Y179" s="21" t="s">
+        <v>1</v>
+      </c>
+      <c r="Z179" s="21" t="s">
+        <v>2</v>
+      </c>
+      <c r="AA179" s="21" t="s">
+        <v>3</v>
+      </c>
+      <c r="AB179" s="21" t="s">
+        <v>4</v>
+      </c>
+      <c r="AC179" s="21" t="s">
+        <v>5</v>
+      </c>
+      <c r="AD179" s="21" t="s">
+        <v>6</v>
+      </c>
+      <c r="AE179" s="21" t="s">
+        <v>7</v>
+      </c>
+      <c r="AF179" s="27" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="180" spans="23:32">
+      <c r="W180" s="22" t="s">
+        <v>24</v>
+      </c>
+      <c r="X180" s="23">
+        <v>1039722</v>
+      </c>
+      <c r="Y180" s="23">
+        <v>1083568</v>
+      </c>
+      <c r="Z180" s="23">
+        <v>997663</v>
+      </c>
+      <c r="AA180" s="23">
+        <v>1001733</v>
+      </c>
+      <c r="AB180" s="23">
+        <v>1694616</v>
+      </c>
+      <c r="AC180" s="23">
+        <v>1957027</v>
+      </c>
+      <c r="AD180" s="23">
+        <v>426485</v>
+      </c>
+      <c r="AE180" s="23">
+        <v>855802</v>
+      </c>
+      <c r="AF180" s="28"/>
+    </row>
+    <row r="181" spans="23:32">
+      <c r="W181" s="8"/>
+      <c r="AF181" s="15"/>
+    </row>
+    <row r="182" spans="23:32">
+      <c r="W182" s="6"/>
+      <c r="X182" s="46">
+        <v>0.207255996600315</v>
+      </c>
+      <c r="Y182" s="46">
+        <v>0.170827487785851</v>
+      </c>
+      <c r="Z182" s="33">
+        <v>0.359711307241924</v>
+      </c>
+      <c r="AA182" s="46">
+        <v>0.11166110429993</v>
+      </c>
+      <c r="AB182" s="46">
+        <v>0.0287592032379425</v>
+      </c>
+      <c r="AC182" s="46">
+        <v>0.0031382201640017</v>
+      </c>
+      <c r="AD182" s="46">
+        <v>0.0948727773946742</v>
+      </c>
+      <c r="AE182" s="46">
+        <v>0.0354465761733521</v>
+      </c>
+      <c r="AF182" s="34">
+        <f>SUM(X182:AE182)</f>
+        <v>1.01167267289799</v>
+      </c>
+    </row>
+    <row r="183" spans="23:32">
+      <c r="W183" s="8" t="s">
+        <v>87</v>
+      </c>
+      <c r="X183" s="7"/>
+      <c r="Y183" s="7"/>
+      <c r="Z183" s="7"/>
+      <c r="AA183" s="7"/>
+      <c r="AB183" s="7"/>
+      <c r="AC183" s="7"/>
+      <c r="AD183" s="7"/>
+      <c r="AE183" s="7"/>
+      <c r="AF183" s="14"/>
+    </row>
+    <row r="184" spans="23:32">
+      <c r="W184" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="X184" s="7">
+        <v>0.312495577129818</v>
+      </c>
+      <c r="Y184" s="7">
+        <v>0.267758307206809</v>
+      </c>
+      <c r="Z184" s="7">
+        <v>0.448368500627429</v>
+      </c>
+      <c r="AA184" s="7">
+        <v>0.195158730886677</v>
+      </c>
+      <c r="AB184" s="7">
+        <v>0.110055511151086</v>
+      </c>
+      <c r="AC184" s="7">
+        <v>0.00641399539044994</v>
+      </c>
+      <c r="AD184" s="7">
+        <v>0.158158049120629</v>
+      </c>
+      <c r="AE184" s="7">
+        <v>0.107585926362531</v>
+      </c>
+      <c r="AF184" s="34">
+        <f t="shared" ref="AF184:AF188" si="0">SUM(X184:AE184)</f>
+        <v>1.60599459787543</v>
+      </c>
+    </row>
+    <row r="185" spans="23:32">
+      <c r="W185" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="X185" s="34">
+        <v>201733</v>
+      </c>
+      <c r="Y185" s="34">
+        <v>187508</v>
+      </c>
+      <c r="Z185" s="39">
+        <v>270524</v>
+      </c>
+      <c r="AA185" s="34">
+        <v>231936</v>
+      </c>
+      <c r="AB185" s="34">
+        <v>624256</v>
+      </c>
+      <c r="AC185" s="34">
+        <v>327145</v>
+      </c>
+      <c r="AD185" s="34">
+        <v>109726</v>
+      </c>
+      <c r="AE185" s="34">
+        <v>109685</v>
+      </c>
+      <c r="AF185" s="39">
+        <f t="shared" si="0"/>
+        <v>2062513</v>
+      </c>
+    </row>
+    <row r="187" spans="12:32">
+      <c r="L187" s="8" t="s">
+        <v>88</v>
+      </c>
+      <c r="M187" s="7"/>
+      <c r="N187" s="7"/>
+      <c r="O187" s="7"/>
+      <c r="P187" s="7"/>
+      <c r="Q187" s="7"/>
+      <c r="R187" s="7"/>
+      <c r="S187" s="7"/>
+      <c r="T187" s="7"/>
+      <c r="U187" s="14"/>
+      <c r="W187" s="8" t="s">
+        <v>89</v>
+      </c>
+      <c r="X187" s="7"/>
+      <c r="Y187" s="7"/>
+      <c r="Z187" s="7"/>
+      <c r="AA187" s="7"/>
+      <c r="AB187" s="7"/>
+      <c r="AC187" s="7"/>
+      <c r="AD187" s="7"/>
+      <c r="AE187" s="7"/>
+      <c r="AF187" s="14"/>
+    </row>
+    <row r="188" spans="12:32">
+      <c r="L188" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="M188" s="7">
+        <v>0.207561640493532</v>
+      </c>
+      <c r="N188" s="7">
+        <v>0.172901852187878</v>
+      </c>
+      <c r="O188" s="7">
+        <v>0.343962910788856</v>
+      </c>
+      <c r="P188" s="7">
+        <v>0.118932859856985</v>
+      </c>
+      <c r="Q188" s="7">
+        <v>0.0380822213280371</v>
+      </c>
+      <c r="R188" s="7">
+        <v>0.0374913548145826</v>
+      </c>
+      <c r="S188" s="7">
+        <v>0.0954016384376688</v>
+      </c>
+      <c r="T188" s="7">
+        <v>0.0483419006066361</v>
+      </c>
+      <c r="U188" s="16">
+        <f>SUM(M188:T188)</f>
+        <v>1.06267637851418</v>
+      </c>
+      <c r="W188" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="X188" s="7">
+        <v>0.207247490729589</v>
+      </c>
+      <c r="Y188" s="7">
+        <v>0.170866122856409</v>
+      </c>
+      <c r="Z188" s="7">
+        <v>0.359639932539382</v>
+      </c>
+      <c r="AA188" s="7">
+        <v>0.111495554443925</v>
+      </c>
+      <c r="AB188" s="7">
+        <v>0.0286448603212694</v>
+      </c>
+      <c r="AC188" s="7">
+        <v>0.00216421261328103</v>
+      </c>
+      <c r="AD188" s="7">
+        <v>0.0949402092366402</v>
+      </c>
+      <c r="AE188" s="7">
+        <v>0.0355927093794736</v>
+      </c>
+      <c r="AF188" s="34">
+        <f t="shared" si="0"/>
+        <v>1.01059109211997</v>
+      </c>
+    </row>
+    <row r="189" spans="12:32">
+      <c r="L189" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="M189" s="40">
+        <v>26454</v>
+      </c>
+      <c r="N189" s="40">
+        <v>19443</v>
+      </c>
+      <c r="O189" s="40">
+        <v>43208</v>
+      </c>
+      <c r="P189" s="40">
+        <v>12952</v>
+      </c>
+      <c r="Q189" s="40">
+        <v>56937</v>
+      </c>
+      <c r="R189" s="40">
+        <v>27451</v>
+      </c>
+      <c r="S189" s="40">
+        <v>54086</v>
+      </c>
+      <c r="T189" s="40">
+        <v>16901</v>
+      </c>
+      <c r="U189" s="40">
+        <v>56937</v>
+      </c>
+      <c r="W189" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="X189" s="34">
+        <v>26382</v>
+      </c>
+      <c r="Y189" s="34">
+        <v>31524</v>
+      </c>
+      <c r="Z189" s="39">
+        <v>39771</v>
+      </c>
+      <c r="AA189" s="34">
+        <v>18168</v>
+      </c>
+      <c r="AB189" s="34">
+        <v>49002</v>
+      </c>
+      <c r="AC189" s="34">
+        <v>33240</v>
+      </c>
+      <c r="AD189" s="34">
+        <v>48593</v>
+      </c>
+      <c r="AE189" s="34">
+        <v>16760</v>
+      </c>
+      <c r="AF189" s="39">
+        <v>49002</v>
+      </c>
+    </row>
+    <row r="191" spans="12:32">
+      <c r="L191" s="8"/>
+      <c r="M191" s="7"/>
+      <c r="N191" s="7"/>
+      <c r="O191" s="7"/>
+      <c r="P191" s="7"/>
+      <c r="Q191" s="7"/>
+      <c r="R191" s="7"/>
+      <c r="S191" s="7"/>
+      <c r="T191" s="7"/>
+      <c r="U191" s="14"/>
+      <c r="W191" s="8" t="s">
+        <v>90</v>
+      </c>
+      <c r="X191" s="7"/>
+      <c r="Y191" s="7"/>
+      <c r="Z191" s="7"/>
+      <c r="AA191" s="7"/>
+      <c r="AB191" s="7"/>
+      <c r="AC191" s="7"/>
+      <c r="AD191" s="7"/>
+      <c r="AE191" s="7"/>
+      <c r="AF191" s="14"/>
+    </row>
+    <row r="192" spans="12:32">
+      <c r="L192" s="6"/>
+      <c r="M192" s="7"/>
+      <c r="N192" s="7"/>
+      <c r="O192" s="7"/>
+      <c r="P192" s="7"/>
+      <c r="Q192" s="7"/>
+      <c r="R192" s="7"/>
+      <c r="S192" s="7"/>
+      <c r="T192" s="7"/>
+      <c r="U192" s="16"/>
+      <c r="W192" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="X192" s="7">
+        <v>0.206049947306921</v>
+      </c>
+      <c r="Y192" s="7">
+        <v>0.169594488695383</v>
+      </c>
+      <c r="Z192" s="7">
+        <v>0.35838545768632</v>
+      </c>
+      <c r="AA192" s="7">
+        <v>0.110748998587646</v>
+      </c>
+      <c r="AB192" s="7">
+        <v>0.0307042559830637</v>
+      </c>
+      <c r="AC192" s="7">
+        <v>0.00296818182317827</v>
+      </c>
+      <c r="AD192" s="7">
+        <v>0.093607987367592</v>
+      </c>
+      <c r="AE192" s="7">
+        <v>0.0355902713631438</v>
+      </c>
+      <c r="AF192" s="34">
+        <f>SUM(X192:AE192)</f>
+        <v>1.00764958881325</v>
+      </c>
+    </row>
+    <row r="193" spans="12:32">
+      <c r="L193" s="6"/>
+      <c r="M193" s="40"/>
+      <c r="N193" s="40"/>
+      <c r="O193" s="40"/>
+      <c r="P193" s="40"/>
+      <c r="Q193" s="40"/>
+      <c r="R193" s="40"/>
+      <c r="S193" s="40"/>
+      <c r="T193" s="40"/>
+      <c r="U193" s="40"/>
+      <c r="W193" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="X193" s="40">
+        <v>18985</v>
+      </c>
+      <c r="Y193" s="40">
+        <v>14109</v>
+      </c>
+      <c r="Z193" s="40">
+        <v>24910</v>
+      </c>
+      <c r="AA193" s="40">
+        <v>9141</v>
+      </c>
+      <c r="AB193" s="40">
+        <v>55161</v>
+      </c>
+      <c r="AC193" s="40">
+        <v>9196</v>
+      </c>
+      <c r="AD193" s="40">
+        <v>76013</v>
+      </c>
+      <c r="AE193" s="40">
+        <v>15393</v>
+      </c>
+      <c r="AF193" s="40">
+        <v>76013</v>
+      </c>
+    </row>
+    <row r="195" spans="24:32">
+      <c r="X195"/>
+      <c r="Y195"/>
+      <c r="Z195"/>
+      <c r="AA195"/>
+      <c r="AB195"/>
+      <c r="AC195"/>
+      <c r="AD195"/>
+      <c r="AE195"/>
+      <c r="AF195"/>
     </row>
   </sheetData>
   <pageMargins left="0.699305555555556" right="0.699305555555556" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -7650,7 +8231,7 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+      <selection activeCell="B29" sqref="B29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>

</xml_diff>

<commit_message>
add closeness python result
</commit_message>
<xml_diff>
--- a/overall.xlsx
+++ b/overall.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="20385" windowHeight="8370"/>
+    <workbookView windowWidth="28695" windowHeight="13065" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92">
   <si>
     <t>model1</t>
   </si>
@@ -279,7 +279,7 @@
     <t>17_07_30_13_04_32_3_1_500_8_0.001</t>
   </si>
   <si>
-    <t>pythonResults/17_07_11_23_45_34_-1_2000000_500_3/./pythonControl.sh -1 2000000 3</t>
+    <t>pythonResults/17_07_11_23_45_34_-1_2000000_500_3/./pythonControl.sh -1 2000000 3(betweenness)</t>
   </si>
   <si>
     <t>17_08_02_12_47_32_2_1_500_6_0.001/FirstInFirstOut</t>
@@ -289,6 +289,9 @@
   </si>
   <si>
     <t>17_08_02_08_20_59_2_1_500_7_0.001/Multiple_reinsert</t>
+  </si>
+  <si>
+    <t>pythonResults/17_08_06_09_53_17_-1_2000000_500_2/./pythonControl.sh -1 2000000 2(closeness)</t>
   </si>
 </sst>
 </file>
@@ -296,10 +299,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
   <fonts count="23">
     <font>
@@ -332,6 +335,13 @@
     </font>
     <font>
       <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="0"/>
       <name val="宋体"/>
       <charset val="0"/>
@@ -339,7 +349,83 @@
     </font>
     <font>
       <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -353,84 +439,9 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="11"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color rgb="FF3F3F3F"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -445,15 +456,15 @@
     </font>
     <font>
       <b/>
-      <sz val="18"/>
-      <color theme="3"/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
       <name val="宋体"/>
-      <charset val="134"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <color rgb="FFFA7D00"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -461,15 +472,7 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
+      <color theme="1"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -502,7 +505,109 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -520,19 +625,31 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
+        <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
+        <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -544,7 +661,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -556,133 +685,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -849,26 +852,26 @@
       <diagonal/>
     </border>
     <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
       <right/>
       <top/>
       <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -890,44 +893,9 @@
     <border>
       <left/>
       <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
       <top/>
       <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -946,6 +914,41 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
@@ -954,10 +957,10 @@
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="17" borderId="14" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="15" borderId="14" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -966,137 +969,137 @@
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="12" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="15" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="15" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="28" borderId="16" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="28" borderId="14" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="29" borderId="17" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="18" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="19" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="27" borderId="18" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="17" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="31" borderId="19" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="31" borderId="14" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="16" borderId="13" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="16" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="15" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
   </cellStyleXfs>
-  <cellXfs count="55">
+  <cellXfs count="52">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1217,9 +1220,6 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1255,12 +1255,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1">
       <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="49">
@@ -1315,11 +1309,6 @@
     <cellStyle name="60% - 强调文字颜色 6" xfId="48" builtinId="52"/>
   </cellStyles>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
@@ -1613,7 +1602,7 @@
   <sheetPr/>
   <dimension ref="A1:J42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B42" sqref="B42:J42"/>
     </sheetView>
   </sheetViews>
@@ -1705,7 +1694,7 @@
       <c r="F3">
         <v>0.0522827100851127</v>
       </c>
-      <c r="G3" s="50">
+      <c r="G3" s="49">
         <v>0.106926203216301</v>
       </c>
       <c r="H3">
@@ -1731,7 +1720,7 @@
       <c r="A12" t="s">
         <v>12</v>
       </c>
-      <c r="G12" s="51">
+      <c r="G12" s="50">
         <v>0.0629933219692992</v>
       </c>
     </row>
@@ -1784,7 +1773,7 @@
       <c r="I19">
         <v>0.0755164339928472</v>
       </c>
-      <c r="J19" s="52">
+      <c r="J19" s="51">
         <f t="shared" ref="J19:J21" si="0">SUM(B19:I19)</f>
         <v>1.17870842662782</v>
       </c>
@@ -1793,31 +1782,31 @@
       <c r="A20" t="s">
         <v>17</v>
       </c>
-      <c r="B20" s="52">
+      <c r="B20" s="51">
         <v>0.20800686430345</v>
       </c>
-      <c r="C20" s="52">
+      <c r="C20" s="51">
         <v>0.173239206962822</v>
       </c>
-      <c r="D20" s="52">
+      <c r="D20" s="51">
         <v>0.346041541710196</v>
       </c>
-      <c r="E20" s="52">
+      <c r="E20" s="51">
         <v>0.124928278882666</v>
       </c>
-      <c r="F20" s="52">
+      <c r="F20" s="51">
         <v>0.0409924383808026</v>
       </c>
-      <c r="G20" s="52">
+      <c r="G20" s="51">
         <v>0.0453003114127127</v>
       </c>
-      <c r="H20" s="52">
+      <c r="H20" s="51">
         <v>0.0964368086720679</v>
       </c>
-      <c r="I20" s="52">
+      <c r="I20" s="51">
         <v>0.065879029949852</v>
       </c>
-      <c r="J20" s="52">
+      <c r="J20" s="51">
         <f t="shared" si="0"/>
         <v>1.10082448027457</v>
       </c>
@@ -1826,52 +1815,52 @@
       <c r="A21" t="s">
         <v>18</v>
       </c>
-      <c r="B21" s="51">
+      <c r="B21" s="50">
         <v>0.207894527330402</v>
       </c>
-      <c r="C21" s="51">
+      <c r="C21" s="50">
         <v>0.173165858291852</v>
       </c>
-      <c r="D21" s="51">
+      <c r="D21" s="50">
         <v>0.344628020195683</v>
       </c>
-      <c r="E21" s="51">
+      <c r="E21" s="50">
         <v>0.118862297465155</v>
       </c>
-      <c r="F21" s="51">
+      <c r="F21" s="50">
         <v>0.0388983176119749</v>
       </c>
-      <c r="G21" s="51">
+      <c r="G21" s="50">
         <v>0.0422239303614074</v>
       </c>
-      <c r="H21" s="51">
+      <c r="H21" s="50">
         <v>0.0955131594160284</v>
       </c>
-      <c r="I21" s="51">
+      <c r="I21" s="50">
         <v>0.0488732287830458</v>
       </c>
-      <c r="J21" s="51">
+      <c r="J21" s="50">
         <f t="shared" si="0"/>
         <v>1.07005933945555</v>
       </c>
     </row>
     <row r="22" spans="10:10">
-      <c r="J22" s="52"/>
+      <c r="J22" s="51"/>
     </row>
     <row r="23" spans="10:10">
-      <c r="J23" s="52"/>
+      <c r="J23" s="51"/>
     </row>
     <row r="24" spans="10:10">
-      <c r="J24" s="52"/>
+      <c r="J24" s="51"/>
     </row>
     <row r="25" spans="10:10">
-      <c r="J25" s="52"/>
+      <c r="J25" s="51"/>
     </row>
     <row r="26" spans="1:10">
       <c r="A26" t="s">
         <v>19</v>
       </c>
-      <c r="J26" s="52"/>
+      <c r="J26" s="51"/>
     </row>
     <row r="27" spans="1:10">
       <c r="A27" t="s">
@@ -1892,7 +1881,7 @@
       <c r="F27">
         <v>0.0492015604703379</v>
       </c>
-      <c r="G27" s="52">
+      <c r="G27" s="51">
         <v>0.0766396493470802</v>
       </c>
       <c r="H27">
@@ -1901,7 +1890,7 @@
       <c r="I27">
         <v>0.0926905158740254</v>
       </c>
-      <c r="J27" s="52">
+      <c r="J27" s="51">
         <f>SUM(B27:I27)</f>
         <v>1.27166155848785</v>
       </c>
@@ -1925,7 +1914,7 @@
       <c r="F28">
         <v>0.0533366743677525</v>
       </c>
-      <c r="G28" s="50">
+      <c r="G28" s="49">
         <v>0.110748101588701</v>
       </c>
       <c r="H28">
@@ -1934,7 +1923,7 @@
       <c r="I28">
         <v>0.103230203907768</v>
       </c>
-      <c r="J28" s="52">
+      <c r="J28" s="51">
         <f>SUM(B28:I28)</f>
         <v>1.31676786850071</v>
       </c>
@@ -1953,31 +1942,31 @@
       </c>
     </row>
     <row r="42" spans="2:10">
-      <c r="B42" s="53">
+      <c r="B42" s="42">
         <v>0.206049947306921</v>
       </c>
-      <c r="C42" s="53">
+      <c r="C42" s="42">
         <v>0.169594488695383</v>
       </c>
-      <c r="D42" s="53">
+      <c r="D42" s="42">
         <v>0.343962910788856</v>
       </c>
-      <c r="E42" s="53">
+      <c r="E42" s="42">
         <v>0.110748998587646</v>
       </c>
-      <c r="F42" s="53">
+      <c r="F42" s="42">
         <v>0.0286448603212694</v>
       </c>
-      <c r="G42" s="53">
+      <c r="G42" s="42">
         <v>0.00216421261328103</v>
       </c>
-      <c r="H42" s="53">
+      <c r="H42" s="42">
         <v>0.093607987367592</v>
       </c>
-      <c r="I42" s="46">
+      <c r="I42" s="45">
         <v>0.0354465761733521</v>
       </c>
-      <c r="J42" s="54">
+      <c r="J42" s="33">
         <f>SUM(B42:I42)</f>
         <v>0.990219981854301</v>
       </c>
@@ -1992,10 +1981,10 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr/>
-  <dimension ref="A1:AF195"/>
+  <dimension ref="A1:AF197"/>
   <sheetViews>
-    <sheetView topLeftCell="Z178" workbookViewId="0">
-      <selection activeCell="AF195" sqref="X195:AF195"/>
+    <sheetView tabSelected="1" topLeftCell="T163" workbookViewId="0">
+      <selection activeCell="AF196" sqref="AF196"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
@@ -6330,7 +6319,7 @@
       </c>
     </row>
     <row r="129" spans="23:32">
-      <c r="W129" s="41" t="s">
+      <c r="W129" s="40" t="s">
         <v>69</v>
       </c>
       <c r="X129" s="34">
@@ -6374,18 +6363,18 @@
       <c r="S130" s="7"/>
       <c r="T130" s="7"/>
       <c r="U130" s="14"/>
-      <c r="W130" s="42" t="s">
+      <c r="W130" s="41" t="s">
         <v>29</v>
       </c>
-      <c r="X130" s="43"/>
-      <c r="Y130" s="43"/>
-      <c r="Z130" s="43"/>
-      <c r="AA130" s="43"/>
-      <c r="AB130" s="43"/>
-      <c r="AC130" s="43"/>
-      <c r="AD130" s="43"/>
-      <c r="AE130" s="43"/>
-      <c r="AF130" s="47"/>
+      <c r="X130" s="42"/>
+      <c r="Y130" s="42"/>
+      <c r="Z130" s="42"/>
+      <c r="AA130" s="42"/>
+      <c r="AB130" s="42"/>
+      <c r="AC130" s="42"/>
+      <c r="AD130" s="42"/>
+      <c r="AE130" s="42"/>
+      <c r="AF130" s="46"/>
     </row>
     <row r="131" spans="12:32">
       <c r="L131" s="6" t="s">
@@ -6419,16 +6408,16 @@
         <f>SUM(M131:T131)</f>
         <v>1.19427920902361</v>
       </c>
-      <c r="W131" s="44"/>
-      <c r="X131" s="45"/>
-      <c r="Y131" s="45"/>
-      <c r="Z131" s="45"/>
-      <c r="AA131" s="45"/>
-      <c r="AB131" s="45"/>
-      <c r="AC131" s="45"/>
-      <c r="AD131" s="45"/>
-      <c r="AE131" s="45"/>
-      <c r="AF131" s="48"/>
+      <c r="W131" s="43"/>
+      <c r="X131" s="44"/>
+      <c r="Y131" s="44"/>
+      <c r="Z131" s="44"/>
+      <c r="AA131" s="44"/>
+      <c r="AB131" s="44"/>
+      <c r="AC131" s="44"/>
+      <c r="AD131" s="44"/>
+      <c r="AE131" s="44"/>
+      <c r="AF131" s="47"/>
     </row>
     <row r="132" spans="12:32">
       <c r="L132" s="6" t="s">
@@ -6461,48 +6450,48 @@
       <c r="U132" s="38">
         <v>8928</v>
       </c>
-      <c r="W132" s="43" t="s">
+      <c r="W132" s="42" t="s">
         <v>71</v>
       </c>
-      <c r="X132" s="43"/>
-      <c r="Y132" s="43"/>
-      <c r="Z132" s="43"/>
-      <c r="AA132" s="43"/>
-      <c r="AB132" s="43"/>
-      <c r="AC132" s="43"/>
-      <c r="AD132" s="43"/>
-      <c r="AE132" s="43"/>
-      <c r="AF132" s="43"/>
+      <c r="X132" s="42"/>
+      <c r="Y132" s="42"/>
+      <c r="Z132" s="42"/>
+      <c r="AA132" s="42"/>
+      <c r="AB132" s="42"/>
+      <c r="AC132" s="42"/>
+      <c r="AD132" s="42"/>
+      <c r="AE132" s="42"/>
+      <c r="AF132" s="42"/>
     </row>
     <row r="133" spans="23:32">
-      <c r="W133" s="42" t="s">
+      <c r="W133" s="41" t="s">
         <v>26</v>
       </c>
-      <c r="X133" s="43">
+      <c r="X133" s="42">
         <v>0.20726823279994</v>
       </c>
-      <c r="Y133" s="43">
+      <c r="Y133" s="42">
         <v>0.170985023438374</v>
       </c>
-      <c r="Z133" s="43">
+      <c r="Z133" s="42">
         <v>0.359664208360988</v>
       </c>
-      <c r="AA133" s="43">
+      <c r="AA133" s="42">
         <v>0.112089923569473</v>
       </c>
-      <c r="AB133" s="43">
+      <c r="AB133" s="42">
         <v>0.029467659671068</v>
       </c>
-      <c r="AC133" s="43">
+      <c r="AC133" s="42">
         <v>0.00370557094652351</v>
       </c>
-      <c r="AD133" s="43">
+      <c r="AD133" s="42">
         <v>0.0955302550359815</v>
       </c>
-      <c r="AE133" s="43">
+      <c r="AE133" s="42">
         <v>0.0365722018037902</v>
       </c>
-      <c r="AF133" s="47">
+      <c r="AF133" s="46">
         <f>SUM(X133:AE133)</f>
         <v>1.01528307562614</v>
       </c>
@@ -6520,7 +6509,7 @@
       <c r="S134" s="7"/>
       <c r="T134" s="7"/>
       <c r="U134" s="14"/>
-      <c r="W134" s="42" t="s">
+      <c r="W134" s="41" t="s">
         <v>27</v>
       </c>
       <c r="X134" s="33">
@@ -6583,7 +6572,7 @@
         <f>SUM(M135:T135)</f>
         <v>1.11768511223654</v>
       </c>
-      <c r="W135" s="43" t="s">
+      <c r="W135" s="42" t="s">
         <v>73</v>
       </c>
       <c r="X135" s="33">
@@ -6645,18 +6634,18 @@
       <c r="U136" s="34">
         <v>49407</v>
       </c>
-      <c r="W136" s="42" t="s">
+      <c r="W136" s="41" t="s">
         <v>29</v>
       </c>
-      <c r="X136" s="43"/>
-      <c r="Y136" s="43"/>
-      <c r="Z136" s="43"/>
-      <c r="AA136" s="43"/>
-      <c r="AB136" s="43"/>
-      <c r="AC136" s="43"/>
-      <c r="AD136" s="43"/>
-      <c r="AE136" s="43"/>
-      <c r="AF136" s="43"/>
+      <c r="X136" s="42"/>
+      <c r="Y136" s="42"/>
+      <c r="Z136" s="42"/>
+      <c r="AA136" s="42"/>
+      <c r="AB136" s="42"/>
+      <c r="AC136" s="42"/>
+      <c r="AD136" s="42"/>
+      <c r="AE136" s="42"/>
+      <c r="AF136" s="42"/>
     </row>
     <row r="137" spans="23:32">
       <c r="W137" s="7"/>
@@ -6760,7 +6749,7 @@
       <c r="U140" s="38">
         <v>10515</v>
       </c>
-      <c r="W140" s="42" t="s">
+      <c r="W140" s="41" t="s">
         <v>26</v>
       </c>
       <c r="X140" s="34">
@@ -6787,13 +6776,13 @@
       <c r="AE140" s="34">
         <v>0.0400224015997118</v>
       </c>
-      <c r="AF140" s="49">
+      <c r="AF140" s="48">
         <f>SUM(X140:AE140)</f>
         <v>1.01852769482818</v>
       </c>
     </row>
     <row r="141" spans="23:32">
-      <c r="W141" s="42" t="s">
+      <c r="W141" s="41" t="s">
         <v>27</v>
       </c>
       <c r="X141" s="34">
@@ -6914,7 +6903,7 @@
       <c r="U144" s="38">
         <v>53817</v>
       </c>
-      <c r="W144" s="42" t="s">
+      <c r="W144" s="41" t="s">
         <v>26</v>
       </c>
       <c r="X144" s="34">
@@ -6947,7 +6936,7 @@
       </c>
     </row>
     <row r="145" spans="23:32">
-      <c r="W145" s="42" t="s">
+      <c r="W145" s="41" t="s">
         <v>27</v>
       </c>
       <c r="X145" s="34">
@@ -7078,7 +7067,7 @@
       <c r="U148" s="38">
         <v>21172</v>
       </c>
-      <c r="W148" s="42" t="s">
+      <c r="W148" s="41" t="s">
         <v>26</v>
       </c>
       <c r="X148" s="34">
@@ -7111,7 +7100,7 @@
       </c>
     </row>
     <row r="149" spans="23:32">
-      <c r="W149" s="42" t="s">
+      <c r="W149" s="41" t="s">
         <v>27</v>
       </c>
       <c r="X149" s="34">
@@ -7232,31 +7221,31 @@
       <c r="U152" s="38">
         <v>88904</v>
       </c>
-      <c r="W152" s="42" t="s">
+      <c r="W152" s="41" t="s">
         <v>26</v>
       </c>
-      <c r="X152" s="46">
+      <c r="X152" s="45">
         <v>0.207255996600315</v>
       </c>
-      <c r="Y152" s="46">
+      <c r="Y152" s="45">
         <v>0.170827487785851</v>
       </c>
       <c r="Z152" s="33">
         <v>0.359711307241924</v>
       </c>
-      <c r="AA152" s="46">
+      <c r="AA152" s="45">
         <v>0.11166110429993</v>
       </c>
-      <c r="AB152" s="46">
+      <c r="AB152" s="45">
         <v>0.0287592032379425</v>
       </c>
-      <c r="AC152" s="46">
+      <c r="AC152" s="45">
         <v>0.0031382201640017</v>
       </c>
-      <c r="AD152" s="46">
+      <c r="AD152" s="45">
         <v>0.0948727773946742</v>
       </c>
-      <c r="AE152" s="46">
+      <c r="AE152" s="45">
         <v>0.0354465761733521</v>
       </c>
       <c r="AF152" s="34">
@@ -7265,7 +7254,7 @@
       </c>
     </row>
     <row r="153" spans="23:32">
-      <c r="W153" s="42" t="s">
+      <c r="W153" s="41" t="s">
         <v>27</v>
       </c>
       <c r="X153" s="34">
@@ -7311,7 +7300,7 @@
       <c r="AF155" s="16"/>
     </row>
     <row r="156" spans="23:32">
-      <c r="W156" s="42" t="s">
+      <c r="W156" s="41" t="s">
         <v>26</v>
       </c>
       <c r="X156" s="34">
@@ -7344,7 +7333,7 @@
       </c>
     </row>
     <row r="157" spans="23:32">
-      <c r="W157" s="42" t="s">
+      <c r="W157" s="41" t="s">
         <v>27</v>
       </c>
       <c r="X157" s="34">
@@ -7390,7 +7379,7 @@
       <c r="AF159" s="16"/>
     </row>
     <row r="160" spans="23:32">
-      <c r="W160" s="42" t="s">
+      <c r="W160" s="41" t="s">
         <v>26</v>
       </c>
       <c r="X160" s="34">
@@ -7423,7 +7412,7 @@
       </c>
     </row>
     <row r="161" spans="23:32">
-      <c r="W161" s="42" t="s">
+      <c r="W161" s="41" t="s">
         <v>27</v>
       </c>
       <c r="X161" s="34">
@@ -7469,7 +7458,7 @@
       <c r="AF163" s="16"/>
     </row>
     <row r="164" spans="23:32">
-      <c r="W164" s="42" t="s">
+      <c r="W164" s="41" t="s">
         <v>26</v>
       </c>
       <c r="X164" s="34">
@@ -7502,7 +7491,7 @@
       </c>
     </row>
     <row r="165" spans="23:32">
-      <c r="W165" s="42" t="s">
+      <c r="W165" s="41" t="s">
         <v>27</v>
       </c>
       <c r="X165" s="34">
@@ -7548,7 +7537,7 @@
       <c r="AF167" s="16"/>
     </row>
     <row r="168" spans="23:32">
-      <c r="W168" s="42" t="s">
+      <c r="W168" s="41" t="s">
         <v>26</v>
       </c>
       <c r="X168" s="34">
@@ -7581,7 +7570,7 @@
       </c>
     </row>
     <row r="169" spans="23:32">
-      <c r="W169" s="42" t="s">
+      <c r="W169" s="41" t="s">
         <v>27</v>
       </c>
       <c r="X169" s="34">
@@ -7627,7 +7616,7 @@
       <c r="AF171" s="16"/>
     </row>
     <row r="172" spans="23:32">
-      <c r="W172" s="42" t="s">
+      <c r="W172" s="41" t="s">
         <v>26</v>
       </c>
       <c r="X172" s="34">
@@ -7660,7 +7649,7 @@
       </c>
     </row>
     <row r="173" spans="23:32">
-      <c r="W173" s="42" t="s">
+      <c r="W173" s="41" t="s">
         <v>27</v>
       </c>
       <c r="X173" s="34">
@@ -7706,7 +7695,7 @@
       <c r="AF175" s="16"/>
     </row>
     <row r="176" spans="23:32">
-      <c r="W176" s="42" t="s">
+      <c r="W176" s="41" t="s">
         <v>26</v>
       </c>
       <c r="X176" s="34">
@@ -7739,7 +7728,7 @@
       </c>
     </row>
     <row r="177" spans="23:32">
-      <c r="W177" s="42" t="s">
+      <c r="W177" s="41" t="s">
         <v>27</v>
       </c>
       <c r="X177" s="34">
@@ -7837,28 +7826,28 @@
     </row>
     <row r="182" spans="23:32">
       <c r="W182" s="6"/>
-      <c r="X182" s="46">
+      <c r="X182" s="45">
         <v>0.207255996600315</v>
       </c>
-      <c r="Y182" s="46">
+      <c r="Y182" s="45">
         <v>0.170827487785851</v>
       </c>
       <c r="Z182" s="33">
         <v>0.359711307241924</v>
       </c>
-      <c r="AA182" s="46">
+      <c r="AA182" s="45">
         <v>0.11166110429993</v>
       </c>
-      <c r="AB182" s="46">
+      <c r="AB182" s="45">
         <v>0.0287592032379425</v>
       </c>
-      <c r="AC182" s="46">
+      <c r="AC182" s="45">
         <v>0.0031382201640017</v>
       </c>
-      <c r="AD182" s="46">
+      <c r="AD182" s="45">
         <v>0.0948727773946742</v>
       </c>
-      <c r="AE182" s="46">
+      <c r="AE182" s="45">
         <v>0.0354465761733521</v>
       </c>
       <c r="AF182" s="34">
@@ -8040,31 +8029,31 @@
       <c r="L189" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="M189" s="40">
+      <c r="M189" s="39">
         <v>26454</v>
       </c>
-      <c r="N189" s="40">
+      <c r="N189" s="39">
         <v>19443</v>
       </c>
-      <c r="O189" s="40">
+      <c r="O189" s="39">
         <v>43208</v>
       </c>
-      <c r="P189" s="40">
+      <c r="P189" s="39">
         <v>12952</v>
       </c>
-      <c r="Q189" s="40">
+      <c r="Q189" s="39">
         <v>56937</v>
       </c>
-      <c r="R189" s="40">
+      <c r="R189" s="39">
         <v>27451</v>
       </c>
-      <c r="S189" s="40">
+      <c r="S189" s="39">
         <v>54086</v>
       </c>
-      <c r="T189" s="40">
+      <c r="T189" s="39">
         <v>16901</v>
       </c>
-      <c r="U189" s="40">
+      <c r="U189" s="39">
         <v>56937</v>
       </c>
       <c r="W189" s="6" t="s">
@@ -8167,56 +8156,125 @@
     </row>
     <row r="193" spans="12:32">
       <c r="L193" s="6"/>
-      <c r="M193" s="40"/>
-      <c r="N193" s="40"/>
-      <c r="O193" s="40"/>
-      <c r="P193" s="40"/>
-      <c r="Q193" s="40"/>
-      <c r="R193" s="40"/>
-      <c r="S193" s="40"/>
-      <c r="T193" s="40"/>
-      <c r="U193" s="40"/>
+      <c r="M193" s="39"/>
+      <c r="N193" s="39"/>
+      <c r="O193" s="39"/>
+      <c r="P193" s="39"/>
+      <c r="Q193" s="39"/>
+      <c r="R193" s="39"/>
+      <c r="S193" s="39"/>
+      <c r="T193" s="39"/>
+      <c r="U193" s="39"/>
       <c r="W193" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="X193" s="40">
+      <c r="X193" s="39">
         <v>18985</v>
       </c>
-      <c r="Y193" s="40">
+      <c r="Y193" s="39">
         <v>14109</v>
       </c>
-      <c r="Z193" s="40">
+      <c r="Z193" s="39">
         <v>24910</v>
       </c>
-      <c r="AA193" s="40">
+      <c r="AA193" s="39">
         <v>9141</v>
       </c>
-      <c r="AB193" s="40">
+      <c r="AB193" s="39">
         <v>55161</v>
       </c>
-      <c r="AC193" s="40">
+      <c r="AC193" s="39">
         <v>9196</v>
       </c>
-      <c r="AD193" s="40">
+      <c r="AD193" s="39">
         <v>76013</v>
       </c>
-      <c r="AE193" s="40">
+      <c r="AE193" s="39">
         <v>15393</v>
       </c>
-      <c r="AF193" s="40">
+      <c r="AF193" s="39">
         <v>76013</v>
       </c>
     </row>
-    <row r="195" spans="24:32">
-      <c r="X195"/>
-      <c r="Y195"/>
-      <c r="Z195"/>
-      <c r="AA195"/>
-      <c r="AB195"/>
-      <c r="AC195"/>
-      <c r="AD195"/>
-      <c r="AE195"/>
-      <c r="AF195"/>
+    <row r="195" spans="23:32">
+      <c r="W195" s="8" t="s">
+        <v>91</v>
+      </c>
+      <c r="X195" s="7"/>
+      <c r="Y195" s="7"/>
+      <c r="Z195" s="7"/>
+      <c r="AA195" s="7"/>
+      <c r="AB195" s="7"/>
+      <c r="AC195" s="7"/>
+      <c r="AD195" s="7"/>
+      <c r="AE195" s="7"/>
+      <c r="AF195" s="14"/>
+    </row>
+    <row r="196" spans="23:32">
+      <c r="W196" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="X196" s="7">
+        <v>0.414046852052083</v>
+      </c>
+      <c r="Y196" s="7">
+        <v>0.376463348201881</v>
+      </c>
+      <c r="Z196" s="7">
+        <v>0.462389953359366</v>
+      </c>
+      <c r="AA196" s="7">
+        <v>0.371686148674771</v>
+      </c>
+      <c r="AB196" s="7">
+        <v>0.249523364035694</v>
+      </c>
+      <c r="AC196" s="7">
+        <v>0.445369332660109</v>
+      </c>
+      <c r="AD196" s="7">
+        <v>0.273837458022987</v>
+      </c>
+      <c r="AE196" s="7">
+        <v>0.286777024588501</v>
+      </c>
+      <c r="AF196" s="34">
+        <f>SUM(X196:AE196)</f>
+        <v>2.88009348159539</v>
+      </c>
+    </row>
+    <row r="197" spans="23:32">
+      <c r="W197" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="X197" s="34">
+        <v>63095</v>
+      </c>
+      <c r="Y197" s="34">
+        <v>63552</v>
+      </c>
+      <c r="Z197" s="39">
+        <v>71382</v>
+      </c>
+      <c r="AA197" s="34">
+        <v>46107</v>
+      </c>
+      <c r="AB197" s="34">
+        <v>136945</v>
+      </c>
+      <c r="AC197" s="34">
+        <v>161397</v>
+      </c>
+      <c r="AD197" s="34">
+        <v>17992</v>
+      </c>
+      <c r="AE197" s="34">
+        <v>31564</v>
+      </c>
+      <c r="AF197" s="39">
+        <f>SUM(X197:AE197)</f>
+        <v>592034</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.699305555555556" right="0.699305555555556" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>